<commit_message>
Updated DIRECTION for Leukocytosis
</commit_message>
<xml_diff>
--- a/inst/adlb_grading/adlb_grading_spec.xlsx
+++ b/inst/adlb_grading/adlb_grading_spec.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\admiral\inst\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\admiral\inst\adlb_grading\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1459,8 +1459,8 @@
   </sheetPr>
   <dimension ref="A1:Z975"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1615,7 +1615,7 @@
         <v>4</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="M3" s="3"/>
       <c r="N3" s="5"/>

</xml_diff>

<commit_message>
More unit tests added for NCICTCv5
</commit_message>
<xml_diff>
--- a/inst/adlb_grading/adlb_grading_spec.xlsx
+++ b/inst/adlb_grading/adlb_grading_spec.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="310">
   <si>
     <t>Anemia</t>
   </si>
@@ -1211,36 +1211,6 @@
   <si>
     <t>case_when(
 is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
-(is.na(BASE) | BASE &lt;= ANRHI) &amp; AVAL &gt;  10*ANRHI ~ "4",
-(!is.na(BASE) &amp; BASE &gt; ANRHI) &amp; AVAL &gt;  10*BASE ~ "4",
-(is.na(BASE) | BASE &lt;= ANRHI) &amp; AVAL &gt;  3*ANRHI ~ "3",
-(!is.na(BASE) &amp; BASE &gt; ANRHI) &amp; AVAL &gt;  3*BASE ~ "3",
-(is.na(BASE) | BASE &lt;= ANRHI) &amp; AVAL &gt; 1.5*ANRHI ~ "2",
-(!is.na(BASE) &amp; BASE &gt; ANRHI) &amp; AVAL &gt;  1.5*BASE ~ "2",
-(is.na(BASE) ! BASE &lt;= ANRHI) &amp; AVAL &gt; ANRHI ~ "1",
-(!is.na(BASE) &amp; BASE &gt; ANRHI) &amp; AVAL &gt;  BASE ~ "1",
-(is.na(BASE) ! BASE &lt;= ANRHI) &amp; AVAL &lt;= ANRHI ~ "0",
-(!is.na(BASE) &amp; BASE &gt; ANRHI) &amp; AVAL &lt;= BASE ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
-(is.na(BASE) | BASE &lt;= ANRHI) &amp; AVAL &gt;  20*ANRHI ~ "4",
-(!is.na(BASE) &amp; BASE &gt; ANRHI) &amp; AVAL &gt;  20*BASE ~ "4",
-(is.na(BASE) | BASE &lt;= ANRHI) &amp; AVAL &gt;  5*ANRHI ~ "3",
-(!is.na(BASE) &amp; BASE &gt; ANRHI) &amp; AVAL &gt;  5*BASE ~ "3",
-(is.na(BASE) | BASE &lt;= ANRHI) &amp; AVAL &gt; 3*ANRHI ~ "2",
-(!is.na(BASE) &amp; BASE &gt; ANRHI) &amp; AVAL &gt;  3*BASE ~ "2",
-(is.na(BASE) ! BASE &lt;= ANRHI) &amp; AVAL &gt; ANRHI ~ "1",
-(!is.na(BASE) &amp; BASE &gt; ANRHI) &amp; AVAL &gt;=  1.5*BASE ~ "1",
-(is.na(BASE) ! BASE &lt;= ANRHI) &amp; AVAL &lt;= ANRHI ~ "0",
-(!is.na(BASE) &amp; BASE &gt; ANRHI) &amp; AVAL &lt;  1.5*BASE ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
 (is.na(BASE) | BASE &lt;= ANRHI) &amp; AVAL &gt;  20*ANRHI ~ "4",
 (!is.na(BASE) &amp; BASE &gt; ANRHI) &amp; AVAL &gt;  20*BASE ~ "4",
 (is.na(BASE) | BASE &lt;= ANRHI) &amp; AVAL &gt;  5*ANRHI ~ "3",
@@ -1342,6 +1312,21 @@
 is.na(ANRLO) ~ NA_character_,
 AVAL &lt; ANRLO ~ "1",
 AVAL &gt;= ANRLO ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
+(is.na(BASE) | BASE &lt;= ANRHI) &amp; AVAL &gt;  10*ANRHI ~ "4",
+(!is.na(BASE) &amp; BASE &gt; ANRHI) &amp; AVAL &gt;  10*BASE ~ "4",
+(is.na(BASE) | BASE &lt;= ANRHI) &amp; AVAL &gt;  3*ANRHI ~ "3",
+(!is.na(BASE) &amp; BASE &gt; ANRHI) &amp; AVAL &gt;  3*BASE ~ "3",
+(is.na(BASE) | BASE &lt;= ANRHI) &amp; AVAL &gt; 1.5*ANRHI ~ "2",
+(!is.na(BASE) &amp; BASE &gt; ANRHI) &amp; AVAL &gt;  1.5*BASE ~ "2",
+(is.na(BASE) | BASE &lt;= ANRHI) &amp; AVAL &gt; ANRHI ~ "1",
+(!is.na(BASE) &amp; BASE &gt; ANRHI) &amp; AVAL &gt;  BASE ~ "1",
+(is.na(BASE) | BASE &lt;= ANRHI) &amp; AVAL &lt;= ANRHI ~ "0",
+(!is.na(BASE) &amp; BASE &gt; ANRHI) &amp; AVAL &lt;= BASE ~ "0"
 )</t>
   </si>
 </sst>
@@ -24471,8 +24456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z972"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -24720,7 +24705,7 @@
         <v>25</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
@@ -24770,7 +24755,7 @@
         <v>30</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
@@ -24870,7 +24855,7 @@
         <v>38</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>289</v>
+        <v>309</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="4" t="s">
@@ -25310,10 +25295,10 @@
         <v>78</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E17" s="10" t="s">
         <v>81</v>
@@ -25328,7 +25313,7 @@
         <v>82</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J17" s="12"/>
       <c r="K17" s="4" t="s">
@@ -25365,13 +25350,13 @@
         <v>15</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G18" s="17" t="s">
         <v>188</v>
@@ -25390,7 +25375,7 @@
         <v>13</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="N18" s="28"/>
       <c r="O18" s="28"/>
@@ -25625,13 +25610,13 @@
         <v>15</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F23" s="24" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>188</v>
@@ -25650,7 +25635,7 @@
         <v>13</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
@@ -25837,7 +25822,7 @@
         <v>126</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E27" s="24" t="s">
         <v>128</v>
@@ -25941,7 +25926,7 @@
         <v>135</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E29" s="20" t="s">
         <v>137</v>
@@ -26042,16 +26027,16 @@
         <v>144</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D31" s="24" t="s">
         <v>215</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F31" s="22" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G31" s="19" t="s">
         <v>186</v>
@@ -26060,7 +26045,7 @@
         <v>222</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="J31" s="17" t="s">
         <v>253</v>
@@ -26311,7 +26296,7 @@
         <v>163</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E36" s="20" t="s">
         <v>165</v>
@@ -26338,7 +26323,7 @@
         <v>8</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
@@ -26417,10 +26402,10 @@
         <v>173</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F38" s="24" t="s">
         <v>175</v>
@@ -26432,7 +26417,7 @@
         <v>228</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J38" s="17" t="s">
         <v>230</v>
@@ -26444,7 +26429,7 @@
         <v>8</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>

</xml_diff>

<commit_message>
1560 Removed unit check for HYPERURICEMIA (version 5 only)
</commit_message>
<xml_diff>
--- a/inst/adlb_grading/adlb_grading_spec.xlsx
+++ b/inst/adlb_grading/adlb_grading_spec.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="310">
   <si>
     <t>Anemia</t>
   </si>
@@ -24456,8 +24456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z972"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -26047,9 +26047,7 @@
       <c r="I31" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="J31" s="17" t="s">
-        <v>253</v>
-      </c>
+      <c r="J31" s="17"/>
       <c r="K31" s="4" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
1859 metadata for DAIDs finalised
</commit_message>
<xml_diff>
--- a/inst/adlb_grading/adlb_grading_spec.xlsx
+++ b/inst/adlb_grading/adlb_grading_spec.xlsx
@@ -17,7 +17,7 @@
     <sheet name="DAIDS" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DAIDS!$J$1:$J$992</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DAIDS!$C$1:$C$992</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2238" uniqueCount="680">
   <si>
     <t>Anemia</t>
   </si>
@@ -1374,9 +1374,6 @@
     <t>&lt; 7.0 g/dL, &lt; 4.34 mmol/L</t>
   </si>
   <si>
-    <t>AVAL, sex, agecurr</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">9.5 to 10.4 g/dL, 5.88 to 6.48 </t>
     </r>
@@ -2019,13 +2016,6 @@
     <t>Assume worst case of "lifethreatening consequences (e.g., signs and symptoms of liver failure)"</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
-AVAL &gt;  ANRHI ~ "4",
-AVAL &lt;= ANRHI ~ "0"
-)</t>
-  </si>
-  <si>
     <t>&gt; 2 mg/dL</t>
   </si>
   <si>
@@ -2048,16 +2038,6 @@
   </si>
   <si>
     <t>1.1 - &lt;1.6 x ULN</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
-AVAL &gt;=  5*ANRHI ~ "4",
-AVAL &gt;=  2.6*ANRHI ~ "3",
-AVAL &gt;= 1.6*ANRHI ~ "2",
-AVAL &gt;= 1.1*ANRHI ~ "1",
-AVAL &lt; 1.1*ANRHI ~ "0"
-)</t>
   </si>
   <si>
     <t>Calcium (Ionized), High</t>
@@ -2093,30 +2073,10 @@
     <t>&gt;=13.5 mg/dL; &gt;=3.38 mmol/L</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &gt;= 3.38 ~ "4",
-AVAL &gt;= 3.13 ~ "3",
-AVAL &gt;= 2.88 ~ "2",
-AVAL &gt;= 2.65 ~ "1",
-AVAL &lt; 2.65 ~ "0"
-)</t>
-  </si>
-  <si>
     <t>&lt; 7 days of age</t>
   </si>
   <si>
     <t>12.9 - &lt;13.5 mg/dL; 3.23 - &lt;3.38 mmol/L</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &gt;= 3.38 ~ "4",
-AVAL &gt;= 3.23 ~ "3",
-AVAL &gt;= 3.1 ~ "2",
-AVAL &gt;= 2.88 ~ "1",
-AVAL &lt; 2.88 ~ "0"
-)</t>
   </si>
   <si>
     <t>Calcium, Low</t>
@@ -2135,16 +2095,6 @@
   </si>
   <si>
     <t>&lt; 3.2 mg/dL; &lt; 0.8 mmol/L</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &lt; 1.53 ~ "4",
-AVAL &lt; 1.75 ~ "3",
-AVAL &lt; 1.95 ~ "2",
-AVAL &lt; 2.1 ~ "1",
-AVAL &gt;= 2.1 ~ "0"
-)</t>
   </si>
   <si>
     <t>7.8 to &lt; 8.4 mg/dL; 1.95 to &lt; 2.10 mmol/L</t>
@@ -2169,16 +2119,6 @@
   </si>
   <si>
     <t>&lt; 5.50 mg/dL; &lt; 1.38 mmol/L</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &lt; 1.38 ~ "4",
-AVAL &lt; 1.5 ~ "3",
-AVAL &lt; 1.63 ~ "2",
-AVAL &lt; 1.88 ~ "1",
-AVAL &gt;= 1.88 ~ "0"
-)</t>
   </si>
   <si>
     <t>Creatine Kinase, High</t>
@@ -2277,30 +2217,10 @@
     <t>&lt; 30 mg/dL; &lt; 1.67 mmol/L</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &lt; 1.67 ~ "4",
-AVAL &lt; 2.22 ~ "3",
-AVAL &lt; 3.05 ~ "2",
-AVAL &lt; 3.55 ~ "1",
-AVAL &gt;= 3.55 ~ "0"
-)</t>
-  </si>
-  <si>
     <t>&lt; 1 month of age</t>
   </si>
   <si>
     <t>40 to &lt; 50 mg/dL; 2.22 to &lt; 2.78 mmol/L</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &lt; 1.67 ~ "4",
-AVAL &lt; 2.22 ~ "3",
-AVAL &lt; 2.78 ~ "2",
-AVAL &lt; 3 ~ "1",
-AVAL &gt;= 3 ~ "0"
-)</t>
   </si>
   <si>
     <t>50 to 54 mg/dL; 2.78 to &lt;3.00 mmol/L</t>
@@ -2329,9 +2249,6 @@
 AVAL &gt;= ANRHI ~ "1",
 AVAL &lt; ANRHI ~ "0"
 )</t>
-  </si>
-  <si>
-    <t>AVAL, ANRHI, agecurr</t>
   </si>
   <si>
     <t>Assume "without acidosis" (only grade 1 and 2)</t>
@@ -2364,15 +2281,6 @@
     <t>200 to &lt; 240 mg/dL; 5.18 to &lt; 6.19 mmol/L</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &gt;= 7.77 ~ "3",
-AVAL &gt;= 6.19 ~ "2",
-AVAL &gt;= 5.18 ~ "1",
-AVAL &lt; 5.18 ~ "0"
-)</t>
-  </si>
-  <si>
     <t>&lt;18 years of age</t>
   </si>
   <si>
@@ -2380,15 +2288,6 @@
   </si>
   <si>
     <t>170 to &lt; 200 mg/dL; 4.4 to &lt; 5.15 mmol/L</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &gt;= 7.77 ~ "3",
-AVAL &gt;= 5.15 ~ "2",
-AVAL &gt;= 4.14 ~ "1",
-AVAL &lt; 4.14 ~ "0"
-)</t>
   </si>
   <si>
     <t>LDL, Fasting, High</t>
@@ -2403,15 +2302,6 @@
     <t>≥ 190 mg/dL; ≥ 4.90 mmol/L</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &gt;= 4.9 ~ "3",
-AVAL &gt;= 4.12 ~ "2",
-AVAL &gt;= 3.37 ~ "1",
-AVAL &lt; 3.37 ~ "0"
-)</t>
-  </si>
-  <si>
     <t>&gt; 2 to &lt; 18 years of age</t>
   </si>
   <si>
@@ -2419,15 +2309,6 @@
   </si>
   <si>
     <t>130 to &lt; 190 mg/dL; 3.34 to &lt; 4.90 mmol/L</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &gt;= 4.9 ~ "3",
-AVAL &gt;= 3.34 ~ "2",
-AVAL &gt;= 2.85 ~ "1",
-AVAL &lt; 2.85 ~ "0"
-)</t>
   </si>
   <si>
     <t>Triglycerides, Fasting, High</t>
@@ -2476,21 +2357,7 @@
     <t>&gt; 14 years of age</t>
   </si>
   <si>
-    <t>AVAL, ANRLO, agecurr</t>
-  </si>
-  <si>
     <t>2.0 mg/dL to &lt; LLN; 0.65 mmol/L to &lt; LLN</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &lt; 0.32 ~ "4",
-AVAL &lt; 0.45 ~ "3",
-AVAL &lt; 0.65 ~ "2",
-is.na(ANRLO) ~ NA_character_,
-AVAL &lt; ANRLO ~ "1",
-AVAL &gt;= ANRLO ~ "0"
-)</t>
   </si>
   <si>
     <t>1.4 to &lt; 2.0 mg/dL; 0.45 to &lt; 0.65 mmol/L</t>
@@ -2517,16 +2384,6 @@
     <t>3.0 to &lt; 3.5 mg/dL; 0.97 to &lt; 1.13 mmol/L</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &lt; 0.48 ~ "4",
-AVAL &lt; 0.81 ~ "3",
-AVAL &lt; 0.97 ~ "2",
-AVAL &lt; 1.13 ~ "1",
-AVAL &gt;= 1.13 ~ "0"
-)</t>
-  </si>
-  <si>
     <t>&lt; 1 year of age</t>
   </si>
   <si>
@@ -2534,16 +2391,6 @@
   </si>
   <si>
     <t>3.5 to &lt; 4.5 mg/dL; 1.13 to &lt; 1.45 mmol/L</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &lt; 0.48 ~ "4",
-AVAL &lt; 0.81 ~ "3",
-AVAL &lt; 1.13 ~ "2",
-AVAL &lt; 1.45 ~ "1",
-AVAL &gt;= 1.45 ~ "0"
-)</t>
   </si>
   <si>
     <t>Potassium, Low</t>
@@ -2691,17 +2538,6 @@
 )</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL*0.05848 &gt;  2 ~ "4",
-AVAL*0.05848 &gt;  1.5 ~ "3",
-AVAL*0.05848 &gt;  1 ~ "2",
-is.na(ANRHI) ~ NA_character_,
-AVAL &gt;= ANRHI ~ "1",
-AVAL &lt; ANRHI ~ "0"
-)</t>
-  </si>
-  <si>
     <t>0.05848 used as conversion from "umol/L" to "mg/dL"</t>
   </si>
   <si>
@@ -2729,45 +2565,6 @@
   </si>
   <si>
     <t>&gt;= 500 mg/dL &gt;= 27.75 mmol/L</t>
-  </si>
-  <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "months", add_one = FALSE) &lt; 1</t>
-  </si>
-  <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "months", add_one = FALSE) &gt;= 1</t>
-  </si>
-  <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &gt; 28</t>
-  </si>
-  <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &lt;= 28</t>
-  </si>
-  <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &gt;= 7</t>
-  </si>
-  <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &lt; 7</t>
-  </si>
-  <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &gt;= 18</t>
-  </si>
-  <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &lt; 18</t>
-  </si>
-  <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &gt; 14</t>
-  </si>
-  <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &lt; 1</t>
-  </si>
-  <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &gt; 5</t>
-  </si>
-  <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &gt; 7</t>
-  </si>
-  <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &lt;= 1</t>
   </si>
   <si>
     <t>300 to &lt;400/mm3; 0.30 to &lt;0.40 x 10^9 /L</t>
@@ -2815,40 +2612,389 @@
     <t>1500 to 2999/mm3; 1.500 to 2.999 x 10e9 /L</t>
   </si>
   <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &lt; 13 &amp; compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &gt;= 57</t>
-  </si>
-  <si>
-    <t>SEX == "F" &amp; compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &gt;= 13</t>
-  </si>
-  <si>
-    <t>SEX == "M" &amp; compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &gt;= 13</t>
-  </si>
-  <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &lt;= 7</t>
-  </si>
-  <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &lt;= 21 &amp; compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &gt;= 8</t>
-  </si>
-  <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &lt;= 56 &amp; compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &gt;= 36</t>
-  </si>
-  <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &lt;= 35 &amp; compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &gt;= 22</t>
-  </si>
-  <si>
     <t>1.5 - &lt;2.0 x ULN</t>
   </si>
   <si>
     <t>2.0 - &lt;3.0 x ULN</t>
   </si>
   <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &gt; 2 &amp; compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &lt; 18</t>
+    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &gt; 28 | is.na(BRTHDT) | is.na(LBDT)</t>
   </si>
   <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &gt;= 1 &amp; compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &lt; 14</t>
+    <t>case_when(
+is.na(AVAL) | is.na(ANRHI) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &gt;  ANRHI ~ "4",
+AVAL &lt;= ANRHI ~ "0"
+)</t>
   </si>
   <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &gt;= 2 &amp; compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &lt;= 7</t>
+    <t>AVAL, ANRHI, LBDT, BRTHDT</t>
+  </si>
+  <si>
+    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &lt;= 28 | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL*0.05848 &gt;  2 ~ "4",
+AVAL*0.05848 &gt;  1.5 ~ "3",
+AVAL*0.05848 &gt;  1 ~ "2",
+is.na(ANRHI) ~ NA_character_,
+AVAL &gt;= ANRHI ~ "1",
+AVAL &lt; ANRHI ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &gt;= 7 | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &lt; 7 | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(ANRHI) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &gt;=  5*ANRHI ~ "4",
+AVAL &gt;=  2.6*ANRHI ~ "3",
+AVAL &gt;= 1.6*ANRHI ~ "2",
+AVAL &gt;= 1.1*ANRHI ~ "1",
+AVAL &lt; 1.1*ANRHI ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &gt;= 3.38 ~ "4",
+AVAL &gt;= 3.13 ~ "3",
+AVAL &gt;= 2.88 ~ "2",
+AVAL &gt;= 2.65 ~ "1",
+AVAL &lt; 2.65 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &gt;= 3.38 ~ "4",
+AVAL &gt;= 3.23 ~ "3",
+AVAL &gt;= 3.1 ~ "2",
+AVAL &gt;= 2.88 ~ "1",
+AVAL &lt; 2.88 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &lt; 1.53 ~ "4",
+AVAL &lt; 1.75 ~ "3",
+AVAL &lt; 1.95 ~ "2",
+AVAL &lt; 2.1 ~ "1",
+AVAL &gt;= 2.1 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>AVAL, LBDT, BRTHDT</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &lt; 1.38 ~ "4",
+AVAL &lt; 1.5 ~ "3",
+AVAL &lt; 1.63 ~ "2",
+AVAL &lt; 1.88 ~ "1",
+AVAL &gt;= 1.88 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &lt; 1.67 ~ "4",
+AVAL &lt; 2.22 ~ "3",
+AVAL &lt; 3.05 ~ "2",
+AVAL &lt; 3.55 ~ "1",
+AVAL &gt;= 3.55 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &lt; 1.67 ~ "4",
+AVAL &lt; 2.22 ~ "3",
+AVAL &lt; 2.78 ~ "2",
+AVAL &lt; 3 ~ "1",
+AVAL &gt;= 3 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>AVAL, BRTHDT, LBDT</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &gt;= 7.77 ~ "3",
+AVAL &gt;= 6.19 ~ "2",
+AVAL &gt;= 5.18 ~ "1",
+AVAL &lt; 5.18 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &gt;= 7.77 ~ "3",
+AVAL &gt;= 5.15 ~ "2",
+AVAL &gt;= 4.14 ~ "1",
+AVAL &lt; 4.14 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &gt;= 4.9 ~ "3",
+AVAL &gt;= 4.12 ~ "2",
+AVAL &gt;= 3.37 ~ "1",
+AVAL &lt; 3.37 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &gt;= 4.9 ~ "3",
+AVAL &gt;= 3.34 ~ "2",
+AVAL &gt;= 2.85 ~ "1",
+AVAL &lt; 2.85 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &lt; 0.32 ~ "4",
+AVAL &lt; 0.45 ~ "3",
+AVAL &lt; 0.65 ~ "2",
+is.na(ANRLO) ~ NA_character_,
+AVAL &lt; ANRLO ~ "1",
+AVAL &gt;= ANRLO ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &lt; 0.48 ~ "4",
+AVAL &lt; 0.81 ~ "3",
+AVAL &lt; 0.97 ~ "2",
+AVAL &lt; 1.13 ~ "1",
+AVAL &gt;= 1.13 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &lt; 0.48 ~ "4",
+AVAL &lt; 0.81 ~ "3",
+AVAL &lt; 1.13 ~ "2",
+AVAL &lt; 1.45 ~ "1",
+AVAL &gt;= 1.45 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "months", add_one = FALSE) &gt;= 1 | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "months", add_one = FALSE) &lt; 1 | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &gt;= 18 | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &lt; 18 | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>(compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &gt; 2 &amp; compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &lt; 18)  | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &gt; 14 | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>(compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &gt;= 1 &amp; compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &lt; 14) | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &lt; 1 | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &gt; 5 | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &gt; 7 | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>(compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &gt;= 2 &amp; compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &lt;= 7) | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &lt;= 1 | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>(SEX == "M" | is.na(SEX)) &amp; (compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &gt;= 13 | is.na(BRTHDT) | is.na(LBDT))</t>
+  </si>
+  <si>
+    <t>(SEX == "F" | is.na(SEX)) &amp; (compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &gt;= 13 | is.na(BRTHDT) | is.na(LBDT))</t>
+  </si>
+  <si>
+    <t>(compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &lt; 13 &amp; compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &gt;= 57) | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>(compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &lt;= 56 &amp; compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &gt;= 36) | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>(compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &lt;= 35 &amp; compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &gt;= 22) | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>(compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &lt;= 21 &amp; compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &gt;= 8) | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &lt;= 7 | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>AVAL, ANRLO, LBDT, BRTHDT</t>
+  </si>
+  <si>
+    <t>AVAL, SEX, LBDT, BRTHDT</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &lt; 0.1 ~ "4",
+AVAL &lt; 0.2 ~ "3",
+AVAL &lt; 0.3 ~ "2",
+AVAL &lt; 0.4 ~ "1",
+AVAL &gt;= 0.4 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &lt; 0.35 ~ "4",
+AVAL &lt; 0.5 ~ "3",
+AVAL &lt; 0.6 ~ "2",
+AVAL &lt; 0.65 ~ "1",
+AVAL &gt;= 0.65 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &lt; 0.4 ~ "4",
+AVAL &lt; 0.6 ~ "3",
+AVAL &lt; 0.8 ~ "2",
+AVAL &lt;= 1 ~ "1",
+AVAL &gt; 1 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &lt; 0.75 ~ "4",
+AVAL &lt; 1 ~ "3",
+AVAL &lt; 1.25 ~ "2",
+AVAL &lt;= 1.5 ~ "1",
+AVAL &gt; 1.5 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &lt; 1.5 ~ "4",
+AVAL &lt; 3 ~ "3",
+AVAL &lt; 4 ~ "2",
+AVAL &lt;= 5 ~ "1",
+AVAL &gt; 5 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(SEX) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &lt; 70 ~ "4",
+AVAL &lt; 90 ~ "3",
+AVAL &lt; 100 ~ "2",
+AVAL &lt;= 109 ~ "1",
+AVAL &gt; 109 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(SEX)  | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &lt; 65 ~ "4",
+AVAL &lt; 85 ~ "3",
+AVAL &lt; 95 ~ "2",
+AVAL &lt;= 104 ~ "1",
+AVAL &gt; 104 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &lt; 65 ~ "4",
+AVAL &lt; 85 ~ "3",
+AVAL &lt; 95 ~ "2",
+AVAL &lt;= 104 ~ "1",
+AVAL &gt; 104 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &lt; 60 ~ "4",
+AVAL &lt; 70 ~ "3",
+AVAL &lt; 85 ~ "2",
+AVAL &lt;= 96 ~ "1",
+AVAL &gt; 96 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &lt; 67 ~ "4",
+AVAL &lt; 80 ~ "3",
+AVAL &lt; 95 ~ "2",
+AVAL &lt;= 110 ~ "1",
+AVAL &gt; 110 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &lt; 80 ~ "4",
+AVAL &lt; 90 ~ "3",
+AVAL &lt; 110 ~ "2",
+AVAL &lt;= 130 ~ "1",
+AVAL &gt; 130 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &lt; 90 ~ "4",
+AVAL &lt; 100 ~ "3",
+AVAL &lt; 130 ~ "2",
+AVAL &lt;= 140 ~ "1",
+AVAL &gt; 140 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &lt; 1 ~ "4",
+AVAL &lt; 1.5 ~ "3",
+AVAL &lt; 2 ~ "2",
+AVAL &lt; 2.5 ~ "1",
+AVAL &gt;= 2.5 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &lt; 2.5 ~ "4",
+AVAL &lt; 4 ~ "3",
+AVAL &lt; 5.5 ~ "2",
+AVAL &lt; 7 ~ "1",
+AVAL &gt;= 7 ~ "0"
+)</t>
   </si>
 </sst>
 </file>
@@ -48569,8 +48715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB992"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -48594,7 +48740,7 @@
         <v>201</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>614</v>
+        <v>596</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>261</v>
@@ -48648,27 +48794,27 @@
     </row>
     <row r="2" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E2" t="s">
+        <v>426</v>
+      </c>
+      <c r="F2" t="s">
         <v>427</v>
-      </c>
-      <c r="F2" t="s">
-        <v>428</v>
       </c>
       <c r="G2" s="32"/>
       <c r="H2" s="10"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="8" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>2</v>
@@ -48696,29 +48842,29 @@
     </row>
     <row r="3" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
+        <v>418</v>
+      </c>
+      <c r="B3" t="s">
         <v>419</v>
-      </c>
-      <c r="B3" t="s">
-        <v>420</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="31" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F3" s="32" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G3" s="32" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H3" s="10"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="8" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="4" t="s">
@@ -48744,29 +48890,29 @@
     </row>
     <row r="4" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="8" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4" t="s">
@@ -48792,29 +48938,29 @@
     </row>
     <row r="5" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="33" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E5" s="34" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F5" s="33" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L5" s="12"/>
       <c r="M5" s="4" t="s">
@@ -48840,29 +48986,29 @@
     </row>
     <row r="6" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="8" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4" t="s">
@@ -48888,29 +49034,29 @@
     </row>
     <row r="7" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B7" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="8" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="L7" s="4" t="s">
         <v>46</v>
@@ -48936,43 +49082,43 @@
       <c r="AA7" s="5"/>
       <c r="AB7" s="5"/>
     </row>
-    <row r="8" spans="1:28" s="44" customFormat="1" ht="63.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" s="44" customFormat="1" ht="76" x14ac:dyDescent="0.35">
       <c r="A8" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B8" s="37" t="s">
+        <v>445</v>
+      </c>
+      <c r="C8" s="37" t="s">
         <v>446</v>
-      </c>
-      <c r="C8" s="37" t="s">
-        <v>447</v>
       </c>
       <c r="D8" s="32"/>
       <c r="E8" s="32"/>
       <c r="F8" s="37" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G8" s="32" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="H8" s="36" t="s">
         <v>188</v>
       </c>
       <c r="I8" s="38"/>
       <c r="J8" s="38" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="K8" s="39" t="s">
-        <v>452</v>
+        <v>623</v>
       </c>
       <c r="L8" s="40"/>
       <c r="M8" s="4" t="s">
-        <v>529</v>
+        <v>624</v>
       </c>
       <c r="N8" s="41" t="s">
         <v>13</v>
       </c>
       <c r="O8" s="37" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P8" s="43"/>
       <c r="Q8" s="43"/>
@@ -48988,46 +49134,46 @@
       <c r="AA8" s="43"/>
       <c r="AB8" s="43"/>
     </row>
-    <row r="9" spans="1:28" s="44" customFormat="1" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" s="44" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A9" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F9" s="32" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="G9" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="H9"/>
       <c r="J9" s="38" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="K9" s="39" t="s">
-        <v>617</v>
+        <v>626</v>
       </c>
       <c r="L9" s="40" t="s">
-        <v>615</v>
+        <v>597</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>529</v>
+        <v>624</v>
       </c>
       <c r="N9" s="41" t="s">
         <v>13</v>
       </c>
       <c r="O9" s="42" t="s">
-        <v>618</v>
+        <v>599</v>
       </c>
       <c r="P9" s="43"/>
       <c r="Q9" s="43"/>
@@ -49043,41 +49189,41 @@
       <c r="AA9" s="43"/>
       <c r="AB9" s="43"/>
     </row>
-    <row r="10" spans="1:28" s="44" customFormat="1" ht="101" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" s="44" customFormat="1" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A10" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B10" t="s">
+        <v>455</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>446</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>458</v>
+      </c>
+      <c r="E10" s="34" t="s">
         <v>457</v>
       </c>
-      <c r="C10" s="37" t="s">
-        <v>447</v>
-      </c>
-      <c r="D10" s="33" t="s">
-        <v>460</v>
-      </c>
-      <c r="E10" s="34" t="s">
-        <v>459</v>
-      </c>
       <c r="F10" s="33" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="G10" s="33" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H10" s="36" t="s">
         <v>188</v>
       </c>
       <c r="I10" s="38"/>
       <c r="J10" s="38" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>461</v>
+        <v>629</v>
       </c>
       <c r="L10" s="40"/>
       <c r="M10" s="4" t="s">
-        <v>529</v>
+        <v>624</v>
       </c>
       <c r="N10" s="41" t="s">
         <v>13</v>
@@ -49097,41 +49243,41 @@
       <c r="AA10" s="43"/>
       <c r="AB10" s="43"/>
     </row>
-    <row r="11" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A11" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B11" s="15" t="s">
+        <v>464</v>
+      </c>
+      <c r="C11" t="s">
+        <v>465</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>466</v>
+      </c>
+      <c r="E11" s="19" t="s">
         <v>467</v>
       </c>
-      <c r="C11" t="s">
+      <c r="F11" s="19" t="s">
         <v>468</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="G11" s="19" t="s">
         <v>469</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>470</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>471</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>472</v>
       </c>
       <c r="H11" s="19"/>
       <c r="I11" s="18"/>
       <c r="J11" s="38" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>473</v>
+        <v>630</v>
       </c>
       <c r="L11" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>325</v>
+        <v>633</v>
       </c>
       <c r="N11" s="4" t="s">
         <v>13</v>
@@ -49151,41 +49297,41 @@
       <c r="AA11" s="5"/>
       <c r="AB11" s="5"/>
     </row>
-    <row r="12" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A12" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="C12" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>620</v>
+        <v>601</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>619</v>
+        <v>600</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="G12" s="19" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="H12" s="19"/>
       <c r="I12" s="18"/>
       <c r="J12" s="38" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>476</v>
+        <v>631</v>
       </c>
       <c r="L12" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>325</v>
+        <v>633</v>
       </c>
       <c r="N12" s="4" t="s">
         <v>13</v>
@@ -49207,29 +49353,29 @@
     </row>
     <row r="13" spans="1:28" ht="113" x14ac:dyDescent="0.3">
       <c r="A13" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="19" t="s">
+        <v>460</v>
+      </c>
+      <c r="E13" s="19" t="s">
         <v>463</v>
       </c>
-      <c r="E13" s="19" t="s">
-        <v>466</v>
-      </c>
       <c r="F13" s="19" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="H13" s="19"/>
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
       <c r="K13" s="1" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="L13" s="14" t="s">
         <v>46</v>
@@ -49255,41 +49401,41 @@
       <c r="AA13" s="5"/>
       <c r="AB13" s="5"/>
     </row>
-    <row r="14" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A14" s="45" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B14" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="C14" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="D14" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="E14" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="F14" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="G14" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="H14" s="19"/>
       <c r="I14" s="18"/>
       <c r="J14" s="38" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>483</v>
+        <v>632</v>
       </c>
       <c r="L14" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>325</v>
+        <v>633</v>
       </c>
       <c r="N14" s="4" t="s">
         <v>8</v>
@@ -49309,41 +49455,41 @@
       <c r="AA14" s="5"/>
       <c r="AB14" s="5"/>
     </row>
-    <row r="15" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A15" s="45" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B15" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="C15" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="D15" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="E15" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="F15" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="G15" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="18"/>
       <c r="J15" s="38" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>492</v>
+        <v>634</v>
       </c>
       <c r="L15" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>325</v>
+        <v>633</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>8</v>
@@ -49365,23 +49511,23 @@
     </row>
     <row r="16" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A16" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B16" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="E16" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="F16" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="G16" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="18"/>
@@ -49415,29 +49561,29 @@
     </row>
     <row r="17" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A17" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B17" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="H17" s="10"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="1" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="L17" s="12"/>
       <c r="M17" s="4" t="s">
@@ -49463,29 +49609,29 @@
     </row>
     <row r="18" spans="1:28" ht="151" x14ac:dyDescent="0.35">
       <c r="A18" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B18" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="E18" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
       <c r="F18" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
       <c r="G18" t="s">
-        <v>621</v>
+        <v>602</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="1" t="s">
-        <v>622</v>
+        <v>603</v>
       </c>
       <c r="L18" s="12"/>
       <c r="M18" s="4" t="s">
@@ -49511,29 +49657,29 @@
     </row>
     <row r="19" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A19" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B19" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
       <c r="E19" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="F19" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="G19" t="s">
-        <v>623</v>
+        <v>604</v>
       </c>
       <c r="H19" s="20"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="1" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="L19" s="14" t="s">
         <v>46</v>
@@ -49561,29 +49707,29 @@
     </row>
     <row r="20" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A20" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B20" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="C20" s="16"/>
       <c r="D20" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
       <c r="E20" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="F20" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="G20" t="s">
-        <v>623</v>
+        <v>604</v>
       </c>
       <c r="H20" s="20"/>
       <c r="I20" s="18"/>
       <c r="J20" s="18"/>
       <c r="K20" s="1" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
       <c r="L20" s="14" t="s">
         <v>46</v>
@@ -49609,41 +49755,41 @@
       <c r="AA20" s="5"/>
       <c r="AB20" s="5"/>
     </row>
-    <row r="21" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A21" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B21" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
       <c r="C21" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
       <c r="D21" t="s">
-        <v>514</v>
+        <v>507</v>
       </c>
       <c r="E21" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
       <c r="F21" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
       <c r="G21" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
       <c r="H21" s="20"/>
       <c r="I21" s="18"/>
       <c r="J21" s="38" t="s">
-        <v>625</v>
+        <v>645</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>518</v>
+        <v>635</v>
       </c>
       <c r="L21" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>325</v>
+        <v>637</v>
       </c>
       <c r="N21" s="4" t="s">
         <v>8</v>
@@ -49663,41 +49809,41 @@
       <c r="AA21" s="5"/>
       <c r="AB21" s="5"/>
     </row>
-    <row r="22" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A22" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B22" t="s">
+        <v>505</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>511</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>513</v>
+      </c>
+      <c r="E22" s="30" t="s">
         <v>512</v>
       </c>
-      <c r="C22" s="30" t="s">
-        <v>519</v>
-      </c>
-      <c r="D22" s="30" t="s">
-        <v>522</v>
-      </c>
-      <c r="E22" s="30" t="s">
-        <v>520</v>
-      </c>
       <c r="F22" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
       <c r="G22" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="18"/>
       <c r="J22" s="38" t="s">
-        <v>624</v>
+        <v>646</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>521</v>
+        <v>636</v>
       </c>
       <c r="L22" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>325</v>
+        <v>637</v>
       </c>
       <c r="N22" s="4" t="s">
         <v>8</v>
@@ -49719,28 +49865,28 @@
     </row>
     <row r="23" spans="1:28" ht="87" x14ac:dyDescent="0.35">
       <c r="A23" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>523</v>
+        <v>514</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>524</v>
+        <v>515</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>525</v>
+        <v>516</v>
       </c>
       <c r="F23" s="35" t="s">
-        <v>526</v>
+        <v>517</v>
       </c>
       <c r="G23" s="30" t="s">
-        <v>527</v>
+        <v>518</v>
       </c>
       <c r="H23" s="20"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="K23" s="1" t="s">
-        <v>528</v>
+        <v>519</v>
       </c>
       <c r="L23" s="14" t="s">
         <v>46</v>
@@ -49752,7 +49898,7 @@
         <v>13</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>530</v>
+        <v>520</v>
       </c>
       <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
@@ -49770,29 +49916,29 @@
     </row>
     <row r="24" spans="1:28" s="29" customFormat="1" ht="101" x14ac:dyDescent="0.35">
       <c r="A24" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>531</v>
+        <v>521</v>
       </c>
       <c r="C24" s="17"/>
       <c r="D24" s="30" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>533</v>
+        <v>523</v>
       </c>
       <c r="F24" s="33" t="s">
-        <v>532</v>
+        <v>522</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H24" s="17"/>
       <c r="I24" s="17"/>
       <c r="J24" s="17"/>
       <c r="K24" s="26" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L24" s="27"/>
       <c r="M24" s="27" t="s">
@@ -49816,39 +49962,39 @@
       <c r="AA24" s="28"/>
       <c r="AB24" s="28"/>
     </row>
-    <row r="25" spans="1:28" ht="88.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A25" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B25" t="s">
-        <v>535</v>
+        <v>525</v>
       </c>
       <c r="C25" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>539</v>
+        <v>529</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>538</v>
+        <v>528</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>537</v>
+        <v>527</v>
       </c>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
       <c r="I25" s="7"/>
       <c r="J25" s="38" t="s">
-        <v>630</v>
+        <v>647</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>540</v>
+        <v>638</v>
       </c>
       <c r="L25" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>325</v>
+        <v>637</v>
       </c>
       <c r="N25" s="4" t="s">
         <v>13</v>
@@ -49868,39 +50014,39 @@
       <c r="AA25" s="5"/>
       <c r="AB25" s="5"/>
     </row>
-    <row r="26" spans="1:28" ht="88.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A26" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B26" t="s">
-        <v>535</v>
+        <v>525</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>541</v>
+        <v>530</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>543</v>
+        <v>532</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>542</v>
+        <v>531</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>537</v>
+        <v>527</v>
       </c>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
       <c r="I26" s="7"/>
       <c r="J26" s="38" t="s">
-        <v>631</v>
+        <v>648</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>544</v>
+        <v>639</v>
       </c>
       <c r="L26" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>325</v>
+        <v>637</v>
       </c>
       <c r="N26" s="4" t="s">
         <v>13</v>
@@ -49920,39 +50066,39 @@
       <c r="AA26" s="5"/>
       <c r="AB26" s="5"/>
     </row>
-    <row r="27" spans="1:28" ht="88.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A27" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>545</v>
+        <v>533</v>
       </c>
       <c r="C27" t="s">
+        <v>526</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>534</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>535</v>
+      </c>
+      <c r="F27" s="30" t="s">
         <v>536</v>
-      </c>
-      <c r="D27" s="30" t="s">
-        <v>546</v>
-      </c>
-      <c r="E27" s="30" t="s">
-        <v>547</v>
-      </c>
-      <c r="F27" s="30" t="s">
-        <v>548</v>
       </c>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
       <c r="I27" s="7"/>
       <c r="J27" s="38" t="s">
-        <v>630</v>
+        <v>647</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>549</v>
+        <v>640</v>
       </c>
       <c r="L27" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>325</v>
+        <v>637</v>
       </c>
       <c r="N27" s="4" t="s">
         <v>13</v>
@@ -49972,39 +50118,39 @@
       <c r="AA27" s="5"/>
       <c r="AB27" s="5"/>
     </row>
-    <row r="28" spans="1:28" ht="88.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A28" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>545</v>
+        <v>533</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>550</v>
+        <v>537</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>551</v>
+        <v>538</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>552</v>
+        <v>539</v>
       </c>
       <c r="F28" s="30" t="s">
-        <v>548</v>
+        <v>536</v>
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
       <c r="I28" s="7"/>
       <c r="J28" s="38" t="s">
-        <v>661</v>
+        <v>649</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>553</v>
+        <v>641</v>
       </c>
       <c r="L28" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>325</v>
+        <v>637</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>13</v>
@@ -50026,23 +50172,23 @@
     </row>
     <row r="29" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A29" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B29" s="30" t="s">
-        <v>554</v>
+        <v>540</v>
       </c>
       <c r="C29" s="16"/>
       <c r="D29" s="30" t="s">
-        <v>555</v>
+        <v>541</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>556</v>
+        <v>542</v>
       </c>
       <c r="F29" s="30" t="s">
-        <v>557</v>
+        <v>543</v>
       </c>
       <c r="G29" s="30" t="s">
-        <v>558</v>
+        <v>544</v>
       </c>
       <c r="H29" s="20"/>
       <c r="I29" s="18"/>
@@ -50076,29 +50222,29 @@
     </row>
     <row r="30" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A30" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>559</v>
+        <v>545</v>
       </c>
       <c r="C30" s="16"/>
       <c r="D30" s="30" t="s">
-        <v>560</v>
+        <v>546</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>561</v>
+        <v>547</v>
       </c>
       <c r="F30" s="30" t="s">
-        <v>562</v>
+        <v>548</v>
       </c>
       <c r="G30" s="30" t="s">
-        <v>563</v>
+        <v>549</v>
       </c>
       <c r="H30" s="20"/>
       <c r="I30" s="18"/>
       <c r="J30" s="18"/>
       <c r="K30" s="1" t="s">
-        <v>564</v>
+        <v>550</v>
       </c>
       <c r="L30" s="14" t="s">
         <v>46</v>
@@ -50124,41 +50270,41 @@
       <c r="AA30" s="5"/>
       <c r="AB30" s="5"/>
     </row>
-    <row r="31" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:28" ht="126" x14ac:dyDescent="0.35">
       <c r="A31" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>565</v>
+        <v>551</v>
       </c>
       <c r="C31" s="30" t="s">
-        <v>566</v>
+        <v>552</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>570</v>
+        <v>554</v>
       </c>
       <c r="F31" s="30" t="s">
-        <v>571</v>
+        <v>555</v>
       </c>
       <c r="G31" s="30" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="H31" s="20"/>
       <c r="I31" s="18"/>
       <c r="J31" s="38" t="s">
-        <v>632</v>
+        <v>650</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>569</v>
+        <v>642</v>
       </c>
       <c r="L31" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>567</v>
+        <v>664</v>
       </c>
       <c r="N31" s="4" t="s">
         <v>8</v>
@@ -50178,41 +50324,41 @@
       <c r="AA31" s="5"/>
       <c r="AB31" s="5"/>
     </row>
-    <row r="32" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A32" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>565</v>
+        <v>551</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>573</v>
+        <v>557</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>577</v>
+        <v>561</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>576</v>
+        <v>560</v>
       </c>
       <c r="F32" s="30" t="s">
-        <v>575</v>
+        <v>559</v>
       </c>
       <c r="G32" s="30" t="s">
-        <v>574</v>
+        <v>558</v>
       </c>
       <c r="H32" s="20"/>
       <c r="I32" s="18"/>
       <c r="J32" s="38" t="s">
-        <v>662</v>
+        <v>651</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>578</v>
+        <v>643</v>
       </c>
       <c r="L32" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>567</v>
+        <v>664</v>
       </c>
       <c r="N32" s="4" t="s">
         <v>8</v>
@@ -50232,41 +50378,41 @@
       <c r="AA32" s="5"/>
       <c r="AB32" s="5"/>
     </row>
-    <row r="33" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A33" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>565</v>
+        <v>551</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>579</v>
+        <v>562</v>
       </c>
       <c r="D33" s="30" t="s">
-        <v>581</v>
+        <v>564</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>580</v>
+        <v>563</v>
       </c>
       <c r="F33" s="30" t="s">
-        <v>575</v>
+        <v>559</v>
       </c>
       <c r="G33" s="30" t="s">
-        <v>574</v>
+        <v>558</v>
       </c>
       <c r="H33" s="20"/>
       <c r="I33" s="18"/>
       <c r="J33" s="38" t="s">
-        <v>633</v>
+        <v>652</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>582</v>
+        <v>644</v>
       </c>
       <c r="L33" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>567</v>
+        <v>664</v>
       </c>
       <c r="N33" s="4" t="s">
         <v>8</v>
@@ -50288,29 +50434,29 @@
     </row>
     <row r="34" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A34" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>589</v>
+        <v>571</v>
       </c>
       <c r="C34" s="30"/>
       <c r="D34" s="30" t="s">
-        <v>593</v>
+        <v>575</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>592</v>
+        <v>574</v>
       </c>
       <c r="F34" s="30" t="s">
-        <v>591</v>
+        <v>573</v>
       </c>
       <c r="G34" s="30" t="s">
-        <v>590</v>
+        <v>572</v>
       </c>
       <c r="H34" s="20"/>
       <c r="I34" s="18"/>
       <c r="J34" s="18"/>
       <c r="K34" s="1" t="s">
-        <v>594</v>
+        <v>576</v>
       </c>
       <c r="L34" s="14" t="s">
         <v>46</v>
@@ -50338,29 +50484,29 @@
     </row>
     <row r="35" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A35" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B35" s="30" t="s">
-        <v>583</v>
+        <v>565</v>
       </c>
       <c r="C35" s="30"/>
       <c r="D35" s="30" t="s">
-        <v>584</v>
+        <v>566</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>587</v>
+        <v>569</v>
       </c>
       <c r="F35" s="30" t="s">
-        <v>586</v>
+        <v>568</v>
       </c>
       <c r="G35" s="30" t="s">
-        <v>585</v>
+        <v>567</v>
       </c>
       <c r="H35" s="20"/>
       <c r="I35" s="18"/>
       <c r="J35" s="18"/>
       <c r="K35" s="1" t="s">
-        <v>588</v>
+        <v>570</v>
       </c>
       <c r="L35" s="14" t="s">
         <v>46</v>
@@ -50388,29 +50534,29 @@
     </row>
     <row r="36" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A36" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>601</v>
+        <v>583</v>
       </c>
       <c r="C36" s="16"/>
       <c r="D36" s="30" t="s">
-        <v>605</v>
+        <v>587</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>604</v>
+        <v>586</v>
       </c>
       <c r="F36" s="30" t="s">
-        <v>603</v>
+        <v>585</v>
       </c>
       <c r="G36" s="20" t="s">
-        <v>602</v>
+        <v>584</v>
       </c>
       <c r="H36" s="20"/>
       <c r="I36" s="18"/>
       <c r="J36" s="18"/>
       <c r="K36" s="1" t="s">
-        <v>606</v>
+        <v>588</v>
       </c>
       <c r="L36" s="14" t="s">
         <v>46</v>
@@ -50438,29 +50584,29 @@
     </row>
     <row r="37" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A37" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B37" s="30" t="s">
-        <v>595</v>
+        <v>577</v>
       </c>
       <c r="C37" s="16"/>
       <c r="D37" s="30" t="s">
-        <v>599</v>
+        <v>581</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>598</v>
+        <v>580</v>
       </c>
       <c r="F37" s="30" t="s">
-        <v>597</v>
+        <v>579</v>
       </c>
       <c r="G37" s="33" t="s">
-        <v>596</v>
+        <v>578</v>
       </c>
       <c r="H37" s="20"/>
       <c r="I37" s="18"/>
       <c r="J37" s="18"/>
       <c r="K37" s="1" t="s">
-        <v>600</v>
+        <v>582</v>
       </c>
       <c r="L37" s="14" t="s">
         <v>46</v>
@@ -50488,29 +50634,29 @@
     </row>
     <row r="38" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A38" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B38" s="30" t="s">
-        <v>607</v>
+        <v>589</v>
       </c>
       <c r="C38" s="15"/>
       <c r="D38" s="30" t="s">
-        <v>611</v>
+        <v>593</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>610</v>
+        <v>592</v>
       </c>
       <c r="F38" s="30" t="s">
-        <v>609</v>
+        <v>591</v>
       </c>
       <c r="G38" s="30" t="s">
-        <v>608</v>
+        <v>590</v>
       </c>
       <c r="H38" s="19"/>
       <c r="I38" s="18"/>
       <c r="J38" s="18"/>
       <c r="K38" s="1" t="s">
-        <v>613</v>
+        <v>595</v>
       </c>
       <c r="L38" s="14" t="s">
         <v>46</v>
@@ -50522,7 +50668,7 @@
         <v>13</v>
       </c>
       <c r="O38" s="3" t="s">
-        <v>612</v>
+        <v>594</v>
       </c>
       <c r="P38" s="5"/>
       <c r="Q38" s="5"/>
@@ -50538,49 +50684,49 @@
       <c r="AA38" s="5"/>
       <c r="AB38" s="5"/>
     </row>
-    <row r="39" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B39" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C39" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>637</v>
+        <v>605</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>638</v>
+        <v>606</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>639</v>
+        <v>607</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>640</v>
+        <v>608</v>
       </c>
       <c r="H39" s="10" t="s">
         <v>188</v>
       </c>
       <c r="I39" s="7"/>
       <c r="J39" s="38" t="s">
-        <v>634</v>
+        <v>653</v>
       </c>
       <c r="K39" s="8" t="s">
-        <v>376</v>
+        <v>666</v>
       </c>
       <c r="L39" s="11" t="s">
         <v>11</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>325</v>
+        <v>633</v>
       </c>
       <c r="N39" s="4" t="s">
         <v>8</v>
       </c>
       <c r="O39" s="3" t="s">
-        <v>641</v>
+        <v>609</v>
       </c>
       <c r="P39" s="5"/>
       <c r="Q39" s="5"/>
@@ -50596,43 +50742,43 @@
       <c r="AA39" s="5"/>
       <c r="AB39" s="5"/>
     </row>
-    <row r="40" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B40" t="s">
+        <v>368</v>
+      </c>
+      <c r="C40" t="s">
         <v>369</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" s="7" t="s">
+        <v>610</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="G40" s="7" t="s">
         <v>370</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>642</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>372</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>371</v>
       </c>
       <c r="H40" s="7" t="s">
         <v>188</v>
       </c>
       <c r="I40" s="7"/>
       <c r="J40" s="38" t="s">
-        <v>634</v>
+        <v>653</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>374</v>
+        <v>667</v>
       </c>
       <c r="L40" s="11" t="s">
         <v>11</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>325</v>
+        <v>633</v>
       </c>
       <c r="N40" s="4" t="s">
         <v>8</v>
@@ -50652,43 +50798,43 @@
       <c r="AA40" s="5"/>
       <c r="AB40" s="5"/>
     </row>
-    <row r="41" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B41" t="s">
+        <v>358</v>
+      </c>
+      <c r="C41" t="s">
         <v>359</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" s="10" t="s">
+        <v>611</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>612</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>613</v>
+      </c>
+      <c r="G41" s="10" t="s">
         <v>360</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>643</v>
-      </c>
-      <c r="E41" s="10" t="s">
-        <v>644</v>
-      </c>
-      <c r="F41" s="10" t="s">
-        <v>645</v>
-      </c>
-      <c r="G41" s="10" t="s">
-        <v>361</v>
       </c>
       <c r="H41" s="10" t="s">
         <v>188</v>
       </c>
       <c r="I41" s="7"/>
       <c r="J41" s="38" t="s">
-        <v>635</v>
+        <v>654</v>
       </c>
       <c r="K41" s="8" t="s">
-        <v>365</v>
+        <v>668</v>
       </c>
       <c r="L41" s="11" t="s">
         <v>11</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>325</v>
+        <v>633</v>
       </c>
       <c r="N41" s="4" t="s">
         <v>8</v>
@@ -50708,43 +50854,43 @@
       <c r="AA41" s="5"/>
       <c r="AB41" s="5"/>
     </row>
-    <row r="42" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B42" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C42" t="s">
+        <v>361</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>614</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>615</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>616</v>
+      </c>
+      <c r="G42" s="10" t="s">
         <v>362</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>646</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>647</v>
-      </c>
-      <c r="F42" s="10" t="s">
-        <v>648</v>
-      </c>
-      <c r="G42" s="10" t="s">
-        <v>363</v>
       </c>
       <c r="H42" s="10" t="s">
         <v>188</v>
       </c>
       <c r="I42" s="7"/>
       <c r="J42" s="38" t="s">
-        <v>663</v>
+        <v>655</v>
       </c>
       <c r="K42" s="8" t="s">
-        <v>364</v>
+        <v>669</v>
       </c>
       <c r="L42" s="11" t="s">
         <v>11</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>325</v>
+        <v>633</v>
       </c>
       <c r="N42" s="4" t="s">
         <v>8</v>
@@ -50764,43 +50910,43 @@
       <c r="AA42" s="5"/>
       <c r="AB42" s="5"/>
     </row>
-    <row r="43" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A43" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B43" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C43" t="s">
+        <v>365</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>617</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>618</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>619</v>
+      </c>
+      <c r="G43" s="10" t="s">
         <v>366</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>649</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>650</v>
-      </c>
-      <c r="F43" s="10" t="s">
-        <v>651</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>367</v>
       </c>
       <c r="H43" s="10" t="s">
         <v>188</v>
       </c>
       <c r="I43" s="7"/>
       <c r="J43" s="38" t="s">
-        <v>636</v>
+        <v>656</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>368</v>
+        <v>670</v>
       </c>
       <c r="L43" s="11" t="s">
         <v>11</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>325</v>
+        <v>633</v>
       </c>
       <c r="N43" s="4" t="s">
         <v>8</v>
@@ -50825,20 +50971,20 @@
         <v>310</v>
       </c>
       <c r="B44" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C44"/>
       <c r="D44" t="s">
+        <v>353</v>
+      </c>
+      <c r="E44" t="s">
         <v>354</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F44" t="s">
         <v>355</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>356</v>
-      </c>
-      <c r="G44" t="s">
-        <v>357</v>
       </c>
       <c r="H44" s="10" t="s">
         <v>188</v>
@@ -50846,7 +50992,7 @@
       <c r="I44" s="7"/>
       <c r="J44" s="7"/>
       <c r="K44" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="L44" s="4" t="s">
         <v>2</v>
@@ -50897,16 +51043,16 @@
       <c r="H45" s="7"/>
       <c r="I45" s="7"/>
       <c r="J45" s="38" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>341</v>
+        <v>671</v>
       </c>
       <c r="L45" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>319</v>
+        <v>665</v>
       </c>
       <c r="N45" s="4" t="s">
         <v>8</v>
@@ -50937,30 +51083,30 @@
         <v>314</v>
       </c>
       <c r="D46" s="30" t="s">
+        <v>319</v>
+      </c>
+      <c r="E46" s="30" t="s">
         <v>320</v>
       </c>
-      <c r="E46" s="30" t="s">
+      <c r="F46" s="30" t="s">
         <v>321</v>
       </c>
-      <c r="F46" s="30" t="s">
+      <c r="G46" s="30" t="s">
         <v>322</v>
-      </c>
-      <c r="G46" s="30" t="s">
-        <v>323</v>
       </c>
       <c r="H46" s="7"/>
       <c r="I46" s="7"/>
       <c r="J46" s="38" t="s">
-        <v>653</v>
+        <v>658</v>
       </c>
       <c r="K46" s="8" t="s">
-        <v>340</v>
+        <v>672</v>
       </c>
       <c r="L46" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>319</v>
+        <v>665</v>
       </c>
       <c r="N46" s="4" t="s">
         <v>8</v>
@@ -50980,7 +51126,7 @@
       <c r="AA46" s="5"/>
       <c r="AB46" s="5"/>
     </row>
-    <row r="47" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
         <v>310</v>
       </c>
@@ -50988,33 +51134,33 @@
         <v>311</v>
       </c>
       <c r="C47" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D47" s="30" t="s">
+        <v>319</v>
+      </c>
+      <c r="E47" s="30" t="s">
         <v>320</v>
       </c>
-      <c r="E47" s="30" t="s">
+      <c r="F47" s="30" t="s">
         <v>321</v>
       </c>
-      <c r="F47" s="30" t="s">
+      <c r="G47" s="30" t="s">
         <v>322</v>
-      </c>
-      <c r="G47" s="30" t="s">
-        <v>323</v>
       </c>
       <c r="H47" s="7"/>
       <c r="I47" s="7"/>
       <c r="J47" s="38" t="s">
-        <v>652</v>
+        <v>659</v>
       </c>
       <c r="K47" s="8" t="s">
-        <v>339</v>
+        <v>673</v>
       </c>
       <c r="L47" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>325</v>
+        <v>633</v>
       </c>
       <c r="N47" s="4" t="s">
         <v>8</v>
@@ -51034,7 +51180,7 @@
       <c r="AA47" s="5"/>
       <c r="AB47" s="5"/>
     </row>
-    <row r="48" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
         <v>310</v>
       </c>
@@ -51042,33 +51188,33 @@
         <v>311</v>
       </c>
       <c r="C48" t="s">
+        <v>325</v>
+      </c>
+      <c r="D48" s="30" t="s">
         <v>326</v>
       </c>
-      <c r="D48" s="30" t="s">
+      <c r="E48" s="30" t="s">
         <v>327</v>
       </c>
-      <c r="E48" s="30" t="s">
+      <c r="F48" s="30" t="s">
         <v>328</v>
       </c>
-      <c r="F48" s="30" t="s">
+      <c r="G48" s="30" t="s">
         <v>329</v>
-      </c>
-      <c r="G48" s="30" t="s">
-        <v>330</v>
       </c>
       <c r="H48" s="7"/>
       <c r="I48" s="7"/>
       <c r="J48" s="38" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="K48" s="8" t="s">
-        <v>338</v>
+        <v>674</v>
       </c>
       <c r="L48" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>325</v>
+        <v>633</v>
       </c>
       <c r="N48" s="4" t="s">
         <v>8</v>
@@ -51088,7 +51234,7 @@
       <c r="AA48" s="5"/>
       <c r="AB48" s="5"/>
     </row>
-    <row r="49" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
         <v>310</v>
       </c>
@@ -51096,33 +51242,33 @@
         <v>311</v>
       </c>
       <c r="C49" t="s">
+        <v>330</v>
+      </c>
+      <c r="D49" s="30" t="s">
         <v>331</v>
       </c>
-      <c r="D49" s="30" t="s">
+      <c r="E49" s="30" t="s">
         <v>332</v>
       </c>
-      <c r="E49" s="30" t="s">
-        <v>333</v>
-      </c>
       <c r="F49" s="30" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G49" s="30" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H49" s="7"/>
       <c r="I49" s="7"/>
       <c r="J49" s="38" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>337</v>
+        <v>675</v>
       </c>
       <c r="L49" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>325</v>
+        <v>633</v>
       </c>
       <c r="N49" s="4" t="s">
         <v>8</v>
@@ -51142,7 +51288,7 @@
       <c r="AA49" s="5"/>
       <c r="AB49" s="5"/>
     </row>
-    <row r="50" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A50" s="7" t="s">
         <v>310</v>
       </c>
@@ -51150,33 +51296,33 @@
         <v>311</v>
       </c>
       <c r="C50" t="s">
+        <v>341</v>
+      </c>
+      <c r="D50" s="30" t="s">
         <v>342</v>
       </c>
-      <c r="D50" s="30" t="s">
+      <c r="E50" s="30" t="s">
         <v>343</v>
       </c>
-      <c r="E50" s="30" t="s">
+      <c r="F50" s="30" t="s">
+        <v>333</v>
+      </c>
+      <c r="G50" s="30" t="s">
         <v>344</v>
-      </c>
-      <c r="F50" s="30" t="s">
-        <v>334</v>
-      </c>
-      <c r="G50" s="30" t="s">
-        <v>345</v>
       </c>
       <c r="H50" s="7"/>
       <c r="I50" s="7"/>
       <c r="J50" s="38" t="s">
-        <v>656</v>
+        <v>662</v>
       </c>
       <c r="K50" s="8" t="s">
-        <v>346</v>
+        <v>676</v>
       </c>
       <c r="L50" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>325</v>
+        <v>633</v>
       </c>
       <c r="N50" s="4" t="s">
         <v>8</v>
@@ -51196,7 +51342,7 @@
       <c r="AA50" s="5"/>
       <c r="AB50" s="5"/>
     </row>
-    <row r="51" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A51" s="7" t="s">
         <v>310</v>
       </c>
@@ -51204,33 +51350,33 @@
         <v>311</v>
       </c>
       <c r="C51" t="s">
+        <v>346</v>
+      </c>
+      <c r="D51" s="30" t="s">
         <v>347</v>
       </c>
-      <c r="D51" s="30" t="s">
+      <c r="E51" s="30" t="s">
         <v>348</v>
       </c>
-      <c r="E51" s="30" t="s">
+      <c r="F51" s="30" t="s">
         <v>349</v>
       </c>
-      <c r="F51" s="30" t="s">
+      <c r="G51" s="30" t="s">
         <v>350</v>
-      </c>
-      <c r="G51" s="30" t="s">
-        <v>351</v>
       </c>
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
       <c r="J51" s="38" t="s">
-        <v>655</v>
+        <v>663</v>
       </c>
       <c r="K51" s="8" t="s">
-        <v>352</v>
+        <v>677</v>
       </c>
       <c r="L51" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>325</v>
+        <v>633</v>
       </c>
       <c r="N51" s="4" t="s">
         <v>8</v>
@@ -51255,28 +51401,28 @@
         <v>310</v>
       </c>
       <c r="B52" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C52" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>659</v>
+        <v>620</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>660</v>
+        <v>621</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H52" s="10"/>
       <c r="I52" s="7"/>
       <c r="J52" s="7"/>
       <c r="K52" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="L52" s="12"/>
       <c r="M52" s="4" t="s">
@@ -51286,7 +51432,7 @@
         <v>13</v>
       </c>
       <c r="O52" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="P52" s="5"/>
       <c r="Q52" s="5"/>
@@ -51307,31 +51453,31 @@
         <v>310</v>
       </c>
       <c r="B53" t="s">
+        <v>380</v>
+      </c>
+      <c r="C53" t="s">
         <v>381</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
+        <v>385</v>
+      </c>
+      <c r="E53" t="s">
+        <v>384</v>
+      </c>
+      <c r="F53" t="s">
+        <v>383</v>
+      </c>
+      <c r="G53" s="10" t="s">
         <v>382</v>
-      </c>
-      <c r="D53" t="s">
-        <v>386</v>
-      </c>
-      <c r="E53" t="s">
-        <v>385</v>
-      </c>
-      <c r="F53" t="s">
-        <v>384</v>
-      </c>
-      <c r="G53" s="10" t="s">
-        <v>383</v>
       </c>
       <c r="H53" s="10"/>
       <c r="I53" s="7"/>
       <c r="J53" s="7"/>
       <c r="K53" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="L53" s="12" t="s">
         <v>387</v>
-      </c>
-      <c r="L53" s="12" t="s">
-        <v>388</v>
       </c>
       <c r="M53" s="4" t="s">
         <v>4</v>
@@ -51359,28 +51505,28 @@
         <v>310</v>
       </c>
       <c r="B54" t="s">
+        <v>388</v>
+      </c>
+      <c r="C54" t="s">
         <v>389</v>
       </c>
-      <c r="C54" t="s">
-        <v>390</v>
-      </c>
       <c r="D54" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E54" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G54" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H54" s="7"/>
       <c r="I54" s="7"/>
       <c r="J54" s="7"/>
       <c r="K54" s="8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="L54" s="4"/>
       <c r="M54" s="4" t="s">
@@ -51390,7 +51536,7 @@
         <v>13</v>
       </c>
       <c r="O54" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="P54" s="5"/>
       <c r="Q54" s="5"/>
@@ -51411,20 +51557,20 @@
         <v>310</v>
       </c>
       <c r="B55" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C55" s="10"/>
       <c r="D55" s="10" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="H55" s="10" t="s">
         <v>188</v>
@@ -51432,7 +51578,7 @@
       <c r="I55" s="7"/>
       <c r="J55" s="7"/>
       <c r="K55" s="8" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="L55" s="11" t="s">
         <v>11</v>
@@ -51463,28 +51609,28 @@
         <v>310</v>
       </c>
       <c r="B56" t="s">
+        <v>401</v>
+      </c>
+      <c r="C56" t="s">
+        <v>389</v>
+      </c>
+      <c r="D56" t="s">
         <v>402</v>
       </c>
-      <c r="C56" t="s">
-        <v>390</v>
-      </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>403</v>
       </c>
-      <c r="E56" t="s">
+      <c r="F56" s="7" t="s">
         <v>404</v>
       </c>
-      <c r="F56" s="7" t="s">
-        <v>405</v>
-      </c>
       <c r="G56" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
       <c r="J56" s="7"/>
       <c r="K56" s="8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="L56" s="4"/>
       <c r="M56" s="4" t="s">
@@ -51494,7 +51640,7 @@
         <v>13</v>
       </c>
       <c r="O56" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="P56" s="5"/>
       <c r="Q56" s="5"/>
@@ -51510,41 +51656,41 @@
       <c r="AA56" s="5"/>
       <c r="AB56" s="5"/>
     </row>
-    <row r="57" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A57" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B57" t="s">
+        <v>406</v>
+      </c>
+      <c r="C57" t="s">
+        <v>359</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>409</v>
+      </c>
+      <c r="F57" s="10" t="s">
         <v>407</v>
       </c>
-      <c r="C57" t="s">
-        <v>360</v>
-      </c>
-      <c r="D57" s="10" t="s">
-        <v>409</v>
-      </c>
-      <c r="E57" s="10" t="s">
+      <c r="G57" s="10" t="s">
         <v>410</v>
-      </c>
-      <c r="F57" s="10" t="s">
-        <v>408</v>
-      </c>
-      <c r="G57" s="10" t="s">
-        <v>411</v>
       </c>
       <c r="H57" s="10"/>
       <c r="I57" s="7"/>
       <c r="J57" s="38" t="s">
-        <v>635</v>
+        <v>654</v>
       </c>
       <c r="K57" s="8" t="s">
-        <v>412</v>
+        <v>678</v>
       </c>
       <c r="L57" s="11" t="s">
         <v>11</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>325</v>
+        <v>633</v>
       </c>
       <c r="N57" s="4" t="s">
         <v>8</v>
@@ -51564,41 +51710,41 @@
       <c r="AA57" s="5"/>
       <c r="AB57" s="5"/>
     </row>
-    <row r="58" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A58" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B58" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C58" t="s">
+        <v>412</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>416</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>415</v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>414</v>
+      </c>
+      <c r="G58" s="10" t="s">
         <v>413</v>
-      </c>
-      <c r="D58" s="10" t="s">
-        <v>417</v>
-      </c>
-      <c r="E58" s="10" t="s">
-        <v>416</v>
-      </c>
-      <c r="F58" s="10" t="s">
-        <v>415</v>
-      </c>
-      <c r="G58" s="10" t="s">
-        <v>414</v>
       </c>
       <c r="H58" s="10"/>
       <c r="I58" s="7"/>
       <c r="J58" s="38" t="s">
-        <v>655</v>
+        <v>663</v>
       </c>
       <c r="K58" s="8" t="s">
-        <v>418</v>
+        <v>679</v>
       </c>
       <c r="L58" s="11" t="s">
         <v>11</v>
       </c>
       <c r="M58" s="4" t="s">
-        <v>325</v>
+        <v>633</v>
       </c>
       <c r="N58" s="4" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
1859 added Acidosis and Alkalosis and more unit tests
</commit_message>
<xml_diff>
--- a/inst/adlb_grading/adlb_grading_spec.xlsx
+++ b/inst/adlb_grading/adlb_grading_spec.xlsx
@@ -17,7 +17,7 @@
     <sheet name="DAIDS" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DAIDS!$C$1:$C$992</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DAIDS!$C$1:$C$994</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2238" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1609" uniqueCount="676">
   <si>
     <t>Anemia</t>
   </si>
@@ -1402,9 +1402,6 @@
     <t>57 days of age to &lt; 13 years of age (male and female)</t>
   </si>
   <si>
-    <t>AVAL, agecurr</t>
-  </si>
-  <si>
     <t>36 to 56 days of age (male and female)</t>
   </si>
   <si>
@@ -1464,56 +1461,6 @@
     <t>6.7 to &lt; 8.0 g/dL, 4.15 to &lt; 4.94 mmol/L</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) | is.na(agecurr) ~ NA_character_,
-AVAL &lt; 67 ~ "4",
-AVAL &lt; 80 ~ "3",
-AVAL &lt; 95 ~ "2",
-AVAL &lt;= 110 ~ "1",
-AVAL &gt; 110 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(agecurr) ~ NA_character_,
-AVAL &lt; 60 ~ "4",
-AVAL &lt; 70 ~ "3",
-AVAL &lt; 85 ~ "2",
-AVAL &lt;= 96 ~ "1",
-AVAL &gt; 96 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(agecurr) ~ NA_character_,
-AVAL &lt; 65 ~ "4",
-AVAL &lt; 85 ~ "3",
-AVAL &lt; 95 ~ "2",
-AVAL &lt;= 104 ~ "1",
-AVAL &gt; 104 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(sex) | is.na(agecurr) ~ NA_character_,
-AVAL &lt; 65 ~ "4",
-AVAL &lt; 85 ~ "3",
-AVAL &lt; 95 ~ "2",
-AVAL &lt;= 104 ~ "1",
-AVAL &gt; 104 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(sex) | is.na(agecurr) ~ NA_character_,
-AVAL &lt; 70 ~ "4",
-AVAL &lt; 90 ~ "3",
-AVAL &lt; 100 ~ "2",
-AVAL &lt;= 109 ~ "1",
-AVAL &gt; 109 ~ "0"
-)</t>
-  </si>
-  <si>
     <t>8 to ≤ 21 days of age (male and female)</t>
   </si>
   <si>
@@ -1537,16 +1484,6 @@
   </si>
   <si>
     <t>&lt; 8.0 g/dL, &lt; 4.96 mmol/L</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(agecurr) ~ NA_character_,
-AVAL &lt; 80 ~ "4",
-AVAL &lt; 90 ~ "3",
-AVAL &lt; 110 ~ "2",
-AVAL &lt;= 130 ~ "1",
-AVAL &gt; 130 ~ "0"
-)</t>
   </si>
   <si>
     <t>≤ 7 days of age (male and female)</t>
@@ -1575,16 +1512,6 @@
   </si>
   <si>
     <t>&lt; 9.0 g/dL, &lt; 5.59 mmol/L</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(agecurr) ~ NA_character_,
-AVAL &lt; 90 ~ "4",
-AVAL &lt; 100 ~ "3",
-AVAL &lt; 130 ~ "2",
-AVAL &lt;= 140 ~ "1",
-AVAL &gt; 140 ~ "0"
-)</t>
   </si>
   <si>
     <t>Fibrinogen Decreased</t>
@@ -1632,40 +1559,10 @@
     <t>&lt;750/mm3; &lt;0.750 x 10e9 /L</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &lt; 0.75 ~ "4",
-AVAL &lt; 1 ~ "3",
-AVAL &lt; 1.25 ~ "2",
-AVAL &lt;= 1.5 ~ "1",
-AVAL &gt; 1.5 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &lt; 0.4 ~ "4",
-AVAL &lt; 0.6 ~ "3",
-AVAL &lt; 0.8 ~ "2",
-AVAL &lt;= 1 ~ "1",
-AVAL &gt; 1 ~ "0"
-)</t>
-  </si>
-  <si>
     <t>≤ 1 day of age</t>
   </si>
   <si>
     <t>&lt;1550/mm3; &lt;1.500 x 10e9 /L</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &lt; 1.5 ~ "4",
-AVAL &lt; 3 ~ "3",
-AVAL &lt; 4 ~ "2",
-AVAL &lt;= 5 ~ "1",
-AVAL &gt; 5 ~ "0"
-)</t>
   </si>
   <si>
     <t>Absolute Lymphocyte Count, Low</t>
@@ -1683,27 +1580,7 @@
     <t>500 to &lt;600/mm3; 0.500 to &lt;0.600 x 10e9 /L</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &lt; 0.35 ~ "4",
-AVAL &lt; 0.5 ~ "3",
-AVAL &lt; 0.6 ~ "2",
-AVAL &lt; 0.65 ~ "1",
-AVAL &gt;= 0.65 ~ "0"
-)</t>
-  </si>
-  <si>
     <t>Absolute CD4+ Count, Low</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &lt; 0.1 ~ "4",
-AVAL &lt; 0.2 ~ "3",
-AVAL &lt; 0.3 ~ "2",
-AVAL &lt; 0.4 ~ "1",
-AVAL &gt;= 0.4 ~ "0"
-)</t>
   </si>
   <si>
     <t>INR, High</t>
@@ -1796,9 +1673,6 @@
     <t>50,000 to &lt;100,000 - /mm3; 50.0 to &lt;100.000 - x 10e9 /L</t>
   </si>
   <si>
-    <t>100,000 to &lt;125,000/mm3; 100.00 - 125.000 x 10e9 /L</t>
-  </si>
-  <si>
     <t>case_when(
 is.na(AVAL) ~ NA_character_,
 AVAL &lt; 25 ~ "4",
@@ -1846,16 +1720,6 @@
     <t>&lt;1000/mm3; &lt;1.000 x 10e9/L</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &lt; 1 ~ "4",
-AVAL &lt; 1.5 ~ "3",
-AVAL &lt; 2 ~ "2",
-AVAL &lt; 2.5 ~ "1",
-AVAL &gt;= 2.5 ~ "0"
-)</t>
-  </si>
-  <si>
     <t>≤ 7 days of age</t>
   </si>
   <si>
@@ -1869,16 +1733,6 @@
   </si>
   <si>
     <t>5500 to 6999/mm3; 5.500 to 6.999 x 10e9/L</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &lt; 2.5 ~ "4",
-AVAL &lt; 4 ~ "3",
-AVAL &lt; 5.5 ~ "2",
-AVAL &lt; 7 ~ "1",
-AVAL &gt;= 7 ~ "0"
-)</t>
   </si>
   <si>
     <t>Chemistries</t>
@@ -2996,6 +2850,54 @@
 AVAL &gt;= 7 ~ "0"
 )</t>
   </si>
+  <si>
+    <t>100,000 to &lt;125,000/mm3; 100.00 - &lt;125.000 x 10e9 /L</t>
+  </si>
+  <si>
+    <t>Acidosis</t>
+  </si>
+  <si>
+    <t>pH &gt;= 7.3 to &lt; LLN</t>
+  </si>
+  <si>
+    <t>pH &lt; 7.3 without lifethreatening consequences</t>
+  </si>
+  <si>
+    <t>pH &lt; 7.3 with lifethreatening consequences</t>
+  </si>
+  <si>
+    <t>Assume "with lifethreatening consequences"</t>
+  </si>
+  <si>
+    <t>Alkalosis</t>
+  </si>
+  <si>
+    <t>pH &gt; ULN to ≤ 7.5</t>
+  </si>
+  <si>
+    <t>pH &gt; 7.5 without lifethreatening consequences</t>
+  </si>
+  <si>
+    <t>pH &gt; 7.5 with lifethreatening consequences</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+AVAL &lt; 7.3 ~ "4",
+is.na(ANRLO) ~ NA_character_,
+AVAL &lt; ANRLO ~ "2",
+AVAL &gt;= ANRLO ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+AVAL &gt; 7.5 ~ "4",
+is.na(ANRHI) ~ NA_character_,
+AVAL &gt; ANRHI ~ "2",
+AVAL &lt;= ANRLO ~ "0"
+)</t>
+  </si>
 </sst>
 </file>
 
@@ -48713,10 +48615,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB992"/>
+  <dimension ref="A1:AB994"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -48740,7 +48642,7 @@
         <v>201</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>596</v>
+        <v>580</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>261</v>
@@ -48792,40 +48694,40 @@
       <c r="AA1" s="5"/>
       <c r="AB1" s="5"/>
     </row>
-    <row r="2" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" ht="88.5" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="B2" t="s">
-        <v>425</v>
+        <v>665</v>
       </c>
       <c r="C2" s="10"/>
-      <c r="D2" t="s">
-        <v>428</v>
-      </c>
+      <c r="D2"/>
       <c r="E2" t="s">
-        <v>426</v>
+        <v>666</v>
       </c>
       <c r="F2" t="s">
-        <v>427</v>
-      </c>
-      <c r="G2" s="32"/>
+        <v>667</v>
+      </c>
+      <c r="G2" t="s">
+        <v>668</v>
+      </c>
       <c r="H2" s="10"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="8" t="s">
-        <v>429</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>674</v>
+      </c>
+      <c r="L2" s="4"/>
       <c r="M2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="3"/>
+      <c r="O2" s="3" t="s">
+        <v>669</v>
+      </c>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
@@ -48842,36 +48744,36 @@
     </row>
     <row r="3" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="B3" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="C3" s="10"/>
-      <c r="D3" s="31" t="s">
-        <v>423</v>
-      </c>
-      <c r="E3" s="31" t="s">
-        <v>422</v>
-      </c>
-      <c r="F3" s="32" t="s">
-        <v>421</v>
-      </c>
-      <c r="G3" s="32" t="s">
-        <v>420</v>
-      </c>
+      <c r="D3" t="s">
+        <v>412</v>
+      </c>
+      <c r="E3" t="s">
+        <v>410</v>
+      </c>
+      <c r="F3" t="s">
+        <v>411</v>
+      </c>
+      <c r="G3" s="32"/>
       <c r="H3" s="10"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="8" t="s">
-        <v>424</v>
-      </c>
-      <c r="L3" s="4"/>
+        <v>413</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="M3" s="4" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="O3" s="3"/>
       <c r="P3" s="5"/>
@@ -48890,29 +48792,29 @@
     </row>
     <row r="4" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="B4" t="s">
-        <v>430</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7" t="s">
-        <v>423</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>422</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>421</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>420</v>
-      </c>
-      <c r="H4" s="7"/>
+        <v>403</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="31" t="s">
+        <v>407</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>406</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>405</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>404</v>
+      </c>
+      <c r="H4" s="10"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="8" t="s">
-        <v>431</v>
+        <v>408</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4" t="s">
@@ -48936,40 +48838,40 @@
       <c r="AA4" s="5"/>
       <c r="AB4" s="5"/>
     </row>
-    <row r="5" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" ht="88.5" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="B5" t="s">
-        <v>433</v>
+        <v>670</v>
       </c>
       <c r="C5" s="10"/>
-      <c r="D5" s="33" t="s">
-        <v>437</v>
-      </c>
-      <c r="E5" s="34" t="s">
-        <v>436</v>
-      </c>
-      <c r="F5" s="33" t="s">
-        <v>435</v>
-      </c>
-      <c r="G5" s="33" t="s">
-        <v>434</v>
+      <c r="D5"/>
+      <c r="E5" t="s">
+        <v>671</v>
+      </c>
+      <c r="F5" t="s">
+        <v>672</v>
+      </c>
+      <c r="G5" t="s">
+        <v>673</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="L5" s="12"/>
+      <c r="K5" s="8" t="s">
+        <v>675</v>
+      </c>
+      <c r="L5" s="4"/>
       <c r="M5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O5" s="3"/>
+      <c r="O5" s="3" t="s">
+        <v>669</v>
+      </c>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
@@ -48986,29 +48888,29 @@
     </row>
     <row r="6" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="B6" t="s">
-        <v>432</v>
+        <v>414</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>423</v>
+        <v>407</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>422</v>
+        <v>406</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>421</v>
+        <v>405</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>420</v>
+        <v>404</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="8" t="s">
-        <v>431</v>
+        <v>415</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4" t="s">
@@ -49032,40 +48934,38 @@
       <c r="AA6" s="5"/>
       <c r="AB6" s="5"/>
     </row>
-    <row r="7" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="B7" t="s">
+        <v>417</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="33" t="s">
+        <v>421</v>
+      </c>
+      <c r="E7" s="34" t="s">
+        <v>420</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="G7" s="33" t="s">
         <v>418</v>
       </c>
-      <c r="B7" t="s">
-        <v>439</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7" t="s">
-        <v>443</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>442</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>441</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>440</v>
-      </c>
-      <c r="H7" s="7"/>
+      <c r="H7" s="10"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
-      <c r="K7" s="8" t="s">
-        <v>444</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="K7" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="L7" s="12"/>
       <c r="M7" s="4" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="O7" s="3"/>
       <c r="P7" s="5"/>
@@ -49082,153 +48982,142 @@
       <c r="AA7" s="5"/>
       <c r="AB7" s="5"/>
     </row>
-    <row r="8" spans="1:28" s="44" customFormat="1" ht="76" x14ac:dyDescent="0.35">
-      <c r="A8" s="36" t="s">
-        <v>418</v>
-      </c>
-      <c r="B8" s="37" t="s">
-        <v>445</v>
-      </c>
-      <c r="C8" s="37" t="s">
-        <v>446</v>
-      </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="37" t="s">
-        <v>449</v>
-      </c>
-      <c r="G8" s="32" t="s">
-        <v>448</v>
-      </c>
-      <c r="H8" s="36" t="s">
-        <v>188</v>
-      </c>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38" t="s">
-        <v>622</v>
-      </c>
-      <c r="K8" s="39" t="s">
-        <v>623</v>
-      </c>
-      <c r="L8" s="40"/>
+    <row r="8" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+      <c r="A8" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="B8" t="s">
+        <v>416</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="8" t="s">
+        <v>415</v>
+      </c>
+      <c r="L8" s="4"/>
       <c r="M8" s="4" t="s">
-        <v>624</v>
-      </c>
-      <c r="N8" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="N8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O8" s="37" t="s">
-        <v>450</v>
-      </c>
-      <c r="P8" s="43"/>
-      <c r="Q8" s="43"/>
-      <c r="R8" s="43"/>
-      <c r="S8" s="43"/>
-      <c r="T8" s="43"/>
-      <c r="U8" s="43"/>
-      <c r="V8" s="43"/>
-      <c r="W8" s="43"/>
-      <c r="X8" s="43"/>
-      <c r="Y8" s="43"/>
-      <c r="Z8" s="43"/>
-      <c r="AA8" s="43"/>
-      <c r="AB8" s="43"/>
-    </row>
-    <row r="9" spans="1:28" s="44" customFormat="1" ht="126" x14ac:dyDescent="0.35">
-      <c r="A9" s="36" t="s">
-        <v>418</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>445</v>
-      </c>
-      <c r="C9" s="37" t="s">
-        <v>447</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>454</v>
-      </c>
-      <c r="E9" s="32" t="s">
-        <v>453</v>
-      </c>
-      <c r="F9" s="32" t="s">
-        <v>452</v>
-      </c>
-      <c r="G9" t="s">
-        <v>451</v>
-      </c>
-      <c r="H9"/>
-      <c r="J9" s="38" t="s">
-        <v>625</v>
-      </c>
-      <c r="K9" s="39" t="s">
-        <v>626</v>
-      </c>
-      <c r="L9" s="40" t="s">
-        <v>597</v>
+      <c r="O8" s="3"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="5"/>
+      <c r="AB8" s="5"/>
+    </row>
+    <row r="9" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="B9" t="s">
+        <v>423</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>624</v>
-      </c>
-      <c r="N9" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="O9" s="42" t="s">
-        <v>599</v>
-      </c>
-      <c r="P9" s="43"/>
-      <c r="Q9" s="43"/>
-      <c r="R9" s="43"/>
-      <c r="S9" s="43"/>
-      <c r="T9" s="43"/>
-      <c r="U9" s="43"/>
-      <c r="V9" s="43"/>
-      <c r="W9" s="43"/>
-      <c r="X9" s="43"/>
-      <c r="Y9" s="43"/>
-      <c r="Z9" s="43"/>
-      <c r="AA9" s="43"/>
-      <c r="AB9" s="43"/>
-    </row>
-    <row r="10" spans="1:28" s="44" customFormat="1" ht="113.5" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="O9" s="3"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="5"/>
+      <c r="AB9" s="5"/>
+    </row>
+    <row r="10" spans="1:28" s="44" customFormat="1" ht="76" x14ac:dyDescent="0.35">
       <c r="A10" s="36" t="s">
-        <v>418</v>
-      </c>
-      <c r="B10" t="s">
-        <v>455</v>
+        <v>402</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>429</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>446</v>
-      </c>
-      <c r="D10" s="33" t="s">
-        <v>458</v>
-      </c>
-      <c r="E10" s="34" t="s">
-        <v>457</v>
-      </c>
-      <c r="F10" s="33" t="s">
-        <v>456</v>
-      </c>
-      <c r="G10" s="33" t="s">
-        <v>434</v>
+        <v>430</v>
+      </c>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="37" t="s">
+        <v>433</v>
+      </c>
+      <c r="G10" s="32" t="s">
+        <v>432</v>
       </c>
       <c r="H10" s="36" t="s">
         <v>188</v>
       </c>
       <c r="I10" s="38"/>
       <c r="J10" s="38" t="s">
-        <v>622</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>629</v>
+        <v>606</v>
+      </c>
+      <c r="K10" s="39" t="s">
+        <v>607</v>
       </c>
       <c r="L10" s="40"/>
       <c r="M10" s="4" t="s">
-        <v>624</v>
+        <v>608</v>
       </c>
       <c r="N10" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="O10" s="37"/>
+      <c r="O10" s="37" t="s">
+        <v>434</v>
+      </c>
       <c r="P10" s="43"/>
       <c r="Q10" s="43"/>
       <c r="R10" s="43"/>
@@ -49243,145 +49132,150 @@
       <c r="AA10" s="43"/>
       <c r="AB10" s="43"/>
     </row>
-    <row r="11" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" s="44" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A11" s="36" t="s">
+        <v>402</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>429</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>431</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>438</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>437</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>436</v>
+      </c>
+      <c r="G11" t="s">
+        <v>435</v>
+      </c>
+      <c r="H11"/>
+      <c r="J11" s="38" t="s">
+        <v>609</v>
+      </c>
+      <c r="K11" s="39" t="s">
+        <v>610</v>
+      </c>
+      <c r="L11" s="40" t="s">
+        <v>581</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="N11" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="O11" s="42" t="s">
+        <v>583</v>
+      </c>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="43"/>
+      <c r="S11" s="43"/>
+      <c r="T11" s="43"/>
+      <c r="U11" s="43"/>
+      <c r="V11" s="43"/>
+      <c r="W11" s="43"/>
+      <c r="X11" s="43"/>
+      <c r="Y11" s="43"/>
+      <c r="Z11" s="43"/>
+      <c r="AA11" s="43"/>
+      <c r="AB11" s="43"/>
+    </row>
+    <row r="12" spans="1:28" s="44" customFormat="1" ht="113.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="36" t="s">
+        <v>402</v>
+      </c>
+      <c r="B12" t="s">
+        <v>439</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>430</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>442</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>441</v>
+      </c>
+      <c r="F12" s="33" t="s">
+        <v>440</v>
+      </c>
+      <c r="G12" s="33" t="s">
         <v>418</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>464</v>
-      </c>
-      <c r="C11" t="s">
-        <v>465</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>466</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>467</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>468</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>469</v>
-      </c>
-      <c r="H11" s="19"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="38" t="s">
-        <v>627</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>630</v>
-      </c>
-      <c r="L11" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>633</v>
-      </c>
-      <c r="N11" s="4" t="s">
+      <c r="H12" s="36" t="s">
+        <v>188</v>
+      </c>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38" t="s">
+        <v>606</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="L12" s="40"/>
+      <c r="M12" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="N12" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="O11" s="3"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
-      <c r="U11" s="5"/>
-      <c r="V11" s="5"/>
-      <c r="W11" s="5"/>
-      <c r="X11" s="5"/>
-      <c r="Y11" s="5"/>
-      <c r="Z11" s="5"/>
-      <c r="AA11" s="5"/>
-      <c r="AB11" s="5"/>
-    </row>
-    <row r="12" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="36" t="s">
-        <v>418</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>464</v>
-      </c>
-      <c r="C12" t="s">
-        <v>470</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>601</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>600</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>471</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>469</v>
-      </c>
-      <c r="H12" s="19"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="38" t="s">
-        <v>628</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>631</v>
-      </c>
-      <c r="L12" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>633</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O12" s="3"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
-      <c r="U12" s="5"/>
-      <c r="V12" s="5"/>
-      <c r="W12" s="5"/>
-      <c r="X12" s="5"/>
-      <c r="Y12" s="5"/>
-      <c r="Z12" s="5"/>
-      <c r="AA12" s="5"/>
-      <c r="AB12" s="5"/>
-    </row>
-    <row r="13" spans="1:28" ht="113" x14ac:dyDescent="0.3">
+      <c r="O12" s="37"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="43"/>
+      <c r="R12" s="43"/>
+      <c r="S12" s="43"/>
+      <c r="T12" s="43"/>
+      <c r="U12" s="43"/>
+      <c r="V12" s="43"/>
+      <c r="W12" s="43"/>
+      <c r="X12" s="43"/>
+      <c r="Y12" s="43"/>
+      <c r="Z12" s="43"/>
+      <c r="AA12" s="43"/>
+      <c r="AB12" s="43"/>
+    </row>
+    <row r="13" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A13" s="36" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>459</v>
-      </c>
-      <c r="C13" s="15"/>
+        <v>448</v>
+      </c>
+      <c r="C13" t="s">
+        <v>449</v>
+      </c>
       <c r="D13" s="19" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>463</v>
+        <v>451</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>462</v>
+        <v>452</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="H13" s="19"/>
       <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
+      <c r="J13" s="38" t="s">
+        <v>611</v>
+      </c>
       <c r="K13" s="1" t="s">
-        <v>598</v>
+        <v>614</v>
       </c>
       <c r="L13" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>16</v>
+        <v>617</v>
       </c>
       <c r="N13" s="4" t="s">
         <v>13</v>
@@ -49402,43 +49296,43 @@
       <c r="AB13" s="5"/>
     </row>
     <row r="14" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="45" t="s">
-        <v>418</v>
-      </c>
-      <c r="B14" t="s">
-        <v>472</v>
+      <c r="A14" s="36" t="s">
+        <v>402</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>448</v>
       </c>
       <c r="C14" t="s">
-        <v>465</v>
-      </c>
-      <c r="D14" t="s">
-        <v>478</v>
-      </c>
-      <c r="E14" t="s">
-        <v>479</v>
-      </c>
-      <c r="F14" t="s">
-        <v>480</v>
-      </c>
-      <c r="G14" t="s">
-        <v>481</v>
+        <v>454</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>585</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>584</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>455</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>453</v>
       </c>
       <c r="H14" s="19"/>
       <c r="I14" s="18"/>
       <c r="J14" s="38" t="s">
-        <v>627</v>
+        <v>612</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>632</v>
+        <v>615</v>
       </c>
       <c r="L14" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>633</v>
+        <v>617</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="O14" s="3"/>
       <c r="P14" s="5"/>
@@ -49455,44 +49349,40 @@
       <c r="AA14" s="5"/>
       <c r="AB14" s="5"/>
     </row>
-    <row r="15" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="45" t="s">
-        <v>418</v>
-      </c>
-      <c r="B15" t="s">
-        <v>472</v>
-      </c>
-      <c r="C15" t="s">
-        <v>470</v>
-      </c>
-      <c r="D15" t="s">
-        <v>482</v>
-      </c>
-      <c r="E15" t="s">
-        <v>483</v>
-      </c>
-      <c r="F15" t="s">
-        <v>484</v>
-      </c>
-      <c r="G15" t="s">
-        <v>485</v>
+    <row r="15" spans="1:28" ht="113" x14ac:dyDescent="0.3">
+      <c r="A15" s="36" t="s">
+        <v>402</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>443</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="19" t="s">
+        <v>444</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>447</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>446</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>445</v>
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="18"/>
-      <c r="J15" s="38" t="s">
-        <v>628</v>
-      </c>
+      <c r="J15" s="18"/>
       <c r="K15" s="1" t="s">
-        <v>634</v>
+        <v>582</v>
       </c>
       <c r="L15" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>633</v>
+        <v>16</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="O15" s="3"/>
       <c r="P15" s="5"/>
@@ -49510,36 +49400,40 @@
       <c r="AB15" s="5"/>
     </row>
     <row r="16" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="36" t="s">
-        <v>418</v>
+      <c r="A16" s="45" t="s">
+        <v>402</v>
       </c>
       <c r="B16" t="s">
-        <v>473</v>
-      </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15" t="s">
-        <v>474</v>
+        <v>456</v>
+      </c>
+      <c r="C16" t="s">
+        <v>449</v>
+      </c>
+      <c r="D16" t="s">
+        <v>462</v>
       </c>
       <c r="E16" t="s">
-        <v>475</v>
+        <v>463</v>
       </c>
       <c r="F16" t="s">
-        <v>476</v>
+        <v>464</v>
       </c>
       <c r="G16" t="s">
-        <v>477</v>
+        <v>465</v>
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
+      <c r="J16" s="38" t="s">
+        <v>611</v>
+      </c>
       <c r="K16" s="1" t="s">
-        <v>245</v>
+        <v>616</v>
       </c>
       <c r="L16" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>3</v>
+        <v>617</v>
       </c>
       <c r="N16" s="4" t="s">
         <v>8</v>
@@ -49559,38 +49453,44 @@
       <c r="AA16" s="5"/>
       <c r="AB16" s="5"/>
     </row>
-    <row r="17" spans="1:28" ht="101" x14ac:dyDescent="0.35">
-      <c r="A17" s="36" t="s">
-        <v>418</v>
+    <row r="17" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="45" t="s">
+        <v>402</v>
       </c>
       <c r="B17" t="s">
-        <v>486</v>
-      </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10" t="s">
-        <v>490</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>489</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>488</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>487</v>
-      </c>
-      <c r="H17" s="10"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
+        <v>456</v>
+      </c>
+      <c r="C17" t="s">
+        <v>454</v>
+      </c>
+      <c r="D17" t="s">
+        <v>466</v>
+      </c>
+      <c r="E17" t="s">
+        <v>467</v>
+      </c>
+      <c r="F17" t="s">
+        <v>468</v>
+      </c>
+      <c r="G17" t="s">
+        <v>469</v>
+      </c>
+      <c r="H17" s="19"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="38" t="s">
+        <v>612</v>
+      </c>
       <c r="K17" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="L17" s="12"/>
+        <v>618</v>
+      </c>
+      <c r="L17" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="M17" s="4" t="s">
-        <v>16</v>
+        <v>617</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="O17" s="3"/>
       <c r="P17" s="5"/>
@@ -49607,38 +49507,40 @@
       <c r="AA17" s="5"/>
       <c r="AB17" s="5"/>
     </row>
-    <row r="18" spans="1:28" ht="151" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A18" s="36" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="B18" t="s">
-        <v>492</v>
-      </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10" t="s">
-        <v>493</v>
+        <v>457</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15" t="s">
+        <v>458</v>
       </c>
       <c r="E18" t="s">
-        <v>494</v>
+        <v>459</v>
       </c>
       <c r="F18" t="s">
-        <v>495</v>
+        <v>460</v>
       </c>
       <c r="G18" t="s">
-        <v>602</v>
-      </c>
-      <c r="H18" s="10"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
+        <v>461</v>
+      </c>
+      <c r="H18" s="19"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
       <c r="K18" s="1" t="s">
-        <v>603</v>
-      </c>
-      <c r="L18" s="12"/>
+        <v>245</v>
+      </c>
+      <c r="L18" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="M18" s="4" t="s">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="O18" s="3"/>
       <c r="P18" s="5"/>
@@ -49657,35 +49559,33 @@
     </row>
     <row r="19" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A19" s="36" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="B19" t="s">
-        <v>496</v>
-      </c>
-      <c r="C19" s="16"/>
-      <c r="D19" t="s">
-        <v>497</v>
-      </c>
-      <c r="E19" t="s">
-        <v>498</v>
-      </c>
-      <c r="F19" t="s">
-        <v>499</v>
-      </c>
-      <c r="G19" t="s">
-        <v>604</v>
-      </c>
-      <c r="H19" s="20"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
+        <v>470</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>473</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="H19" s="10"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
       <c r="K19" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="L19" s="14" t="s">
-        <v>46</v>
-      </c>
+        <v>475</v>
+      </c>
+      <c r="L19" s="12"/>
       <c r="M19" s="4" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="N19" s="4" t="s">
         <v>13</v>
@@ -49705,37 +49605,35 @@
       <c r="AA19" s="5"/>
       <c r="AB19" s="5"/>
     </row>
-    <row r="20" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:28" ht="151" x14ac:dyDescent="0.35">
       <c r="A20" s="36" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="B20" t="s">
-        <v>501</v>
-      </c>
-      <c r="C20" s="16"/>
-      <c r="D20" t="s">
-        <v>503</v>
+        <v>476</v>
+      </c>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10" t="s">
+        <v>477</v>
       </c>
       <c r="E20" t="s">
-        <v>502</v>
+        <v>478</v>
       </c>
       <c r="F20" t="s">
-        <v>499</v>
+        <v>479</v>
       </c>
       <c r="G20" t="s">
-        <v>604</v>
-      </c>
-      <c r="H20" s="20"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+        <v>586</v>
+      </c>
+      <c r="H20" s="10"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
       <c r="K20" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="L20" s="14" t="s">
-        <v>46</v>
-      </c>
+        <v>587</v>
+      </c>
+      <c r="L20" s="12"/>
       <c r="M20" s="4" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="N20" s="4" t="s">
         <v>13</v>
@@ -49755,44 +49653,40 @@
       <c r="AA20" s="5"/>
       <c r="AB20" s="5"/>
     </row>
-    <row r="21" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A21" s="36" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="B21" t="s">
-        <v>505</v>
-      </c>
-      <c r="C21" t="s">
-        <v>506</v>
-      </c>
+        <v>480</v>
+      </c>
+      <c r="C21" s="16"/>
       <c r="D21" t="s">
-        <v>507</v>
+        <v>481</v>
       </c>
       <c r="E21" t="s">
-        <v>508</v>
+        <v>482</v>
       </c>
       <c r="F21" t="s">
-        <v>509</v>
+        <v>483</v>
       </c>
       <c r="G21" t="s">
-        <v>510</v>
+        <v>588</v>
       </c>
       <c r="H21" s="20"/>
       <c r="I21" s="18"/>
-      <c r="J21" s="38" t="s">
-        <v>645</v>
-      </c>
+      <c r="J21" s="18"/>
       <c r="K21" s="1" t="s">
-        <v>635</v>
+        <v>484</v>
       </c>
       <c r="L21" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>637</v>
+        <v>4</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="O21" s="3"/>
       <c r="P21" s="5"/>
@@ -49809,44 +49703,40 @@
       <c r="AA21" s="5"/>
       <c r="AB21" s="5"/>
     </row>
-    <row r="22" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A22" s="36" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="B22" t="s">
-        <v>505</v>
-      </c>
-      <c r="C22" s="30" t="s">
-        <v>511</v>
-      </c>
-      <c r="D22" s="30" t="s">
-        <v>513</v>
-      </c>
-      <c r="E22" s="30" t="s">
-        <v>512</v>
+        <v>485</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" t="s">
+        <v>487</v>
+      </c>
+      <c r="E22" t="s">
+        <v>486</v>
       </c>
       <c r="F22" t="s">
-        <v>509</v>
+        <v>483</v>
       </c>
       <c r="G22" t="s">
-        <v>510</v>
+        <v>588</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="18"/>
-      <c r="J22" s="38" t="s">
-        <v>646</v>
-      </c>
+      <c r="J22" s="18"/>
       <c r="K22" s="1" t="s">
-        <v>636</v>
+        <v>488</v>
       </c>
       <c r="L22" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>637</v>
+        <v>4</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="O22" s="3"/>
       <c r="P22" s="5"/>
@@ -49863,43 +49753,46 @@
       <c r="AA22" s="5"/>
       <c r="AB22" s="5"/>
     </row>
-    <row r="23" spans="1:28" ht="87" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A23" s="36" t="s">
-        <v>418</v>
-      </c>
-      <c r="B23" s="30" t="s">
-        <v>514</v>
-      </c>
-      <c r="D23" s="30" t="s">
-        <v>515</v>
-      </c>
-      <c r="E23" s="30" t="s">
-        <v>516</v>
-      </c>
-      <c r="F23" s="35" t="s">
-        <v>517</v>
-      </c>
-      <c r="G23" s="30" t="s">
-        <v>518</v>
+        <v>402</v>
+      </c>
+      <c r="B23" t="s">
+        <v>489</v>
+      </c>
+      <c r="C23" t="s">
+        <v>490</v>
+      </c>
+      <c r="D23" t="s">
+        <v>491</v>
+      </c>
+      <c r="E23" t="s">
+        <v>492</v>
+      </c>
+      <c r="F23" t="s">
+        <v>493</v>
+      </c>
+      <c r="G23" t="s">
+        <v>494</v>
       </c>
       <c r="H23" s="20"/>
       <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
+      <c r="J23" s="38" t="s">
+        <v>629</v>
+      </c>
       <c r="K23" s="1" t="s">
-        <v>519</v>
+        <v>619</v>
       </c>
       <c r="L23" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>16</v>
+        <v>621</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O23" s="3" t="s">
-        <v>520</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="O23" s="3"/>
       <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
       <c r="R23" s="5"/>
@@ -49914,92 +49807,97 @@
       <c r="AA23" s="5"/>
       <c r="AB23" s="5"/>
     </row>
-    <row r="24" spans="1:28" s="29" customFormat="1" ht="101" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A24" s="36" t="s">
-        <v>418</v>
-      </c>
-      <c r="B24" s="30" t="s">
-        <v>521</v>
-      </c>
-      <c r="C24" s="17"/>
+        <v>402</v>
+      </c>
+      <c r="B24" t="s">
+        <v>489</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>495</v>
+      </c>
       <c r="D24" s="30" t="s">
-        <v>524</v>
+        <v>497</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>523</v>
-      </c>
-      <c r="F24" s="33" t="s">
-        <v>522</v>
-      </c>
-      <c r="G24" s="17" t="s">
-        <v>434</v>
-      </c>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="26" t="s">
-        <v>438</v>
-      </c>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="N24" s="27" t="s">
-        <v>13</v>
+        <v>496</v>
+      </c>
+      <c r="F24" t="s">
+        <v>493</v>
+      </c>
+      <c r="G24" t="s">
+        <v>494</v>
+      </c>
+      <c r="H24" s="20"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="38" t="s">
+        <v>630</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="L24" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>621</v>
+      </c>
+      <c r="N24" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="O24" s="3"/>
-      <c r="P24" s="28"/>
-      <c r="Q24" s="28"/>
-      <c r="R24" s="28"/>
-      <c r="S24" s="28"/>
-      <c r="T24" s="28"/>
-      <c r="U24" s="28"/>
-      <c r="V24" s="28"/>
-      <c r="W24" s="28"/>
-      <c r="X24" s="28"/>
-      <c r="Y24" s="28"/>
-      <c r="Z24" s="28"/>
-      <c r="AA24" s="28"/>
-      <c r="AB24" s="28"/>
-    </row>
-    <row r="25" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="5"/>
+      <c r="T24" s="5"/>
+      <c r="U24" s="5"/>
+      <c r="V24" s="5"/>
+      <c r="W24" s="5"/>
+      <c r="X24" s="5"/>
+      <c r="Y24" s="5"/>
+      <c r="Z24" s="5"/>
+      <c r="AA24" s="5"/>
+      <c r="AB24" s="5"/>
+    </row>
+    <row r="25" spans="1:28" ht="87" x14ac:dyDescent="0.35">
       <c r="A25" s="36" t="s">
-        <v>418</v>
-      </c>
-      <c r="B25" t="s">
-        <v>525</v>
-      </c>
-      <c r="C25" t="s">
-        <v>526</v>
+        <v>402</v>
+      </c>
+      <c r="B25" s="30" t="s">
+        <v>498</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>529</v>
+        <v>499</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>528</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>527</v>
-      </c>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="38" t="s">
-        <v>647</v>
-      </c>
-      <c r="K25" s="8" t="s">
-        <v>638</v>
+        <v>500</v>
+      </c>
+      <c r="F25" s="35" t="s">
+        <v>501</v>
+      </c>
+      <c r="G25" s="30" t="s">
+        <v>502</v>
+      </c>
+      <c r="H25" s="20"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="1" t="s">
+        <v>503</v>
       </c>
       <c r="L25" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>637</v>
+        <v>16</v>
       </c>
       <c r="N25" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O25" s="3"/>
+      <c r="O25" s="3" t="s">
+        <v>504</v>
+      </c>
       <c r="P25" s="5"/>
       <c r="Q25" s="5"/>
       <c r="R25" s="5"/>
@@ -50014,91 +49912,87 @@
       <c r="AA25" s="5"/>
       <c r="AB25" s="5"/>
     </row>
-    <row r="26" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:28" s="29" customFormat="1" ht="101" x14ac:dyDescent="0.35">
       <c r="A26" s="36" t="s">
+        <v>402</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>505</v>
+      </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="30" t="s">
+        <v>508</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>507</v>
+      </c>
+      <c r="F26" s="33" t="s">
+        <v>506</v>
+      </c>
+      <c r="G26" s="17" t="s">
         <v>418</v>
       </c>
-      <c r="B26" t="s">
-        <v>525</v>
-      </c>
-      <c r="C26" s="30" t="s">
-        <v>530</v>
-      </c>
-      <c r="D26" s="30" t="s">
-        <v>532</v>
-      </c>
-      <c r="E26" s="30" t="s">
-        <v>531</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>527</v>
-      </c>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="38" t="s">
-        <v>648</v>
-      </c>
-      <c r="K26" s="8" t="s">
-        <v>639</v>
-      </c>
-      <c r="L26" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="M26" s="4" t="s">
-        <v>637</v>
-      </c>
-      <c r="N26" s="4" t="s">
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="26" t="s">
+        <v>422</v>
+      </c>
+      <c r="L26" s="27"/>
+      <c r="M26" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="N26" s="27" t="s">
         <v>13</v>
       </c>
       <c r="O26" s="3"/>
-      <c r="P26" s="5"/>
-      <c r="Q26" s="5"/>
-      <c r="R26" s="5"/>
-      <c r="S26" s="5"/>
-      <c r="T26" s="5"/>
-      <c r="U26" s="5"/>
-      <c r="V26" s="5"/>
-      <c r="W26" s="5"/>
-      <c r="X26" s="5"/>
-      <c r="Y26" s="5"/>
-      <c r="Z26" s="5"/>
-      <c r="AA26" s="5"/>
-      <c r="AB26" s="5"/>
+      <c r="P26" s="28"/>
+      <c r="Q26" s="28"/>
+      <c r="R26" s="28"/>
+      <c r="S26" s="28"/>
+      <c r="T26" s="28"/>
+      <c r="U26" s="28"/>
+      <c r="V26" s="28"/>
+      <c r="W26" s="28"/>
+      <c r="X26" s="28"/>
+      <c r="Y26" s="28"/>
+      <c r="Z26" s="28"/>
+      <c r="AA26" s="28"/>
+      <c r="AB26" s="28"/>
     </row>
     <row r="27" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A27" s="36" t="s">
-        <v>418</v>
-      </c>
-      <c r="B27" s="30" t="s">
-        <v>533</v>
+        <v>402</v>
+      </c>
+      <c r="B27" t="s">
+        <v>509</v>
       </c>
       <c r="C27" t="s">
-        <v>526</v>
+        <v>510</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>534</v>
+        <v>513</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>535</v>
-      </c>
-      <c r="F27" s="30" t="s">
-        <v>536</v>
+        <v>512</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>511</v>
       </c>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
       <c r="I27" s="7"/>
       <c r="J27" s="38" t="s">
-        <v>647</v>
+        <v>631</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>640</v>
+        <v>622</v>
       </c>
       <c r="L27" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>637</v>
+        <v>621</v>
       </c>
       <c r="N27" s="4" t="s">
         <v>13</v>
@@ -50120,37 +50014,37 @@
     </row>
     <row r="28" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A28" s="36" t="s">
-        <v>418</v>
-      </c>
-      <c r="B28" s="30" t="s">
-        <v>533</v>
+        <v>402</v>
+      </c>
+      <c r="B28" t="s">
+        <v>509</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>537</v>
+        <v>514</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>538</v>
+        <v>516</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>539</v>
-      </c>
-      <c r="F28" s="30" t="s">
-        <v>536</v>
+        <v>515</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>511</v>
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
       <c r="I28" s="7"/>
       <c r="J28" s="38" t="s">
-        <v>649</v>
+        <v>632</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>641</v>
+        <v>623</v>
       </c>
       <c r="L28" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>637</v>
+        <v>621</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>13</v>
@@ -50172,35 +50066,37 @@
     </row>
     <row r="29" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A29" s="36" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="B29" s="30" t="s">
-        <v>540</v>
-      </c>
-      <c r="C29" s="16"/>
+        <v>517</v>
+      </c>
+      <c r="C29" t="s">
+        <v>510</v>
+      </c>
       <c r="D29" s="30" t="s">
-        <v>541</v>
+        <v>518</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>542</v>
+        <v>519</v>
       </c>
       <c r="F29" s="30" t="s">
-        <v>543</v>
-      </c>
-      <c r="G29" s="30" t="s">
-        <v>544</v>
-      </c>
-      <c r="H29" s="20"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="1" t="s">
-        <v>240</v>
+        <v>520</v>
+      </c>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="38" t="s">
+        <v>631</v>
+      </c>
+      <c r="K29" s="8" t="s">
+        <v>624</v>
       </c>
       <c r="L29" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>4</v>
+        <v>621</v>
       </c>
       <c r="N29" s="4" t="s">
         <v>13</v>
@@ -50222,38 +50118,40 @@
     </row>
     <row r="30" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A30" s="36" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>545</v>
-      </c>
-      <c r="C30" s="16"/>
+        <v>517</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>521</v>
+      </c>
       <c r="D30" s="30" t="s">
-        <v>546</v>
+        <v>522</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>547</v>
+        <v>523</v>
       </c>
       <c r="F30" s="30" t="s">
-        <v>548</v>
-      </c>
-      <c r="G30" s="30" t="s">
-        <v>549</v>
-      </c>
-      <c r="H30" s="20"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="1" t="s">
-        <v>550</v>
+        <v>520</v>
+      </c>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="38" t="s">
+        <v>633</v>
+      </c>
+      <c r="K30" s="8" t="s">
+        <v>625</v>
       </c>
       <c r="L30" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>4</v>
+        <v>621</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="O30" s="3"/>
       <c r="P30" s="5"/>
@@ -50270,44 +50168,40 @@
       <c r="AA30" s="5"/>
       <c r="AB30" s="5"/>
     </row>
-    <row r="31" spans="1:28" ht="126" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A31" s="36" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>551</v>
-      </c>
-      <c r="C31" s="30" t="s">
-        <v>552</v>
-      </c>
+        <v>524</v>
+      </c>
+      <c r="C31" s="16"/>
       <c r="D31" s="30" t="s">
-        <v>553</v>
+        <v>525</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>554</v>
+        <v>526</v>
       </c>
       <c r="F31" s="30" t="s">
-        <v>555</v>
+        <v>527</v>
       </c>
       <c r="G31" s="30" t="s">
-        <v>556</v>
+        <v>528</v>
       </c>
       <c r="H31" s="20"/>
       <c r="I31" s="18"/>
-      <c r="J31" s="38" t="s">
-        <v>650</v>
-      </c>
+      <c r="J31" s="18"/>
       <c r="K31" s="1" t="s">
-        <v>642</v>
+        <v>240</v>
       </c>
       <c r="L31" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>664</v>
+        <v>4</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="O31" s="3"/>
       <c r="P31" s="5"/>
@@ -50324,41 +50218,37 @@
       <c r="AA31" s="5"/>
       <c r="AB31" s="5"/>
     </row>
-    <row r="32" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A32" s="36" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>551</v>
-      </c>
-      <c r="C32" s="30" t="s">
-        <v>557</v>
-      </c>
+        <v>529</v>
+      </c>
+      <c r="C32" s="16"/>
       <c r="D32" s="30" t="s">
-        <v>561</v>
+        <v>530</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>560</v>
+        <v>531</v>
       </c>
       <c r="F32" s="30" t="s">
-        <v>559</v>
+        <v>532</v>
       </c>
       <c r="G32" s="30" t="s">
-        <v>558</v>
+        <v>533</v>
       </c>
       <c r="H32" s="20"/>
       <c r="I32" s="18"/>
-      <c r="J32" s="38" t="s">
-        <v>651</v>
-      </c>
+      <c r="J32" s="18"/>
       <c r="K32" s="1" t="s">
-        <v>643</v>
+        <v>534</v>
       </c>
       <c r="L32" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>664</v>
+        <v>4</v>
       </c>
       <c r="N32" s="4" t="s">
         <v>8</v>
@@ -50378,41 +50268,41 @@
       <c r="AA32" s="5"/>
       <c r="AB32" s="5"/>
     </row>
-    <row r="33" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:28" ht="126" x14ac:dyDescent="0.35">
       <c r="A33" s="36" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>551</v>
+        <v>535</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>562</v>
+        <v>536</v>
       </c>
       <c r="D33" s="30" t="s">
-        <v>564</v>
+        <v>537</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>563</v>
+        <v>538</v>
       </c>
       <c r="F33" s="30" t="s">
-        <v>559</v>
+        <v>539</v>
       </c>
       <c r="G33" s="30" t="s">
-        <v>558</v>
+        <v>540</v>
       </c>
       <c r="H33" s="20"/>
       <c r="I33" s="18"/>
       <c r="J33" s="38" t="s">
-        <v>652</v>
+        <v>634</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>644</v>
+        <v>626</v>
       </c>
       <c r="L33" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>664</v>
+        <v>648</v>
       </c>
       <c r="N33" s="4" t="s">
         <v>8</v>
@@ -50432,40 +50322,44 @@
       <c r="AA33" s="5"/>
       <c r="AB33" s="5"/>
     </row>
-    <row r="34" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A34" s="36" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>571</v>
-      </c>
-      <c r="C34" s="30"/>
+        <v>535</v>
+      </c>
+      <c r="C34" s="30" t="s">
+        <v>541</v>
+      </c>
       <c r="D34" s="30" t="s">
-        <v>575</v>
+        <v>545</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>574</v>
+        <v>544</v>
       </c>
       <c r="F34" s="30" t="s">
-        <v>573</v>
+        <v>543</v>
       </c>
       <c r="G34" s="30" t="s">
-        <v>572</v>
+        <v>542</v>
       </c>
       <c r="H34" s="20"/>
       <c r="I34" s="18"/>
-      <c r="J34" s="18"/>
+      <c r="J34" s="38" t="s">
+        <v>635</v>
+      </c>
       <c r="K34" s="1" t="s">
-        <v>576</v>
+        <v>627</v>
       </c>
       <c r="L34" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>4</v>
+        <v>648</v>
       </c>
       <c r="N34" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="O34" s="3"/>
       <c r="P34" s="5"/>
@@ -50482,37 +50376,41 @@
       <c r="AA34" s="5"/>
       <c r="AB34" s="5"/>
     </row>
-    <row r="35" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A35" s="36" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="B35" s="30" t="s">
-        <v>565</v>
-      </c>
-      <c r="C35" s="30"/>
+        <v>535</v>
+      </c>
+      <c r="C35" s="30" t="s">
+        <v>546</v>
+      </c>
       <c r="D35" s="30" t="s">
-        <v>566</v>
+        <v>548</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>569</v>
+        <v>547</v>
       </c>
       <c r="F35" s="30" t="s">
-        <v>568</v>
+        <v>543</v>
       </c>
       <c r="G35" s="30" t="s">
-        <v>567</v>
+        <v>542</v>
       </c>
       <c r="H35" s="20"/>
       <c r="I35" s="18"/>
-      <c r="J35" s="18"/>
+      <c r="J35" s="38" t="s">
+        <v>636</v>
+      </c>
       <c r="K35" s="1" t="s">
-        <v>570</v>
+        <v>628</v>
       </c>
       <c r="L35" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>4</v>
+        <v>648</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>8</v>
@@ -50534,29 +50432,29 @@
     </row>
     <row r="36" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A36" s="36" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>583</v>
-      </c>
-      <c r="C36" s="16"/>
+        <v>555</v>
+      </c>
+      <c r="C36" s="30"/>
       <c r="D36" s="30" t="s">
-        <v>587</v>
+        <v>559</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>586</v>
+        <v>558</v>
       </c>
       <c r="F36" s="30" t="s">
-        <v>585</v>
-      </c>
-      <c r="G36" s="20" t="s">
-        <v>584</v>
+        <v>557</v>
+      </c>
+      <c r="G36" s="30" t="s">
+        <v>556</v>
       </c>
       <c r="H36" s="20"/>
       <c r="I36" s="18"/>
       <c r="J36" s="18"/>
       <c r="K36" s="1" t="s">
-        <v>588</v>
+        <v>560</v>
       </c>
       <c r="L36" s="14" t="s">
         <v>46</v>
@@ -50584,29 +50482,29 @@
     </row>
     <row r="37" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A37" s="36" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="B37" s="30" t="s">
-        <v>577</v>
-      </c>
-      <c r="C37" s="16"/>
+        <v>549</v>
+      </c>
+      <c r="C37" s="30"/>
       <c r="D37" s="30" t="s">
-        <v>581</v>
+        <v>550</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>580</v>
+        <v>553</v>
       </c>
       <c r="F37" s="30" t="s">
-        <v>579</v>
-      </c>
-      <c r="G37" s="33" t="s">
-        <v>578</v>
+        <v>552</v>
+      </c>
+      <c r="G37" s="30" t="s">
+        <v>551</v>
       </c>
       <c r="H37" s="20"/>
       <c r="I37" s="18"/>
       <c r="J37" s="18"/>
       <c r="K37" s="1" t="s">
-        <v>582</v>
+        <v>554</v>
       </c>
       <c r="L37" s="14" t="s">
         <v>46</v>
@@ -50634,29 +50532,29 @@
     </row>
     <row r="38" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A38" s="36" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="B38" s="30" t="s">
-        <v>589</v>
-      </c>
-      <c r="C38" s="15"/>
+        <v>567</v>
+      </c>
+      <c r="C38" s="16"/>
       <c r="D38" s="30" t="s">
-        <v>593</v>
+        <v>571</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>592</v>
+        <v>570</v>
       </c>
       <c r="F38" s="30" t="s">
-        <v>591</v>
-      </c>
-      <c r="G38" s="30" t="s">
-        <v>590</v>
-      </c>
-      <c r="H38" s="19"/>
+        <v>569</v>
+      </c>
+      <c r="G38" s="20" t="s">
+        <v>568</v>
+      </c>
+      <c r="H38" s="20"/>
       <c r="I38" s="18"/>
       <c r="J38" s="18"/>
       <c r="K38" s="1" t="s">
-        <v>595</v>
+        <v>572</v>
       </c>
       <c r="L38" s="14" t="s">
         <v>46</v>
@@ -50667,9 +50565,7 @@
       <c r="N38" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O38" s="3" t="s">
-        <v>594</v>
-      </c>
+      <c r="O38" s="3"/>
       <c r="P38" s="5"/>
       <c r="Q38" s="5"/>
       <c r="R38" s="5"/>
@@ -50684,50 +50580,42 @@
       <c r="AA38" s="5"/>
       <c r="AB38" s="5"/>
     </row>
-    <row r="39" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="B39" t="s">
-        <v>374</v>
-      </c>
-      <c r="C39" t="s">
-        <v>369</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>605</v>
-      </c>
-      <c r="E39" s="10" t="s">
-        <v>606</v>
-      </c>
-      <c r="F39" s="10" t="s">
-        <v>607</v>
-      </c>
-      <c r="G39" s="10" t="s">
-        <v>608</v>
-      </c>
-      <c r="H39" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="I39" s="7"/>
-      <c r="J39" s="38" t="s">
-        <v>653</v>
-      </c>
-      <c r="K39" s="8" t="s">
-        <v>666</v>
-      </c>
-      <c r="L39" s="11" t="s">
-        <v>11</v>
+    <row r="39" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+      <c r="A39" s="36" t="s">
+        <v>402</v>
+      </c>
+      <c r="B39" s="30" t="s">
+        <v>561</v>
+      </c>
+      <c r="C39" s="16"/>
+      <c r="D39" s="30" t="s">
+        <v>565</v>
+      </c>
+      <c r="E39" s="30" t="s">
+        <v>564</v>
+      </c>
+      <c r="F39" s="30" t="s">
+        <v>563</v>
+      </c>
+      <c r="G39" s="33" t="s">
+        <v>562</v>
+      </c>
+      <c r="H39" s="20"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="L39" s="14" t="s">
+        <v>46</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>633</v>
+        <v>4</v>
       </c>
       <c r="N39" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O39" s="3" t="s">
-        <v>609</v>
-      </c>
+      <c r="O39" s="3"/>
       <c r="P39" s="5"/>
       <c r="Q39" s="5"/>
       <c r="R39" s="5"/>
@@ -50742,48 +50630,44 @@
       <c r="AA39" s="5"/>
       <c r="AB39" s="5"/>
     </row>
-    <row r="40" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="B40" t="s">
-        <v>368</v>
-      </c>
-      <c r="C40" t="s">
-        <v>369</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>610</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>372</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>371</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>370</v>
-      </c>
-      <c r="H40" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="I40" s="7"/>
-      <c r="J40" s="38" t="s">
-        <v>653</v>
-      </c>
-      <c r="K40" s="8" t="s">
-        <v>667</v>
-      </c>
-      <c r="L40" s="11" t="s">
-        <v>11</v>
+    <row r="40" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+      <c r="A40" s="36" t="s">
+        <v>402</v>
+      </c>
+      <c r="B40" s="30" t="s">
+        <v>573</v>
+      </c>
+      <c r="C40" s="15"/>
+      <c r="D40" s="30" t="s">
+        <v>577</v>
+      </c>
+      <c r="E40" s="30" t="s">
+        <v>576</v>
+      </c>
+      <c r="F40" s="30" t="s">
+        <v>575</v>
+      </c>
+      <c r="G40" s="30" t="s">
+        <v>574</v>
+      </c>
+      <c r="H40" s="19"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
+      <c r="K40" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="L40" s="14" t="s">
+        <v>46</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>633</v>
+        <v>4</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="O40" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="O40" s="3" t="s">
+        <v>578</v>
+      </c>
       <c r="P40" s="5"/>
       <c r="Q40" s="5"/>
       <c r="R40" s="5"/>
@@ -50803,43 +50687,45 @@
         <v>310</v>
       </c>
       <c r="B41" t="s">
+        <v>362</v>
+      </c>
+      <c r="C41" t="s">
         <v>358</v>
       </c>
-      <c r="C41" t="s">
-        <v>359</v>
-      </c>
       <c r="D41" s="10" t="s">
-        <v>611</v>
+        <v>589</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>612</v>
+        <v>590</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>613</v>
+        <v>591</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>360</v>
+        <v>592</v>
       </c>
       <c r="H41" s="10" t="s">
         <v>188</v>
       </c>
       <c r="I41" s="7"/>
       <c r="J41" s="38" t="s">
-        <v>654</v>
+        <v>637</v>
       </c>
       <c r="K41" s="8" t="s">
-        <v>668</v>
+        <v>650</v>
       </c>
       <c r="L41" s="11" t="s">
         <v>11</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>633</v>
+        <v>617</v>
       </c>
       <c r="N41" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O41" s="3"/>
+      <c r="O41" s="3" t="s">
+        <v>593</v>
+      </c>
       <c r="P41" s="5"/>
       <c r="Q41" s="5"/>
       <c r="R41" s="5"/>
@@ -50859,38 +50745,38 @@
         <v>310</v>
       </c>
       <c r="B42" t="s">
+        <v>357</v>
+      </c>
+      <c r="C42" t="s">
         <v>358</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" s="7" t="s">
+        <v>594</v>
+      </c>
+      <c r="E42" s="7" t="s">
         <v>361</v>
       </c>
-      <c r="D42" s="10" t="s">
-        <v>614</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>615</v>
-      </c>
-      <c r="F42" s="10" t="s">
-        <v>616</v>
-      </c>
-      <c r="G42" s="10" t="s">
-        <v>362</v>
-      </c>
-      <c r="H42" s="10" t="s">
+      <c r="F42" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="H42" s="7" t="s">
         <v>188</v>
       </c>
       <c r="I42" s="7"/>
       <c r="J42" s="38" t="s">
-        <v>655</v>
+        <v>637</v>
       </c>
       <c r="K42" s="8" t="s">
-        <v>669</v>
+        <v>651</v>
       </c>
       <c r="L42" s="11" t="s">
         <v>11</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>633</v>
+        <v>617</v>
       </c>
       <c r="N42" s="4" t="s">
         <v>8</v>
@@ -50915,38 +50801,38 @@
         <v>310</v>
       </c>
       <c r="B43" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="C43" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>617</v>
+        <v>595</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>618</v>
+        <v>596</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>619</v>
+        <v>597</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
       <c r="H43" s="10" t="s">
         <v>188</v>
       </c>
       <c r="I43" s="7"/>
       <c r="J43" s="38" t="s">
-        <v>656</v>
+        <v>638</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>670</v>
+        <v>652</v>
       </c>
       <c r="L43" s="11" t="s">
         <v>11</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>633</v>
+        <v>617</v>
       </c>
       <c r="N43" s="4" t="s">
         <v>8</v>
@@ -50966,39 +50852,43 @@
       <c r="AA43" s="5"/>
       <c r="AB43" s="5"/>
     </row>
-    <row r="44" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B44" t="s">
-        <v>352</v>
-      </c>
-      <c r="C44"/>
-      <c r="D44" t="s">
+        <v>350</v>
+      </c>
+      <c r="C44" t="s">
         <v>353</v>
       </c>
-      <c r="E44" t="s">
+      <c r="D44" s="10" t="s">
+        <v>598</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>599</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>600</v>
+      </c>
+      <c r="G44" s="10" t="s">
         <v>354</v>
-      </c>
-      <c r="F44" t="s">
-        <v>355</v>
-      </c>
-      <c r="G44" t="s">
-        <v>356</v>
       </c>
       <c r="H44" s="10" t="s">
         <v>188</v>
       </c>
       <c r="I44" s="7"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="L44" s="4" t="s">
-        <v>2</v>
+      <c r="J44" s="38" t="s">
+        <v>639</v>
+      </c>
+      <c r="K44" s="8" t="s">
+        <v>653</v>
+      </c>
+      <c r="L44" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>3</v>
+        <v>617</v>
       </c>
       <c r="N44" s="4" t="s">
         <v>8</v>
@@ -51023,36 +50913,38 @@
         <v>310</v>
       </c>
       <c r="B45" t="s">
-        <v>311</v>
+        <v>350</v>
       </c>
       <c r="C45" t="s">
-        <v>313</v>
-      </c>
-      <c r="D45" s="30" t="s">
-        <v>315</v>
-      </c>
-      <c r="E45" s="30" t="s">
-        <v>316</v>
-      </c>
-      <c r="F45" s="30" t="s">
-        <v>317</v>
-      </c>
-      <c r="G45" s="30" t="s">
-        <v>318</v>
-      </c>
-      <c r="H45" s="7"/>
+        <v>355</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>601</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>602</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>603</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>188</v>
+      </c>
       <c r="I45" s="7"/>
       <c r="J45" s="38" t="s">
-        <v>657</v>
+        <v>640</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>671</v>
-      </c>
-      <c r="L45" s="4" t="s">
-        <v>2</v>
+        <v>654</v>
+      </c>
+      <c r="L45" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>665</v>
+        <v>617</v>
       </c>
       <c r="N45" s="4" t="s">
         <v>8</v>
@@ -51072,41 +50964,39 @@
       <c r="AA45" s="5"/>
       <c r="AB45" s="5"/>
     </row>
-    <row r="46" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B46" t="s">
-        <v>311</v>
-      </c>
-      <c r="C46" t="s">
-        <v>314</v>
-      </c>
-      <c r="D46" s="30" t="s">
-        <v>319</v>
-      </c>
-      <c r="E46" s="30" t="s">
-        <v>320</v>
-      </c>
-      <c r="F46" s="30" t="s">
-        <v>321</v>
-      </c>
-      <c r="G46" s="30" t="s">
-        <v>322</v>
-      </c>
-      <c r="H46" s="7"/>
+        <v>344</v>
+      </c>
+      <c r="C46"/>
+      <c r="D46" t="s">
+        <v>345</v>
+      </c>
+      <c r="E46" t="s">
+        <v>346</v>
+      </c>
+      <c r="F46" t="s">
+        <v>347</v>
+      </c>
+      <c r="G46" t="s">
+        <v>348</v>
+      </c>
+      <c r="H46" s="10" t="s">
+        <v>188</v>
+      </c>
       <c r="I46" s="7"/>
-      <c r="J46" s="38" t="s">
-        <v>658</v>
-      </c>
-      <c r="K46" s="8" t="s">
-        <v>672</v>
+      <c r="J46" s="7"/>
+      <c r="K46" s="1" t="s">
+        <v>349</v>
       </c>
       <c r="L46" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>665</v>
+        <v>3</v>
       </c>
       <c r="N46" s="4" t="s">
         <v>8</v>
@@ -51134,33 +51024,33 @@
         <v>311</v>
       </c>
       <c r="C47" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="D47" s="30" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="E47" s="30" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F47" s="30" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="G47" s="30" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="H47" s="7"/>
       <c r="I47" s="7"/>
       <c r="J47" s="38" t="s">
-        <v>659</v>
+        <v>641</v>
       </c>
       <c r="K47" s="8" t="s">
-        <v>673</v>
+        <v>655</v>
       </c>
       <c r="L47" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>633</v>
+        <v>649</v>
       </c>
       <c r="N47" s="4" t="s">
         <v>8</v>
@@ -51188,33 +51078,33 @@
         <v>311</v>
       </c>
       <c r="C48" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="D48" s="30" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="E48" s="30" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="F48" s="30" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="G48" s="30" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="H48" s="7"/>
       <c r="I48" s="7"/>
       <c r="J48" s="38" t="s">
-        <v>660</v>
+        <v>642</v>
       </c>
       <c r="K48" s="8" t="s">
-        <v>674</v>
+        <v>656</v>
       </c>
       <c r="L48" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>633</v>
+        <v>649</v>
       </c>
       <c r="N48" s="4" t="s">
         <v>8</v>
@@ -51242,33 +51132,33 @@
         <v>311</v>
       </c>
       <c r="C49" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="D49" s="30" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="E49" s="30" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="F49" s="30" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="G49" s="30" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="H49" s="7"/>
       <c r="I49" s="7"/>
       <c r="J49" s="38" t="s">
-        <v>661</v>
+        <v>643</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>675</v>
+        <v>657</v>
       </c>
       <c r="L49" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>633</v>
+        <v>617</v>
       </c>
       <c r="N49" s="4" t="s">
         <v>8</v>
@@ -51296,33 +51186,33 @@
         <v>311</v>
       </c>
       <c r="C50" t="s">
-        <v>341</v>
+        <v>324</v>
       </c>
       <c r="D50" s="30" t="s">
-        <v>342</v>
+        <v>325</v>
       </c>
       <c r="E50" s="30" t="s">
-        <v>343</v>
+        <v>326</v>
       </c>
       <c r="F50" s="30" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="G50" s="30" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="H50" s="7"/>
       <c r="I50" s="7"/>
       <c r="J50" s="38" t="s">
-        <v>662</v>
+        <v>644</v>
       </c>
       <c r="K50" s="8" t="s">
-        <v>676</v>
+        <v>658</v>
       </c>
       <c r="L50" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>633</v>
+        <v>617</v>
       </c>
       <c r="N50" s="4" t="s">
         <v>8</v>
@@ -51350,33 +51240,33 @@
         <v>311</v>
       </c>
       <c r="C51" t="s">
-        <v>346</v>
+        <v>329</v>
       </c>
       <c r="D51" s="30" t="s">
-        <v>347</v>
+        <v>330</v>
       </c>
       <c r="E51" s="30" t="s">
-        <v>348</v>
+        <v>331</v>
       </c>
       <c r="F51" s="30" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="G51" s="30" t="s">
-        <v>350</v>
+        <v>333</v>
       </c>
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
       <c r="J51" s="38" t="s">
-        <v>663</v>
+        <v>645</v>
       </c>
       <c r="K51" s="8" t="s">
-        <v>677</v>
+        <v>659</v>
       </c>
       <c r="L51" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>633</v>
+        <v>617</v>
       </c>
       <c r="N51" s="4" t="s">
         <v>8</v>
@@ -51396,44 +51286,46 @@
       <c r="AA51" s="5"/>
       <c r="AB51" s="5"/>
     </row>
-    <row r="52" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A52" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B52" t="s">
-        <v>376</v>
+        <v>311</v>
       </c>
       <c r="C52" t="s">
-        <v>389</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>437</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>620</v>
-      </c>
-      <c r="F52" s="10" t="s">
-        <v>621</v>
-      </c>
-      <c r="G52" s="10" t="s">
-        <v>378</v>
-      </c>
-      <c r="H52" s="10"/>
+        <v>335</v>
+      </c>
+      <c r="D52" s="30" t="s">
+        <v>336</v>
+      </c>
+      <c r="E52" s="30" t="s">
+        <v>337</v>
+      </c>
+      <c r="F52" s="30" t="s">
+        <v>332</v>
+      </c>
+      <c r="G52" s="30" t="s">
+        <v>338</v>
+      </c>
+      <c r="H52" s="7"/>
       <c r="I52" s="7"/>
-      <c r="J52" s="7"/>
-      <c r="K52" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="L52" s="12"/>
+      <c r="J52" s="38" t="s">
+        <v>646</v>
+      </c>
+      <c r="K52" s="8" t="s">
+        <v>660</v>
+      </c>
+      <c r="L52" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="M52" s="4" t="s">
-        <v>16</v>
+        <v>617</v>
       </c>
       <c r="N52" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O52" s="3" t="s">
-        <v>377</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="O52" s="3"/>
       <c r="P52" s="5"/>
       <c r="Q52" s="5"/>
       <c r="R52" s="5"/>
@@ -51448,42 +51340,44 @@
       <c r="AA52" s="5"/>
       <c r="AB52" s="5"/>
     </row>
-    <row r="53" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A53" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B53" t="s">
-        <v>380</v>
+        <v>311</v>
       </c>
       <c r="C53" t="s">
-        <v>381</v>
-      </c>
-      <c r="D53" t="s">
-        <v>385</v>
-      </c>
-      <c r="E53" t="s">
-        <v>384</v>
-      </c>
-      <c r="F53" t="s">
-        <v>383</v>
-      </c>
-      <c r="G53" s="10" t="s">
-        <v>382</v>
-      </c>
-      <c r="H53" s="10"/>
+        <v>339</v>
+      </c>
+      <c r="D53" s="30" t="s">
+        <v>340</v>
+      </c>
+      <c r="E53" s="30" t="s">
+        <v>341</v>
+      </c>
+      <c r="F53" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="G53" s="30" t="s">
+        <v>343</v>
+      </c>
+      <c r="H53" s="7"/>
       <c r="I53" s="7"/>
-      <c r="J53" s="7"/>
-      <c r="K53" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="L53" s="12" t="s">
-        <v>387</v>
+      <c r="J53" s="38" t="s">
+        <v>647</v>
+      </c>
+      <c r="K53" s="8" t="s">
+        <v>661</v>
+      </c>
+      <c r="L53" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>4</v>
+        <v>617</v>
       </c>
       <c r="N53" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="O53" s="3"/>
       <c r="P53" s="5"/>
@@ -51505,30 +51399,30 @@
         <v>310</v>
       </c>
       <c r="B54" t="s">
-        <v>388</v>
+        <v>363</v>
       </c>
       <c r="C54" t="s">
-        <v>389</v>
-      </c>
-      <c r="D54" t="s">
-        <v>394</v>
-      </c>
-      <c r="E54" t="s">
-        <v>393</v>
-      </c>
-      <c r="F54" s="7" t="s">
-        <v>392</v>
-      </c>
-      <c r="G54" t="s">
-        <v>391</v>
-      </c>
-      <c r="H54" s="7"/>
+        <v>376</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>604</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>605</v>
+      </c>
+      <c r="G54" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="H54" s="10"/>
       <c r="I54" s="7"/>
       <c r="J54" s="7"/>
-      <c r="K54" s="8" t="s">
-        <v>390</v>
-      </c>
-      <c r="L54" s="4"/>
+      <c r="K54" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="L54" s="12"/>
       <c r="M54" s="4" t="s">
         <v>16</v>
       </c>
@@ -51536,7 +51430,7 @@
         <v>13</v>
       </c>
       <c r="O54" s="3" t="s">
-        <v>377</v>
+        <v>364</v>
       </c>
       <c r="P54" s="5"/>
       <c r="Q54" s="5"/>
@@ -51557,37 +51451,37 @@
         <v>310</v>
       </c>
       <c r="B55" t="s">
-        <v>395</v>
-      </c>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10" t="s">
-        <v>399</v>
-      </c>
-      <c r="E55" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="F55" s="10" t="s">
-        <v>397</v>
+        <v>367</v>
+      </c>
+      <c r="C55" t="s">
+        <v>368</v>
+      </c>
+      <c r="D55" t="s">
+        <v>372</v>
+      </c>
+      <c r="E55" t="s">
+        <v>371</v>
+      </c>
+      <c r="F55" t="s">
+        <v>370</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>396</v>
-      </c>
-      <c r="H55" s="10" t="s">
-        <v>188</v>
-      </c>
+        <v>369</v>
+      </c>
+      <c r="H55" s="10"/>
       <c r="I55" s="7"/>
       <c r="J55" s="7"/>
-      <c r="K55" s="8" t="s">
-        <v>400</v>
-      </c>
-      <c r="L55" s="11" t="s">
-        <v>11</v>
+      <c r="K55" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="L55" s="12" t="s">
+        <v>374</v>
       </c>
       <c r="M55" s="4" t="s">
         <v>4</v>
       </c>
       <c r="N55" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="O55" s="3"/>
       <c r="P55" s="5"/>
@@ -51609,28 +51503,28 @@
         <v>310</v>
       </c>
       <c r="B56" t="s">
-        <v>401</v>
+        <v>375</v>
       </c>
       <c r="C56" t="s">
-        <v>389</v>
+        <v>376</v>
       </c>
       <c r="D56" t="s">
-        <v>402</v>
+        <v>381</v>
       </c>
       <c r="E56" t="s">
-        <v>403</v>
+        <v>380</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>404</v>
+        <v>379</v>
       </c>
       <c r="G56" t="s">
-        <v>391</v>
+        <v>378</v>
       </c>
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
       <c r="J56" s="7"/>
       <c r="K56" s="8" t="s">
-        <v>405</v>
+        <v>377</v>
       </c>
       <c r="L56" s="4"/>
       <c r="M56" s="4" t="s">
@@ -51640,7 +51534,7 @@
         <v>13</v>
       </c>
       <c r="O56" s="3" t="s">
-        <v>377</v>
+        <v>364</v>
       </c>
       <c r="P56" s="5"/>
       <c r="Q56" s="5"/>
@@ -51656,41 +51550,39 @@
       <c r="AA56" s="5"/>
       <c r="AB56" s="5"/>
     </row>
-    <row r="57" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A57" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B57" t="s">
-        <v>406</v>
-      </c>
-      <c r="C57" t="s">
-        <v>359</v>
-      </c>
+        <v>382</v>
+      </c>
+      <c r="C57" s="10"/>
       <c r="D57" s="10" t="s">
-        <v>408</v>
+        <v>664</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>409</v>
+        <v>385</v>
       </c>
       <c r="F57" s="10" t="s">
-        <v>407</v>
+        <v>384</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>410</v>
-      </c>
-      <c r="H57" s="10"/>
+        <v>383</v>
+      </c>
+      <c r="H57" s="10" t="s">
+        <v>188</v>
+      </c>
       <c r="I57" s="7"/>
-      <c r="J57" s="38" t="s">
-        <v>654</v>
-      </c>
+      <c r="J57" s="7"/>
       <c r="K57" s="8" t="s">
-        <v>678</v>
+        <v>386</v>
       </c>
       <c r="L57" s="11" t="s">
         <v>11</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>633</v>
+        <v>4</v>
       </c>
       <c r="N57" s="4" t="s">
         <v>8</v>
@@ -51710,46 +51602,44 @@
       <c r="AA57" s="5"/>
       <c r="AB57" s="5"/>
     </row>
-    <row r="58" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A58" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B58" t="s">
-        <v>406</v>
+        <v>387</v>
       </c>
       <c r="C58" t="s">
-        <v>412</v>
-      </c>
-      <c r="D58" s="10" t="s">
-        <v>416</v>
-      </c>
-      <c r="E58" s="10" t="s">
-        <v>415</v>
-      </c>
-      <c r="F58" s="10" t="s">
-        <v>414</v>
-      </c>
-      <c r="G58" s="10" t="s">
-        <v>413</v>
-      </c>
-      <c r="H58" s="10"/>
+        <v>376</v>
+      </c>
+      <c r="D58" t="s">
+        <v>388</v>
+      </c>
+      <c r="E58" t="s">
+        <v>389</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="G58" t="s">
+        <v>378</v>
+      </c>
+      <c r="H58" s="7"/>
       <c r="I58" s="7"/>
-      <c r="J58" s="38" t="s">
-        <v>663</v>
-      </c>
+      <c r="J58" s="7"/>
       <c r="K58" s="8" t="s">
-        <v>679</v>
-      </c>
-      <c r="L58" s="11" t="s">
-        <v>11</v>
-      </c>
+        <v>391</v>
+      </c>
+      <c r="L58" s="4"/>
       <c r="M58" s="4" t="s">
-        <v>633</v>
+        <v>16</v>
       </c>
       <c r="N58" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="O58" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="O58" s="3" t="s">
+        <v>364</v>
+      </c>
       <c r="P58" s="5"/>
       <c r="Q58" s="5"/>
       <c r="R58" s="5"/>
@@ -51764,14 +51654,45 @@
       <c r="AA58" s="5"/>
       <c r="AB58" s="5"/>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="K59" s="5"/>
-      <c r="L59" s="13"/>
-      <c r="M59" s="4"/>
-      <c r="N59" s="4"/>
+    <row r="59" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+      <c r="A59" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B59" t="s">
+        <v>392</v>
+      </c>
+      <c r="C59" t="s">
+        <v>351</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="G59" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="H59" s="10"/>
+      <c r="I59" s="7"/>
+      <c r="J59" s="38" t="s">
+        <v>638</v>
+      </c>
+      <c r="K59" s="8" t="s">
+        <v>662</v>
+      </c>
+      <c r="L59" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M59" s="4" t="s">
+        <v>617</v>
+      </c>
+      <c r="N59" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="O59" s="3"/>
       <c r="P59" s="5"/>
       <c r="Q59" s="5"/>
@@ -51787,14 +51708,45 @@
       <c r="AA59" s="5"/>
       <c r="AB59" s="5"/>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="K60" s="5"/>
-      <c r="L60" s="13"/>
-      <c r="M60" s="4"/>
-      <c r="N60" s="4"/>
+    <row r="60" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+      <c r="A60" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B60" t="s">
+        <v>392</v>
+      </c>
+      <c r="C60" t="s">
+        <v>397</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>399</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="H60" s="10"/>
+      <c r="I60" s="7"/>
+      <c r="J60" s="38" t="s">
+        <v>647</v>
+      </c>
+      <c r="K60" s="8" t="s">
+        <v>663</v>
+      </c>
+      <c r="L60" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M60" s="4" t="s">
+        <v>617</v>
+      </c>
+      <c r="N60" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="O60" s="3"/>
       <c r="P60" s="5"/>
       <c r="Q60" s="5"/>
@@ -73246,6 +73198,52 @@
       <c r="AA992" s="5"/>
       <c r="AB992" s="5"/>
     </row>
+    <row r="993" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A993" s="5"/>
+      <c r="B993" s="5"/>
+      <c r="C993" s="5"/>
+      <c r="K993" s="5"/>
+      <c r="L993" s="13"/>
+      <c r="M993" s="4"/>
+      <c r="N993" s="4"/>
+      <c r="O993" s="3"/>
+      <c r="P993" s="5"/>
+      <c r="Q993" s="5"/>
+      <c r="R993" s="5"/>
+      <c r="S993" s="5"/>
+      <c r="T993" s="5"/>
+      <c r="U993" s="5"/>
+      <c r="V993" s="5"/>
+      <c r="W993" s="5"/>
+      <c r="X993" s="5"/>
+      <c r="Y993" s="5"/>
+      <c r="Z993" s="5"/>
+      <c r="AA993" s="5"/>
+      <c r="AB993" s="5"/>
+    </row>
+    <row r="994" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A994" s="5"/>
+      <c r="B994" s="5"/>
+      <c r="C994" s="5"/>
+      <c r="K994" s="5"/>
+      <c r="L994" s="13"/>
+      <c r="M994" s="4"/>
+      <c r="N994" s="4"/>
+      <c r="O994" s="3"/>
+      <c r="P994" s="5"/>
+      <c r="Q994" s="5"/>
+      <c r="R994" s="5"/>
+      <c r="S994" s="5"/>
+      <c r="T994" s="5"/>
+      <c r="U994" s="5"/>
+      <c r="V994" s="5"/>
+      <c r="W994" s="5"/>
+      <c r="X994" s="5"/>
+      <c r="Y994" s="5"/>
+      <c r="Z994" s="5"/>
+      <c r="AA994" s="5"/>
+      <c r="AB994" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
1859 added more tests and partiallyy update gradin vignette
</commit_message>
<xml_diff>
--- a/inst/adlb_grading/adlb_grading_spec.xlsx
+++ b/inst/adlb_grading/adlb_grading_spec.xlsx
@@ -17,7 +17,7 @@
     <sheet name="DAIDS" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DAIDS!$C$1:$C$994</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DAIDS!$C$1:$C$996</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1609" uniqueCount="676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1626" uniqueCount="680">
   <si>
     <t>Anemia</t>
   </si>
@@ -2898,6 +2898,18 @@
 AVAL &lt;= ANRLO ~ "0"
 )</t>
   </si>
+  <si>
+    <t>&lt;= 5 years of age</t>
+  </si>
+  <si>
+    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &lt;= 5 | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>No criteria given for this age range</t>
+  </si>
+  <si>
+    <t>NA_character_</t>
+  </si>
 </sst>
 </file>
 
@@ -48615,10 +48627,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB994"/>
+  <dimension ref="A1:AB996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -50704,9 +50716,7 @@
       <c r="G41" s="10" t="s">
         <v>592</v>
       </c>
-      <c r="H41" s="10" t="s">
-        <v>188</v>
-      </c>
+      <c r="H41" s="10"/>
       <c r="I41" s="7"/>
       <c r="J41" s="38" t="s">
         <v>637</v>
@@ -50740,37 +50750,27 @@
       <c r="AA41" s="5"/>
       <c r="AB41" s="5"/>
     </row>
-    <row r="42" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B42" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="C42" t="s">
-        <v>358</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>594</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>361</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>360</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>359</v>
-      </c>
-      <c r="H42" s="7" t="s">
-        <v>188</v>
-      </c>
+        <v>676</v>
+      </c>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
       <c r="I42" s="7"/>
       <c r="J42" s="38" t="s">
-        <v>637</v>
+        <v>677</v>
       </c>
       <c r="K42" s="8" t="s">
-        <v>651</v>
+        <v>679</v>
       </c>
       <c r="L42" s="11" t="s">
         <v>11</v>
@@ -50781,7 +50781,9 @@
       <c r="N42" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O42" s="3"/>
+      <c r="O42" s="3" t="s">
+        <v>678</v>
+      </c>
       <c r="P42" s="5"/>
       <c r="Q42" s="5"/>
       <c r="R42" s="5"/>
@@ -50801,32 +50803,30 @@
         <v>310</v>
       </c>
       <c r="B43" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="C43" t="s">
-        <v>351</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>595</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>596</v>
-      </c>
-      <c r="F43" s="10" t="s">
-        <v>597</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>352</v>
-      </c>
-      <c r="H43" s="10" t="s">
-        <v>188</v>
-      </c>
+        <v>358</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>594</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="H43" s="7"/>
       <c r="I43" s="7"/>
       <c r="J43" s="38" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="L43" s="11" t="s">
         <v>11</v>
@@ -50837,7 +50837,9 @@
       <c r="N43" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O43" s="3"/>
+      <c r="O43" s="3" t="s">
+        <v>593</v>
+      </c>
       <c r="P43" s="5"/>
       <c r="Q43" s="5"/>
       <c r="R43" s="5"/>
@@ -50852,37 +50854,27 @@
       <c r="AA43" s="5"/>
       <c r="AB43" s="5"/>
     </row>
-    <row r="44" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B44" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="C44" t="s">
-        <v>353</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>598</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>599</v>
-      </c>
-      <c r="F44" s="10" t="s">
-        <v>600</v>
-      </c>
-      <c r="G44" s="10" t="s">
-        <v>354</v>
-      </c>
-      <c r="H44" s="10" t="s">
-        <v>188</v>
-      </c>
+        <v>676</v>
+      </c>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
       <c r="I44" s="7"/>
       <c r="J44" s="38" t="s">
-        <v>639</v>
+        <v>677</v>
       </c>
       <c r="K44" s="8" t="s">
-        <v>653</v>
+        <v>679</v>
       </c>
       <c r="L44" s="11" t="s">
         <v>11</v>
@@ -50893,7 +50885,9 @@
       <c r="N44" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O44" s="3"/>
+      <c r="O44" s="3" t="s">
+        <v>678</v>
+      </c>
       <c r="P44" s="5"/>
       <c r="Q44" s="5"/>
       <c r="R44" s="5"/>
@@ -50916,29 +50910,29 @@
         <v>350</v>
       </c>
       <c r="C45" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="H45" s="10" t="s">
         <v>188</v>
       </c>
       <c r="I45" s="7"/>
       <c r="J45" s="38" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="L45" s="11" t="s">
         <v>11</v>
@@ -50964,39 +50958,43 @@
       <c r="AA45" s="5"/>
       <c r="AB45" s="5"/>
     </row>
-    <row r="46" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B46" t="s">
-        <v>344</v>
-      </c>
-      <c r="C46"/>
-      <c r="D46" t="s">
-        <v>345</v>
-      </c>
-      <c r="E46" t="s">
-        <v>346</v>
-      </c>
-      <c r="F46" t="s">
-        <v>347</v>
-      </c>
-      <c r="G46" t="s">
-        <v>348</v>
+        <v>350</v>
+      </c>
+      <c r="C46" t="s">
+        <v>353</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>598</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>599</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>600</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>354</v>
       </c>
       <c r="H46" s="10" t="s">
         <v>188</v>
       </c>
       <c r="I46" s="7"/>
-      <c r="J46" s="7"/>
-      <c r="K46" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="L46" s="4" t="s">
-        <v>2</v>
+      <c r="J46" s="38" t="s">
+        <v>639</v>
+      </c>
+      <c r="K46" s="8" t="s">
+        <v>653</v>
+      </c>
+      <c r="L46" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>3</v>
+        <v>617</v>
       </c>
       <c r="N46" s="4" t="s">
         <v>8</v>
@@ -51021,36 +51019,38 @@
         <v>310</v>
       </c>
       <c r="B47" t="s">
-        <v>311</v>
+        <v>350</v>
       </c>
       <c r="C47" t="s">
-        <v>313</v>
-      </c>
-      <c r="D47" s="30" t="s">
-        <v>315</v>
-      </c>
-      <c r="E47" s="30" t="s">
-        <v>316</v>
-      </c>
-      <c r="F47" s="30" t="s">
-        <v>317</v>
-      </c>
-      <c r="G47" s="30" t="s">
-        <v>318</v>
-      </c>
-      <c r="H47" s="7"/>
+        <v>355</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>601</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>602</v>
+      </c>
+      <c r="F47" s="10" t="s">
+        <v>603</v>
+      </c>
+      <c r="G47" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H47" s="10" t="s">
+        <v>188</v>
+      </c>
       <c r="I47" s="7"/>
       <c r="J47" s="38" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="K47" s="8" t="s">
-        <v>655</v>
-      </c>
-      <c r="L47" s="4" t="s">
-        <v>2</v>
+        <v>654</v>
+      </c>
+      <c r="L47" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>649</v>
+        <v>617</v>
       </c>
       <c r="N47" s="4" t="s">
         <v>8</v>
@@ -51070,41 +51070,39 @@
       <c r="AA47" s="5"/>
       <c r="AB47" s="5"/>
     </row>
-    <row r="48" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B48" t="s">
-        <v>311</v>
-      </c>
-      <c r="C48" t="s">
-        <v>314</v>
-      </c>
-      <c r="D48" s="30" t="s">
-        <v>319</v>
-      </c>
-      <c r="E48" s="30" t="s">
-        <v>320</v>
-      </c>
-      <c r="F48" s="30" t="s">
-        <v>321</v>
-      </c>
-      <c r="G48" s="30" t="s">
-        <v>322</v>
-      </c>
-      <c r="H48" s="7"/>
+        <v>344</v>
+      </c>
+      <c r="C48"/>
+      <c r="D48" t="s">
+        <v>345</v>
+      </c>
+      <c r="E48" t="s">
+        <v>346</v>
+      </c>
+      <c r="F48" t="s">
+        <v>347</v>
+      </c>
+      <c r="G48" t="s">
+        <v>348</v>
+      </c>
+      <c r="H48" s="10" t="s">
+        <v>188</v>
+      </c>
       <c r="I48" s="7"/>
-      <c r="J48" s="38" t="s">
-        <v>642</v>
-      </c>
-      <c r="K48" s="8" t="s">
-        <v>656</v>
+      <c r="J48" s="7"/>
+      <c r="K48" s="1" t="s">
+        <v>349</v>
       </c>
       <c r="L48" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>649</v>
+        <v>3</v>
       </c>
       <c r="N48" s="4" t="s">
         <v>8</v>
@@ -51132,33 +51130,33 @@
         <v>311</v>
       </c>
       <c r="C49" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="D49" s="30" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="E49" s="30" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F49" s="30" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="G49" s="30" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="H49" s="7"/>
       <c r="I49" s="7"/>
       <c r="J49" s="38" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="L49" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>617</v>
+        <v>649</v>
       </c>
       <c r="N49" s="4" t="s">
         <v>8</v>
@@ -51186,33 +51184,33 @@
         <v>311</v>
       </c>
       <c r="C50" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="D50" s="30" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="E50" s="30" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="F50" s="30" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="G50" s="30" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="H50" s="7"/>
       <c r="I50" s="7"/>
       <c r="J50" s="38" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="K50" s="8" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="L50" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>617</v>
+        <v>649</v>
       </c>
       <c r="N50" s="4" t="s">
         <v>8</v>
@@ -51240,27 +51238,27 @@
         <v>311</v>
       </c>
       <c r="C51" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="D51" s="30" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="E51" s="30" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="F51" s="30" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="G51" s="30" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
       <c r="J51" s="38" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="K51" s="8" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="L51" s="4" t="s">
         <v>2</v>
@@ -51294,27 +51292,27 @@
         <v>311</v>
       </c>
       <c r="C52" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="D52" s="30" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="E52" s="30" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="F52" s="30" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="G52" s="30" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="H52" s="7"/>
       <c r="I52" s="7"/>
       <c r="J52" s="38" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="K52" s="8" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="L52" s="4" t="s">
         <v>2</v>
@@ -51348,27 +51346,27 @@
         <v>311</v>
       </c>
       <c r="C53" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="D53" s="30" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="E53" s="30" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="F53" s="30" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="G53" s="30" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="H53" s="7"/>
       <c r="I53" s="7"/>
       <c r="J53" s="38" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="K53" s="8" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="L53" s="4" t="s">
         <v>2</v>
@@ -51394,44 +51392,46 @@
       <c r="AA53" s="5"/>
       <c r="AB53" s="5"/>
     </row>
-    <row r="54" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A54" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B54" t="s">
-        <v>363</v>
+        <v>311</v>
       </c>
       <c r="C54" t="s">
-        <v>376</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>421</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>604</v>
-      </c>
-      <c r="F54" s="10" t="s">
-        <v>605</v>
-      </c>
-      <c r="G54" s="10" t="s">
-        <v>365</v>
-      </c>
-      <c r="H54" s="10"/>
+        <v>335</v>
+      </c>
+      <c r="D54" s="30" t="s">
+        <v>336</v>
+      </c>
+      <c r="E54" s="30" t="s">
+        <v>337</v>
+      </c>
+      <c r="F54" s="30" t="s">
+        <v>332</v>
+      </c>
+      <c r="G54" s="30" t="s">
+        <v>338</v>
+      </c>
+      <c r="H54" s="7"/>
       <c r="I54" s="7"/>
-      <c r="J54" s="7"/>
-      <c r="K54" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="L54" s="12"/>
+      <c r="J54" s="38" t="s">
+        <v>646</v>
+      </c>
+      <c r="K54" s="8" t="s">
+        <v>660</v>
+      </c>
+      <c r="L54" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="M54" s="4" t="s">
-        <v>16</v>
+        <v>617</v>
       </c>
       <c r="N54" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O54" s="3" t="s">
-        <v>364</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="O54" s="3"/>
       <c r="P54" s="5"/>
       <c r="Q54" s="5"/>
       <c r="R54" s="5"/>
@@ -51446,42 +51446,44 @@
       <c r="AA54" s="5"/>
       <c r="AB54" s="5"/>
     </row>
-    <row r="55" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B55" t="s">
-        <v>367</v>
+        <v>311</v>
       </c>
       <c r="C55" t="s">
-        <v>368</v>
-      </c>
-      <c r="D55" t="s">
-        <v>372</v>
-      </c>
-      <c r="E55" t="s">
-        <v>371</v>
-      </c>
-      <c r="F55" t="s">
-        <v>370</v>
-      </c>
-      <c r="G55" s="10" t="s">
-        <v>369</v>
-      </c>
-      <c r="H55" s="10"/>
+        <v>339</v>
+      </c>
+      <c r="D55" s="30" t="s">
+        <v>340</v>
+      </c>
+      <c r="E55" s="30" t="s">
+        <v>341</v>
+      </c>
+      <c r="F55" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="G55" s="30" t="s">
+        <v>343</v>
+      </c>
+      <c r="H55" s="7"/>
       <c r="I55" s="7"/>
-      <c r="J55" s="7"/>
-      <c r="K55" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="L55" s="12" t="s">
-        <v>374</v>
+      <c r="J55" s="38" t="s">
+        <v>647</v>
+      </c>
+      <c r="K55" s="8" t="s">
+        <v>661</v>
+      </c>
+      <c r="L55" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="M55" s="4" t="s">
-        <v>4</v>
+        <v>617</v>
       </c>
       <c r="N55" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="O55" s="3"/>
       <c r="P55" s="5"/>
@@ -51503,30 +51505,30 @@
         <v>310</v>
       </c>
       <c r="B56" t="s">
-        <v>375</v>
+        <v>363</v>
       </c>
       <c r="C56" t="s">
         <v>376</v>
       </c>
-      <c r="D56" t="s">
-        <v>381</v>
-      </c>
-      <c r="E56" t="s">
-        <v>380</v>
-      </c>
-      <c r="F56" s="7" t="s">
-        <v>379</v>
-      </c>
-      <c r="G56" t="s">
-        <v>378</v>
-      </c>
-      <c r="H56" s="7"/>
+      <c r="D56" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>604</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>605</v>
+      </c>
+      <c r="G56" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="H56" s="10"/>
       <c r="I56" s="7"/>
       <c r="J56" s="7"/>
-      <c r="K56" s="8" t="s">
-        <v>377</v>
-      </c>
-      <c r="L56" s="4"/>
+      <c r="K56" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="L56" s="12"/>
       <c r="M56" s="4" t="s">
         <v>16</v>
       </c>
@@ -51555,37 +51557,37 @@
         <v>310</v>
       </c>
       <c r="B57" t="s">
-        <v>382</v>
-      </c>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10" t="s">
-        <v>664</v>
-      </c>
-      <c r="E57" s="10" t="s">
-        <v>385</v>
-      </c>
-      <c r="F57" s="10" t="s">
-        <v>384</v>
+        <v>367</v>
+      </c>
+      <c r="C57" t="s">
+        <v>368</v>
+      </c>
+      <c r="D57" t="s">
+        <v>372</v>
+      </c>
+      <c r="E57" t="s">
+        <v>371</v>
+      </c>
+      <c r="F57" t="s">
+        <v>370</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>383</v>
-      </c>
-      <c r="H57" s="10" t="s">
-        <v>188</v>
-      </c>
+        <v>369</v>
+      </c>
+      <c r="H57" s="10"/>
       <c r="I57" s="7"/>
       <c r="J57" s="7"/>
-      <c r="K57" s="8" t="s">
-        <v>386</v>
-      </c>
-      <c r="L57" s="11" t="s">
-        <v>11</v>
+      <c r="K57" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="L57" s="12" t="s">
+        <v>374</v>
       </c>
       <c r="M57" s="4" t="s">
         <v>4</v>
       </c>
       <c r="N57" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="O57" s="3"/>
       <c r="P57" s="5"/>
@@ -51607,19 +51609,19 @@
         <v>310</v>
       </c>
       <c r="B58" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="C58" t="s">
         <v>376</v>
       </c>
       <c r="D58" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="E58" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="G58" t="s">
         <v>378</v>
@@ -51628,7 +51630,7 @@
       <c r="I58" s="7"/>
       <c r="J58" s="7"/>
       <c r="K58" s="8" t="s">
-        <v>391</v>
+        <v>377</v>
       </c>
       <c r="L58" s="4"/>
       <c r="M58" s="4" t="s">
@@ -51654,41 +51656,39 @@
       <c r="AA58" s="5"/>
       <c r="AB58" s="5"/>
     </row>
-    <row r="59" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A59" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B59" t="s">
-        <v>392</v>
-      </c>
-      <c r="C59" t="s">
-        <v>351</v>
-      </c>
+        <v>382</v>
+      </c>
+      <c r="C59" s="10"/>
       <c r="D59" s="10" t="s">
-        <v>394</v>
+        <v>664</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="F59" s="10" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>396</v>
-      </c>
-      <c r="H59" s="10"/>
+        <v>383</v>
+      </c>
+      <c r="H59" s="10" t="s">
+        <v>188</v>
+      </c>
       <c r="I59" s="7"/>
-      <c r="J59" s="38" t="s">
-        <v>638</v>
-      </c>
+      <c r="J59" s="7"/>
       <c r="K59" s="8" t="s">
-        <v>662</v>
+        <v>386</v>
       </c>
       <c r="L59" s="11" t="s">
         <v>11</v>
       </c>
       <c r="M59" s="4" t="s">
-        <v>617</v>
+        <v>4</v>
       </c>
       <c r="N59" s="4" t="s">
         <v>8</v>
@@ -51708,46 +51708,44 @@
       <c r="AA59" s="5"/>
       <c r="AB59" s="5"/>
     </row>
-    <row r="60" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A60" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B60" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C60" t="s">
-        <v>397</v>
-      </c>
-      <c r="D60" s="10" t="s">
-        <v>401</v>
-      </c>
-      <c r="E60" s="10" t="s">
-        <v>400</v>
-      </c>
-      <c r="F60" s="10" t="s">
-        <v>399</v>
-      </c>
-      <c r="G60" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="H60" s="10"/>
+        <v>376</v>
+      </c>
+      <c r="D60" t="s">
+        <v>388</v>
+      </c>
+      <c r="E60" t="s">
+        <v>389</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="G60" t="s">
+        <v>378</v>
+      </c>
+      <c r="H60" s="7"/>
       <c r="I60" s="7"/>
-      <c r="J60" s="38" t="s">
-        <v>647</v>
-      </c>
+      <c r="J60" s="7"/>
       <c r="K60" s="8" t="s">
-        <v>663</v>
-      </c>
-      <c r="L60" s="11" t="s">
-        <v>11</v>
-      </c>
+        <v>391</v>
+      </c>
+      <c r="L60" s="4"/>
       <c r="M60" s="4" t="s">
-        <v>617</v>
+        <v>16</v>
       </c>
       <c r="N60" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="O60" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="O60" s="3" t="s">
+        <v>364</v>
+      </c>
       <c r="P60" s="5"/>
       <c r="Q60" s="5"/>
       <c r="R60" s="5"/>
@@ -51762,14 +51760,45 @@
       <c r="AA60" s="5"/>
       <c r="AB60" s="5"/>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="K61" s="5"/>
-      <c r="L61" s="13"/>
-      <c r="M61" s="4"/>
-      <c r="N61" s="4"/>
+    <row r="61" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+      <c r="A61" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B61" t="s">
+        <v>392</v>
+      </c>
+      <c r="C61" t="s">
+        <v>351</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="G61" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="H61" s="10"/>
+      <c r="I61" s="7"/>
+      <c r="J61" s="38" t="s">
+        <v>638</v>
+      </c>
+      <c r="K61" s="8" t="s">
+        <v>662</v>
+      </c>
+      <c r="L61" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M61" s="4" t="s">
+        <v>617</v>
+      </c>
+      <c r="N61" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="O61" s="3"/>
       <c r="P61" s="5"/>
       <c r="Q61" s="5"/>
@@ -51785,14 +51814,45 @@
       <c r="AA61" s="5"/>
       <c r="AB61" s="5"/>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A62" s="5"/>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-      <c r="K62" s="5"/>
-      <c r="L62" s="13"/>
-      <c r="M62" s="4"/>
-      <c r="N62" s="4"/>
+    <row r="62" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+      <c r="A62" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B62" t="s">
+        <v>392</v>
+      </c>
+      <c r="C62" t="s">
+        <v>397</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>399</v>
+      </c>
+      <c r="G62" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="H62" s="10"/>
+      <c r="I62" s="7"/>
+      <c r="J62" s="38" t="s">
+        <v>647</v>
+      </c>
+      <c r="K62" s="8" t="s">
+        <v>663</v>
+      </c>
+      <c r="L62" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M62" s="4" t="s">
+        <v>617</v>
+      </c>
+      <c r="N62" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="O62" s="3"/>
       <c r="P62" s="5"/>
       <c r="Q62" s="5"/>
@@ -73244,6 +73304,52 @@
       <c r="AA994" s="5"/>
       <c r="AB994" s="5"/>
     </row>
+    <row r="995" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A995" s="5"/>
+      <c r="B995" s="5"/>
+      <c r="C995" s="5"/>
+      <c r="K995" s="5"/>
+      <c r="L995" s="13"/>
+      <c r="M995" s="4"/>
+      <c r="N995" s="4"/>
+      <c r="O995" s="3"/>
+      <c r="P995" s="5"/>
+      <c r="Q995" s="5"/>
+      <c r="R995" s="5"/>
+      <c r="S995" s="5"/>
+      <c r="T995" s="5"/>
+      <c r="U995" s="5"/>
+      <c r="V995" s="5"/>
+      <c r="W995" s="5"/>
+      <c r="X995" s="5"/>
+      <c r="Y995" s="5"/>
+      <c r="Z995" s="5"/>
+      <c r="AA995" s="5"/>
+      <c r="AB995" s="5"/>
+    </row>
+    <row r="996" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A996" s="5"/>
+      <c r="B996" s="5"/>
+      <c r="C996" s="5"/>
+      <c r="K996" s="5"/>
+      <c r="L996" s="13"/>
+      <c r="M996" s="4"/>
+      <c r="N996" s="4"/>
+      <c r="O996" s="3"/>
+      <c r="P996" s="5"/>
+      <c r="Q996" s="5"/>
+      <c r="R996" s="5"/>
+      <c r="S996" s="5"/>
+      <c r="T996" s="5"/>
+      <c r="U996" s="5"/>
+      <c r="V996" s="5"/>
+      <c r="W996" s="5"/>
+      <c r="X996" s="5"/>
+      <c r="Y996" s="5"/>
+      <c r="Z996" s="5"/>
+      <c r="AA996" s="5"/>
+      <c r="AB996" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
1859 all unit tests added
</commit_message>
<xml_diff>
--- a/inst/adlb_grading/adlb_grading_spec.xlsx
+++ b/inst/adlb_grading/adlb_grading_spec.xlsx
@@ -17,7 +17,7 @@
     <sheet name="DAIDS" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DAIDS!$C$1:$C$996</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DAIDS!$C$1:$C$998</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1626" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1640" uniqueCount="684">
   <si>
     <t>Anemia</t>
   </si>
@@ -1343,12 +1343,6 @@
     <t>FILTER</t>
   </si>
   <si>
-    <t>≥ 13 years of age (male only)</t>
-  </si>
-  <si>
-    <t>≥ 13 years of age (female only)</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">10.0 to 10.9 g/dL, 6.19 to 6.76 </t>
     </r>
@@ -1461,9 +1455,6 @@
     <t>6.7 to &lt; 8.0 g/dL, 4.15 to &lt; 4.94 mmol/L</t>
   </si>
   <si>
-    <t>8 to ≤ 21 days of age (male and female)</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">11.0 to 13.0 g/dL, 6.81 to 8.10 </t>
     </r>
@@ -1484,9 +1475,6 @@
   </si>
   <si>
     <t>&lt; 8.0 g/dL, &lt; 4.96 mmol/L</t>
-  </si>
-  <si>
-    <t>≤ 7 days of age (male and female)</t>
   </si>
   <si>
     <r>
@@ -1557,9 +1545,6 @@
   </si>
   <si>
     <t>&lt;750/mm3; &lt;0.750 x 10e9 /L</t>
-  </si>
-  <si>
-    <t>≤ 1 day of age</t>
   </si>
   <si>
     <t>&lt;1550/mm3; &lt;1.500 x 10e9 /L</t>
@@ -1720,9 +1705,6 @@
     <t>&lt;1000/mm3; &lt;1.000 x 10e9/L</t>
   </si>
   <si>
-    <t>≤ 7 days of age</t>
-  </si>
-  <si>
     <t>&lt;2500/mm3; &lt;2.500 x 10e9/L</t>
   </si>
   <si>
@@ -1785,9 +1767,6 @@
 )</t>
   </si>
   <si>
-    <t>ALT or SGPT, High</t>
-  </si>
-  <si>
     <t>case_when(
 is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
 AVAL &gt;= 10*ANRHI ~ "4",
@@ -1796,9 +1775,6 @@
 AVAL &gt;= 1.25*ANRHI ~ "1",
 AVAL &lt; 1.25*ANRHI ~ "0"
 )</t>
-  </si>
-  <si>
-    <t>AST or SGOT, High</t>
   </si>
   <si>
     <t>Amylase, High</t>
@@ -1839,17 +1815,6 @@
   </si>
   <si>
     <t>16.0 to &lt;LLN</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &lt; 8 ~ "4",
-AVAL &lt; 11 ~ "3",
-AVAL &lt; 16 ~ "2",(
-is.na(ANRLO) ~ NA_character_,
-AVAL &lt; ANRLO ~ "1",
-AVAL &gt;= ANRLO ~ "0"
-)</t>
   </si>
   <si>
     <t>Direct Bilirubin, High</t>
@@ -1910,9 +1875,6 @@
   </si>
   <si>
     <t>Calcium, High</t>
-  </si>
-  <si>
-    <t>≥ 7 days of age</t>
   </si>
   <si>
     <t>10.6 - &lt;11.5 mg/dL; 2.65 - &lt;2.88 mmol/L</t>
@@ -2392,9 +2354,6 @@
 )</t>
   </si>
   <si>
-    <t>0.05848 used as conversion from "umol/L" to "mg/dL"</t>
-  </si>
-  <si>
     <t>12.4 - &lt;12.9 mg/dL; 3.10 - &lt;3.23 mmol/L</t>
   </si>
   <si>
@@ -2402,20 +2361,6 @@
   </si>
   <si>
     <t>&gt;= 3.5 x ULN OR Increase of &gt;= 2.0 x participant’s baseline</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-!is.na(ANRHI) &amp; AVAL &gt;=  3.5*ANRHI ~ "4",
-!is.na(BASE) &amp; AVAL &gt;=  2*BASE ~ "4",
-!is.na(ANRHI) &amp; AVAL &gt;  1.8*ANRHI ~ "3",
-!is.na(BASE) &amp; AVAL &gt;= 1.5*BASE) ~ "3",
-!is.na(ANRHI) &amp; AVAL &gt; 1.3*ANRHI~ "2",
-!is.na(BASE) &amp; AVAL &gt;= 1.3*BASE ~ "2",
-is.na(ANRHI) ~ NA_character_,
-AVAL &gt;= 1.1*ANRHI ~ "1",
-AVAL &lt; 1.1*ANRHI ~ "0"
-)</t>
   </si>
   <si>
     <t>&gt;= 500 mg/dL &gt;= 27.75 mmol/L</t>
@@ -2486,17 +2431,6 @@
   </si>
   <si>
     <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &lt;= 28 | is.na(BRTHDT) | is.na(LBDT)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL*0.05848 &gt;  2 ~ "4",
-AVAL*0.05848 &gt;  1.5 ~ "3",
-AVAL*0.05848 &gt;  1 ~ "2",
-is.na(ANRHI) ~ NA_character_,
-AVAL &gt;= ANRHI ~ "1",
-AVAL &lt; ANRHI ~ "0"
-)</t>
   </si>
   <si>
     <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &gt;= 7 | is.na(BRTHDT) | is.na(LBDT)</t>
@@ -2587,15 +2521,6 @@
 AVAL &gt;= 6.19 ~ "2",
 AVAL &gt;= 5.18 ~ "1",
 AVAL &lt; 5.18 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &gt;= 7.77 ~ "3",
-AVAL &gt;= 5.15 ~ "2",
-AVAL &gt;= 4.14 ~ "1",
-AVAL &lt; 4.14 ~ "0"
 )</t>
   </si>
   <si>
@@ -2881,9 +2806,21 @@
     <t>pH &gt; 7.5 with lifethreatening consequences</t>
   </si>
   <si>
+    <t>&lt;= 5 years of age</t>
+  </si>
+  <si>
+    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &lt;= 5 | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>No criteria given for this age range</t>
+  </si>
+  <si>
+    <t>NA_character_</t>
+  </si>
+  <si>
     <t>case_when(
 is.na(AVAL) ~ NA_character_,
-AVAL &lt; 7.3 ~ "4",
+AVAL &lt; 7.3  ~ "4",
 is.na(ANRLO) ~ NA_character_,
 AVAL &lt; ANRLO ~ "2",
 AVAL &gt;= ANRLO ~ "0"
@@ -2895,31 +2832,120 @@
 AVAL &gt; 7.5 ~ "4",
 is.na(ANRHI) ~ NA_character_,
 AVAL &gt; ANRHI ~ "2",
-AVAL &lt;= ANRLO ~ "0"
+AVAL &lt;= ANRHI ~ "0"
 )</t>
   </si>
   <si>
-    <t>&lt;= 5 years of age</t>
+    <t>ALT, High</t>
   </si>
   <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &lt;= 5 | is.na(BRTHDT) | is.na(LBDT)</t>
+    <t>AST, High</t>
   </si>
   <si>
-    <t>No criteria given for this age range</t>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+AVAL &lt; 8 ~ "4",
+AVAL &lt; 11 ~ "3",
+AVAL &lt; 16 ~ "2",
+is.na(ANRLO) ~ NA_character_,
+AVAL &lt; ANRLO ~ "1",
+AVAL &gt;= ANRLO ~ "0"
+)</t>
   </si>
   <si>
-    <t>NA_character_</t>
+    <t>17.1 used as conversion from "mg/dL" to "umol/L"</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &gt;  2*17.1 ~ "4",
+AVAL &gt;  1.5*17.1 ~ "3",
+AVAL &gt;  17.1 ~ "2",
+is.na(ANRHI) ~ NA_character_,
+AVAL &gt;= ANRHI ~ "1",
+AVAL &lt; ANRHI ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>Did not grade</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+!is.na(ANRHI) &amp; AVAL &gt;=  3.5*ANRHI ~ "4",
+!is.na(BASE) &amp; AVAL &gt;=  2*BASE ~ "4",
+!is.na(ANRHI) &amp; AVAL &gt;  1.8*ANRHI ~ "3",
+!is.na(BASE) &amp; AVAL &gt;= 1.5*BASE ~ "3",
+!is.na(ANRHI) &amp; AVAL &gt; 1.3*ANRHI~ "2",
+!is.na(BASE) &amp; AVAL &gt;= 1.3*BASE ~ "2",
+is.na(ANRHI) ~ NA_character_,
+AVAL &gt;= 1.1*ANRHI ~ "1",
+AVAL &lt; 1.1*ANRHI ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+AVAL &gt;= 7.77 ~ "3",
+AVAL &gt;= 5.15 ~ "2",
+AVAL &gt;= 4.4 ~ "1",
+AVAL &lt; 4.4 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+AVAL &gt; 11.4 ~ "4",
+AVAL &gt; 5.7 ~ "3",
+AVAL &gt; 3.42 ~ "2",
+AVAL &gt;= 1.71 ~ "1",
+AVAL &lt; 1.71 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>&lt;= 2 years of age</t>
+  </si>
+  <si>
+    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &lt;= 2  | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>&gt;= 7 days of age</t>
+  </si>
+  <si>
+    <t>&lt;= 1 day of age</t>
+  </si>
+  <si>
+    <t>&lt;= 7 days of age (male and female)</t>
+  </si>
+  <si>
+    <t>&gt;= 13 years of age (female only)</t>
+  </si>
+  <si>
+    <t>&gt;= 13 years of age (male only)</t>
+  </si>
+  <si>
+    <t>8 to  21 days of age (male and female)</t>
+  </si>
+  <si>
+    <t>&lt;= 7 days of age</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3058,108 +3084,109 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3384,8 +3411,8 @@
   </sheetPr>
   <dimension ref="A1:Z975"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -26085,8 +26112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z972"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -48627,10 +48654,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB996"/>
+  <dimension ref="A1:AB998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -48654,7 +48681,7 @@
         <v>201</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>580</v>
+        <v>570</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>261</v>
@@ -48708,27 +48735,27 @@
     </row>
     <row r="2" spans="1:28" ht="88.5" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B2" t="s">
-        <v>665</v>
+        <v>651</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>666</v>
+        <v>652</v>
       </c>
       <c r="F2" t="s">
-        <v>667</v>
+        <v>653</v>
       </c>
       <c r="G2" t="s">
-        <v>668</v>
+        <v>654</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="8" t="s">
-        <v>674</v>
+        <v>664</v>
       </c>
       <c r="L2" s="4"/>
       <c r="M2" s="4" t="s">
@@ -48738,7 +48765,7 @@
         <v>8</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>669</v>
+        <v>655</v>
       </c>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
@@ -48756,27 +48783,27 @@
     </row>
     <row r="3" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B3" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="E3" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="F3" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="G3" s="32"/>
       <c r="H3" s="10"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="8" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>2</v>
@@ -48804,29 +48831,29 @@
     </row>
     <row r="4" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B4" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="31" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="G4" s="32" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="8" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4" t="s">
@@ -48852,27 +48879,27 @@
     </row>
     <row r="5" spans="1:28" ht="88.5" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B5" t="s">
-        <v>670</v>
+        <v>656</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>671</v>
+        <v>657</v>
       </c>
       <c r="F5" t="s">
-        <v>672</v>
+        <v>658</v>
       </c>
       <c r="G5" t="s">
-        <v>673</v>
+        <v>659</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8" t="s">
-        <v>675</v>
+        <v>665</v>
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="4" t="s">
@@ -48882,7 +48909,7 @@
         <v>13</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>669</v>
+        <v>655</v>
       </c>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
@@ -48900,29 +48927,29 @@
     </row>
     <row r="6" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B6" t="s">
-        <v>414</v>
+        <v>666</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="8" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4" t="s">
@@ -48948,29 +48975,29 @@
     </row>
     <row r="7" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B7" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="33" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="G7" s="33" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="1" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="L7" s="12"/>
       <c r="M7" s="4" t="s">
@@ -48996,29 +49023,29 @@
     </row>
     <row r="8" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B8" t="s">
-        <v>416</v>
+        <v>667</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="8" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4" t="s">
@@ -49044,29 +49071,29 @@
     </row>
     <row r="9" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B9" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="8" t="s">
-        <v>428</v>
+        <v>668</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>46</v>
@@ -49094,41 +49121,39 @@
     </row>
     <row r="10" spans="1:28" s="44" customFormat="1" ht="76" x14ac:dyDescent="0.35">
       <c r="A10" s="36" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="32"/>
       <c r="F10" s="37" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>432</v>
-      </c>
-      <c r="H10" s="36" t="s">
-        <v>188</v>
-      </c>
+        <v>423</v>
+      </c>
+      <c r="H10" s="36"/>
       <c r="I10" s="38"/>
       <c r="J10" s="38" t="s">
-        <v>606</v>
+        <v>594</v>
       </c>
       <c r="K10" s="39" t="s">
-        <v>607</v>
+        <v>595</v>
       </c>
       <c r="L10" s="40"/>
       <c r="M10" s="4" t="s">
-        <v>608</v>
+        <v>596</v>
       </c>
       <c r="N10" s="41" t="s">
         <v>13</v>
       </c>
       <c r="O10" s="37" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
       <c r="P10" s="43"/>
       <c r="Q10" s="43"/>
@@ -49146,44 +49171,44 @@
     </row>
     <row r="11" spans="1:28" s="44" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A11" s="36" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B11" s="37" t="s">
+        <v>420</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>422</v>
+      </c>
+      <c r="D11" s="32" t="s">
         <v>429</v>
       </c>
-      <c r="C11" s="37" t="s">
-        <v>431</v>
-      </c>
-      <c r="D11" s="32" t="s">
-        <v>438</v>
-      </c>
       <c r="E11" s="32" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="F11" s="32" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="G11" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="H11"/>
       <c r="J11" s="38" t="s">
-        <v>609</v>
+        <v>597</v>
       </c>
       <c r="K11" s="39" t="s">
-        <v>610</v>
+        <v>670</v>
       </c>
       <c r="L11" s="40" t="s">
-        <v>581</v>
+        <v>571</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>608</v>
+        <v>596</v>
       </c>
       <c r="N11" s="41" t="s">
         <v>13</v>
       </c>
       <c r="O11" s="42" t="s">
-        <v>583</v>
+        <v>669</v>
       </c>
       <c r="P11" s="43"/>
       <c r="Q11" s="43"/>
@@ -49201,39 +49226,37 @@
     </row>
     <row r="12" spans="1:28" s="44" customFormat="1" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A12" s="36" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B12" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="F12" s="33" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="G12" s="33" t="s">
-        <v>418</v>
-      </c>
-      <c r="H12" s="36" t="s">
-        <v>188</v>
-      </c>
+        <v>410</v>
+      </c>
+      <c r="H12" s="36"/>
       <c r="I12" s="38"/>
       <c r="J12" s="38" t="s">
-        <v>606</v>
+        <v>594</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>613</v>
+        <v>600</v>
       </c>
       <c r="L12" s="40"/>
       <c r="M12" s="4" t="s">
-        <v>608</v>
+        <v>596</v>
       </c>
       <c r="N12" s="41" t="s">
         <v>13</v>
@@ -49253,95 +49276,87 @@
       <c r="AA12" s="43"/>
       <c r="AB12" s="43"/>
     </row>
-    <row r="13" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" s="44" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>448</v>
-      </c>
-      <c r="C13" t="s">
-        <v>449</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>451</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>452</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>453</v>
-      </c>
-      <c r="H13" s="19"/>
-      <c r="I13" s="18"/>
+        <v>396</v>
+      </c>
+      <c r="B13" t="s">
+        <v>430</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>422</v>
+      </c>
+      <c r="D13" s="33"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="38"/>
       <c r="J13" s="38" t="s">
-        <v>611</v>
+        <v>597</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>614</v>
-      </c>
-      <c r="L13" s="14" t="s">
-        <v>46</v>
-      </c>
+        <v>663</v>
+      </c>
+      <c r="L13" s="40"/>
       <c r="M13" s="4" t="s">
-        <v>617</v>
-      </c>
-      <c r="N13" s="4" t="s">
+        <v>596</v>
+      </c>
+      <c r="N13" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="O13" s="3"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
-      <c r="U13" s="5"/>
-      <c r="V13" s="5"/>
-      <c r="W13" s="5"/>
-      <c r="X13" s="5"/>
-      <c r="Y13" s="5"/>
-      <c r="Z13" s="5"/>
-      <c r="AA13" s="5"/>
-      <c r="AB13" s="5"/>
+      <c r="O13" s="37" t="s">
+        <v>671</v>
+      </c>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="43"/>
+      <c r="R13" s="43"/>
+      <c r="S13" s="43"/>
+      <c r="T13" s="43"/>
+      <c r="U13" s="43"/>
+      <c r="V13" s="43"/>
+      <c r="W13" s="43"/>
+      <c r="X13" s="43"/>
+      <c r="Y13" s="43"/>
+      <c r="Z13" s="43"/>
+      <c r="AA13" s="43"/>
+      <c r="AB13" s="43"/>
     </row>
     <row r="14" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A14" s="36" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="C14" t="s">
-        <v>454</v>
+        <v>677</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>585</v>
+        <v>440</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>584</v>
+        <v>441</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>455</v>
+        <v>442</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>453</v>
+        <v>443</v>
       </c>
       <c r="H14" s="19"/>
       <c r="I14" s="18"/>
       <c r="J14" s="38" t="s">
-        <v>612</v>
+        <v>598</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>615</v>
+        <v>601</v>
       </c>
       <c r="L14" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>617</v>
+        <v>604</v>
       </c>
       <c r="N14" s="4" t="s">
         <v>13</v>
@@ -49361,37 +49376,41 @@
       <c r="AA14" s="5"/>
       <c r="AB14" s="5"/>
     </row>
-    <row r="15" spans="1:28" ht="113" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A15" s="36" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B15" s="15" t="s">
+        <v>439</v>
+      </c>
+      <c r="C15" t="s">
+        <v>444</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>574</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>573</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>445</v>
+      </c>
+      <c r="G15" s="19" t="s">
         <v>443</v>
-      </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="19" t="s">
-        <v>444</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>447</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>446</v>
-      </c>
-      <c r="G15" s="19" t="s">
-        <v>445</v>
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
+      <c r="J15" s="38" t="s">
+        <v>599</v>
+      </c>
       <c r="K15" s="1" t="s">
-        <v>582</v>
+        <v>602</v>
       </c>
       <c r="L15" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>16</v>
+        <v>604</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>13</v>
@@ -49411,44 +49430,40 @@
       <c r="AA15" s="5"/>
       <c r="AB15" s="5"/>
     </row>
-    <row r="16" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="45" t="s">
-        <v>402</v>
-      </c>
-      <c r="B16" t="s">
-        <v>456</v>
-      </c>
-      <c r="C16" t="s">
-        <v>449</v>
-      </c>
-      <c r="D16" t="s">
-        <v>462</v>
-      </c>
-      <c r="E16" t="s">
-        <v>463</v>
-      </c>
-      <c r="F16" t="s">
-        <v>464</v>
-      </c>
-      <c r="G16" t="s">
-        <v>465</v>
+    <row r="16" spans="1:28" ht="113" x14ac:dyDescent="0.3">
+      <c r="A16" s="36" t="s">
+        <v>396</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>434</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="19" t="s">
+        <v>435</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>438</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>437</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>436</v>
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="18"/>
-      <c r="J16" s="38" t="s">
-        <v>611</v>
-      </c>
+      <c r="J16" s="18"/>
       <c r="K16" s="1" t="s">
-        <v>616</v>
+        <v>572</v>
       </c>
       <c r="L16" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>617</v>
+        <v>16</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="O16" s="3"/>
       <c r="P16" s="5"/>
@@ -49467,39 +49482,39 @@
     </row>
     <row r="17" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A17" s="45" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B17" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
       <c r="C17" t="s">
+        <v>677</v>
+      </c>
+      <c r="D17" t="s">
+        <v>452</v>
+      </c>
+      <c r="E17" t="s">
+        <v>453</v>
+      </c>
+      <c r="F17" t="s">
         <v>454</v>
       </c>
-      <c r="D17" t="s">
-        <v>466</v>
-      </c>
-      <c r="E17" t="s">
-        <v>467</v>
-      </c>
-      <c r="F17" t="s">
-        <v>468</v>
-      </c>
       <c r="G17" t="s">
-        <v>469</v>
+        <v>455</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="18"/>
       <c r="J17" s="38" t="s">
-        <v>612</v>
+        <v>598</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>618</v>
+        <v>603</v>
       </c>
       <c r="L17" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>617</v>
+        <v>604</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>8</v>
@@ -49520,36 +49535,40 @@
       <c r="AB17" s="5"/>
     </row>
     <row r="18" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="36" t="s">
-        <v>402</v>
+      <c r="A18" s="45" t="s">
+        <v>396</v>
       </c>
       <c r="B18" t="s">
+        <v>446</v>
+      </c>
+      <c r="C18" t="s">
+        <v>444</v>
+      </c>
+      <c r="D18" t="s">
+        <v>456</v>
+      </c>
+      <c r="E18" t="s">
         <v>457</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15" t="s">
+      <c r="F18" t="s">
         <v>458</v>
       </c>
-      <c r="E18" t="s">
+      <c r="G18" t="s">
         <v>459</v>
-      </c>
-      <c r="F18" t="s">
-        <v>460</v>
-      </c>
-      <c r="G18" t="s">
-        <v>461</v>
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
+      <c r="J18" s="38" t="s">
+        <v>599</v>
+      </c>
       <c r="K18" s="1" t="s">
-        <v>245</v>
+        <v>605</v>
       </c>
       <c r="L18" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>3</v>
+        <v>604</v>
       </c>
       <c r="N18" s="4" t="s">
         <v>8</v>
@@ -49569,38 +49588,40 @@
       <c r="AA18" s="5"/>
       <c r="AB18" s="5"/>
     </row>
-    <row r="19" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A19" s="36" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B19" t="s">
-        <v>470</v>
-      </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>473</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>472</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="H19" s="10"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
+        <v>447</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15" t="s">
+        <v>448</v>
+      </c>
+      <c r="E19" t="s">
+        <v>449</v>
+      </c>
+      <c r="F19" t="s">
+        <v>450</v>
+      </c>
+      <c r="G19" t="s">
+        <v>451</v>
+      </c>
+      <c r="H19" s="19"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
       <c r="K19" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="L19" s="12"/>
+        <v>245</v>
+      </c>
+      <c r="L19" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="M19" s="4" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="O19" s="3"/>
       <c r="P19" s="5"/>
@@ -49617,35 +49638,35 @@
       <c r="AA19" s="5"/>
       <c r="AB19" s="5"/>
     </row>
-    <row r="20" spans="1:28" ht="151" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A20" s="36" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B20" t="s">
-        <v>476</v>
+        <v>460</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10" t="s">
-        <v>477</v>
-      </c>
-      <c r="E20" t="s">
-        <v>478</v>
-      </c>
-      <c r="F20" t="s">
-        <v>479</v>
-      </c>
-      <c r="G20" t="s">
-        <v>586</v>
+        <v>464</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>463</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>462</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>461</v>
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="1" t="s">
-        <v>587</v>
+        <v>465</v>
       </c>
       <c r="L20" s="12"/>
       <c r="M20" s="4" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="N20" s="4" t="s">
         <v>13</v>
@@ -49665,37 +49686,35 @@
       <c r="AA20" s="5"/>
       <c r="AB20" s="5"/>
     </row>
-    <row r="21" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:28" ht="151" x14ac:dyDescent="0.35">
       <c r="A21" s="36" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B21" t="s">
-        <v>480</v>
-      </c>
-      <c r="C21" s="16"/>
-      <c r="D21" t="s">
-        <v>481</v>
+        <v>466</v>
+      </c>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10" t="s">
+        <v>467</v>
       </c>
       <c r="E21" t="s">
-        <v>482</v>
+        <v>468</v>
       </c>
       <c r="F21" t="s">
-        <v>483</v>
+        <v>469</v>
       </c>
       <c r="G21" t="s">
-        <v>588</v>
-      </c>
-      <c r="H21" s="20"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
+        <v>575</v>
+      </c>
+      <c r="H21" s="10"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
       <c r="K21" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="L21" s="14" t="s">
-        <v>46</v>
-      </c>
+        <v>672</v>
+      </c>
+      <c r="L21" s="12"/>
       <c r="M21" s="4" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="N21" s="4" t="s">
         <v>13</v>
@@ -49717,29 +49736,29 @@
     </row>
     <row r="22" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A22" s="36" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B22" t="s">
-        <v>485</v>
+        <v>470</v>
       </c>
       <c r="C22" s="16"/>
       <c r="D22" t="s">
-        <v>487</v>
+        <v>471</v>
       </c>
       <c r="E22" t="s">
-        <v>486</v>
+        <v>472</v>
       </c>
       <c r="F22" t="s">
-        <v>483</v>
+        <v>473</v>
       </c>
       <c r="G22" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="18"/>
       <c r="J22" s="18"/>
       <c r="K22" s="1" t="s">
-        <v>488</v>
+        <v>474</v>
       </c>
       <c r="L22" s="14" t="s">
         <v>46</v>
@@ -49765,44 +49784,40 @@
       <c r="AA22" s="5"/>
       <c r="AB22" s="5"/>
     </row>
-    <row r="23" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A23" s="36" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B23" t="s">
-        <v>489</v>
-      </c>
-      <c r="C23" t="s">
-        <v>490</v>
-      </c>
+        <v>475</v>
+      </c>
+      <c r="C23" s="16"/>
       <c r="D23" t="s">
-        <v>491</v>
+        <v>477</v>
       </c>
       <c r="E23" t="s">
-        <v>492</v>
+        <v>476</v>
       </c>
       <c r="F23" t="s">
-        <v>493</v>
+        <v>473</v>
       </c>
       <c r="G23" t="s">
-        <v>494</v>
+        <v>576</v>
       </c>
       <c r="H23" s="20"/>
       <c r="I23" s="18"/>
-      <c r="J23" s="38" t="s">
-        <v>629</v>
-      </c>
+      <c r="J23" s="18"/>
       <c r="K23" s="1" t="s">
-        <v>619</v>
+        <v>478</v>
       </c>
       <c r="L23" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>621</v>
+        <v>4</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="O23" s="3"/>
       <c r="P23" s="5"/>
@@ -49821,39 +49836,39 @@
     </row>
     <row r="24" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A24" s="36" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B24" t="s">
-        <v>489</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>495</v>
-      </c>
-      <c r="D24" s="30" t="s">
-        <v>497</v>
-      </c>
-      <c r="E24" s="30" t="s">
-        <v>496</v>
+        <v>479</v>
+      </c>
+      <c r="C24" t="s">
+        <v>480</v>
+      </c>
+      <c r="D24" t="s">
+        <v>481</v>
+      </c>
+      <c r="E24" t="s">
+        <v>482</v>
       </c>
       <c r="F24" t="s">
-        <v>493</v>
+        <v>483</v>
       </c>
       <c r="G24" t="s">
-        <v>494</v>
+        <v>484</v>
       </c>
       <c r="H24" s="20"/>
       <c r="I24" s="18"/>
       <c r="J24" s="38" t="s">
-        <v>630</v>
+        <v>615</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>620</v>
+        <v>606</v>
       </c>
       <c r="L24" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>621</v>
+        <v>608</v>
       </c>
       <c r="N24" s="4" t="s">
         <v>8</v>
@@ -49873,43 +49888,46 @@
       <c r="AA24" s="5"/>
       <c r="AB24" s="5"/>
     </row>
-    <row r="25" spans="1:28" ht="87" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A25" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B25" s="30" t="s">
-        <v>498</v>
+        <v>396</v>
+      </c>
+      <c r="B25" t="s">
+        <v>479</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>485</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>499</v>
+        <v>487</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>500</v>
-      </c>
-      <c r="F25" s="35" t="s">
-        <v>501</v>
-      </c>
-      <c r="G25" s="30" t="s">
-        <v>502</v>
+        <v>486</v>
+      </c>
+      <c r="F25" t="s">
+        <v>483</v>
+      </c>
+      <c r="G25" t="s">
+        <v>484</v>
       </c>
       <c r="H25" s="20"/>
       <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
+      <c r="J25" s="38" t="s">
+        <v>616</v>
+      </c>
       <c r="K25" s="1" t="s">
-        <v>503</v>
+        <v>607</v>
       </c>
       <c r="L25" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>16</v>
+        <v>608</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O25" s="3" t="s">
-        <v>504</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="O25" s="3"/>
       <c r="P25" s="5"/>
       <c r="Q25" s="5"/>
       <c r="R25" s="5"/>
@@ -49924,139 +49942,136 @@
       <c r="AA25" s="5"/>
       <c r="AB25" s="5"/>
     </row>
-    <row r="26" spans="1:28" s="29" customFormat="1" ht="101" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:28" ht="87" x14ac:dyDescent="0.35">
       <c r="A26" s="36" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>505</v>
-      </c>
-      <c r="C26" s="17"/>
+        <v>488</v>
+      </c>
       <c r="D26" s="30" t="s">
-        <v>508</v>
+        <v>489</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>507</v>
-      </c>
-      <c r="F26" s="33" t="s">
-        <v>506</v>
-      </c>
-      <c r="G26" s="17" t="s">
-        <v>418</v>
-      </c>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="26" t="s">
-        <v>422</v>
-      </c>
-      <c r="L26" s="27"/>
-      <c r="M26" s="27" t="s">
+        <v>490</v>
+      </c>
+      <c r="F26" s="35" t="s">
+        <v>491</v>
+      </c>
+      <c r="G26" s="30" t="s">
+        <v>492</v>
+      </c>
+      <c r="H26" s="20"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="L26" s="14"/>
+      <c r="M26" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N26" s="27" t="s">
+      <c r="N26" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O26" s="3"/>
-      <c r="P26" s="28"/>
-      <c r="Q26" s="28"/>
-      <c r="R26" s="28"/>
-      <c r="S26" s="28"/>
-      <c r="T26" s="28"/>
-      <c r="U26" s="28"/>
-      <c r="V26" s="28"/>
-      <c r="W26" s="28"/>
-      <c r="X26" s="28"/>
-      <c r="Y26" s="28"/>
-      <c r="Z26" s="28"/>
-      <c r="AA26" s="28"/>
-      <c r="AB26" s="28"/>
-    </row>
-    <row r="27" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+      <c r="O26" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="5"/>
+      <c r="V26" s="5"/>
+      <c r="W26" s="5"/>
+      <c r="X26" s="5"/>
+      <c r="Y26" s="5"/>
+      <c r="Z26" s="5"/>
+      <c r="AA26" s="5"/>
+      <c r="AB26" s="5"/>
+    </row>
+    <row r="27" spans="1:28" s="29" customFormat="1" ht="101" x14ac:dyDescent="0.35">
       <c r="A27" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B27" t="s">
-        <v>509</v>
-      </c>
-      <c r="C27" t="s">
-        <v>510</v>
-      </c>
+        <v>396</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>495</v>
+      </c>
+      <c r="C27" s="17"/>
       <c r="D27" s="30" t="s">
-        <v>513</v>
+        <v>498</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>512</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>511</v>
-      </c>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="38" t="s">
-        <v>631</v>
-      </c>
-      <c r="K27" s="8" t="s">
-        <v>622</v>
-      </c>
-      <c r="L27" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="M27" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="N27" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="F27" s="33" t="s">
+        <v>496</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>410</v>
+      </c>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="26" t="s">
+        <v>414</v>
+      </c>
+      <c r="L27" s="27"/>
+      <c r="M27" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="N27" s="27" t="s">
         <v>13</v>
       </c>
       <c r="O27" s="3"/>
-      <c r="P27" s="5"/>
-      <c r="Q27" s="5"/>
-      <c r="R27" s="5"/>
-      <c r="S27" s="5"/>
-      <c r="T27" s="5"/>
-      <c r="U27" s="5"/>
-      <c r="V27" s="5"/>
-      <c r="W27" s="5"/>
-      <c r="X27" s="5"/>
-      <c r="Y27" s="5"/>
-      <c r="Z27" s="5"/>
-      <c r="AA27" s="5"/>
-      <c r="AB27" s="5"/>
+      <c r="P27" s="28"/>
+      <c r="Q27" s="28"/>
+      <c r="R27" s="28"/>
+      <c r="S27" s="28"/>
+      <c r="T27" s="28"/>
+      <c r="U27" s="28"/>
+      <c r="V27" s="28"/>
+      <c r="W27" s="28"/>
+      <c r="X27" s="28"/>
+      <c r="Y27" s="28"/>
+      <c r="Z27" s="28"/>
+      <c r="AA27" s="28"/>
+      <c r="AB27" s="28"/>
     </row>
     <row r="28" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A28" s="36" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B28" t="s">
-        <v>509</v>
-      </c>
-      <c r="C28" s="30" t="s">
-        <v>514</v>
+        <v>499</v>
+      </c>
+      <c r="C28" t="s">
+        <v>500</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>516</v>
+        <v>503</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>515</v>
+        <v>502</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>511</v>
+        <v>501</v>
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
       <c r="I28" s="7"/>
       <c r="J28" s="38" t="s">
-        <v>632</v>
+        <v>617</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>623</v>
+        <v>609</v>
       </c>
       <c r="L28" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>621</v>
+        <v>608</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>13</v>
@@ -50078,37 +50093,37 @@
     </row>
     <row r="29" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A29" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B29" s="30" t="s">
-        <v>517</v>
-      </c>
-      <c r="C29" t="s">
-        <v>510</v>
+        <v>396</v>
+      </c>
+      <c r="B29" t="s">
+        <v>499</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>504</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>518</v>
+        <v>506</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>519</v>
-      </c>
-      <c r="F29" s="30" t="s">
-        <v>520</v>
+        <v>505</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>501</v>
       </c>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
       <c r="I29" s="7"/>
       <c r="J29" s="38" t="s">
-        <v>631</v>
+        <v>618</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>624</v>
+        <v>673</v>
       </c>
       <c r="L29" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>621</v>
+        <v>608</v>
       </c>
       <c r="N29" s="4" t="s">
         <v>13</v>
@@ -50130,37 +50145,37 @@
     </row>
     <row r="30" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A30" s="36" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>517</v>
-      </c>
-      <c r="C30" s="30" t="s">
-        <v>521</v>
+        <v>507</v>
+      </c>
+      <c r="C30" t="s">
+        <v>500</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>522</v>
+        <v>508</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>523</v>
+        <v>509</v>
       </c>
       <c r="F30" s="30" t="s">
-        <v>520</v>
+        <v>510</v>
       </c>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
       <c r="I30" s="7"/>
       <c r="J30" s="38" t="s">
-        <v>633</v>
+        <v>617</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>625</v>
+        <v>610</v>
       </c>
       <c r="L30" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>621</v>
+        <v>608</v>
       </c>
       <c r="N30" s="4" t="s">
         <v>13</v>
@@ -50182,35 +50197,37 @@
     </row>
     <row r="31" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A31" s="36" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>524</v>
-      </c>
-      <c r="C31" s="16"/>
+        <v>507</v>
+      </c>
+      <c r="C31" s="30" t="s">
+        <v>511</v>
+      </c>
       <c r="D31" s="30" t="s">
-        <v>525</v>
+        <v>512</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>526</v>
+        <v>513</v>
       </c>
       <c r="F31" s="30" t="s">
-        <v>527</v>
-      </c>
-      <c r="G31" s="30" t="s">
-        <v>528</v>
-      </c>
-      <c r="H31" s="20"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="1" t="s">
-        <v>240</v>
+        <v>510</v>
+      </c>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="38" t="s">
+        <v>619</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>611</v>
       </c>
       <c r="L31" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>4</v>
+        <v>608</v>
       </c>
       <c r="N31" s="4" t="s">
         <v>13</v>
@@ -50230,42 +50247,40 @@
       <c r="AA31" s="5"/>
       <c r="AB31" s="5"/>
     </row>
-    <row r="32" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A32" s="36" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>529</v>
-      </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="30" t="s">
-        <v>530</v>
-      </c>
-      <c r="E32" s="30" t="s">
-        <v>531</v>
-      </c>
-      <c r="F32" s="30" t="s">
-        <v>532</v>
-      </c>
-      <c r="G32" s="30" t="s">
-        <v>533</v>
-      </c>
-      <c r="H32" s="20"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="1" t="s">
-        <v>534</v>
+        <v>507</v>
+      </c>
+      <c r="C32" s="47" t="s">
+        <v>675</v>
+      </c>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="38" t="s">
+        <v>676</v>
+      </c>
+      <c r="K32" s="8" t="s">
+        <v>663</v>
       </c>
       <c r="L32" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>4</v>
+        <v>608</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="O32" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="O32" s="3" t="s">
+        <v>662</v>
+      </c>
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
       <c r="R32" s="5"/>
@@ -50280,44 +50295,40 @@
       <c r="AA32" s="5"/>
       <c r="AB32" s="5"/>
     </row>
-    <row r="33" spans="1:28" ht="126" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A33" s="36" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>535</v>
-      </c>
-      <c r="C33" s="30" t="s">
-        <v>536</v>
-      </c>
+        <v>514</v>
+      </c>
+      <c r="C33" s="16"/>
       <c r="D33" s="30" t="s">
-        <v>537</v>
+        <v>515</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>538</v>
+        <v>516</v>
       </c>
       <c r="F33" s="30" t="s">
-        <v>539</v>
+        <v>517</v>
       </c>
       <c r="G33" s="30" t="s">
-        <v>540</v>
+        <v>518</v>
       </c>
       <c r="H33" s="20"/>
       <c r="I33" s="18"/>
-      <c r="J33" s="38" t="s">
-        <v>634</v>
-      </c>
+      <c r="J33" s="18"/>
       <c r="K33" s="1" t="s">
-        <v>626</v>
+        <v>674</v>
       </c>
       <c r="L33" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>648</v>
+        <v>4</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="O33" s="3"/>
       <c r="P33" s="5"/>
@@ -50334,41 +50345,37 @@
       <c r="AA33" s="5"/>
       <c r="AB33" s="5"/>
     </row>
-    <row r="34" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A34" s="36" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>535</v>
-      </c>
-      <c r="C34" s="30" t="s">
-        <v>541</v>
-      </c>
+        <v>519</v>
+      </c>
+      <c r="C34" s="16"/>
       <c r="D34" s="30" t="s">
-        <v>545</v>
+        <v>520</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>544</v>
+        <v>521</v>
       </c>
       <c r="F34" s="30" t="s">
-        <v>543</v>
+        <v>522</v>
       </c>
       <c r="G34" s="30" t="s">
-        <v>542</v>
+        <v>523</v>
       </c>
       <c r="H34" s="20"/>
       <c r="I34" s="18"/>
-      <c r="J34" s="38" t="s">
-        <v>635</v>
-      </c>
+      <c r="J34" s="18"/>
       <c r="K34" s="1" t="s">
-        <v>627</v>
+        <v>524</v>
       </c>
       <c r="L34" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>648</v>
+        <v>4</v>
       </c>
       <c r="N34" s="4" t="s">
         <v>8</v>
@@ -50388,41 +50395,41 @@
       <c r="AA34" s="5"/>
       <c r="AB34" s="5"/>
     </row>
-    <row r="35" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:28" ht="126" x14ac:dyDescent="0.35">
       <c r="A35" s="36" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B35" s="30" t="s">
-        <v>535</v>
+        <v>525</v>
       </c>
       <c r="C35" s="30" t="s">
-        <v>546</v>
+        <v>526</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>548</v>
+        <v>527</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>547</v>
+        <v>528</v>
       </c>
       <c r="F35" s="30" t="s">
-        <v>543</v>
+        <v>529</v>
       </c>
       <c r="G35" s="30" t="s">
-        <v>542</v>
+        <v>530</v>
       </c>
       <c r="H35" s="20"/>
       <c r="I35" s="18"/>
       <c r="J35" s="38" t="s">
-        <v>636</v>
+        <v>620</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>628</v>
+        <v>612</v>
       </c>
       <c r="L35" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>648</v>
+        <v>634</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>8</v>
@@ -50442,40 +50449,44 @@
       <c r="AA35" s="5"/>
       <c r="AB35" s="5"/>
     </row>
-    <row r="36" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A36" s="36" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>555</v>
-      </c>
-      <c r="C36" s="30"/>
+        <v>525</v>
+      </c>
+      <c r="C36" s="30" t="s">
+        <v>531</v>
+      </c>
       <c r="D36" s="30" t="s">
-        <v>559</v>
+        <v>535</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>558</v>
+        <v>534</v>
       </c>
       <c r="F36" s="30" t="s">
-        <v>557</v>
+        <v>533</v>
       </c>
       <c r="G36" s="30" t="s">
-        <v>556</v>
+        <v>532</v>
       </c>
       <c r="H36" s="20"/>
       <c r="I36" s="18"/>
-      <c r="J36" s="18"/>
+      <c r="J36" s="38" t="s">
+        <v>621</v>
+      </c>
       <c r="K36" s="1" t="s">
-        <v>560</v>
+        <v>613</v>
       </c>
       <c r="L36" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>4</v>
+        <v>634</v>
       </c>
       <c r="N36" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="O36" s="3"/>
       <c r="P36" s="5"/>
@@ -50492,37 +50503,41 @@
       <c r="AA36" s="5"/>
       <c r="AB36" s="5"/>
     </row>
-    <row r="37" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A37" s="36" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B37" s="30" t="s">
-        <v>549</v>
-      </c>
-      <c r="C37" s="30"/>
+        <v>525</v>
+      </c>
+      <c r="C37" s="30" t="s">
+        <v>536</v>
+      </c>
       <c r="D37" s="30" t="s">
-        <v>550</v>
+        <v>538</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>553</v>
+        <v>537</v>
       </c>
       <c r="F37" s="30" t="s">
-        <v>552</v>
+        <v>533</v>
       </c>
       <c r="G37" s="30" t="s">
-        <v>551</v>
+        <v>532</v>
       </c>
       <c r="H37" s="20"/>
       <c r="I37" s="18"/>
-      <c r="J37" s="18"/>
+      <c r="J37" s="38" t="s">
+        <v>622</v>
+      </c>
       <c r="K37" s="1" t="s">
-        <v>554</v>
+        <v>614</v>
       </c>
       <c r="L37" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>4</v>
+        <v>634</v>
       </c>
       <c r="N37" s="4" t="s">
         <v>8</v>
@@ -50544,29 +50559,29 @@
     </row>
     <row r="38" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A38" s="36" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B38" s="30" t="s">
-        <v>567</v>
-      </c>
-      <c r="C38" s="16"/>
+        <v>545</v>
+      </c>
+      <c r="C38" s="30"/>
       <c r="D38" s="30" t="s">
-        <v>571</v>
+        <v>549</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>570</v>
+        <v>548</v>
       </c>
       <c r="F38" s="30" t="s">
-        <v>569</v>
-      </c>
-      <c r="G38" s="20" t="s">
-        <v>568</v>
+        <v>547</v>
+      </c>
+      <c r="G38" s="30" t="s">
+        <v>546</v>
       </c>
       <c r="H38" s="20"/>
       <c r="I38" s="18"/>
       <c r="J38" s="18"/>
       <c r="K38" s="1" t="s">
-        <v>572</v>
+        <v>550</v>
       </c>
       <c r="L38" s="14" t="s">
         <v>46</v>
@@ -50594,29 +50609,29 @@
     </row>
     <row r="39" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A39" s="36" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B39" s="30" t="s">
-        <v>561</v>
-      </c>
-      <c r="C39" s="16"/>
+        <v>539</v>
+      </c>
+      <c r="C39" s="30"/>
       <c r="D39" s="30" t="s">
-        <v>565</v>
+        <v>540</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>564</v>
+        <v>543</v>
       </c>
       <c r="F39" s="30" t="s">
-        <v>563</v>
-      </c>
-      <c r="G39" s="33" t="s">
-        <v>562</v>
+        <v>542</v>
+      </c>
+      <c r="G39" s="30" t="s">
+        <v>541</v>
       </c>
       <c r="H39" s="20"/>
       <c r="I39" s="18"/>
       <c r="J39" s="18"/>
       <c r="K39" s="1" t="s">
-        <v>566</v>
+        <v>544</v>
       </c>
       <c r="L39" s="14" t="s">
         <v>46</v>
@@ -50644,29 +50659,29 @@
     </row>
     <row r="40" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A40" s="36" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B40" s="30" t="s">
-        <v>573</v>
-      </c>
-      <c r="C40" s="15"/>
+        <v>557</v>
+      </c>
+      <c r="C40" s="16"/>
       <c r="D40" s="30" t="s">
-        <v>577</v>
+        <v>561</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>576</v>
+        <v>560</v>
       </c>
       <c r="F40" s="30" t="s">
-        <v>575</v>
-      </c>
-      <c r="G40" s="30" t="s">
-        <v>574</v>
-      </c>
-      <c r="H40" s="19"/>
+        <v>559</v>
+      </c>
+      <c r="G40" s="20" t="s">
+        <v>558</v>
+      </c>
+      <c r="H40" s="20"/>
       <c r="I40" s="18"/>
       <c r="J40" s="18"/>
       <c r="K40" s="1" t="s">
-        <v>579</v>
+        <v>562</v>
       </c>
       <c r="L40" s="14" t="s">
         <v>46</v>
@@ -50677,9 +50692,7 @@
       <c r="N40" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O40" s="3" t="s">
-        <v>578</v>
-      </c>
+      <c r="O40" s="3"/>
       <c r="P40" s="5"/>
       <c r="Q40" s="5"/>
       <c r="R40" s="5"/>
@@ -50694,48 +50707,42 @@
       <c r="AA40" s="5"/>
       <c r="AB40" s="5"/>
     </row>
-    <row r="41" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="B41" t="s">
-        <v>362</v>
-      </c>
-      <c r="C41" t="s">
-        <v>358</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>589</v>
-      </c>
-      <c r="E41" s="10" t="s">
-        <v>590</v>
-      </c>
-      <c r="F41" s="10" t="s">
-        <v>591</v>
-      </c>
-      <c r="G41" s="10" t="s">
-        <v>592</v>
-      </c>
-      <c r="H41" s="10"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="38" t="s">
-        <v>637</v>
-      </c>
-      <c r="K41" s="8" t="s">
-        <v>650</v>
-      </c>
-      <c r="L41" s="11" t="s">
-        <v>11</v>
+    <row r="41" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+      <c r="A41" s="36" t="s">
+        <v>396</v>
+      </c>
+      <c r="B41" s="30" t="s">
+        <v>551</v>
+      </c>
+      <c r="C41" s="16"/>
+      <c r="D41" s="30" t="s">
+        <v>555</v>
+      </c>
+      <c r="E41" s="30" t="s">
+        <v>554</v>
+      </c>
+      <c r="F41" s="30" t="s">
+        <v>553</v>
+      </c>
+      <c r="G41" s="33" t="s">
+        <v>552</v>
+      </c>
+      <c r="H41" s="20"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="L41" s="14" t="s">
+        <v>46</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>617</v>
+        <v>4</v>
       </c>
       <c r="N41" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O41" s="3" t="s">
-        <v>593</v>
-      </c>
+      <c r="O41" s="3"/>
       <c r="P41" s="5"/>
       <c r="Q41" s="5"/>
       <c r="R41" s="5"/>
@@ -50750,39 +50757,43 @@
       <c r="AA41" s="5"/>
       <c r="AB41" s="5"/>
     </row>
-    <row r="42" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="B42" t="s">
-        <v>362</v>
-      </c>
-      <c r="C42" t="s">
-        <v>676</v>
-      </c>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="38" t="s">
-        <v>677</v>
-      </c>
-      <c r="K42" s="8" t="s">
-        <v>679</v>
-      </c>
-      <c r="L42" s="11" t="s">
-        <v>11</v>
+    <row r="42" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+      <c r="A42" s="36" t="s">
+        <v>396</v>
+      </c>
+      <c r="B42" s="30" t="s">
+        <v>563</v>
+      </c>
+      <c r="C42" s="15"/>
+      <c r="D42" s="30" t="s">
+        <v>567</v>
+      </c>
+      <c r="E42" s="30" t="s">
+        <v>566</v>
+      </c>
+      <c r="F42" s="30" t="s">
+        <v>565</v>
+      </c>
+      <c r="G42" s="30" t="s">
+        <v>564</v>
+      </c>
+      <c r="H42" s="19"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="18"/>
+      <c r="K42" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="L42" s="14" t="s">
+        <v>571</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>617</v>
+        <v>4</v>
       </c>
       <c r="N42" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="O42" s="3" t="s">
-        <v>678</v>
+        <v>568</v>
       </c>
       <c r="P42" s="5"/>
       <c r="Q42" s="5"/>
@@ -50806,39 +50817,39 @@
         <v>357</v>
       </c>
       <c r="C43" t="s">
-        <v>358</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>594</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>361</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>360</v>
-      </c>
-      <c r="G43" s="7" t="s">
-        <v>359</v>
-      </c>
-      <c r="H43" s="7"/>
+        <v>353</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>577</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>578</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>579</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>580</v>
+      </c>
+      <c r="H43" s="10"/>
       <c r="I43" s="7"/>
       <c r="J43" s="38" t="s">
-        <v>637</v>
+        <v>623</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>651</v>
+        <v>636</v>
       </c>
       <c r="L43" s="11" t="s">
         <v>11</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>617</v>
+        <v>604</v>
       </c>
       <c r="N43" s="4" t="s">
         <v>8</v>
       </c>
       <c r="O43" s="3" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
       <c r="P43" s="5"/>
       <c r="Q43" s="5"/>
@@ -50862,31 +50873,31 @@
         <v>357</v>
       </c>
       <c r="C44" t="s">
-        <v>676</v>
-      </c>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="7"/>
+        <v>660</v>
+      </c>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
       <c r="I44" s="7"/>
       <c r="J44" s="38" t="s">
-        <v>677</v>
+        <v>661</v>
       </c>
       <c r="K44" s="8" t="s">
-        <v>679</v>
+        <v>663</v>
       </c>
       <c r="L44" s="11" t="s">
         <v>11</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>617</v>
+        <v>604</v>
       </c>
       <c r="N44" s="4" t="s">
         <v>8</v>
       </c>
       <c r="O44" s="3" t="s">
-        <v>678</v>
+        <v>662</v>
       </c>
       <c r="P44" s="5"/>
       <c r="Q44" s="5"/>
@@ -50907,43 +50918,43 @@
         <v>310</v>
       </c>
       <c r="B45" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C45" t="s">
-        <v>351</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>595</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>596</v>
-      </c>
-      <c r="F45" s="10" t="s">
-        <v>597</v>
-      </c>
-      <c r="G45" s="10" t="s">
-        <v>352</v>
-      </c>
-      <c r="H45" s="10" t="s">
-        <v>188</v>
-      </c>
+        <v>353</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>582</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="H45" s="7"/>
       <c r="I45" s="7"/>
       <c r="J45" s="38" t="s">
-        <v>638</v>
+        <v>623</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>652</v>
+        <v>637</v>
       </c>
       <c r="L45" s="11" t="s">
         <v>11</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>617</v>
+        <v>604</v>
       </c>
       <c r="N45" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O45" s="3"/>
+      <c r="O45" s="3" t="s">
+        <v>581</v>
+      </c>
       <c r="P45" s="5"/>
       <c r="Q45" s="5"/>
       <c r="R45" s="5"/>
@@ -50958,48 +50969,40 @@
       <c r="AA45" s="5"/>
       <c r="AB45" s="5"/>
     </row>
-    <row r="46" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B46" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C46" t="s">
-        <v>353</v>
-      </c>
-      <c r="D46" s="10" t="s">
-        <v>598</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>599</v>
-      </c>
-      <c r="F46" s="10" t="s">
-        <v>600</v>
-      </c>
-      <c r="G46" s="10" t="s">
-        <v>354</v>
-      </c>
-      <c r="H46" s="10" t="s">
-        <v>188</v>
-      </c>
+        <v>660</v>
+      </c>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
       <c r="I46" s="7"/>
       <c r="J46" s="38" t="s">
-        <v>639</v>
+        <v>661</v>
       </c>
       <c r="K46" s="8" t="s">
-        <v>653</v>
+        <v>663</v>
       </c>
       <c r="L46" s="11" t="s">
         <v>11</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>617</v>
+        <v>604</v>
       </c>
       <c r="N46" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O46" s="3"/>
+      <c r="O46" s="3" t="s">
+        <v>662</v>
+      </c>
       <c r="P46" s="5"/>
       <c r="Q46" s="5"/>
       <c r="R46" s="5"/>
@@ -51019,38 +51022,38 @@
         <v>310</v>
       </c>
       <c r="B47" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C47" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>601</v>
+        <v>583</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>602</v>
+        <v>584</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>603</v>
+        <v>585</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="H47" s="10" t="s">
         <v>188</v>
       </c>
       <c r="I47" s="7"/>
       <c r="J47" s="38" t="s">
-        <v>640</v>
+        <v>624</v>
       </c>
       <c r="K47" s="8" t="s">
-        <v>654</v>
+        <v>638</v>
       </c>
       <c r="L47" s="11" t="s">
         <v>11</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>617</v>
+        <v>604</v>
       </c>
       <c r="N47" s="4" t="s">
         <v>8</v>
@@ -51070,39 +51073,43 @@
       <c r="AA47" s="5"/>
       <c r="AB47" s="5"/>
     </row>
-    <row r="48" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B48" t="s">
-        <v>344</v>
-      </c>
-      <c r="C48"/>
-      <c r="D48" t="s">
-        <v>345</v>
-      </c>
-      <c r="E48" t="s">
         <v>346</v>
       </c>
-      <c r="F48" t="s">
-        <v>347</v>
-      </c>
-      <c r="G48" t="s">
-        <v>348</v>
+      <c r="C48" t="s">
+        <v>349</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>586</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>587</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="G48" s="10" t="s">
+        <v>350</v>
       </c>
       <c r="H48" s="10" t="s">
         <v>188</v>
       </c>
       <c r="I48" s="7"/>
-      <c r="J48" s="7"/>
-      <c r="K48" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="L48" s="4" t="s">
-        <v>2</v>
+      <c r="J48" s="38" t="s">
+        <v>625</v>
+      </c>
+      <c r="K48" s="8" t="s">
+        <v>639</v>
+      </c>
+      <c r="L48" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>3</v>
+        <v>604</v>
       </c>
       <c r="N48" s="4" t="s">
         <v>8</v>
@@ -51127,36 +51134,38 @@
         <v>310</v>
       </c>
       <c r="B49" t="s">
-        <v>311</v>
+        <v>346</v>
       </c>
       <c r="C49" t="s">
-        <v>313</v>
-      </c>
-      <c r="D49" s="30" t="s">
-        <v>315</v>
-      </c>
-      <c r="E49" s="30" t="s">
-        <v>316</v>
-      </c>
-      <c r="F49" s="30" t="s">
-        <v>317</v>
-      </c>
-      <c r="G49" s="30" t="s">
-        <v>318</v>
-      </c>
-      <c r="H49" s="7"/>
+        <v>678</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>589</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>590</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>591</v>
+      </c>
+      <c r="G49" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="H49" s="10" t="s">
+        <v>188</v>
+      </c>
       <c r="I49" s="7"/>
       <c r="J49" s="38" t="s">
-        <v>641</v>
+        <v>626</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>655</v>
-      </c>
-      <c r="L49" s="4" t="s">
-        <v>2</v>
+        <v>640</v>
+      </c>
+      <c r="L49" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>649</v>
+        <v>604</v>
       </c>
       <c r="N49" s="4" t="s">
         <v>8</v>
@@ -51176,41 +51185,39 @@
       <c r="AA49" s="5"/>
       <c r="AB49" s="5"/>
     </row>
-    <row r="50" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A50" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B50" t="s">
-        <v>311</v>
-      </c>
-      <c r="C50" t="s">
-        <v>314</v>
-      </c>
-      <c r="D50" s="30" t="s">
-        <v>319</v>
-      </c>
-      <c r="E50" s="30" t="s">
-        <v>320</v>
-      </c>
-      <c r="F50" s="30" t="s">
-        <v>321</v>
-      </c>
-      <c r="G50" s="30" t="s">
-        <v>322</v>
-      </c>
-      <c r="H50" s="7"/>
+        <v>340</v>
+      </c>
+      <c r="C50"/>
+      <c r="D50" t="s">
+        <v>341</v>
+      </c>
+      <c r="E50" t="s">
+        <v>342</v>
+      </c>
+      <c r="F50" t="s">
+        <v>343</v>
+      </c>
+      <c r="G50" t="s">
+        <v>344</v>
+      </c>
+      <c r="H50" s="10" t="s">
+        <v>188</v>
+      </c>
       <c r="I50" s="7"/>
-      <c r="J50" s="38" t="s">
-        <v>642</v>
-      </c>
-      <c r="K50" s="8" t="s">
-        <v>656</v>
+      <c r="J50" s="7"/>
+      <c r="K50" s="1" t="s">
+        <v>345</v>
       </c>
       <c r="L50" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>649</v>
+        <v>3</v>
       </c>
       <c r="N50" s="4" t="s">
         <v>8</v>
@@ -51238,33 +51245,33 @@
         <v>311</v>
       </c>
       <c r="C51" t="s">
-        <v>323</v>
+        <v>681</v>
       </c>
       <c r="D51" s="30" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="E51" s="30" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F51" s="30" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="G51" s="30" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
       <c r="J51" s="38" t="s">
-        <v>643</v>
+        <v>627</v>
       </c>
       <c r="K51" s="8" t="s">
-        <v>657</v>
+        <v>641</v>
       </c>
       <c r="L51" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>617</v>
+        <v>635</v>
       </c>
       <c r="N51" s="4" t="s">
         <v>8</v>
@@ -51292,33 +51299,33 @@
         <v>311</v>
       </c>
       <c r="C52" t="s">
-        <v>324</v>
+        <v>680</v>
       </c>
       <c r="D52" s="30" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="E52" s="30" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="F52" s="30" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="G52" s="30" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="H52" s="7"/>
       <c r="I52" s="7"/>
       <c r="J52" s="38" t="s">
-        <v>644</v>
+        <v>628</v>
       </c>
       <c r="K52" s="8" t="s">
-        <v>658</v>
+        <v>642</v>
       </c>
       <c r="L52" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>617</v>
+        <v>635</v>
       </c>
       <c r="N52" s="4" t="s">
         <v>8</v>
@@ -51346,33 +51353,33 @@
         <v>311</v>
       </c>
       <c r="C53" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="D53" s="30" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="E53" s="30" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="F53" s="30" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="G53" s="30" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="H53" s="7"/>
       <c r="I53" s="7"/>
       <c r="J53" s="38" t="s">
-        <v>645</v>
+        <v>629</v>
       </c>
       <c r="K53" s="8" t="s">
-        <v>659</v>
+        <v>643</v>
       </c>
       <c r="L53" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>617</v>
+        <v>604</v>
       </c>
       <c r="N53" s="4" t="s">
         <v>8</v>
@@ -51400,33 +51407,33 @@
         <v>311</v>
       </c>
       <c r="C54" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="D54" s="30" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="E54" s="30" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
       <c r="F54" s="30" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="G54" s="30" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="H54" s="7"/>
       <c r="I54" s="7"/>
       <c r="J54" s="38" t="s">
-        <v>646</v>
+        <v>630</v>
       </c>
       <c r="K54" s="8" t="s">
-        <v>660</v>
+        <v>644</v>
       </c>
       <c r="L54" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>617</v>
+        <v>604</v>
       </c>
       <c r="N54" s="4" t="s">
         <v>8</v>
@@ -51454,33 +51461,33 @@
         <v>311</v>
       </c>
       <c r="C55" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="D55" s="30" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="E55" s="30" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="F55" s="30" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="G55" s="30" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="H55" s="7"/>
       <c r="I55" s="7"/>
       <c r="J55" s="38" t="s">
-        <v>647</v>
+        <v>631</v>
       </c>
       <c r="K55" s="8" t="s">
-        <v>661</v>
+        <v>645</v>
       </c>
       <c r="L55" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M55" s="4" t="s">
-        <v>617</v>
+        <v>604</v>
       </c>
       <c r="N55" s="4" t="s">
         <v>8</v>
@@ -51500,44 +51507,46 @@
       <c r="AA55" s="5"/>
       <c r="AB55" s="5"/>
     </row>
-    <row r="56" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B56" t="s">
-        <v>363</v>
+        <v>311</v>
       </c>
       <c r="C56" t="s">
-        <v>376</v>
-      </c>
-      <c r="D56" s="10" t="s">
-        <v>421</v>
-      </c>
-      <c r="E56" s="10" t="s">
+        <v>682</v>
+      </c>
+      <c r="D56" s="30" t="s">
+        <v>333</v>
+      </c>
+      <c r="E56" s="30" t="s">
+        <v>334</v>
+      </c>
+      <c r="F56" s="30" t="s">
+        <v>330</v>
+      </c>
+      <c r="G56" s="30" t="s">
+        <v>335</v>
+      </c>
+      <c r="H56" s="7"/>
+      <c r="I56" s="7"/>
+      <c r="J56" s="38" t="s">
+        <v>632</v>
+      </c>
+      <c r="K56" s="8" t="s">
+        <v>646</v>
+      </c>
+      <c r="L56" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="M56" s="4" t="s">
         <v>604</v>
       </c>
-      <c r="F56" s="10" t="s">
-        <v>605</v>
-      </c>
-      <c r="G56" s="10" t="s">
-        <v>365</v>
-      </c>
-      <c r="H56" s="10"/>
-      <c r="I56" s="7"/>
-      <c r="J56" s="7"/>
-      <c r="K56" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="L56" s="12"/>
-      <c r="M56" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="N56" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O56" s="3" t="s">
-        <v>364</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="O56" s="3"/>
       <c r="P56" s="5"/>
       <c r="Q56" s="5"/>
       <c r="R56" s="5"/>
@@ -51552,42 +51561,44 @@
       <c r="AA56" s="5"/>
       <c r="AB56" s="5"/>
     </row>
-    <row r="57" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A57" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B57" t="s">
-        <v>367</v>
+        <v>311</v>
       </c>
       <c r="C57" t="s">
-        <v>368</v>
-      </c>
-      <c r="D57" t="s">
-        <v>372</v>
-      </c>
-      <c r="E57" t="s">
-        <v>371</v>
-      </c>
-      <c r="F57" t="s">
-        <v>370</v>
-      </c>
-      <c r="G57" s="10" t="s">
-        <v>369</v>
-      </c>
-      <c r="H57" s="10"/>
+        <v>679</v>
+      </c>
+      <c r="D57" s="30" t="s">
+        <v>336</v>
+      </c>
+      <c r="E57" s="30" t="s">
+        <v>337</v>
+      </c>
+      <c r="F57" s="30" t="s">
+        <v>338</v>
+      </c>
+      <c r="G57" s="30" t="s">
+        <v>339</v>
+      </c>
+      <c r="H57" s="7"/>
       <c r="I57" s="7"/>
-      <c r="J57" s="7"/>
-      <c r="K57" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="L57" s="12" t="s">
-        <v>374</v>
+      <c r="J57" s="38" t="s">
+        <v>633</v>
+      </c>
+      <c r="K57" s="8" t="s">
+        <v>647</v>
+      </c>
+      <c r="L57" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>4</v>
+        <v>604</v>
       </c>
       <c r="N57" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="O57" s="3"/>
       <c r="P57" s="5"/>
@@ -51609,30 +51620,30 @@
         <v>310</v>
       </c>
       <c r="B58" t="s">
-        <v>375</v>
+        <v>358</v>
       </c>
       <c r="C58" t="s">
-        <v>376</v>
-      </c>
-      <c r="D58" t="s">
-        <v>381</v>
-      </c>
-      <c r="E58" t="s">
-        <v>380</v>
-      </c>
-      <c r="F58" s="7" t="s">
-        <v>379</v>
-      </c>
-      <c r="G58" t="s">
-        <v>378</v>
-      </c>
-      <c r="H58" s="7"/>
+        <v>371</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>413</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>592</v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>593</v>
+      </c>
+      <c r="G58" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H58" s="10"/>
       <c r="I58" s="7"/>
       <c r="J58" s="7"/>
-      <c r="K58" s="8" t="s">
-        <v>377</v>
-      </c>
-      <c r="L58" s="4"/>
+      <c r="K58" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="L58" s="12"/>
       <c r="M58" s="4" t="s">
         <v>16</v>
       </c>
@@ -51640,7 +51651,7 @@
         <v>13</v>
       </c>
       <c r="O58" s="3" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="P58" s="5"/>
       <c r="Q58" s="5"/>
@@ -51661,37 +51672,37 @@
         <v>310</v>
       </c>
       <c r="B59" t="s">
-        <v>382</v>
-      </c>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10" t="s">
-        <v>664</v>
-      </c>
-      <c r="E59" s="10" t="s">
-        <v>385</v>
-      </c>
-      <c r="F59" s="10" t="s">
-        <v>384</v>
+        <v>362</v>
+      </c>
+      <c r="C59" t="s">
+        <v>363</v>
+      </c>
+      <c r="D59" t="s">
+        <v>367</v>
+      </c>
+      <c r="E59" t="s">
+        <v>366</v>
+      </c>
+      <c r="F59" t="s">
+        <v>365</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>383</v>
-      </c>
-      <c r="H59" s="10" t="s">
-        <v>188</v>
-      </c>
+        <v>364</v>
+      </c>
+      <c r="H59" s="10"/>
       <c r="I59" s="7"/>
       <c r="J59" s="7"/>
-      <c r="K59" s="8" t="s">
-        <v>386</v>
-      </c>
-      <c r="L59" s="11" t="s">
-        <v>11</v>
+      <c r="K59" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="L59" s="12" t="s">
+        <v>369</v>
       </c>
       <c r="M59" s="4" t="s">
         <v>4</v>
       </c>
       <c r="N59" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="O59" s="3"/>
       <c r="P59" s="5"/>
@@ -51713,28 +51724,28 @@
         <v>310</v>
       </c>
       <c r="B60" t="s">
-        <v>387</v>
+        <v>370</v>
       </c>
       <c r="C60" t="s">
+        <v>371</v>
+      </c>
+      <c r="D60" t="s">
         <v>376</v>
       </c>
-      <c r="D60" t="s">
-        <v>388</v>
-      </c>
       <c r="E60" t="s">
-        <v>389</v>
+        <v>375</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>390</v>
+        <v>374</v>
       </c>
       <c r="G60" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="H60" s="7"/>
       <c r="I60" s="7"/>
       <c r="J60" s="7"/>
       <c r="K60" s="8" t="s">
-        <v>391</v>
+        <v>372</v>
       </c>
       <c r="L60" s="4"/>
       <c r="M60" s="4" t="s">
@@ -51744,7 +51755,7 @@
         <v>13</v>
       </c>
       <c r="O60" s="3" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="P60" s="5"/>
       <c r="Q60" s="5"/>
@@ -51760,41 +51771,39 @@
       <c r="AA60" s="5"/>
       <c r="AB60" s="5"/>
     </row>
-    <row r="61" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A61" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B61" t="s">
-        <v>392</v>
-      </c>
-      <c r="C61" t="s">
-        <v>351</v>
-      </c>
+        <v>377</v>
+      </c>
+      <c r="C61" s="10"/>
       <c r="D61" s="10" t="s">
-        <v>394</v>
+        <v>650</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>393</v>
+        <v>379</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>396</v>
-      </c>
-      <c r="H61" s="10"/>
+        <v>378</v>
+      </c>
+      <c r="H61" s="10" t="s">
+        <v>188</v>
+      </c>
       <c r="I61" s="7"/>
-      <c r="J61" s="38" t="s">
-        <v>638</v>
-      </c>
+      <c r="J61" s="7"/>
       <c r="K61" s="8" t="s">
-        <v>662</v>
+        <v>381</v>
       </c>
       <c r="L61" s="11" t="s">
         <v>11</v>
       </c>
       <c r="M61" s="4" t="s">
-        <v>617</v>
+        <v>4</v>
       </c>
       <c r="N61" s="4" t="s">
         <v>8</v>
@@ -51814,46 +51823,44 @@
       <c r="AA61" s="5"/>
       <c r="AB61" s="5"/>
     </row>
-    <row r="62" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A62" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B62" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="C62" t="s">
-        <v>397</v>
-      </c>
-      <c r="D62" s="10" t="s">
-        <v>401</v>
-      </c>
-      <c r="E62" s="10" t="s">
-        <v>400</v>
-      </c>
-      <c r="F62" s="10" t="s">
-        <v>399</v>
-      </c>
-      <c r="G62" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="H62" s="10"/>
+        <v>371</v>
+      </c>
+      <c r="D62" t="s">
+        <v>383</v>
+      </c>
+      <c r="E62" t="s">
+        <v>384</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="G62" t="s">
+        <v>373</v>
+      </c>
+      <c r="H62" s="7"/>
       <c r="I62" s="7"/>
-      <c r="J62" s="38" t="s">
-        <v>647</v>
-      </c>
+      <c r="J62" s="7"/>
       <c r="K62" s="8" t="s">
-        <v>663</v>
-      </c>
-      <c r="L62" s="11" t="s">
-        <v>11</v>
-      </c>
+        <v>386</v>
+      </c>
+      <c r="L62" s="4"/>
       <c r="M62" s="4" t="s">
-        <v>617</v>
+        <v>16</v>
       </c>
       <c r="N62" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="O62" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="O62" s="3" t="s">
+        <v>359</v>
+      </c>
       <c r="P62" s="5"/>
       <c r="Q62" s="5"/>
       <c r="R62" s="5"/>
@@ -51868,14 +51875,45 @@
       <c r="AA62" s="5"/>
       <c r="AB62" s="5"/>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="K63" s="5"/>
-      <c r="L63" s="13"/>
-      <c r="M63" s="4"/>
-      <c r="N63" s="4"/>
+    <row r="63" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+      <c r="A63" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B63" t="s">
+        <v>387</v>
+      </c>
+      <c r="C63" t="s">
+        <v>347</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>389</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="G63" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="H63" s="10"/>
+      <c r="I63" s="7"/>
+      <c r="J63" s="38" t="s">
+        <v>624</v>
+      </c>
+      <c r="K63" s="8" t="s">
+        <v>648</v>
+      </c>
+      <c r="L63" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M63" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="N63" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="O63" s="3"/>
       <c r="P63" s="5"/>
       <c r="Q63" s="5"/>
@@ -51891,14 +51929,45 @@
       <c r="AA63" s="5"/>
       <c r="AB63" s="5"/>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A64" s="5"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="K64" s="5"/>
-      <c r="L64" s="13"/>
-      <c r="M64" s="4"/>
-      <c r="N64" s="4"/>
+    <row r="64" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+      <c r="A64" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B64" t="s">
+        <v>387</v>
+      </c>
+      <c r="C64" t="s">
+        <v>683</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="F64" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="G64" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="H64" s="10"/>
+      <c r="I64" s="7"/>
+      <c r="J64" s="38" t="s">
+        <v>633</v>
+      </c>
+      <c r="K64" s="8" t="s">
+        <v>649</v>
+      </c>
+      <c r="L64" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M64" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="N64" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="O64" s="3"/>
       <c r="P64" s="5"/>
       <c r="Q64" s="5"/>
@@ -73350,6 +73419,52 @@
       <c r="AA996" s="5"/>
       <c r="AB996" s="5"/>
     </row>
+    <row r="997" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A997" s="5"/>
+      <c r="B997" s="5"/>
+      <c r="C997" s="5"/>
+      <c r="K997" s="5"/>
+      <c r="L997" s="13"/>
+      <c r="M997" s="4"/>
+      <c r="N997" s="4"/>
+      <c r="O997" s="3"/>
+      <c r="P997" s="5"/>
+      <c r="Q997" s="5"/>
+      <c r="R997" s="5"/>
+      <c r="S997" s="5"/>
+      <c r="T997" s="5"/>
+      <c r="U997" s="5"/>
+      <c r="V997" s="5"/>
+      <c r="W997" s="5"/>
+      <c r="X997" s="5"/>
+      <c r="Y997" s="5"/>
+      <c r="Z997" s="5"/>
+      <c r="AA997" s="5"/>
+      <c r="AB997" s="5"/>
+    </row>
+    <row r="998" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A998" s="5"/>
+      <c r="B998" s="5"/>
+      <c r="C998" s="5"/>
+      <c r="K998" s="5"/>
+      <c r="L998" s="13"/>
+      <c r="M998" s="4"/>
+      <c r="N998" s="4"/>
+      <c r="O998" s="3"/>
+      <c r="P998" s="5"/>
+      <c r="Q998" s="5"/>
+      <c r="R998" s="5"/>
+      <c r="S998" s="5"/>
+      <c r="T998" s="5"/>
+      <c r="U998" s="5"/>
+      <c r="V998" s="5"/>
+      <c r="W998" s="5"/>
+      <c r="X998" s="5"/>
+      <c r="Y998" s="5"/>
+      <c r="Z998" s="5"/>
+      <c r="AA998" s="5"/>
+      <c r="AB998" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
1859 use signif function in metadata
</commit_message>
<xml_diff>
--- a/inst/adlb_grading/adlb_grading_spec.xlsx
+++ b/inst/adlb_grading/adlb_grading_spec.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1640" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1640" uniqueCount="685">
   <si>
     <t>Anemia</t>
   </si>
@@ -1517,21 +1517,6 @@
     <t>&lt; 50 mg/dL, &lt; 0.50 g/L OR &lt; 0.25 x LLN OR Associated with gross bleeding</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &lt;  0.5 ~ "4",
-is.na(ANRLO) ~ NA_character_,
-AVAL &lt;  0.25*ANRLO ~ "4",
-AVAL &lt; 0.75 ~ "3",
-AVAL &lt;  0.5*ANRLO ~ "3",
-AVAL &lt;  1 ~ "2",
-AVAL &lt;  0.75*ANRLO ~ "2",
-AVAL &lt;  2 ~ "1",
-AVAL &lt;  ANRLO ~ "1",
-AVAL &gt;= ANRLO ~ "0"
-)</t>
-  </si>
-  <si>
     <t>Absolute Neutrophil Count (ANC), Low</t>
   </si>
   <si>
@@ -1577,16 +1562,6 @@
     <t>&gt;=3.0 x ULN</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
-AVAL &gt;=  3*ANRHI ~ "4",
-AVAL &gt;=  2*ANRHI ~ "3",
-AVAL &gt;= 1.5*ANRHI ~ "2",
-AVAL &gt;= 1.1*ANRHI ~ "1",
-AVAL &lt; 1.1*ANRHI ~ "0"
-)</t>
-  </si>
-  <si>
     <t>Methemoglobin</t>
   </si>
   <si>
@@ -1605,16 +1580,6 @@
     <t>5.0 to &lt; 10.0%</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &gt;=  20 ~ "4",
-AVAL &gt;=  15 ~ "3",
-AVAL &gt;= 10 ~ "2",
-AVAL &gt;= 5 ~ "1",
-AVAL &lt; 5 ~ "0"
-)</t>
-  </si>
-  <si>
     <t>%</t>
   </si>
   <si>
@@ -1622,16 +1587,6 @@
   </si>
   <si>
     <t>not on anticoagulation therapy</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
-AVAL &gt;=  3*ANRHI ~ "4",
-AVAL &gt;=  2.33*ANRHI ~ "3",
-AVAL &gt;= 1.66*ANRHI ~ "2",
-AVAL &gt;= 1.1*ANRHI ~ "1",
-AVAL &lt; 1.1*ANRHI ~ "0"
-)</t>
   </si>
   <si>
     <t>&gt;=3.00 x ULN</t>
@@ -1658,16 +1613,6 @@
     <t>50,000 to &lt;100,000 - /mm3; 50.0 to &lt;100.000 - x 10e9 /L</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &lt; 25 ~ "4",
-AVAL &lt; 50 ~ "3",
-AVAL &lt; 100 ~ "2",
-AVAL &lt; 125 ~ "1",
-AVAL &gt;= 125 ~ "0"
-)</t>
-  </si>
-  <si>
     <t>PT, High</t>
   </si>
   <si>
@@ -1678,16 +1623,6 @@
   </si>
   <si>
     <t xml:space="preserve">1.50 to &lt; 3.00 x ULN </t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
-AVAL &gt;=  3*ANRHI ~ "4",
-AVAL &gt;=  1.5*ANRHI ~ "3",
-AVAL &gt;= 1.25*ANRHI ~ "2",
-AVAL &gt;= 1.1*ANRHI ~ "1",
-AVAL &lt; 1.1*ANRHI ~ "0"
-)</t>
   </si>
   <si>
     <t>WBC, Decreased</t>
@@ -1735,16 +1670,6 @@
     <t>1.25 to &lt;2.5 x ULN</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
-AVAL &gt;=  10*ANRHI ~ "4",
-AVAL &gt;=  5*ANRHI ~ "3",
-AVAL &gt;= 2.5*ANRHI ~ "2",
-AVAL &gt;= 1.25*ANRHI ~ "1",
-AVAL &lt; 1.25*ANRHI ~ "0"
-)</t>
-  </si>
-  <si>
     <t>Albumin, Low</t>
   </si>
   <si>
@@ -1755,26 +1680,6 @@
   </si>
   <si>
     <t>3.0 g/dL to &lt; LLN 30 g/L to &lt; LLN</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &lt;  20 ~ "3",
-AVAL &lt; 30 ~ "2",
-is.na(ANRLO) ~ NA_character_,
-AVAL &lt; ANRLO ~ "1",
-AVAL &gt;= ANRLO ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
-AVAL &gt;= 10*ANRHI ~ "4",
-AVAL &gt;= 5*ANRHI ~ "3",
-AVAL &gt;= 2.5*ANRHI ~ "2",
-AVAL &gt;= 1.25*ANRHI ~ "1",
-AVAL &lt; 1.25*ANRHI ~ "0"
-)</t>
   </si>
   <si>
     <t>Amylase, High</t>
@@ -1790,16 +1695,6 @@
   </si>
   <si>
     <t>1.1 - &lt;1.5 x ULN</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
-AVAL &gt;=  5*ANRHI ~ "4",
-AVAL &gt;=  3*ANRHI ~ "3",
-AVAL &gt;= 1.5*ANRHI ~ "2",
-AVAL &gt;= 1.1*ANRHI ~ "1",
-AVAL &lt; 1.1*ANRHI ~ "0"
-)</t>
   </si>
   <si>
     <t>Bicarbonate, Low</t>
@@ -1952,16 +1847,6 @@
     <t>3 to &lt;6 x ULN</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
-AVAL &gt;=  20*ANRHI ~ "4",
-AVAL &gt;=  10*ANRHI ~ "3",
-AVAL &gt;= 6*ANRHI ~ "2",
-AVAL &gt;= 3*ANRHI ~ "1",
-AVAL &lt; 3*ANRHI ~ "0"
-)</t>
-  </si>
-  <si>
     <t>Creatinine, High</t>
   </si>
   <si>
@@ -1986,16 +1871,6 @@
     <t>&gt; 250 to 500 mg/dL; 13.89 to &lt; 27.75 mmol/L</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &gt;= 27.75 ~ "4",
-AVAL &gt;= 13.89 ~ "3",
-AVAL &gt;= 6.95 ~ "2",
-AVAL &gt;= 6.11 ~ "1",
-AVAL &lt; 6.11 ~ "0"
-)</t>
-  </si>
-  <si>
     <t>Glucose Nonfasting, High</t>
   </si>
   <si>
@@ -2003,16 +1878,6 @@
   </si>
   <si>
     <t>116 to 160 mg/dL; 6.44 to &lt; 8.89 mmol/L</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &gt;= 27.75 ~ "4",
-AVAL &gt;= 13.89 ~ "3",
-AVAL &gt;= 8.89 ~ "2",
-AVAL &gt;= 6.44 ~ "1",
-AVAL &lt; 6.44 ~ "0"
-)</t>
   </si>
   <si>
     <t>Glucose, Low</t>
@@ -2057,14 +1922,6 @@
   </si>
   <si>
     <t>Increased lactate with pH &lt; 7.3 with lifethreatening consequences</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
-AVAL &gt;= 2*ANRHI ~ "2",
-AVAL &gt;= ANRHI ~ "1",
-AVAL &lt; ANRHI ~ "0"
-)</t>
   </si>
   <si>
     <t>Assume "without acidosis" (only grade 1 and 2)</t>
@@ -2157,16 +2014,6 @@
     <t>&lt; 0.6 mEq/L; &lt; 0.30 mmol/L</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &lt; 0.3 ~ "4",
-AVAL &lt; 0.45 ~ "3",
-AVAL &lt; 0.6 ~ "2",
-AVAL &lt; 0.7 ~ "1",
-AVAL &gt;= 0.7 ~ "0"
-)</t>
-  </si>
-  <si>
     <t>Phosphate, Low</t>
   </si>
   <si>
@@ -2224,16 +2071,6 @@
     <t>2.5 to &lt; 3.0 mmol/L</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &lt; 2 ~ "4",
-AVAL &lt; 2.5 ~ "3",
-AVAL &lt; 3 ~ "2",
-AVAL &lt; 3.4 ~ "1",
-AVAL &gt;= 3.4 ~ "0"
-)</t>
-  </si>
-  <si>
     <t>Potassium, High</t>
   </si>
   <si>
@@ -2247,16 +2084,6 @@
   </si>
   <si>
     <t>5.6 to &lt; 6.0 mmol/L</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &gt;= 7 ~ "4",
-AVAL &gt;= 6.5 ~ "3",
-AVAL &gt;= 6 ~ "2",
-AVAL &gt;= 5.6 ~ "1",
-AVAL &lt; 5.6 ~ "0"
-)</t>
   </si>
   <si>
     <t>Sodium, Low</t>
@@ -2274,16 +2101,6 @@
     <t>130 to &lt; 135 mmol/L</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &lt;= 120 ~ "4",
-AVAL &lt; 125 ~ "3",
-AVAL &lt; 130 ~ "2",
-AVAL &lt; 135 ~ "1",
-AVAL &gt;= 135 ~ "0"
-)</t>
-  </si>
-  <si>
     <t>Sodium, High</t>
   </si>
   <si>
@@ -2297,16 +2114,6 @@
   </si>
   <si>
     <t>146 to &lt; 150 mmol/L</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &gt;= 160 ~ "4",
-AVAL &gt;= 154 ~ "3",
-AVAL &gt;= 150 ~ "2",
-AVAL &gt;= 146 ~ "1",
-AVAL &lt; 146 ~ "0"
-)</t>
   </si>
   <si>
     <t>Uric Acid, High</t>
@@ -2327,31 +2134,10 @@
     <t>To convert "mmol/L" to "umol/L" multiply by 1000</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &gt;= 890 ~ "4",
-AVAL &gt;= 710 ~ "3",
-AVAL &gt;= 590 ~ "2",
-AVAL &gt;= 450 ~ "1",
-AVAL &lt; 450 ~ "0"
-)</t>
-  </si>
-  <si>
     <t>SUBGROUP</t>
   </si>
   <si>
     <t>umol/L</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &gt;= 1.8 ~ "4",
-AVAL &gt;= 1.6 ~ "3",
-AVAL &gt;= 1.5 ~ "2",
-is.na(ANRHI) ~ NA_character_,
-AVAL &gt; ANRHI ~ "1",
-AVAL &lt;= ANRHI ~ "0"
-)</t>
   </si>
   <si>
     <t>12.4 - &lt;12.9 mg/dL; 3.10 - &lt;3.23 mmol/L</t>
@@ -2420,13 +2206,6 @@
     <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &gt; 28 | is.na(BRTHDT) | is.na(LBDT)</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) | is.na(ANRHI) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &gt;  ANRHI ~ "4",
-AVAL &lt;= ANRHI ~ "0"
-)</t>
-  </si>
-  <si>
     <t>AVAL, ANRHI, LBDT, BRTHDT</t>
   </si>
   <si>
@@ -2439,165 +2218,10 @@
     <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &lt; 7 | is.na(BRTHDT) | is.na(LBDT)</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) | is.na(ANRHI) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &gt;=  5*ANRHI ~ "4",
-AVAL &gt;=  2.6*ANRHI ~ "3",
-AVAL &gt;= 1.6*ANRHI ~ "2",
-AVAL &gt;= 1.1*ANRHI ~ "1",
-AVAL &lt; 1.1*ANRHI ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &gt;= 3.38 ~ "4",
-AVAL &gt;= 3.13 ~ "3",
-AVAL &gt;= 2.88 ~ "2",
-AVAL &gt;= 2.65 ~ "1",
-AVAL &lt; 2.65 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &gt;= 3.38 ~ "4",
-AVAL &gt;= 3.23 ~ "3",
-AVAL &gt;= 3.1 ~ "2",
-AVAL &gt;= 2.88 ~ "1",
-AVAL &lt; 2.88 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &lt; 1.53 ~ "4",
-AVAL &lt; 1.75 ~ "3",
-AVAL &lt; 1.95 ~ "2",
-AVAL &lt; 2.1 ~ "1",
-AVAL &gt;= 2.1 ~ "0"
-)</t>
-  </si>
-  <si>
     <t>AVAL, LBDT, BRTHDT</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &lt; 1.38 ~ "4",
-AVAL &lt; 1.5 ~ "3",
-AVAL &lt; 1.63 ~ "2",
-AVAL &lt; 1.88 ~ "1",
-AVAL &gt;= 1.88 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &lt; 1.67 ~ "4",
-AVAL &lt; 2.22 ~ "3",
-AVAL &lt; 3.05 ~ "2",
-AVAL &lt; 3.55 ~ "1",
-AVAL &gt;= 3.55 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &lt; 1.67 ~ "4",
-AVAL &lt; 2.22 ~ "3",
-AVAL &lt; 2.78 ~ "2",
-AVAL &lt; 3 ~ "1",
-AVAL &gt;= 3 ~ "0"
-)</t>
-  </si>
-  <si>
     <t>AVAL, BRTHDT, LBDT</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &gt;= 7.77 ~ "3",
-AVAL &gt;= 6.19 ~ "2",
-AVAL &gt;= 5.18 ~ "1",
-AVAL &lt; 5.18 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &gt;= 4.9 ~ "3",
-AVAL &gt;= 4.12 ~ "2",
-AVAL &gt;= 3.37 ~ "1",
-AVAL &lt; 3.37 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &gt;= 4.9 ~ "3",
-AVAL &gt;= 3.34 ~ "2",
-AVAL &gt;= 2.85 ~ "1",
-AVAL &lt; 2.85 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &lt; 0.32 ~ "4",
-AVAL &lt; 0.45 ~ "3",
-AVAL &lt; 0.65 ~ "2",
-is.na(ANRLO) ~ NA_character_,
-AVAL &lt; ANRLO ~ "1",
-AVAL &gt;= ANRLO ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &lt; 0.48 ~ "4",
-AVAL &lt; 0.81 ~ "3",
-AVAL &lt; 0.97 ~ "2",
-AVAL &lt; 1.13 ~ "1",
-AVAL &gt;= 1.13 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &lt; 0.48 ~ "4",
-AVAL &lt; 0.81 ~ "3",
-AVAL &lt; 1.13 ~ "2",
-AVAL &lt; 1.45 ~ "1",
-AVAL &gt;= 1.45 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "months", add_one = FALSE) &gt;= 1 | is.na(BRTHDT) | is.na(LBDT)</t>
-  </si>
-  <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "months", add_one = FALSE) &lt; 1 | is.na(BRTHDT) | is.na(LBDT)</t>
-  </si>
-  <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &gt;= 18 | is.na(BRTHDT) | is.na(LBDT)</t>
-  </si>
-  <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &lt; 18 | is.na(BRTHDT) | is.na(LBDT)</t>
-  </si>
-  <si>
-    <t>(compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &gt; 2 &amp; compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &lt; 18)  | is.na(BRTHDT) | is.na(LBDT)</t>
-  </si>
-  <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &gt; 14 | is.na(BRTHDT) | is.na(LBDT)</t>
-  </si>
-  <si>
-    <t>(compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &gt;= 1 &amp; compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &lt; 14) | is.na(BRTHDT) | is.na(LBDT)</t>
-  </si>
-  <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &lt; 1 | is.na(BRTHDT) | is.na(LBDT)</t>
-  </si>
-  <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &gt; 5 | is.na(BRTHDT) | is.na(LBDT)</t>
   </si>
   <si>
     <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &gt; 7 | is.na(BRTHDT) | is.na(LBDT)</t>
@@ -2607,15 +2231,6 @@
   </si>
   <si>
     <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &lt;= 1 | is.na(BRTHDT) | is.na(LBDT)</t>
-  </si>
-  <si>
-    <t>(SEX == "M" | is.na(SEX)) &amp; (compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &gt;= 13 | is.na(BRTHDT) | is.na(LBDT))</t>
-  </si>
-  <si>
-    <t>(SEX == "F" | is.na(SEX)) &amp; (compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &gt;= 13 | is.na(BRTHDT) | is.na(LBDT))</t>
-  </si>
-  <si>
-    <t>(compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &lt; 13 &amp; compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &gt;= 57) | is.na(BRTHDT) | is.na(LBDT)</t>
   </si>
   <si>
     <t>(compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &lt;= 56 &amp; compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &gt;= 36) | is.na(BRTHDT) | is.na(LBDT)</t>
@@ -2634,146 +2249,6 @@
   </si>
   <si>
     <t>AVAL, SEX, LBDT, BRTHDT</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &lt; 0.1 ~ "4",
-AVAL &lt; 0.2 ~ "3",
-AVAL &lt; 0.3 ~ "2",
-AVAL &lt; 0.4 ~ "1",
-AVAL &gt;= 0.4 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &lt; 0.35 ~ "4",
-AVAL &lt; 0.5 ~ "3",
-AVAL &lt; 0.6 ~ "2",
-AVAL &lt; 0.65 ~ "1",
-AVAL &gt;= 0.65 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &lt; 0.4 ~ "4",
-AVAL &lt; 0.6 ~ "3",
-AVAL &lt; 0.8 ~ "2",
-AVAL &lt;= 1 ~ "1",
-AVAL &gt; 1 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &lt; 0.75 ~ "4",
-AVAL &lt; 1 ~ "3",
-AVAL &lt; 1.25 ~ "2",
-AVAL &lt;= 1.5 ~ "1",
-AVAL &gt; 1.5 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &lt; 1.5 ~ "4",
-AVAL &lt; 3 ~ "3",
-AVAL &lt; 4 ~ "2",
-AVAL &lt;= 5 ~ "1",
-AVAL &gt; 5 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(SEX) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &lt; 70 ~ "4",
-AVAL &lt; 90 ~ "3",
-AVAL &lt; 100 ~ "2",
-AVAL &lt;= 109 ~ "1",
-AVAL &gt; 109 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(SEX)  | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &lt; 65 ~ "4",
-AVAL &lt; 85 ~ "3",
-AVAL &lt; 95 ~ "2",
-AVAL &lt;= 104 ~ "1",
-AVAL &gt; 104 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &lt; 65 ~ "4",
-AVAL &lt; 85 ~ "3",
-AVAL &lt; 95 ~ "2",
-AVAL &lt;= 104 ~ "1",
-AVAL &gt; 104 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &lt; 60 ~ "4",
-AVAL &lt; 70 ~ "3",
-AVAL &lt; 85 ~ "2",
-AVAL &lt;= 96 ~ "1",
-AVAL &gt; 96 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &lt; 67 ~ "4",
-AVAL &lt; 80 ~ "3",
-AVAL &lt; 95 ~ "2",
-AVAL &lt;= 110 ~ "1",
-AVAL &gt; 110 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &lt; 80 ~ "4",
-AVAL &lt; 90 ~ "3",
-AVAL &lt; 110 ~ "2",
-AVAL &lt;= 130 ~ "1",
-AVAL &gt; 130 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &lt; 90 ~ "4",
-AVAL &lt; 100 ~ "3",
-AVAL &lt; 130 ~ "2",
-AVAL &lt;= 140 ~ "1",
-AVAL &gt; 140 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &lt; 1 ~ "4",
-AVAL &lt; 1.5 ~ "3",
-AVAL &lt; 2 ~ "2",
-AVAL &lt; 2.5 ~ "1",
-AVAL &gt;= 2.5 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &lt; 2.5 ~ "4",
-AVAL &lt; 4 ~ "3",
-AVAL &lt; 5.5 ~ "2",
-AVAL &lt; 7 ~ "1",
-AVAL &gt;= 7 ~ "0"
-)</t>
   </si>
   <si>
     <t>100,000 to &lt;125,000/mm3; 100.00 - &lt;125.000 x 10e9 /L</t>
@@ -2809,31 +2284,10 @@
     <t>&lt;= 5 years of age</t>
   </si>
   <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &lt;= 5 | is.na(BRTHDT) | is.na(LBDT)</t>
-  </si>
-  <si>
     <t>No criteria given for this age range</t>
   </si>
   <si>
     <t>NA_character_</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &lt; 7.3  ~ "4",
-is.na(ANRLO) ~ NA_character_,
-AVAL &lt; ANRLO ~ "2",
-AVAL &gt;= ANRLO ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &gt; 7.5 ~ "4",
-is.na(ANRHI) ~ NA_character_,
-AVAL &gt; ANRHI ~ "2",
-AVAL &lt;= ANRHI ~ "0"
-)</t>
   </si>
   <si>
     <t>ALT, High</t>
@@ -2842,71 +2296,13 @@
     <t>AST, High</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &lt; 8 ~ "4",
-AVAL &lt; 11 ~ "3",
-AVAL &lt; 16 ~ "2",
-is.na(ANRLO) ~ NA_character_,
-AVAL &lt; ANRLO ~ "1",
-AVAL &gt;= ANRLO ~ "0"
-)</t>
-  </si>
-  <si>
     <t>17.1 used as conversion from "mg/dL" to "umol/L"</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &gt;  2*17.1 ~ "4",
-AVAL &gt;  1.5*17.1 ~ "3",
-AVAL &gt;  17.1 ~ "2",
-is.na(ANRHI) ~ NA_character_,
-AVAL &gt;= ANRHI ~ "1",
-AVAL &lt; ANRHI ~ "0"
-)</t>
   </si>
   <si>
     <t>Did not grade</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-!is.na(ANRHI) &amp; AVAL &gt;=  3.5*ANRHI ~ "4",
-!is.na(BASE) &amp; AVAL &gt;=  2*BASE ~ "4",
-!is.na(ANRHI) &amp; AVAL &gt;  1.8*ANRHI ~ "3",
-!is.na(BASE) &amp; AVAL &gt;= 1.5*BASE ~ "3",
-!is.na(ANRHI) &amp; AVAL &gt; 1.3*ANRHI~ "2",
-!is.na(BASE) &amp; AVAL &gt;= 1.3*BASE ~ "2",
-is.na(ANRHI) ~ NA_character_,
-AVAL &gt;= 1.1*ANRHI ~ "1",
-AVAL &lt; 1.1*ANRHI ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-AVAL &gt;= 7.77 ~ "3",
-AVAL &gt;= 5.15 ~ "2",
-AVAL &gt;= 4.4 ~ "1",
-AVAL &lt; 4.4 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) ~ NA_character_,
-AVAL &gt; 11.4 ~ "4",
-AVAL &gt; 5.7 ~ "3",
-AVAL &gt; 3.42 ~ "2",
-AVAL &gt;= 1.71 ~ "1",
-AVAL &lt; 1.71 ~ "0"
-)</t>
-  </si>
-  <si>
     <t>&lt;= 2 years of age</t>
-  </si>
-  <si>
-    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE) &lt;= 2  | is.na(BRTHDT) | is.na(LBDT)</t>
   </si>
   <si>
     <t>&gt;= 7 days of age</t>
@@ -2928,6 +2324,621 @@
   </si>
   <si>
     <t>&lt;= 7 days of age</t>
+  </si>
+  <si>
+    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "months", add_one = FALSE, type = "interval") &gt;= 1 | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "months", add_one = FALSE, type = "interval") &lt; 1 | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE, type = "interval") &gt;= 18 | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE, type = "interval") &lt; 18 | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE, type = "interval") &lt;= 2  | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE, type = "interval") &gt; 14 | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>(compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE, type = "interval") &gt;= 1 &amp; compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE, type = "interval") &lt; 14) | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE, type = "interval") &lt; 1 | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE, type = "interval") &gt; 5 | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE, type = "interval") &lt;= 5 | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>(SEX == "M" | is.na(SEX)) &amp; (compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE, type = "interval") &gt;= 13 | is.na(BRTHDT) | is.na(LBDT))</t>
+  </si>
+  <si>
+    <t>(SEX == "F" | is.na(SEX)) &amp; (compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE, type = "interval") &gt;= 13 | is.na(BRTHDT) | is.na(LBDT))</t>
+  </si>
+  <si>
+    <t>(compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE, type = "interval") &lt; 13 &amp; compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "days", add_one = FALSE) &gt;= 57) | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
+signif(AVAL, signif_dig) &gt;=  signif(3*ANRHI, signif_dig) ~ "4",
+signif(AVAL, signif_dig) &gt;=  signif(2.33*ANRHI, signif_dig) ~ "3",
+signif(AVAL, signif_dig) &gt;= signif(1.66*ANRHI, signif_dig) ~ "2",
+signif(AVAL, signif_dig) &gt;= signif(1.1*ANRHI, signif_dig) ~ "1",
+signif(AVAL, signif_dig) &lt; signif(1.1*ANRHI, signif_dig) ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>(compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE, type = "interval") &gt; 2 &amp; compute_duration(start_date = BRTHDT, end_date = LBDT, trunc_out = TRUE, out_unit = "years", add_one = FALSE, type = "interval") &lt; 18)  | is.na(BRTHDT) | is.na(LBDT)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
+signif(AVAL, signif_dig) &gt;=  signif(3*ANRHI, signif_dig) ~ "4",
+signif(AVAL, signif_dig) &gt;=  signif(1.5*ANRHI, signif_dig) ~ "3",
+signif(AVAL, signif_dig) &gt;= signif(1.25*ANRHI, signif_dig) ~ "2",
+signif(AVAL, signif_dig) &gt;= signif(1.1*ANRHI, signif_dig) ~ "1",
+signif(AVAL, signif_dig) &lt; signif(1.1*ANRHI, signif_dig) ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
+signif(AVAL, signif_dig) &gt;=  signif(5*ANRHI, signif_dig) ~ "4",
+signif(AVAL, signif_dig) &gt;=  signif(3*ANRHI, signif_dig) ~ "3",
+signif(AVAL, signif_dig) &gt;= signif(1.5*ANRHI, signif_dig) ~ "2",
+signif(AVAL, signif_dig) &gt;= signif(1.1*ANRHI, signif_dig) ~ "1",
+signif(AVAL, signif_dig) &lt; signif(1.1*ANRHI, signif_dig) ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
+signif(AVAL, signif_dig) &gt;= signif(2*ANRHI, signif_dig) ~ "2",
+signif(AVAL, signif_dig) &gt;= signif(ANRHI, signif_dig) ~ "1",
+signif(AVAL, signif_dig) &lt; signif(ANRHI, signif_dig) ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 1.67 ~ "4",
+signif(AVAL, signif_dig) &lt; 2.22 ~ "3",
+signif(AVAL, signif_dig) &lt; 2.78 ~ "2",
+signif(AVAL, signif_dig) &lt; 3 ~ "1",
+signif(AVAL, signif_dig) &gt;= 3 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 1.67 ~ "4",
+signif(AVAL, signif_dig) &lt; 2.22 ~ "3",
+signif(AVAL, signif_dig) &lt; 3.05 ~ "2",
+signif(AVAL, signif_dig) &lt; 3.55 ~ "1",
+signif(AVAL, signif_dig) &gt;= 3.55 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+signif(AVAL, signif_dig) &gt;= 27.75 ~ "4",
+signif(AVAL, signif_dig) &gt;= 13.89 ~ "3",
+signif(AVAL, signif_dig) &gt;= 8.89 ~ "2",
+signif(AVAL, signif_dig) &gt;= 6.44 ~ "1",
+signif(AVAL, signif_dig) &lt; 6.44 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+signif(AVAL, signif_dig) &gt;= 27.75 ~ "4",
+signif(AVAL, signif_dig) &gt;= 13.89 ~ "3",
+signif(AVAL, signif_dig) &gt;= 6.95 ~ "2",
+signif(AVAL, signif_dig) &gt;= 6.11 ~ "1",
+signif(AVAL, signif_dig) &lt; 6.11 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+!is.na(ANRHI) &amp; signif(AVAL, signif_dig) &gt;=  signif(3.5*ANRHI, signif_dig) ~ "4",
+!is.na(BASE) &amp; signif(AVAL, signif_dig) &gt;=  signif(2*BASE, signif_dig) ~ "4",
+!is.na(ANRHI) &amp; signif(AVAL, signif_dig) &gt;  signif(1.8*ANRHI, signif_dig) ~ "3",
+!is.na(BASE) &amp; signif(AVAL, signif_dig) &gt;= signif(1.5*BASE, signif_dig) ~ "3",
+!is.na(ANRHI) &amp; signif(AVAL, signif_dig) &gt; signif(1.3*ANRHI, signif_dig) ~ "2",
+!is.na(BASE) &amp; signif(AVAL, signif_dig) &gt;= signif(1.3*BASE, signif_dig) ~ "2",
+is.na(ANRHI) ~ NA_character_,
+signif(AVAL, signif_dig) &gt;= signif(1.1*ANRHI, signif_dig) ~ "1",
+signif(AVAL, signif_dig) &lt; signif(1.1*ANRHI, signif_dig) ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
+signif(AVAL, signif_dig) &gt;=  signif(20*ANRHI, signif_dig) ~ "4",
+signif(AVAL, signif_dig) &gt;=  signif(10*ANRHI, signif_dig) ~ "3",
+signif(AVAL, signif_dig) &gt;= signif(6*ANRHI, signif_dig) ~ "2",
+signif(AVAL, signif_dig) &gt;= signif(3*ANRHI, signif_dig) ~ "1",
+signif(AVAL, signif_dig) &lt; signif(3*ANRHI, signif_dig) ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 0.8 ~ "4",
+signif(AVAL, signif_dig) &lt; 0.9 ~ "3",
+signif(AVAL, signif_dig) &lt; 1 ~ "2",
+is.na(ANRLO) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; signif(ANRLO, signif_dig) ~ "1",
+signif(AVAL, signif_dig) &gt;= signif(ANRLO, signif_dig) ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 1.38 ~ "4",
+signif(AVAL, signif_dig) &lt; 1.5 ~ "3",
+signif(AVAL, signif_dig) &lt; 1.63 ~ "2",
+signif(AVAL, signif_dig) &lt; 1.88 ~ "1",
+signif(AVAL, signif_dig) &gt;= 1.88 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 1.53 ~ "4",
+signif(AVAL, signif_dig) &lt; 1.75 ~ "3",
+signif(AVAL, signif_dig) &lt; 1.95 ~ "2",
+signif(AVAL, signif_dig) &lt; 2.1 ~ "1",
+signif(AVAL, signif_dig) &gt;= 2.1 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+signif(AVAL, signif_dig) &gt;= 1.8 ~ "4",
+signif(AVAL, signif_dig) &gt;= 1.6 ~ "3",
+signif(AVAL, signif_dig) &gt;= 1.5 ~ "2",
+is.na(ANRHI) ~ NA_character_,
+signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
+signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &gt;= 3.38 ~ "4",
+signif(AVAL, signif_dig) &gt;= 3.23 ~ "3",
+signif(AVAL, signif_dig) &gt;= 3.1 ~ "2",
+signif(AVAL, signif_dig) &gt;= 2.88 ~ "1",
+signif(AVAL, signif_dig) &lt; 2.88 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &gt;= 3.38 ~ "4",
+signif(AVAL, signif_dig) &gt;= 3.13 ~ "3",
+signif(AVAL, signif_dig) &gt;= 2.88 ~ "2",
+signif(AVAL, signif_dig) &gt;= 2.65 ~ "1",
+signif(AVAL, signif_dig) &lt; 2.65 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(ANRHI) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &gt;=  5*ANRHI ~ "4",
+signif(AVAL, signif_dig) &gt;=  2.6*ANRHI ~ "3",
+signif(AVAL, signif_dig) &gt;= 1.6*ANRHI ~ "2",
+signif(AVAL, signif_dig) &gt;= 1.1*ANRHI ~ "1",
+signif(AVAL, signif_dig) &lt; 1.1*ANRHI ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &gt;  2*17.1 ~ "4",
+signif(AVAL, signif_dig) &gt;  1.5*17.1 ~ "3",
+signif(AVAL, signif_dig) &gt;  17.1 ~ "2",
+is.na(ANRHI) ~ NA_character_,
+signif(AVAL, signif_dig) &gt;= signif(ANRHI, signif_dig) ~ "1",
+signif(AVAL, signif_dig) &lt; signif(ANRHI, signif_dig) ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(ANRHI) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &gt;  signif(ANRHI, signif_dig) ~ "4",
+signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 8 ~ "4",
+signif(AVAL, signif_dig) &lt; 11 ~ "3",
+signif(AVAL, signif_dig) &lt; 16 ~ "2",
+is.na(ANRLO) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; signif(ANRLO, signif_dig) ~ "1",
+signif(AVAL, signif_dig) &gt;= signif(ANRLO, signif_dig) ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 7.3  ~ "4",
+is.na(ANRLO) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; signif(ANRLO, signif_dig) ~ "2",
+signif(AVAL, signif_dig) &gt;= signif(ANRLO, signif_dig) ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+signif(AVAL, signif_dig) &lt;  20 ~ "3",
+signif(AVAL, signif_dig) &lt; 30 ~ "2",
+is.na(ANRLO) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; signif(ANRLO, signif_dig) ~ "1",
+signif(AVAL, signif_dig) &gt;= signif(ANRLO, signif_dig) ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
+signif(AVAL, signif_dig) &gt;=  signif(10*ANRHI, signif_dig) ~ "4",
+signif(AVAL, signif_dig) &gt;=  signif(5*ANRHI, signif_dig) ~ "3",
+signif(AVAL, signif_dig) &gt;= signif(2.5*ANRHI, signif_dig) ~ "2",
+signif(AVAL, signif_dig) &gt;= signif(1.25*ANRHI, signif_dig) ~ "1",
+signif(AVAL, signif_dig) &lt; signif(1.25*ANRHI, signif_dig) ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+signif(AVAL, signif_dig) &gt; 7.5 ~ "4",
+is.na(ANRHI) ~ NA_character_,
+signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "2",
+signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
+signif(AVAL, signif_dig) &gt;= signif(10*ANRHI, signif_dig) ~ "4",
+signif(AVAL, signif_dig) &gt;= signif(5*ANRHI, signif_dig) ~ "3",
+signif(AVAL, signif_dig) &gt;= signif(2.5*ANRHI, signif_dig) ~ "2",
+signif(AVAL, signif_dig) &gt;= signif(1.25*ANRHI, signif_dig) ~ "1",
+signif(AVAL, signif_dig) &lt; signif(1.25*ANRHI, signif_dig) ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &gt;= 7.77 ~ "3",
+signif(AVAL, signif_dig) &gt;= 6.19 ~ "2",
+signif(AVAL, signif_dig) &gt;= 5.18 ~ "1",
+signif(AVAL, signif_dig) &lt; 5.18 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &gt;= 7.77 ~ "3",
+signif(AVAL, signif_dig) &gt;= 5.15 ~ "2",
+signif(AVAL, signif_dig) &gt;= 4.4 ~ "1",
+signif(AVAL, signif_dig) &lt; 4.4 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &gt;= 4.9 ~ "3",
+signif(AVAL, signif_dig) &gt;= 4.12 ~ "2",
+signif(AVAL, signif_dig) &gt;= 3.37 ~ "1",
+signif(AVAL, signif_dig) &lt; 3.37 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &gt;= 4.9 ~ "3",
+signif(AVAL, signif_dig) &gt;= 3.34 ~ "2",
+signif(AVAL, signif_dig) &gt;= 2.85 ~ "1",
+signif(AVAL, signif_dig) &lt; 2.85 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+signif(AVAL, signif_dig) &gt; 11.4 ~ "4",
+signif(AVAL, signif_dig) &gt; 5.7 ~ "3",
+signif(AVAL, signif_dig) &gt; 3.42 ~ "2",
+signif(AVAL, signif_dig) &gt;= 1.71 ~ "1",
+signif(AVAL, signif_dig) &lt; 1.71 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 0.3 ~ "4",
+signif(AVAL, signif_dig) &lt; 0.45 ~ "3",
+signif(AVAL, signif_dig) &lt; 0.6 ~ "2",
+signif(AVAL, signif_dig) &lt; 0.7 ~ "1",
+signif(AVAL, signif_dig) &gt;= 0.7 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 0.32 ~ "4",
+signif(AVAL, signif_dig) &lt; 0.45 ~ "3",
+signif(AVAL, signif_dig) &lt; 0.65 ~ "2",
+is.na(ANRLO) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; signif(ANRLO, signif_dig) ~ "1",
+signif(AVAL, signif_dig) &gt;= signif(ANRLO, signif_dig) ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 0.48 ~ "4",
+signif(AVAL, signif_dig) &lt; 0.81 ~ "3",
+signif(AVAL, signif_dig) &lt; 1.13 ~ "2",
+signif(AVAL, signif_dig) &lt; 1.45 ~ "1",
+signif(AVAL, signif_dig) &gt;= 1.45 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+signif(AVAL, signif_dig) &gt;= 7 ~ "4",
+signif(AVAL, signif_dig) &gt;= 6.5 ~ "3",
+signif(AVAL, signif_dig) &gt;= 6 ~ "2",
+signif(AVAL, signif_dig) &gt;= 5.6 ~ "1",
+signif(AVAL, signif_dig) &lt; 5.6 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 2 ~ "4",
+signif(AVAL, signif_dig) &lt; 2.5 ~ "3",
+signif(AVAL, signif_dig) &lt; 3 ~ "2",
+signif(AVAL, signif_dig) &lt; 3.4 ~ "1",
+signif(AVAL, signif_dig) &gt;= 3.4 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+signif(AVAL, signif_dig) &gt;= 160 ~ "4",
+signif(AVAL, signif_dig) &gt;= 154 ~ "3",
+signif(AVAL, signif_dig) &gt;= 150 ~ "2",
+signif(AVAL, signif_dig) &gt;= 146 ~ "1",
+signif(AVAL, signif_dig) &lt; 146 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+signif(AVAL, signif_dig) &lt;= 120 ~ "4",
+signif(AVAL, signif_dig) &lt; 125 ~ "3",
+signif(AVAL, signif_dig) &lt; 130 ~ "2",
+signif(AVAL, signif_dig) &lt; 135 ~ "1",
+signif(AVAL, signif_dig) &gt;= 135 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+signif(AVAL, signif_dig) &gt;= 890 ~ "4",
+signif(AVAL, signif_dig) &gt;= 710 ~ "3",
+signif(AVAL, signif_dig) &gt;= 590 ~ "2",
+signif(AVAL, signif_dig) &gt;= 450 ~ "1",
+signif(AVAL, signif_dig) &lt; 450 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 0.1 ~ "4",
+signif(AVAL, signif_dig) &lt; 0.2 ~ "3",
+signif(AVAL, signif_dig) &lt; 0.3 ~ "2",
+signif(AVAL, signif_dig) &lt; 0.4 ~ "1",
+signif(AVAL, signif_dig) &gt;= 0.4 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 0.35 ~ "4",
+signif(AVAL, signif_dig) &lt; 0.5 ~ "3",
+signif(AVAL, signif_dig) &lt; 0.6 ~ "2",
+signif(AVAL, signif_dig) &lt; 0.65 ~ "1",
+signif(AVAL, signif_dig) &lt;= 0.65 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 0.4 ~ "4",
+signif(AVAL, signif_dig) &lt; 0.6 ~ "3",
+signif(AVAL, signif_dig) &lt; 0.8 ~ "2",
+signif(AVAL, signif_dig) &lt;= 1 ~ "1",
+signif(AVAL, signif_dig) &gt; 1 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 0.75 ~ "4",
+signif(AVAL, signif_dig) &lt; 1 ~ "3",
+signif(AVAL, signif_dig) &lt; 1.25 ~ "2",
+signif(AVAL, signif_dig) &lt;= 1.5 ~ "1",
+signif(AVAL, signif_dig) &gt; 1.5 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 1.5 ~ "4",
+signif(AVAL, signif_dig) &lt; 3 ~ "3",
+signif(AVAL, signif_dig) &lt; 4 ~ "2",
+signif(AVAL, signif_dig) &lt;= 5 ~ "1",
+signif(AVAL, signif_dig) &gt; 5 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(SEX) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 70 ~ "4",
+signif(AVAL, signif_dig) &lt; 90 ~ "3",
+signif(AVAL, signif_dig) &lt; 100 ~ "2",
+signif(AVAL, signif_dig) &lt;= 109 ~ "1",
+signif(AVAL, signif_dig) &gt; 109 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(SEX)  | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 65 ~ "4",
+signif(AVAL, signif_dig) &lt; 85 ~ "3",
+signif(AVAL, signif_dig) &lt; 95 ~ "2",
+signif(AVAL, signif_dig) &lt;= 104 ~ "1",
+signif(AVAL, signif_dig) &gt; 104 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 65 ~ "4",
+signif(AVAL, signif_dig) &lt; 85 ~ "3",
+signif(AVAL, signif_dig) &lt; 95 ~ "2",
+signif(AVAL, signif_dig) &lt;= 104 ~ "1",
+signif(AVAL, signif_dig) &gt; 104 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 60 ~ "4",
+signif(AVAL, signif_dig) &lt; 70 ~ "3",
+signif(AVAL, signif_dig) &lt; 85 ~ "2",
+signif(AVAL, signif_dig) &lt;= 96 ~ "1",
+signif(AVAL, signif_dig) &gt; 96 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 67 ~ "4",
+signif(AVAL, signif_dig) &lt; 80 ~ "3",
+signif(AVAL, signif_dig) &lt; 95 ~ "2",
+signif(AVAL, signif_dig) &lt;= 110 ~ "1",
+signif(AVAL, signif_dig) &gt; 110 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 80 ~ "4",
+signif(AVAL, signif_dig) &lt; 90 ~ "3",
+signif(AVAL, signif_dig) &lt; 110 ~ "2",
+signif(AVAL, signif_dig) &lt;= 130 ~ "1",
+signif(AVAL, signif_dig) &gt; 130 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 90 ~ "4",
+signif(AVAL, signif_dig) &lt; 100 ~ "3",
+signif(AVAL, signif_dig) &lt; 130 ~ "2",
+signif(AVAL, signif_dig) &lt;= 140 ~ "1",
+signif(AVAL, signif_dig) &gt; 140 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
+signif(AVAL, signif_dig) &gt;=  signif(3*ANRHI, signif_dig) ~ "4",
+signif(AVAL, signif_dig) &gt;=  signif(2*ANRHI, signif_dig) ~ "3",
+signif(AVAL, signif_dig) &gt;= signif(1.5*ANRHI, signif_dig) ~ "2",
+signif(AVAL, signif_dig) &gt;= signif(1.1*ANRHI, signif_dig) ~ "1",
+signif(AVAL, signif_dig) &lt; signif(1.1*ANRHI, signif_dig) ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+signif(AVAL, signif_dig) &gt;=  20 ~ "4",
+signif(AVAL, signif_dig) &gt;=  15 ~ "3",
+signif(AVAL, signif_dig) &gt;= 10 ~ "2",
+signif(AVAL, signif_dig) &gt;= 5 ~ "1",
+signif(AVAL, signif_dig) &lt; 5 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 25 ~ "4",
+signif(AVAL, signif_dig) &lt; 50 ~ "3",
+signif(AVAL, signif_dig) &lt; 100 ~ "2",
+signif(AVAL, signif_dig) &lt; 125 ~ "1",
+signif(AVAL, signif_dig) &gt;= 125 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 1 ~ "4",
+signif(AVAL, signif_dig) &lt; 1.5 ~ "3",
+signif(AVAL, signif_dig) &lt; 2 ~ "2",
+signif(AVAL, signif_dig) &lt; 2.5 ~ "1",
+signif(AVAL, signif_dig) &gt;= 2.5 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 2.5 ~ "4",
+signif(AVAL, signif_dig) &lt; 4 ~ "3",
+signif(AVAL, signif_dig) &lt; 5.5 ~ "2",
+signif(AVAL, signif_dig) &lt; 7 ~ "1",
+signif(AVAL, signif_dig) &gt;= 7 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 0.48 ~ "4",
+signif(AVAL, signif_dig) &lt; 0.81 ~ "3",
+signif(AVAL, signif_dig) &lt; 0.97 ~ "2",
+signif(AVAL, signif_dig) &lt; 1.13 ~ "1",
+signif(AVAL, signif_dig) &gt;= 1.13 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+signif(AVAL, signif_dig) &lt;  0.5 ~ "4",
+is.na(ANRLO) ~ NA_character_,
+signif(AVAL, signif_dig) &lt;  signif(0.25*ANRLO, signif_dig) ~ "4",
+signif(AVAL, signif_dig) &lt; 0.75 ~ "3",
+signif(AVAL, signif_dig) &lt;  signif(0.5*ANRLO, signif_dig) ~ "3",
+signif(AVAL, signif_dig) &lt;  1 ~ "2",
+signif(AVAL, signif_dig) &lt;  signif(0.75*ANRLO, signif_dig) ~ "2",
+signif(AVAL, signif_dig) &lt;  2 ~ "1",
+signif(AVAL, signif_dig) &lt;  signif(ANRLO, signif_dig) ~ "1",
+signif(AVAL, signif_dig) &gt;= signif(ANRLO, signif_dig) ~ "0"
+)</t>
   </si>
 </sst>
 </file>
@@ -48656,8 +48667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -48681,7 +48692,7 @@
         <v>201</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>570</v>
+        <v>550</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>261</v>
@@ -48733,29 +48744,29 @@
       <c r="AA1" s="5"/>
       <c r="AB1" s="5"/>
     </row>
-    <row r="2" spans="1:28" ht="88.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B2" t="s">
-        <v>651</v>
+        <v>590</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>652</v>
+        <v>591</v>
       </c>
       <c r="F2" t="s">
-        <v>653</v>
+        <v>592</v>
       </c>
       <c r="G2" t="s">
-        <v>654</v>
+        <v>593</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="8" t="s">
-        <v>664</v>
+        <v>648</v>
       </c>
       <c r="L2" s="4"/>
       <c r="M2" s="4" t="s">
@@ -48765,7 +48776,7 @@
         <v>8</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>655</v>
+        <v>594</v>
       </c>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
@@ -48781,29 +48792,29 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="5"/>
     </row>
-    <row r="3" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" ht="126" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="B3" t="s">
         <v>396</v>
-      </c>
-      <c r="B3" t="s">
-        <v>403</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="E3" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="F3" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="G3" s="32"/>
       <c r="H3" s="10"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="8" t="s">
-        <v>407</v>
+        <v>649</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>2</v>
@@ -48829,31 +48840,31 @@
       <c r="AA3" s="5"/>
       <c r="AB3" s="5"/>
     </row>
-    <row r="4" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B4" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="31" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="G4" s="32" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="8" t="s">
-        <v>402</v>
+        <v>650</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4" t="s">
@@ -48877,29 +48888,29 @@
       <c r="AA4" s="5"/>
       <c r="AB4" s="5"/>
     </row>
-    <row r="5" spans="1:28" ht="88.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B5" t="s">
-        <v>656</v>
+        <v>595</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>657</v>
+        <v>596</v>
       </c>
       <c r="F5" t="s">
-        <v>658</v>
+        <v>597</v>
       </c>
       <c r="G5" t="s">
-        <v>659</v>
+        <v>598</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8" t="s">
-        <v>665</v>
+        <v>651</v>
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="4" t="s">
@@ -48909,7 +48920,7 @@
         <v>13</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>655</v>
+        <v>594</v>
       </c>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
@@ -48925,31 +48936,31 @@
       <c r="AA5" s="5"/>
       <c r="AB5" s="5"/>
     </row>
-    <row r="6" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B6" t="s">
-        <v>666</v>
+        <v>602</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="8" t="s">
-        <v>408</v>
+        <v>652</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4" t="s">
@@ -48973,31 +48984,31 @@
       <c r="AA6" s="5"/>
       <c r="AB6" s="5"/>
     </row>
-    <row r="7" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B7" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="33" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="G7" s="33" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="1" t="s">
-        <v>414</v>
+        <v>630</v>
       </c>
       <c r="L7" s="12"/>
       <c r="M7" s="4" t="s">
@@ -49021,31 +49032,31 @@
       <c r="AA7" s="5"/>
       <c r="AB7" s="5"/>
     </row>
-    <row r="8" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B8" t="s">
-        <v>667</v>
+        <v>603</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="8" t="s">
-        <v>408</v>
+        <v>652</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4" t="s">
@@ -49069,31 +49080,31 @@
       <c r="AA8" s="5"/>
       <c r="AB8" s="5"/>
     </row>
-    <row r="9" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B9" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="8" t="s">
-        <v>668</v>
+        <v>647</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>46</v>
@@ -49119,41 +49130,41 @@
       <c r="AA9" s="5"/>
       <c r="AB9" s="5"/>
     </row>
-    <row r="10" spans="1:28" s="44" customFormat="1" ht="76" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" s="44" customFormat="1" ht="101" x14ac:dyDescent="0.35">
       <c r="A10" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="32"/>
       <c r="F10" s="37" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
       <c r="H10" s="36"/>
       <c r="I10" s="38"/>
       <c r="J10" s="38" t="s">
-        <v>594</v>
+        <v>573</v>
       </c>
       <c r="K10" s="39" t="s">
-        <v>595</v>
+        <v>646</v>
       </c>
       <c r="L10" s="40"/>
       <c r="M10" s="4" t="s">
-        <v>596</v>
+        <v>574</v>
       </c>
       <c r="N10" s="41" t="s">
         <v>13</v>
       </c>
       <c r="O10" s="37" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="P10" s="43"/>
       <c r="Q10" s="43"/>
@@ -49169,46 +49180,46 @@
       <c r="AA10" s="43"/>
       <c r="AB10" s="43"/>
     </row>
-    <row r="11" spans="1:28" s="44" customFormat="1" ht="126" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" s="44" customFormat="1" ht="151" x14ac:dyDescent="0.35">
       <c r="A11" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>429</v>
+        <v>419</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="F11" s="32" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="G11" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="H11"/>
       <c r="J11" s="38" t="s">
-        <v>597</v>
+        <v>575</v>
       </c>
       <c r="K11" s="39" t="s">
-        <v>670</v>
+        <v>645</v>
       </c>
       <c r="L11" s="40" t="s">
-        <v>571</v>
+        <v>551</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>596</v>
+        <v>574</v>
       </c>
       <c r="N11" s="41" t="s">
         <v>13</v>
       </c>
       <c r="O11" s="42" t="s">
-        <v>669</v>
+        <v>604</v>
       </c>
       <c r="P11" s="43"/>
       <c r="Q11" s="43"/>
@@ -49226,37 +49237,37 @@
     </row>
     <row r="12" spans="1:28" s="44" customFormat="1" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A12" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B12" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="C12" s="37" t="s">
+        <v>411</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>423</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>422</v>
+      </c>
+      <c r="F12" s="33" t="s">
         <v>421</v>
       </c>
-      <c r="D12" s="33" t="s">
-        <v>433</v>
-      </c>
-      <c r="E12" s="34" t="s">
-        <v>432</v>
-      </c>
-      <c r="F12" s="33" t="s">
-        <v>431</v>
-      </c>
       <c r="G12" s="33" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="H12" s="36"/>
       <c r="I12" s="38"/>
       <c r="J12" s="38" t="s">
-        <v>594</v>
+        <v>573</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>600</v>
+        <v>644</v>
       </c>
       <c r="L12" s="40"/>
       <c r="M12" s="4" t="s">
-        <v>596</v>
+        <v>574</v>
       </c>
       <c r="N12" s="41" t="s">
         <v>13</v>
@@ -49278,13 +49289,13 @@
     </row>
     <row r="13" spans="1:28" s="44" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B13" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="D13" s="33"/>
       <c r="E13" s="34"/>
@@ -49293,20 +49304,20 @@
       <c r="H13" s="36"/>
       <c r="I13" s="38"/>
       <c r="J13" s="38" t="s">
-        <v>597</v>
+        <v>575</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>663</v>
+        <v>601</v>
       </c>
       <c r="L13" s="40"/>
       <c r="M13" s="4" t="s">
-        <v>596</v>
+        <v>574</v>
       </c>
       <c r="N13" s="41" t="s">
         <v>13</v>
       </c>
       <c r="O13" s="37" t="s">
-        <v>671</v>
+        <v>605</v>
       </c>
       <c r="P13" s="43"/>
       <c r="Q13" s="43"/>
@@ -49324,39 +49335,39 @@
     </row>
     <row r="14" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A14" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>439</v>
+        <v>429</v>
       </c>
       <c r="C14" t="s">
-        <v>677</v>
+        <v>607</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>440</v>
+        <v>430</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>441</v>
+        <v>431</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>443</v>
+        <v>433</v>
       </c>
       <c r="H14" s="19"/>
       <c r="I14" s="18"/>
       <c r="J14" s="38" t="s">
-        <v>598</v>
+        <v>576</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>601</v>
+        <v>643</v>
       </c>
       <c r="L14" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>604</v>
+        <v>578</v>
       </c>
       <c r="N14" s="4" t="s">
         <v>13</v>
@@ -49378,39 +49389,39 @@
     </row>
     <row r="15" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A15" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>439</v>
+        <v>429</v>
       </c>
       <c r="C15" t="s">
-        <v>444</v>
+        <v>434</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>574</v>
+        <v>553</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>573</v>
+        <v>552</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>443</v>
+        <v>433</v>
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="18"/>
       <c r="J15" s="38" t="s">
-        <v>599</v>
+        <v>577</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>602</v>
+        <v>642</v>
       </c>
       <c r="L15" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>604</v>
+        <v>578</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>13</v>
@@ -49430,31 +49441,31 @@
       <c r="AA15" s="5"/>
       <c r="AB15" s="5"/>
     </row>
-    <row r="16" spans="1:28" ht="113" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" ht="138" x14ac:dyDescent="0.3">
       <c r="A16" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>434</v>
+        <v>424</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="19" t="s">
-        <v>435</v>
+        <v>425</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>438</v>
+        <v>428</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>437</v>
+        <v>427</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
       <c r="K16" s="1" t="s">
-        <v>572</v>
+        <v>641</v>
       </c>
       <c r="L16" s="14" t="s">
         <v>46</v>
@@ -49482,39 +49493,39 @@
     </row>
     <row r="17" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A17" s="45" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B17" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
       <c r="C17" t="s">
-        <v>677</v>
+        <v>607</v>
       </c>
       <c r="D17" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="E17" t="s">
-        <v>453</v>
+        <v>443</v>
       </c>
       <c r="F17" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
       <c r="G17" t="s">
-        <v>455</v>
+        <v>445</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="18"/>
       <c r="J17" s="38" t="s">
-        <v>598</v>
+        <v>576</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>603</v>
+        <v>640</v>
       </c>
       <c r="L17" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>604</v>
+        <v>578</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>8</v>
@@ -49536,39 +49547,39 @@
     </row>
     <row r="18" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A18" s="45" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B18" t="s">
+        <v>436</v>
+      </c>
+      <c r="C18" t="s">
+        <v>434</v>
+      </c>
+      <c r="D18" t="s">
         <v>446</v>
       </c>
-      <c r="C18" t="s">
-        <v>444</v>
-      </c>
-      <c r="D18" t="s">
-        <v>456</v>
-      </c>
       <c r="E18" t="s">
-        <v>457</v>
+        <v>447</v>
       </c>
       <c r="F18" t="s">
-        <v>458</v>
+        <v>448</v>
       </c>
       <c r="G18" t="s">
-        <v>459</v>
+        <v>449</v>
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="18"/>
       <c r="J18" s="38" t="s">
-        <v>599</v>
+        <v>577</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>605</v>
+        <v>639</v>
       </c>
       <c r="L18" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>604</v>
+        <v>578</v>
       </c>
       <c r="N18" s="4" t="s">
         <v>8</v>
@@ -49588,31 +49599,31 @@
       <c r="AA18" s="5"/>
       <c r="AB18" s="5"/>
     </row>
-    <row r="19" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:28" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A19" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B19" t="s">
-        <v>447</v>
+        <v>437</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
-        <v>448</v>
+        <v>438</v>
       </c>
       <c r="E19" t="s">
-        <v>449</v>
+        <v>439</v>
       </c>
       <c r="F19" t="s">
-        <v>450</v>
+        <v>440</v>
       </c>
       <c r="G19" t="s">
-        <v>451</v>
+        <v>441</v>
       </c>
       <c r="H19" s="19"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="1" t="s">
-        <v>245</v>
+        <v>638</v>
       </c>
       <c r="L19" s="14" t="s">
         <v>46</v>
@@ -49638,31 +49649,31 @@
       <c r="AA19" s="5"/>
       <c r="AB19" s="5"/>
     </row>
-    <row r="20" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A20" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B20" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10" t="s">
-        <v>464</v>
+        <v>454</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>463</v>
+        <v>453</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>462</v>
+        <v>452</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>461</v>
+        <v>451</v>
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="1" t="s">
-        <v>465</v>
+        <v>637</v>
       </c>
       <c r="L20" s="12"/>
       <c r="M20" s="4" t="s">
@@ -49686,31 +49697,31 @@
       <c r="AA20" s="5"/>
       <c r="AB20" s="5"/>
     </row>
-    <row r="21" spans="1:28" ht="151" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:28" ht="251" x14ac:dyDescent="0.35">
       <c r="A21" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B21" t="s">
-        <v>466</v>
+        <v>455</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10" t="s">
-        <v>467</v>
+        <v>456</v>
       </c>
       <c r="E21" t="s">
-        <v>468</v>
+        <v>457</v>
       </c>
       <c r="F21" t="s">
-        <v>469</v>
+        <v>458</v>
       </c>
       <c r="G21" t="s">
-        <v>575</v>
+        <v>554</v>
       </c>
       <c r="H21" s="10"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
       <c r="K21" s="1" t="s">
-        <v>672</v>
+        <v>636</v>
       </c>
       <c r="L21" s="12"/>
       <c r="M21" s="4" t="s">
@@ -49736,29 +49747,29 @@
     </row>
     <row r="22" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A22" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B22" t="s">
-        <v>470</v>
+        <v>459</v>
       </c>
       <c r="C22" s="16"/>
       <c r="D22" t="s">
-        <v>471</v>
+        <v>460</v>
       </c>
       <c r="E22" t="s">
-        <v>472</v>
+        <v>461</v>
       </c>
       <c r="F22" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="G22" t="s">
-        <v>576</v>
+        <v>555</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="18"/>
       <c r="J22" s="18"/>
       <c r="K22" s="1" t="s">
-        <v>474</v>
+        <v>635</v>
       </c>
       <c r="L22" s="14" t="s">
         <v>46</v>
@@ -49786,29 +49797,29 @@
     </row>
     <row r="23" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A23" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B23" t="s">
-        <v>475</v>
+        <v>463</v>
       </c>
       <c r="C23" s="16"/>
       <c r="D23" t="s">
-        <v>477</v>
+        <v>465</v>
       </c>
       <c r="E23" t="s">
-        <v>476</v>
+        <v>464</v>
       </c>
       <c r="F23" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="G23" t="s">
-        <v>576</v>
+        <v>555</v>
       </c>
       <c r="H23" s="20"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="K23" s="1" t="s">
-        <v>478</v>
+        <v>634</v>
       </c>
       <c r="L23" s="14" t="s">
         <v>46</v>
@@ -49836,39 +49847,39 @@
     </row>
     <row r="24" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A24" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B24" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="C24" t="s">
-        <v>480</v>
+        <v>467</v>
       </c>
       <c r="D24" t="s">
-        <v>481</v>
+        <v>468</v>
       </c>
       <c r="E24" t="s">
-        <v>482</v>
+        <v>469</v>
       </c>
       <c r="F24" t="s">
-        <v>483</v>
+        <v>470</v>
       </c>
       <c r="G24" t="s">
-        <v>484</v>
+        <v>471</v>
       </c>
       <c r="H24" s="20"/>
       <c r="I24" s="18"/>
       <c r="J24" s="38" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>606</v>
+        <v>633</v>
       </c>
       <c r="L24" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>608</v>
+        <v>579</v>
       </c>
       <c r="N24" s="4" t="s">
         <v>8</v>
@@ -49890,39 +49901,39 @@
     </row>
     <row r="25" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A25" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B25" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>485</v>
+        <v>472</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>487</v>
+        <v>474</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>486</v>
+        <v>473</v>
       </c>
       <c r="F25" t="s">
-        <v>483</v>
+        <v>470</v>
       </c>
       <c r="G25" t="s">
-        <v>484</v>
+        <v>471</v>
       </c>
       <c r="H25" s="20"/>
       <c r="I25" s="18"/>
       <c r="J25" s="38" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>607</v>
+        <v>632</v>
       </c>
       <c r="L25" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>608</v>
+        <v>579</v>
       </c>
       <c r="N25" s="4" t="s">
         <v>8</v>
@@ -49942,30 +49953,30 @@
       <c r="AA25" s="5"/>
       <c r="AB25" s="5"/>
     </row>
-    <row r="26" spans="1:28" ht="87" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A26" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>488</v>
+        <v>475</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>489</v>
+        <v>476</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>490</v>
+        <v>477</v>
       </c>
       <c r="F26" s="35" t="s">
-        <v>491</v>
+        <v>478</v>
       </c>
       <c r="G26" s="30" t="s">
-        <v>492</v>
+        <v>479</v>
       </c>
       <c r="H26" s="20"/>
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
       <c r="K26" s="1" t="s">
-        <v>493</v>
+        <v>631</v>
       </c>
       <c r="L26" s="14"/>
       <c r="M26" s="4" t="s">
@@ -49975,7 +49986,7 @@
         <v>13</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>494</v>
+        <v>480</v>
       </c>
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
@@ -49991,31 +50002,31 @@
       <c r="AA26" s="5"/>
       <c r="AB26" s="5"/>
     </row>
-    <row r="27" spans="1:28" s="29" customFormat="1" ht="101" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:28" s="29" customFormat="1" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A27" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>495</v>
+        <v>481</v>
       </c>
       <c r="C27" s="17"/>
       <c r="D27" s="30" t="s">
-        <v>498</v>
+        <v>484</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>497</v>
+        <v>483</v>
       </c>
       <c r="F27" s="33" t="s">
-        <v>496</v>
+        <v>482</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="H27" s="17"/>
       <c r="I27" s="17"/>
       <c r="J27" s="17"/>
       <c r="K27" s="26" t="s">
-        <v>414</v>
+        <v>630</v>
       </c>
       <c r="L27" s="27"/>
       <c r="M27" s="27" t="s">
@@ -50041,37 +50052,37 @@
     </row>
     <row r="28" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A28" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B28" t="s">
-        <v>499</v>
+        <v>485</v>
       </c>
       <c r="C28" t="s">
-        <v>500</v>
+        <v>486</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>503</v>
+        <v>489</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>502</v>
+        <v>488</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>501</v>
+        <v>487</v>
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
       <c r="I28" s="7"/>
       <c r="J28" s="38" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>609</v>
+        <v>653</v>
       </c>
       <c r="L28" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>608</v>
+        <v>579</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>13</v>
@@ -50093,37 +50104,37 @@
     </row>
     <row r="29" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A29" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B29" t="s">
-        <v>499</v>
+        <v>485</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>504</v>
+        <v>490</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>506</v>
+        <v>492</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>505</v>
+        <v>491</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>501</v>
+        <v>487</v>
       </c>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
       <c r="I29" s="7"/>
       <c r="J29" s="38" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>673</v>
+        <v>654</v>
       </c>
       <c r="L29" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>608</v>
+        <v>579</v>
       </c>
       <c r="N29" s="4" t="s">
         <v>13</v>
@@ -50145,37 +50156,37 @@
     </row>
     <row r="30" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A30" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>507</v>
+        <v>493</v>
       </c>
       <c r="C30" t="s">
-        <v>500</v>
+        <v>486</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>508</v>
+        <v>494</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>509</v>
+        <v>495</v>
       </c>
       <c r="F30" s="30" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
       <c r="I30" s="7"/>
       <c r="J30" s="38" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>610</v>
+        <v>655</v>
       </c>
       <c r="L30" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>608</v>
+        <v>579</v>
       </c>
       <c r="N30" s="4" t="s">
         <v>13</v>
@@ -50197,37 +50208,37 @@
     </row>
     <row r="31" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A31" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>507</v>
+        <v>493</v>
       </c>
       <c r="C31" s="30" t="s">
-        <v>511</v>
+        <v>497</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>512</v>
+        <v>498</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="F31" s="30" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
       <c r="I31" s="7"/>
       <c r="J31" s="38" t="s">
-        <v>619</v>
+        <v>628</v>
       </c>
       <c r="K31" s="8" t="s">
-        <v>611</v>
+        <v>656</v>
       </c>
       <c r="L31" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>608</v>
+        <v>579</v>
       </c>
       <c r="N31" s="4" t="s">
         <v>13</v>
@@ -50249,13 +50260,13 @@
     </row>
     <row r="32" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A32" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>507</v>
+        <v>493</v>
       </c>
       <c r="C32" s="47" t="s">
-        <v>675</v>
+        <v>606</v>
       </c>
       <c r="D32" s="30"/>
       <c r="E32" s="30"/>
@@ -50264,22 +50275,22 @@
       <c r="H32" s="10"/>
       <c r="I32" s="7"/>
       <c r="J32" s="38" t="s">
-        <v>676</v>
+        <v>618</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>663</v>
+        <v>601</v>
       </c>
       <c r="L32" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>608</v>
+        <v>579</v>
       </c>
       <c r="N32" s="4" t="s">
         <v>13</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>662</v>
+        <v>600</v>
       </c>
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
@@ -50297,29 +50308,29 @@
     </row>
     <row r="33" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A33" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>514</v>
+        <v>500</v>
       </c>
       <c r="C33" s="16"/>
       <c r="D33" s="30" t="s">
-        <v>515</v>
+        <v>501</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>516</v>
+        <v>502</v>
       </c>
       <c r="F33" s="30" t="s">
-        <v>517</v>
+        <v>503</v>
       </c>
       <c r="G33" s="30" t="s">
-        <v>518</v>
+        <v>504</v>
       </c>
       <c r="H33" s="20"/>
       <c r="I33" s="18"/>
       <c r="J33" s="18"/>
       <c r="K33" s="1" t="s">
-        <v>674</v>
+        <v>657</v>
       </c>
       <c r="L33" s="14" t="s">
         <v>46</v>
@@ -50347,29 +50358,29 @@
     </row>
     <row r="34" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A34" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>519</v>
+        <v>505</v>
       </c>
       <c r="C34" s="16"/>
       <c r="D34" s="30" t="s">
-        <v>520</v>
+        <v>506</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>521</v>
+        <v>507</v>
       </c>
       <c r="F34" s="30" t="s">
-        <v>522</v>
+        <v>508</v>
       </c>
       <c r="G34" s="30" t="s">
-        <v>523</v>
+        <v>509</v>
       </c>
       <c r="H34" s="20"/>
       <c r="I34" s="18"/>
       <c r="J34" s="18"/>
       <c r="K34" s="1" t="s">
-        <v>524</v>
+        <v>658</v>
       </c>
       <c r="L34" s="14" t="s">
         <v>46</v>
@@ -50395,41 +50406,41 @@
       <c r="AA34" s="5"/>
       <c r="AB34" s="5"/>
     </row>
-    <row r="35" spans="1:28" ht="126" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:28" ht="151" x14ac:dyDescent="0.35">
       <c r="A35" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B35" s="30" t="s">
-        <v>525</v>
+        <v>510</v>
       </c>
       <c r="C35" s="30" t="s">
-        <v>526</v>
+        <v>511</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>527</v>
+        <v>512</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>528</v>
+        <v>513</v>
       </c>
       <c r="F35" s="30" t="s">
-        <v>529</v>
+        <v>514</v>
       </c>
       <c r="G35" s="30" t="s">
-        <v>530</v>
+        <v>515</v>
       </c>
       <c r="H35" s="20"/>
       <c r="I35" s="18"/>
       <c r="J35" s="38" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>612</v>
+        <v>659</v>
       </c>
       <c r="L35" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>634</v>
+        <v>587</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>8</v>
@@ -50451,39 +50462,39 @@
     </row>
     <row r="36" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A36" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>525</v>
+        <v>510</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>531</v>
+        <v>516</v>
       </c>
       <c r="D36" s="30" t="s">
-        <v>535</v>
+        <v>520</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>534</v>
+        <v>519</v>
       </c>
       <c r="F36" s="30" t="s">
-        <v>533</v>
+        <v>518</v>
       </c>
       <c r="G36" s="30" t="s">
-        <v>532</v>
+        <v>517</v>
       </c>
       <c r="H36" s="20"/>
       <c r="I36" s="18"/>
       <c r="J36" s="38" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>613</v>
+        <v>683</v>
       </c>
       <c r="L36" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>634</v>
+        <v>587</v>
       </c>
       <c r="N36" s="4" t="s">
         <v>8</v>
@@ -50505,39 +50516,39 @@
     </row>
     <row r="37" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A37" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B37" s="30" t="s">
-        <v>525</v>
+        <v>510</v>
       </c>
       <c r="C37" s="30" t="s">
-        <v>536</v>
+        <v>521</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>538</v>
+        <v>523</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>537</v>
+        <v>522</v>
       </c>
       <c r="F37" s="30" t="s">
-        <v>533</v>
+        <v>518</v>
       </c>
       <c r="G37" s="30" t="s">
-        <v>532</v>
+        <v>517</v>
       </c>
       <c r="H37" s="20"/>
       <c r="I37" s="18"/>
       <c r="J37" s="38" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>614</v>
+        <v>660</v>
       </c>
       <c r="L37" s="14" t="s">
         <v>46</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>634</v>
+        <v>587</v>
       </c>
       <c r="N37" s="4" t="s">
         <v>8</v>
@@ -50559,29 +50570,29 @@
     </row>
     <row r="38" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A38" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B38" s="30" t="s">
-        <v>545</v>
+        <v>529</v>
       </c>
       <c r="C38" s="30"/>
       <c r="D38" s="30" t="s">
-        <v>549</v>
+        <v>533</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>548</v>
+        <v>532</v>
       </c>
       <c r="F38" s="30" t="s">
-        <v>547</v>
+        <v>531</v>
       </c>
       <c r="G38" s="30" t="s">
-        <v>546</v>
+        <v>530</v>
       </c>
       <c r="H38" s="20"/>
       <c r="I38" s="18"/>
       <c r="J38" s="18"/>
       <c r="K38" s="1" t="s">
-        <v>550</v>
+        <v>661</v>
       </c>
       <c r="L38" s="14" t="s">
         <v>46</v>
@@ -50609,29 +50620,29 @@
     </row>
     <row r="39" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A39" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B39" s="30" t="s">
-        <v>539</v>
+        <v>524</v>
       </c>
       <c r="C39" s="30"/>
       <c r="D39" s="30" t="s">
-        <v>540</v>
+        <v>525</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>543</v>
+        <v>528</v>
       </c>
       <c r="F39" s="30" t="s">
-        <v>542</v>
+        <v>527</v>
       </c>
       <c r="G39" s="30" t="s">
-        <v>541</v>
+        <v>526</v>
       </c>
       <c r="H39" s="20"/>
       <c r="I39" s="18"/>
       <c r="J39" s="18"/>
       <c r="K39" s="1" t="s">
-        <v>544</v>
+        <v>662</v>
       </c>
       <c r="L39" s="14" t="s">
         <v>46</v>
@@ -50659,29 +50670,29 @@
     </row>
     <row r="40" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A40" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B40" s="30" t="s">
-        <v>557</v>
+        <v>539</v>
       </c>
       <c r="C40" s="16"/>
       <c r="D40" s="30" t="s">
-        <v>561</v>
+        <v>543</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>560</v>
+        <v>542</v>
       </c>
       <c r="F40" s="30" t="s">
-        <v>559</v>
+        <v>541</v>
       </c>
       <c r="G40" s="20" t="s">
-        <v>558</v>
+        <v>540</v>
       </c>
       <c r="H40" s="20"/>
       <c r="I40" s="18"/>
       <c r="J40" s="18"/>
       <c r="K40" s="1" t="s">
-        <v>562</v>
+        <v>663</v>
       </c>
       <c r="L40" s="14" t="s">
         <v>46</v>
@@ -50709,29 +50720,29 @@
     </row>
     <row r="41" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A41" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>551</v>
+        <v>534</v>
       </c>
       <c r="C41" s="16"/>
       <c r="D41" s="30" t="s">
-        <v>555</v>
+        <v>538</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>554</v>
+        <v>537</v>
       </c>
       <c r="F41" s="30" t="s">
-        <v>553</v>
+        <v>536</v>
       </c>
       <c r="G41" s="33" t="s">
-        <v>552</v>
+        <v>535</v>
       </c>
       <c r="H41" s="20"/>
       <c r="I41" s="18"/>
       <c r="J41" s="18"/>
       <c r="K41" s="1" t="s">
-        <v>556</v>
+        <v>664</v>
       </c>
       <c r="L41" s="14" t="s">
         <v>46</v>
@@ -50759,32 +50770,32 @@
     </row>
     <row r="42" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A42" s="36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>563</v>
+        <v>544</v>
       </c>
       <c r="C42" s="15"/>
       <c r="D42" s="30" t="s">
-        <v>567</v>
+        <v>548</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>566</v>
+        <v>547</v>
       </c>
       <c r="F42" s="30" t="s">
-        <v>565</v>
+        <v>546</v>
       </c>
       <c r="G42" s="30" t="s">
-        <v>564</v>
+        <v>545</v>
       </c>
       <c r="H42" s="19"/>
       <c r="I42" s="18"/>
       <c r="J42" s="18"/>
       <c r="K42" s="1" t="s">
-        <v>569</v>
+        <v>665</v>
       </c>
       <c r="L42" s="14" t="s">
-        <v>571</v>
+        <v>551</v>
       </c>
       <c r="M42" s="4" t="s">
         <v>4</v>
@@ -50793,7 +50804,7 @@
         <v>13</v>
       </c>
       <c r="O42" s="3" t="s">
-        <v>568</v>
+        <v>549</v>
       </c>
       <c r="P42" s="5"/>
       <c r="Q42" s="5"/>
@@ -50814,42 +50825,42 @@
         <v>310</v>
       </c>
       <c r="B43" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C43" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>577</v>
+        <v>556</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>578</v>
+        <v>557</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>579</v>
+        <v>558</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>580</v>
+        <v>559</v>
       </c>
       <c r="H43" s="10"/>
       <c r="I43" s="7"/>
       <c r="J43" s="38" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>636</v>
+        <v>666</v>
       </c>
       <c r="L43" s="11" t="s">
         <v>11</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>604</v>
+        <v>578</v>
       </c>
       <c r="N43" s="4" t="s">
         <v>8</v>
       </c>
       <c r="O43" s="3" t="s">
-        <v>581</v>
+        <v>560</v>
       </c>
       <c r="P43" s="5"/>
       <c r="Q43" s="5"/>
@@ -50870,10 +50881,10 @@
         <v>310</v>
       </c>
       <c r="B44" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C44" t="s">
-        <v>660</v>
+        <v>599</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
@@ -50882,22 +50893,22 @@
       <c r="H44" s="10"/>
       <c r="I44" s="7"/>
       <c r="J44" s="38" t="s">
-        <v>661</v>
+        <v>623</v>
       </c>
       <c r="K44" s="8" t="s">
-        <v>663</v>
+        <v>601</v>
       </c>
       <c r="L44" s="11" t="s">
         <v>11</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>604</v>
+        <v>578</v>
       </c>
       <c r="N44" s="4" t="s">
         <v>8</v>
       </c>
       <c r="O44" s="3" t="s">
-        <v>662</v>
+        <v>600</v>
       </c>
       <c r="P44" s="5"/>
       <c r="Q44" s="5"/>
@@ -50918,42 +50929,42 @@
         <v>310</v>
       </c>
       <c r="B45" t="s">
+        <v>351</v>
+      </c>
+      <c r="C45" t="s">
         <v>352</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" s="7" t="s">
+        <v>561</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="G45" s="7" t="s">
         <v>353</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>582</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>356</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>355</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>354</v>
       </c>
       <c r="H45" s="7"/>
       <c r="I45" s="7"/>
       <c r="J45" s="38" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>637</v>
+        <v>667</v>
       </c>
       <c r="L45" s="11" t="s">
         <v>11</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>604</v>
+        <v>578</v>
       </c>
       <c r="N45" s="4" t="s">
         <v>8</v>
       </c>
       <c r="O45" s="3" t="s">
-        <v>581</v>
+        <v>560</v>
       </c>
       <c r="P45" s="5"/>
       <c r="Q45" s="5"/>
@@ -50974,10 +50985,10 @@
         <v>310</v>
       </c>
       <c r="B46" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C46" t="s">
-        <v>660</v>
+        <v>599</v>
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
@@ -50986,22 +50997,22 @@
       <c r="H46" s="7"/>
       <c r="I46" s="7"/>
       <c r="J46" s="38" t="s">
-        <v>661</v>
+        <v>623</v>
       </c>
       <c r="K46" s="8" t="s">
-        <v>663</v>
+        <v>601</v>
       </c>
       <c r="L46" s="11" t="s">
         <v>11</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>604</v>
+        <v>578</v>
       </c>
       <c r="N46" s="4" t="s">
         <v>8</v>
       </c>
       <c r="O46" s="3" t="s">
-        <v>662</v>
+        <v>600</v>
       </c>
       <c r="P46" s="5"/>
       <c r="Q46" s="5"/>
@@ -51022,38 +51033,38 @@
         <v>310</v>
       </c>
       <c r="B47" t="s">
+        <v>345</v>
+      </c>
+      <c r="C47" t="s">
         <v>346</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" s="10" t="s">
+        <v>562</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>563</v>
+      </c>
+      <c r="F47" s="10" t="s">
+        <v>564</v>
+      </c>
+      <c r="G47" s="10" t="s">
         <v>347</v>
-      </c>
-      <c r="D47" s="10" t="s">
-        <v>583</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="F47" s="10" t="s">
-        <v>585</v>
-      </c>
-      <c r="G47" s="10" t="s">
-        <v>348</v>
       </c>
       <c r="H47" s="10" t="s">
         <v>188</v>
       </c>
       <c r="I47" s="7"/>
       <c r="J47" s="38" t="s">
-        <v>624</v>
+        <v>580</v>
       </c>
       <c r="K47" s="8" t="s">
-        <v>638</v>
+        <v>668</v>
       </c>
       <c r="L47" s="11" t="s">
         <v>11</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>604</v>
+        <v>578</v>
       </c>
       <c r="N47" s="4" t="s">
         <v>8</v>
@@ -51078,38 +51089,38 @@
         <v>310</v>
       </c>
       <c r="B48" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C48" t="s">
+        <v>348</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>565</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>566</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>567</v>
+      </c>
+      <c r="G48" s="10" t="s">
         <v>349</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>586</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>587</v>
-      </c>
-      <c r="F48" s="10" t="s">
-        <v>588</v>
-      </c>
-      <c r="G48" s="10" t="s">
-        <v>350</v>
       </c>
       <c r="H48" s="10" t="s">
         <v>188</v>
       </c>
       <c r="I48" s="7"/>
       <c r="J48" s="38" t="s">
-        <v>625</v>
+        <v>581</v>
       </c>
       <c r="K48" s="8" t="s">
-        <v>639</v>
+        <v>669</v>
       </c>
       <c r="L48" s="11" t="s">
         <v>11</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>604</v>
+        <v>578</v>
       </c>
       <c r="N48" s="4" t="s">
         <v>8</v>
@@ -51134,38 +51145,38 @@
         <v>310</v>
       </c>
       <c r="B49" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C49" t="s">
-        <v>678</v>
+        <v>608</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>589</v>
+        <v>568</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>590</v>
+        <v>569</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>591</v>
+        <v>570</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H49" s="10" t="s">
         <v>188</v>
       </c>
       <c r="I49" s="7"/>
       <c r="J49" s="38" t="s">
-        <v>626</v>
+        <v>582</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>640</v>
+        <v>670</v>
       </c>
       <c r="L49" s="11" t="s">
         <v>11</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>604</v>
+        <v>578</v>
       </c>
       <c r="N49" s="4" t="s">
         <v>8</v>
@@ -51185,7 +51196,7 @@
       <c r="AA49" s="5"/>
       <c r="AB49" s="5"/>
     </row>
-    <row r="50" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:28" ht="226" x14ac:dyDescent="0.35">
       <c r="A50" s="7" t="s">
         <v>310</v>
       </c>
@@ -51211,7 +51222,7 @@
       <c r="I50" s="7"/>
       <c r="J50" s="7"/>
       <c r="K50" s="1" t="s">
-        <v>345</v>
+        <v>684</v>
       </c>
       <c r="L50" s="4" t="s">
         <v>2</v>
@@ -51245,7 +51256,7 @@
         <v>311</v>
       </c>
       <c r="C51" t="s">
-        <v>681</v>
+        <v>611</v>
       </c>
       <c r="D51" s="30" t="s">
         <v>313</v>
@@ -51262,16 +51273,16 @@
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
       <c r="J51" s="38" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="K51" s="8" t="s">
-        <v>641</v>
+        <v>671</v>
       </c>
       <c r="L51" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>635</v>
+        <v>588</v>
       </c>
       <c r="N51" s="4" t="s">
         <v>8</v>
@@ -51299,7 +51310,7 @@
         <v>311</v>
       </c>
       <c r="C52" t="s">
-        <v>680</v>
+        <v>610</v>
       </c>
       <c r="D52" s="30" t="s">
         <v>317</v>
@@ -51316,16 +51327,16 @@
       <c r="H52" s="7"/>
       <c r="I52" s="7"/>
       <c r="J52" s="38" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="K52" s="8" t="s">
-        <v>642</v>
+        <v>672</v>
       </c>
       <c r="L52" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>635</v>
+        <v>588</v>
       </c>
       <c r="N52" s="4" t="s">
         <v>8</v>
@@ -51370,16 +51381,16 @@
       <c r="H53" s="7"/>
       <c r="I53" s="7"/>
       <c r="J53" s="38" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="K53" s="8" t="s">
-        <v>643</v>
+        <v>673</v>
       </c>
       <c r="L53" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>604</v>
+        <v>578</v>
       </c>
       <c r="N53" s="4" t="s">
         <v>8</v>
@@ -51424,16 +51435,16 @@
       <c r="H54" s="7"/>
       <c r="I54" s="7"/>
       <c r="J54" s="38" t="s">
-        <v>630</v>
+        <v>583</v>
       </c>
       <c r="K54" s="8" t="s">
-        <v>644</v>
+        <v>674</v>
       </c>
       <c r="L54" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>604</v>
+        <v>578</v>
       </c>
       <c r="N54" s="4" t="s">
         <v>8</v>
@@ -51478,16 +51489,16 @@
       <c r="H55" s="7"/>
       <c r="I55" s="7"/>
       <c r="J55" s="38" t="s">
-        <v>631</v>
+        <v>584</v>
       </c>
       <c r="K55" s="8" t="s">
-        <v>645</v>
+        <v>675</v>
       </c>
       <c r="L55" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M55" s="4" t="s">
-        <v>604</v>
+        <v>578</v>
       </c>
       <c r="N55" s="4" t="s">
         <v>8</v>
@@ -51515,7 +51526,7 @@
         <v>311</v>
       </c>
       <c r="C56" t="s">
-        <v>682</v>
+        <v>612</v>
       </c>
       <c r="D56" s="30" t="s">
         <v>333</v>
@@ -51532,16 +51543,16 @@
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
       <c r="J56" s="38" t="s">
-        <v>632</v>
+        <v>585</v>
       </c>
       <c r="K56" s="8" t="s">
-        <v>646</v>
+        <v>676</v>
       </c>
       <c r="L56" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M56" s="4" t="s">
-        <v>604</v>
+        <v>578</v>
       </c>
       <c r="N56" s="4" t="s">
         <v>8</v>
@@ -51569,7 +51580,7 @@
         <v>311</v>
       </c>
       <c r="C57" t="s">
-        <v>679</v>
+        <v>609</v>
       </c>
       <c r="D57" s="30" t="s">
         <v>336</v>
@@ -51586,16 +51597,16 @@
       <c r="H57" s="7"/>
       <c r="I57" s="7"/>
       <c r="J57" s="38" t="s">
-        <v>633</v>
+        <v>586</v>
       </c>
       <c r="K57" s="8" t="s">
-        <v>647</v>
+        <v>677</v>
       </c>
       <c r="L57" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>604</v>
+        <v>578</v>
       </c>
       <c r="N57" s="4" t="s">
         <v>8</v>
@@ -51615,33 +51626,33 @@
       <c r="AA57" s="5"/>
       <c r="AB57" s="5"/>
     </row>
-    <row r="58" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A58" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B58" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C58" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>592</v>
+        <v>571</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>593</v>
+        <v>572</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H58" s="10"/>
       <c r="I58" s="7"/>
       <c r="J58" s="7"/>
       <c r="K58" s="1" t="s">
-        <v>361</v>
+        <v>678</v>
       </c>
       <c r="L58" s="12"/>
       <c r="M58" s="4" t="s">
@@ -51651,7 +51662,7 @@
         <v>13</v>
       </c>
       <c r="O58" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="P58" s="5"/>
       <c r="Q58" s="5"/>
@@ -51672,31 +51683,31 @@
         <v>310</v>
       </c>
       <c r="B59" t="s">
+        <v>360</v>
+      </c>
+      <c r="C59" t="s">
+        <v>361</v>
+      </c>
+      <c r="D59" t="s">
+        <v>365</v>
+      </c>
+      <c r="E59" t="s">
+        <v>364</v>
+      </c>
+      <c r="F59" t="s">
+        <v>363</v>
+      </c>
+      <c r="G59" s="10" t="s">
         <v>362</v>
-      </c>
-      <c r="C59" t="s">
-        <v>363</v>
-      </c>
-      <c r="D59" t="s">
-        <v>367</v>
-      </c>
-      <c r="E59" t="s">
-        <v>366</v>
-      </c>
-      <c r="F59" t="s">
-        <v>365</v>
-      </c>
-      <c r="G59" s="10" t="s">
-        <v>364</v>
       </c>
       <c r="H59" s="10"/>
       <c r="I59" s="7"/>
       <c r="J59" s="7"/>
       <c r="K59" s="1" t="s">
-        <v>368</v>
+        <v>679</v>
       </c>
       <c r="L59" s="12" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="M59" s="4" t="s">
         <v>4</v>
@@ -51719,33 +51730,33 @@
       <c r="AA59" s="5"/>
       <c r="AB59" s="5"/>
     </row>
-    <row r="60" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A60" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B60" t="s">
+        <v>367</v>
+      </c>
+      <c r="C60" t="s">
+        <v>368</v>
+      </c>
+      <c r="D60" t="s">
+        <v>372</v>
+      </c>
+      <c r="E60" t="s">
+        <v>371</v>
+      </c>
+      <c r="F60" s="7" t="s">
         <v>370</v>
       </c>
-      <c r="C60" t="s">
-        <v>371</v>
-      </c>
-      <c r="D60" t="s">
-        <v>376</v>
-      </c>
-      <c r="E60" t="s">
-        <v>375</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>374</v>
-      </c>
       <c r="G60" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="H60" s="7"/>
       <c r="I60" s="7"/>
       <c r="J60" s="7"/>
       <c r="K60" s="8" t="s">
-        <v>372</v>
+        <v>627</v>
       </c>
       <c r="L60" s="4"/>
       <c r="M60" s="4" t="s">
@@ -51755,7 +51766,7 @@
         <v>13</v>
       </c>
       <c r="O60" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="P60" s="5"/>
       <c r="Q60" s="5"/>
@@ -51776,20 +51787,20 @@
         <v>310</v>
       </c>
       <c r="B61" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C61" s="10"/>
       <c r="D61" s="10" t="s">
-        <v>650</v>
+        <v>589</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="H61" s="10" t="s">
         <v>188</v>
@@ -51797,7 +51808,7 @@
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
       <c r="K61" s="8" t="s">
-        <v>381</v>
+        <v>680</v>
       </c>
       <c r="L61" s="11" t="s">
         <v>11</v>
@@ -51823,33 +51834,33 @@
       <c r="AA61" s="5"/>
       <c r="AB61" s="5"/>
     </row>
-    <row r="62" spans="1:28" ht="101" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A62" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B62" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="C62" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D62" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="E62" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="G62" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="H62" s="7"/>
       <c r="I62" s="7"/>
       <c r="J62" s="7"/>
       <c r="K62" s="8" t="s">
-        <v>386</v>
+        <v>629</v>
       </c>
       <c r="L62" s="4"/>
       <c r="M62" s="4" t="s">
@@ -51859,7 +51870,7 @@
         <v>13</v>
       </c>
       <c r="O62" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="P62" s="5"/>
       <c r="Q62" s="5"/>
@@ -51880,36 +51891,36 @@
         <v>310</v>
       </c>
       <c r="B63" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="C63" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="H63" s="10"/>
       <c r="I63" s="7"/>
       <c r="J63" s="38" t="s">
-        <v>624</v>
+        <v>580</v>
       </c>
       <c r="K63" s="8" t="s">
-        <v>648</v>
+        <v>681</v>
       </c>
       <c r="L63" s="11" t="s">
         <v>11</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>604</v>
+        <v>578</v>
       </c>
       <c r="N63" s="4" t="s">
         <v>8</v>
@@ -51934,36 +51945,36 @@
         <v>310</v>
       </c>
       <c r="B64" t="s">
+        <v>381</v>
+      </c>
+      <c r="C64" t="s">
+        <v>613</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>389</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="F64" s="10" t="s">
         <v>387</v>
       </c>
-      <c r="C64" t="s">
-        <v>683</v>
-      </c>
-      <c r="D64" s="10" t="s">
-        <v>395</v>
-      </c>
-      <c r="E64" s="10" t="s">
-        <v>394</v>
-      </c>
-      <c r="F64" s="10" t="s">
-        <v>393</v>
-      </c>
       <c r="G64" s="10" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="H64" s="10"/>
       <c r="I64" s="7"/>
       <c r="J64" s="38" t="s">
-        <v>633</v>
+        <v>586</v>
       </c>
       <c r="K64" s="8" t="s">
-        <v>649</v>
+        <v>682</v>
       </c>
       <c r="L64" s="11" t="s">
         <v>11</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>604</v>
+        <v>578</v>
       </c>
       <c r="N64" s="4" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
2225 tidy up SUBGROUP column
</commit_message>
<xml_diff>
--- a/inst/adlb_grading/adlb_grading_spec.xlsx
+++ b/inst/adlb_grading/adlb_grading_spec.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\millerg1\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\millerg1\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="6090" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="6090" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NCICTCAEv4" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1640" uniqueCount="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="685">
   <si>
     <t>Anemia</t>
   </si>
@@ -1024,9 +1024,6 @@
     <t>Absolute Lymphocyte Count, Low</t>
   </si>
   <si>
-    <t>&gt; 5 years of age (not HIV infected)</t>
-  </si>
-  <si>
     <t>&lt;350/mm3; &lt;0.350 x 10e9 /L</t>
   </si>
   <si>
@@ -1070,9 +1067,6 @@
   </si>
   <si>
     <t>PTT, High</t>
-  </si>
-  <si>
-    <t>not on anticoagulation therapy</t>
   </si>
   <si>
     <t>&gt;=3.00 x ULN</t>
@@ -2955,6 +2949,9 @@
 !is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig) &amp; signif(AVAL, signif_dig) &lt;= signif(BASE, signif_dig) ~ "0"
 )</t>
   </si>
+  <si>
+    <t>&gt; 5 years of age</t>
+  </si>
 </sst>
 </file>
 
@@ -3532,7 +3529,7 @@
         <v>182</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>2</v>
@@ -3584,7 +3581,7 @@
         <v>11</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>10</v>
@@ -3636,7 +3633,7 @@
         <v>186</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
@@ -3686,7 +3683,7 @@
         <v>23</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
@@ -3736,7 +3733,7 @@
         <v>27</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
@@ -3786,7 +3783,7 @@
         <v>29</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4" t="s">
@@ -3836,7 +3833,7 @@
         <v>34</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="4" t="s">
@@ -3886,7 +3883,7 @@
         <v>39</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>10</v>
@@ -3938,7 +3935,7 @@
         <v>46</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="J10" s="14" t="s">
         <v>42</v>
@@ -3990,7 +3987,7 @@
         <v>51</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="4" t="s">
@@ -4040,7 +4037,7 @@
         <v>58</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="4" t="s">
@@ -4090,7 +4087,7 @@
         <v>63</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>2</v>
@@ -4142,7 +4139,7 @@
         <v>65</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="4" t="s">
@@ -4192,7 +4189,7 @@
         <v>68</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="J15" s="12"/>
       <c r="K15" s="4" t="s">
@@ -4242,7 +4239,7 @@
         <v>190</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>2</v>
@@ -4294,7 +4291,7 @@
         <v>77</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="J17" s="12"/>
       <c r="K17" s="4" t="s">
@@ -4346,7 +4343,7 @@
         <v>82</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="J18" s="12"/>
       <c r="K18" s="4" t="s">
@@ -4396,7 +4393,7 @@
         <v>86</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="J19" s="11" t="s">
         <v>10</v>
@@ -4448,7 +4445,7 @@
         <v>192</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="J20" s="11" t="s">
         <v>10</v>
@@ -4500,7 +4497,7 @@
         <v>95</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="J21" s="11" t="s">
         <v>10</v>
@@ -4552,7 +4549,7 @@
         <v>101</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="J22" s="11" t="s">
         <v>10</v>
@@ -4604,7 +4601,7 @@
         <v>103</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="J23" s="12"/>
       <c r="K23" s="4" t="s">
@@ -4654,7 +4651,7 @@
         <v>109</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="J24" s="11" t="s">
         <v>10</v>
@@ -4706,7 +4703,7 @@
         <v>198</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="J25" s="17" t="s">
         <v>212</v>
@@ -4760,7 +4757,7 @@
         <v>198</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="J26" s="17" t="s">
         <v>212</v>
@@ -4814,7 +4811,7 @@
         <v>199</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="J27" s="17" t="s">
         <v>212</v>
@@ -4868,7 +4865,7 @@
         <v>199</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="J28" s="17" t="s">
         <v>212</v>
@@ -4922,7 +4919,7 @@
         <v>200</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="J29" s="17" t="s">
         <v>212</v>
@@ -4974,7 +4971,7 @@
         <v>201</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="J30" s="17" t="s">
         <v>212</v>
@@ -5026,7 +5023,7 @@
         <v>202</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="J31" s="17" t="s">
         <v>212</v>
@@ -5078,7 +5075,7 @@
         <v>203</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="J32" s="17" t="s">
         <v>212</v>
@@ -5130,7 +5127,7 @@
         <v>204</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="J33" s="17" t="s">
         <v>219</v>
@@ -5184,7 +5181,7 @@
         <v>205</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="J34" s="17" t="s">
         <v>2</v>
@@ -5236,7 +5233,7 @@
         <v>206</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="J35" s="17" t="s">
         <v>212</v>
@@ -5290,7 +5287,7 @@
         <v>206</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="J36" s="17" t="s">
         <v>212</v>
@@ -5344,7 +5341,7 @@
         <v>207</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="J37" s="17" t="s">
         <v>212</v>
@@ -5396,7 +5393,7 @@
         <v>208</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="J38" s="17" t="s">
         <v>212</v>
@@ -5450,7 +5447,7 @@
         <v>209</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="J39" s="17" t="s">
         <v>212</v>
@@ -5502,7 +5499,7 @@
         <v>210</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="J40" s="17" t="s">
         <v>212</v>
@@ -5554,7 +5551,7 @@
         <v>211</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="J41" s="17" t="s">
         <v>212</v>
@@ -26138,7 +26135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z972"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -26233,7 +26230,7 @@
         <v>182</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>2</v>
@@ -26285,7 +26282,7 @@
         <v>11</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>10</v>
@@ -26337,7 +26334,7 @@
         <v>186</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
@@ -26387,7 +26384,7 @@
         <v>23</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
@@ -26437,7 +26434,7 @@
         <v>27</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
@@ -26487,7 +26484,7 @@
         <v>29</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4" t="s">
@@ -26537,7 +26534,7 @@
         <v>34</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="4" t="s">
@@ -26587,7 +26584,7 @@
         <v>39</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>10</v>
@@ -26639,7 +26636,7 @@
         <v>46</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="J10" s="14" t="s">
         <v>42</v>
@@ -26691,7 +26688,7 @@
         <v>51</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="4" t="s">
@@ -26741,7 +26738,7 @@
         <v>58</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="4" t="s">
@@ -26791,7 +26788,7 @@
         <v>63</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>2</v>
@@ -26843,7 +26840,7 @@
         <v>65</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="4" t="s">
@@ -26893,7 +26890,7 @@
         <v>68</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="J15" s="12"/>
       <c r="K15" s="4" t="s">
@@ -26943,7 +26940,7 @@
         <v>247</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>2</v>
@@ -26995,7 +26992,7 @@
         <v>77</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="J17" s="12"/>
       <c r="K17" s="4" t="s">
@@ -27047,7 +27044,7 @@
         <v>82</v>
       </c>
       <c r="I18" s="26" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="J18" s="27"/>
       <c r="K18" s="27" t="s">
@@ -27099,7 +27096,7 @@
         <v>86</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="J19" s="11" t="s">
         <v>10</v>
@@ -27151,7 +27148,7 @@
         <v>192</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="J20" s="11" t="s">
         <v>10</v>
@@ -27203,7 +27200,7 @@
         <v>95</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="J21" s="11" t="s">
         <v>10</v>
@@ -27255,7 +27252,7 @@
         <v>101</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="J22" s="11" t="s">
         <v>10</v>
@@ -27307,7 +27304,7 @@
         <v>103</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="J23" s="12"/>
       <c r="K23" s="4" t="s">
@@ -27359,7 +27356,7 @@
         <v>109</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="J24" s="11" t="s">
         <v>10</v>
@@ -27411,7 +27408,7 @@
         <v>198</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="J25" s="17" t="s">
         <v>212</v>
@@ -27465,7 +27462,7 @@
         <v>198</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="J26" s="17" t="s">
         <v>212</v>
@@ -27519,7 +27516,7 @@
         <v>200</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="J27" s="17" t="s">
         <v>212</v>
@@ -27571,7 +27568,7 @@
         <v>201</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="J28" s="17" t="s">
         <v>212</v>
@@ -27623,7 +27620,7 @@
         <v>202</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="J29" s="17" t="s">
         <v>212</v>
@@ -27675,7 +27672,7 @@
         <v>203</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="J30" s="17" t="s">
         <v>212</v>
@@ -27727,7 +27724,7 @@
         <v>204</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="J31" s="17"/>
       <c r="K31" s="4" t="s">
@@ -27779,7 +27776,7 @@
         <v>205</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="J32" s="17" t="s">
         <v>2</v>
@@ -27831,7 +27828,7 @@
         <v>206</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="J33" s="17" t="s">
         <v>212</v>
@@ -27885,7 +27882,7 @@
         <v>206</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="J34" s="17" t="s">
         <v>212</v>
@@ -27939,7 +27936,7 @@
         <v>207</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="J35" s="17" t="s">
         <v>212</v>
@@ -27991,7 +27988,7 @@
         <v>208</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="J36" s="17" t="s">
         <v>212</v>
@@ -28045,7 +28042,7 @@
         <v>209</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="J37" s="17" t="s">
         <v>212</v>
@@ -28097,7 +28094,7 @@
         <v>210</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="J38" s="17" t="s">
         <v>212</v>
@@ -48683,8 +48680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB998"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -48708,7 +48705,7 @@
         <v>193</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>224</v>
@@ -48762,27 +48759,27 @@
     </row>
     <row r="2" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2"/>
       <c r="E2" t="s">
+        <v>542</v>
+      </c>
+      <c r="F2" t="s">
+        <v>543</v>
+      </c>
+      <c r="G2" t="s">
         <v>544</v>
-      </c>
-      <c r="F2" t="s">
-        <v>545</v>
-      </c>
-      <c r="G2" t="s">
-        <v>546</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="8" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L2" s="4"/>
       <c r="M2" s="4" t="s">
@@ -48792,7 +48789,7 @@
         <v>7</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
@@ -48810,27 +48807,27 @@
     </row>
     <row r="3" spans="1:28" ht="126" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="G3" s="32"/>
       <c r="H3" s="10"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="8" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>2</v>
@@ -48858,29 +48855,29 @@
     </row>
     <row r="4" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B4" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="31" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G4" s="32" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="8" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4" t="s">
@@ -48906,27 +48903,27 @@
     </row>
     <row r="5" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B5" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5"/>
       <c r="E5" t="s">
+        <v>547</v>
+      </c>
+      <c r="F5" t="s">
+        <v>548</v>
+      </c>
+      <c r="G5" t="s">
         <v>549</v>
-      </c>
-      <c r="F5" t="s">
-        <v>550</v>
-      </c>
-      <c r="G5" t="s">
-        <v>551</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="4" t="s">
@@ -48936,7 +48933,7 @@
         <v>12</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
@@ -48954,29 +48951,29 @@
     </row>
     <row r="6" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B6" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="8" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4" t="s">
@@ -49002,29 +48999,29 @@
     </row>
     <row r="7" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B7" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="33" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="G7" s="33" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="L7" s="12"/>
       <c r="M7" s="4" t="s">
@@ -49050,29 +49047,29 @@
     </row>
     <row r="8" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B8" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="8" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4" t="s">
@@ -49098,29 +49095,29 @@
     </row>
     <row r="9" spans="1:28" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B9" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="8" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>42</v>
@@ -49148,39 +49145,39 @@
     </row>
     <row r="10" spans="1:28" s="44" customFormat="1" ht="101" x14ac:dyDescent="0.35">
       <c r="A10" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="32"/>
       <c r="F10" s="37" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="H10" s="36"/>
       <c r="I10" s="38"/>
       <c r="J10" s="38" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="K10" s="39" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="L10" s="40"/>
       <c r="M10" s="4" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="N10" s="41" t="s">
         <v>12</v>
       </c>
       <c r="O10" s="37" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="P10" s="43"/>
       <c r="Q10" s="43"/>
@@ -49198,44 +49195,44 @@
     </row>
     <row r="11" spans="1:28" s="44" customFormat="1" ht="151" x14ac:dyDescent="0.35">
       <c r="A11" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B11" s="37" t="s">
+        <v>361</v>
+      </c>
+      <c r="C11" s="37" t="s">
         <v>363</v>
       </c>
-      <c r="C11" s="37" t="s">
-        <v>365</v>
-      </c>
       <c r="D11" s="32" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F11" s="32" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="G11" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="H11"/>
       <c r="J11" s="38" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="K11" s="39" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="L11" s="40" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="N11" s="41" t="s">
         <v>12</v>
       </c>
       <c r="O11" s="42" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="P11" s="43"/>
       <c r="Q11" s="43"/>
@@ -49253,37 +49250,37 @@
     </row>
     <row r="12" spans="1:28" s="44" customFormat="1" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A12" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B12" t="s">
+        <v>371</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>362</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>374</v>
+      </c>
+      <c r="E12" s="34" t="s">
         <v>373</v>
       </c>
-      <c r="C12" s="37" t="s">
-        <v>364</v>
-      </c>
-      <c r="D12" s="33" t="s">
-        <v>376</v>
-      </c>
-      <c r="E12" s="34" t="s">
-        <v>375</v>
-      </c>
       <c r="F12" s="33" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="G12" s="33" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="H12" s="36"/>
       <c r="I12" s="38"/>
       <c r="J12" s="38" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="L12" s="40"/>
       <c r="M12" s="4" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="N12" s="41" t="s">
         <v>12</v>
@@ -49305,13 +49302,13 @@
     </row>
     <row r="13" spans="1:28" s="44" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B13" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D13" s="33"/>
       <c r="E13" s="34"/>
@@ -49320,20 +49317,20 @@
       <c r="H13" s="36"/>
       <c r="I13" s="38"/>
       <c r="J13" s="38" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="L13" s="40"/>
       <c r="M13" s="4" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="N13" s="41" t="s">
         <v>12</v>
       </c>
       <c r="O13" s="37" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="P13" s="43"/>
       <c r="Q13" s="43"/>
@@ -49351,39 +49348,39 @@
     </row>
     <row r="14" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A14" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B14" s="15" t="s">
+        <v>380</v>
+      </c>
+      <c r="C14" t="s">
+        <v>558</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="E14" s="19" t="s">
         <v>382</v>
       </c>
-      <c r="C14" t="s">
-        <v>560</v>
-      </c>
-      <c r="D14" s="19" t="s">
+      <c r="F14" s="19" t="s">
         <v>383</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="G14" s="19" t="s">
         <v>384</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>385</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>386</v>
       </c>
       <c r="H14" s="19"/>
       <c r="I14" s="18"/>
       <c r="J14" s="38" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="L14" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N14" s="4" t="s">
         <v>12</v>
@@ -49405,39 +49402,39 @@
     </row>
     <row r="15" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A15" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C15" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="18"/>
       <c r="J15" s="38" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="L15" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>12</v>
@@ -49459,29 +49456,29 @@
     </row>
     <row r="16" spans="1:28" ht="138" x14ac:dyDescent="0.3">
       <c r="A16" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="19" t="s">
+        <v>376</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>379</v>
+      </c>
+      <c r="F16" s="19" t="s">
         <v>378</v>
       </c>
-      <c r="E16" s="19" t="s">
-        <v>381</v>
-      </c>
-      <c r="F16" s="19" t="s">
-        <v>380</v>
-      </c>
       <c r="G16" s="19" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
       <c r="K16" s="1" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="L16" s="14" t="s">
         <v>42</v>
@@ -49509,39 +49506,39 @@
     </row>
     <row r="17" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A17" s="45" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B17" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C17" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="D17" t="s">
+        <v>393</v>
+      </c>
+      <c r="E17" t="s">
+        <v>394</v>
+      </c>
+      <c r="F17" t="s">
         <v>395</v>
       </c>
-      <c r="E17" t="s">
+      <c r="G17" t="s">
         <v>396</v>
-      </c>
-      <c r="F17" t="s">
-        <v>397</v>
-      </c>
-      <c r="G17" t="s">
-        <v>398</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="18"/>
       <c r="J17" s="38" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="L17" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>7</v>
@@ -49563,39 +49560,39 @@
     </row>
     <row r="18" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A18" s="45" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B18" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C18" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D18" t="s">
+        <v>397</v>
+      </c>
+      <c r="E18" t="s">
+        <v>398</v>
+      </c>
+      <c r="F18" t="s">
         <v>399</v>
       </c>
-      <c r="E18" t="s">
+      <c r="G18" t="s">
         <v>400</v>
-      </c>
-      <c r="F18" t="s">
-        <v>401</v>
-      </c>
-      <c r="G18" t="s">
-        <v>402</v>
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="18"/>
       <c r="J18" s="38" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="L18" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N18" s="4" t="s">
         <v>7</v>
@@ -49617,29 +49614,29 @@
     </row>
     <row r="19" spans="1:28" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A19" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B19" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
+        <v>389</v>
+      </c>
+      <c r="E19" t="s">
+        <v>390</v>
+      </c>
+      <c r="F19" t="s">
         <v>391</v>
       </c>
-      <c r="E19" t="s">
+      <c r="G19" t="s">
         <v>392</v>
-      </c>
-      <c r="F19" t="s">
-        <v>393</v>
-      </c>
-      <c r="G19" t="s">
-        <v>394</v>
       </c>
       <c r="H19" s="19"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="1" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="L19" s="14" t="s">
         <v>42</v>
@@ -49667,29 +49664,29 @@
     </row>
     <row r="20" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A20" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B20" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="1" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="L20" s="12"/>
       <c r="M20" s="4" t="s">
@@ -49715,29 +49712,29 @@
     </row>
     <row r="21" spans="1:28" ht="251" x14ac:dyDescent="0.35">
       <c r="A21" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B21" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="E21" t="s">
+        <v>408</v>
+      </c>
+      <c r="F21" t="s">
         <v>409</v>
       </c>
-      <c r="E21" t="s">
-        <v>410</v>
-      </c>
-      <c r="F21" t="s">
-        <v>411</v>
-      </c>
       <c r="G21" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="H21" s="10"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
       <c r="K21" s="1" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="L21" s="12"/>
       <c r="M21" s="4" t="s">
@@ -49763,29 +49760,29 @@
     </row>
     <row r="22" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A22" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B22" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C22" s="16"/>
       <c r="D22" t="s">
+        <v>411</v>
+      </c>
+      <c r="E22" t="s">
+        <v>412</v>
+      </c>
+      <c r="F22" t="s">
         <v>413</v>
       </c>
-      <c r="E22" t="s">
-        <v>414</v>
-      </c>
-      <c r="F22" t="s">
-        <v>415</v>
-      </c>
       <c r="G22" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="18"/>
       <c r="J22" s="18"/>
       <c r="K22" s="1" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="L22" s="14" t="s">
         <v>42</v>
@@ -49813,29 +49810,29 @@
     </row>
     <row r="23" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A23" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B23" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C23" s="16"/>
       <c r="D23" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E23" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F23" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="G23" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="H23" s="20"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="K23" s="1" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="L23" s="14" t="s">
         <v>42</v>
@@ -49863,39 +49860,39 @@
     </row>
     <row r="24" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A24" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B24" t="s">
+        <v>417</v>
+      </c>
+      <c r="C24" t="s">
+        <v>418</v>
+      </c>
+      <c r="D24" t="s">
         <v>419</v>
       </c>
-      <c r="C24" t="s">
+      <c r="E24" t="s">
         <v>420</v>
       </c>
-      <c r="D24" t="s">
+      <c r="F24" t="s">
         <v>421</v>
       </c>
-      <c r="E24" t="s">
+      <c r="G24" t="s">
         <v>422</v>
-      </c>
-      <c r="F24" t="s">
-        <v>423</v>
-      </c>
-      <c r="G24" t="s">
-        <v>424</v>
       </c>
       <c r="H24" s="20"/>
       <c r="I24" s="18"/>
       <c r="J24" s="38" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="L24" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="N24" s="4" t="s">
         <v>7</v>
@@ -49917,39 +49914,39 @@
     </row>
     <row r="25" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A25" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B25" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C25" s="30" t="s">
+        <v>423</v>
+      </c>
+      <c r="D25" s="30" t="s">
         <v>425</v>
       </c>
-      <c r="D25" s="30" t="s">
-        <v>427</v>
-      </c>
       <c r="E25" s="30" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="F25" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="G25" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="H25" s="20"/>
       <c r="I25" s="18"/>
       <c r="J25" s="38" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="L25" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="N25" s="4" t="s">
         <v>7</v>
@@ -49971,28 +49968,28 @@
     </row>
     <row r="26" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A26" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B26" s="30" t="s">
+        <v>426</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>427</v>
+      </c>
+      <c r="E26" s="30" t="s">
         <v>428</v>
       </c>
-      <c r="D26" s="30" t="s">
+      <c r="F26" s="35" t="s">
         <v>429</v>
       </c>
-      <c r="E26" s="30" t="s">
+      <c r="G26" s="30" t="s">
         <v>430</v>
-      </c>
-      <c r="F26" s="35" t="s">
-        <v>431</v>
-      </c>
-      <c r="G26" s="30" t="s">
-        <v>432</v>
       </c>
       <c r="H26" s="20"/>
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
       <c r="K26" s="1" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="L26" s="14"/>
       <c r="M26" s="4" t="s">
@@ -50002,7 +49999,7 @@
         <v>12</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
@@ -50020,29 +50017,29 @@
     </row>
     <row r="27" spans="1:28" s="29" customFormat="1" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A27" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C27" s="17"/>
       <c r="D27" s="30" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F27" s="33" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="H27" s="17"/>
       <c r="I27" s="17"/>
       <c r="J27" s="17"/>
       <c r="K27" s="26" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="L27" s="27"/>
       <c r="M27" s="27" t="s">
@@ -50068,37 +50065,37 @@
     </row>
     <row r="28" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A28" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B28" t="s">
+        <v>436</v>
+      </c>
+      <c r="C28" t="s">
+        <v>437</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>440</v>
+      </c>
+      <c r="E28" s="30" t="s">
+        <v>439</v>
+      </c>
+      <c r="F28" s="10" t="s">
         <v>438</v>
-      </c>
-      <c r="C28" t="s">
-        <v>439</v>
-      </c>
-      <c r="D28" s="30" t="s">
-        <v>442</v>
-      </c>
-      <c r="E28" s="30" t="s">
-        <v>441</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>440</v>
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
       <c r="I28" s="7"/>
       <c r="J28" s="38" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="L28" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>12</v>
@@ -50120,37 +50117,37 @@
     </row>
     <row r="29" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A29" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B29" t="s">
+        <v>436</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>441</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>443</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>442</v>
+      </c>
+      <c r="F29" s="10" t="s">
         <v>438</v>
-      </c>
-      <c r="C29" s="30" t="s">
-        <v>443</v>
-      </c>
-      <c r="D29" s="30" t="s">
-        <v>445</v>
-      </c>
-      <c r="E29" s="30" t="s">
-        <v>444</v>
-      </c>
-      <c r="F29" s="10" t="s">
-        <v>440</v>
       </c>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
       <c r="I29" s="7"/>
       <c r="J29" s="38" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="L29" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="N29" s="4" t="s">
         <v>12</v>
@@ -50172,37 +50169,37 @@
     </row>
     <row r="30" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A30" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B30" s="30" t="s">
+        <v>444</v>
+      </c>
+      <c r="C30" t="s">
+        <v>437</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>445</v>
+      </c>
+      <c r="E30" s="30" t="s">
         <v>446</v>
       </c>
-      <c r="C30" t="s">
-        <v>439</v>
-      </c>
-      <c r="D30" s="30" t="s">
+      <c r="F30" s="30" t="s">
         <v>447</v>
-      </c>
-      <c r="E30" s="30" t="s">
-        <v>448</v>
-      </c>
-      <c r="F30" s="30" t="s">
-        <v>449</v>
       </c>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
       <c r="I30" s="7"/>
       <c r="J30" s="38" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="L30" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="N30" s="4" t="s">
         <v>12</v>
@@ -50224,37 +50221,37 @@
     </row>
     <row r="31" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A31" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C31" s="30" t="s">
+        <v>448</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>449</v>
+      </c>
+      <c r="E31" s="30" t="s">
         <v>450</v>
       </c>
-      <c r="D31" s="30" t="s">
-        <v>451</v>
-      </c>
-      <c r="E31" s="30" t="s">
-        <v>452</v>
-      </c>
       <c r="F31" s="30" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
       <c r="I31" s="7"/>
       <c r="J31" s="38" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="K31" s="8" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="L31" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="N31" s="4" t="s">
         <v>12</v>
@@ -50276,13 +50273,13 @@
     </row>
     <row r="32" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A32" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C32" s="47" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="D32" s="30"/>
       <c r="E32" s="30"/>
@@ -50291,22 +50288,22 @@
       <c r="H32" s="10"/>
       <c r="I32" s="7"/>
       <c r="J32" s="38" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="L32" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="N32" s="4" t="s">
         <v>12</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
@@ -50324,29 +50321,29 @@
     </row>
     <row r="33" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A33" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C33" s="16"/>
       <c r="D33" s="30" t="s">
+        <v>452</v>
+      </c>
+      <c r="E33" s="30" t="s">
+        <v>453</v>
+      </c>
+      <c r="F33" s="30" t="s">
         <v>454</v>
       </c>
-      <c r="E33" s="30" t="s">
+      <c r="G33" s="30" t="s">
         <v>455</v>
-      </c>
-      <c r="F33" s="30" t="s">
-        <v>456</v>
-      </c>
-      <c r="G33" s="30" t="s">
-        <v>457</v>
       </c>
       <c r="H33" s="20"/>
       <c r="I33" s="18"/>
       <c r="J33" s="18"/>
       <c r="K33" s="1" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="L33" s="14" t="s">
         <v>42</v>
@@ -50374,29 +50371,29 @@
     </row>
     <row r="34" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A34" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C34" s="16"/>
       <c r="D34" s="30" t="s">
+        <v>457</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>458</v>
+      </c>
+      <c r="F34" s="30" t="s">
         <v>459</v>
       </c>
-      <c r="E34" s="30" t="s">
+      <c r="G34" s="30" t="s">
         <v>460</v>
-      </c>
-      <c r="F34" s="30" t="s">
-        <v>461</v>
-      </c>
-      <c r="G34" s="30" t="s">
-        <v>462</v>
       </c>
       <c r="H34" s="20"/>
       <c r="I34" s="18"/>
       <c r="J34" s="18"/>
       <c r="K34" s="1" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L34" s="14" t="s">
         <v>42</v>
@@ -50424,39 +50421,39 @@
     </row>
     <row r="35" spans="1:28" ht="151" x14ac:dyDescent="0.35">
       <c r="A35" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B35" s="30" t="s">
+        <v>461</v>
+      </c>
+      <c r="C35" s="30" t="s">
+        <v>462</v>
+      </c>
+      <c r="D35" s="30" t="s">
         <v>463</v>
       </c>
-      <c r="C35" s="30" t="s">
+      <c r="E35" s="30" t="s">
         <v>464</v>
       </c>
-      <c r="D35" s="30" t="s">
+      <c r="F35" s="30" t="s">
         <v>465</v>
       </c>
-      <c r="E35" s="30" t="s">
+      <c r="G35" s="30" t="s">
         <v>466</v>
-      </c>
-      <c r="F35" s="30" t="s">
-        <v>467</v>
-      </c>
-      <c r="G35" s="30" t="s">
-        <v>468</v>
       </c>
       <c r="H35" s="20"/>
       <c r="I35" s="18"/>
       <c r="J35" s="38" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="L35" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>7</v>
@@ -50478,39 +50475,39 @@
     </row>
     <row r="36" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A36" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C36" s="30" t="s">
+        <v>467</v>
+      </c>
+      <c r="D36" s="30" t="s">
+        <v>471</v>
+      </c>
+      <c r="E36" s="30" t="s">
+        <v>470</v>
+      </c>
+      <c r="F36" s="30" t="s">
         <v>469</v>
       </c>
-      <c r="D36" s="30" t="s">
-        <v>473</v>
-      </c>
-      <c r="E36" s="30" t="s">
-        <v>472</v>
-      </c>
-      <c r="F36" s="30" t="s">
-        <v>471</v>
-      </c>
       <c r="G36" s="30" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="H36" s="20"/>
       <c r="I36" s="18"/>
       <c r="J36" s="38" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="L36" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="N36" s="4" t="s">
         <v>7</v>
@@ -50532,39 +50529,39 @@
     </row>
     <row r="37" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A37" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B37" s="30" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C37" s="30" t="s">
+        <v>472</v>
+      </c>
+      <c r="D37" s="30" t="s">
         <v>474</v>
       </c>
-      <c r="D37" s="30" t="s">
-        <v>476</v>
-      </c>
       <c r="E37" s="30" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="F37" s="30" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="G37" s="30" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="H37" s="20"/>
       <c r="I37" s="18"/>
       <c r="J37" s="38" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L37" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="N37" s="4" t="s">
         <v>7</v>
@@ -50586,29 +50583,29 @@
     </row>
     <row r="38" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A38" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B38" s="30" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C38" s="30"/>
       <c r="D38" s="30" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F38" s="30" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="G38" s="30" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="H38" s="20"/>
       <c r="I38" s="18"/>
       <c r="J38" s="18"/>
       <c r="K38" s="1" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="L38" s="14" t="s">
         <v>42</v>
@@ -50636,29 +50633,29 @@
     </row>
     <row r="39" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A39" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B39" s="30" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C39" s="30"/>
       <c r="D39" s="30" t="s">
+        <v>476</v>
+      </c>
+      <c r="E39" s="30" t="s">
+        <v>479</v>
+      </c>
+      <c r="F39" s="30" t="s">
         <v>478</v>
       </c>
-      <c r="E39" s="30" t="s">
-        <v>481</v>
-      </c>
-      <c r="F39" s="30" t="s">
-        <v>480</v>
-      </c>
       <c r="G39" s="30" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H39" s="20"/>
       <c r="I39" s="18"/>
       <c r="J39" s="18"/>
       <c r="K39" s="1" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="L39" s="14" t="s">
         <v>42</v>
@@ -50686,29 +50683,29 @@
     </row>
     <row r="40" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A40" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B40" s="30" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C40" s="16"/>
       <c r="D40" s="30" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="F40" s="30" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="G40" s="20" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="H40" s="20"/>
       <c r="I40" s="18"/>
       <c r="J40" s="18"/>
       <c r="K40" s="1" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="L40" s="14" t="s">
         <v>42</v>
@@ -50736,29 +50733,29 @@
     </row>
     <row r="41" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A41" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C41" s="16"/>
       <c r="D41" s="30" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="F41" s="30" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="G41" s="33" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="H41" s="20"/>
       <c r="I41" s="18"/>
       <c r="J41" s="18"/>
       <c r="K41" s="1" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="L41" s="14" t="s">
         <v>42</v>
@@ -50786,32 +50783,32 @@
     </row>
     <row r="42" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A42" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C42" s="15"/>
       <c r="D42" s="30" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="F42" s="30" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="G42" s="30" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="H42" s="19"/>
       <c r="I42" s="18"/>
       <c r="J42" s="18"/>
       <c r="K42" s="1" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="L42" s="14" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="M42" s="4" t="s">
         <v>4</v>
@@ -50820,7 +50817,7 @@
         <v>12</v>
       </c>
       <c r="O42" s="3" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="P42" s="5"/>
       <c r="Q42" s="5"/>
@@ -50841,42 +50838,42 @@
         <v>263</v>
       </c>
       <c r="B43" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C43" t="s">
-        <v>305</v>
+        <v>684</v>
       </c>
       <c r="D43" s="10" t="s">
+        <v>507</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>508</v>
+      </c>
+      <c r="F43" s="10" t="s">
         <v>509</v>
       </c>
-      <c r="E43" s="10" t="s">
+      <c r="G43" s="10" t="s">
         <v>510</v>
-      </c>
-      <c r="F43" s="10" t="s">
-        <v>511</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>512</v>
       </c>
       <c r="H43" s="10"/>
       <c r="I43" s="7"/>
       <c r="J43" s="38" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="L43" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N43" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O43" s="3" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="P43" s="5"/>
       <c r="Q43" s="5"/>
@@ -50897,10 +50894,10 @@
         <v>263</v>
       </c>
       <c r="B44" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C44" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
@@ -50909,22 +50906,22 @@
       <c r="H44" s="10"/>
       <c r="I44" s="7"/>
       <c r="J44" s="38" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="K44" s="8" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="L44" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N44" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O44" s="3" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="P44" s="5"/>
       <c r="Q44" s="5"/>
@@ -50948,39 +50945,39 @@
         <v>304</v>
       </c>
       <c r="C45" t="s">
+        <v>684</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>512</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="G45" s="7" t="s">
         <v>305</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>514</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>306</v>
       </c>
       <c r="H45" s="7"/>
       <c r="I45" s="7"/>
       <c r="J45" s="38" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="L45" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N45" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O45" s="3" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="P45" s="5"/>
       <c r="Q45" s="5"/>
@@ -51004,7 +51001,7 @@
         <v>304</v>
       </c>
       <c r="C46" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
@@ -51013,22 +51010,22 @@
       <c r="H46" s="7"/>
       <c r="I46" s="7"/>
       <c r="J46" s="38" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="K46" s="8" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="L46" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N46" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O46" s="3" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="P46" s="5"/>
       <c r="Q46" s="5"/>
@@ -51055,13 +51052,13 @@
         <v>299</v>
       </c>
       <c r="D47" s="10" t="s">
+        <v>513</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>514</v>
+      </c>
+      <c r="F47" s="10" t="s">
         <v>515</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>516</v>
-      </c>
-      <c r="F47" s="10" t="s">
-        <v>517</v>
       </c>
       <c r="G47" s="10" t="s">
         <v>300</v>
@@ -51071,16 +51068,16 @@
       </c>
       <c r="I47" s="7"/>
       <c r="J47" s="38" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K47" s="8" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="L47" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N47" s="4" t="s">
         <v>7</v>
@@ -51111,13 +51108,13 @@
         <v>301</v>
       </c>
       <c r="D48" s="10" t="s">
+        <v>516</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>517</v>
+      </c>
+      <c r="F48" s="10" t="s">
         <v>518</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>519</v>
-      </c>
-      <c r="F48" s="10" t="s">
-        <v>520</v>
       </c>
       <c r="G48" s="10" t="s">
         <v>302</v>
@@ -51127,16 +51124,16 @@
       </c>
       <c r="I48" s="7"/>
       <c r="J48" s="38" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K48" s="8" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="L48" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N48" s="4" t="s">
         <v>7</v>
@@ -51164,16 +51161,16 @@
         <v>298</v>
       </c>
       <c r="C49" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="D49" s="10" t="s">
+        <v>519</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>520</v>
+      </c>
+      <c r="F49" s="10" t="s">
         <v>521</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>522</v>
-      </c>
-      <c r="F49" s="10" t="s">
-        <v>523</v>
       </c>
       <c r="G49" s="10" t="s">
         <v>303</v>
@@ -51183,16 +51180,16 @@
       </c>
       <c r="I49" s="7"/>
       <c r="J49" s="38" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="L49" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N49" s="4" t="s">
         <v>7</v>
@@ -51238,7 +51235,7 @@
       <c r="I50" s="7"/>
       <c r="J50" s="7"/>
       <c r="K50" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="L50" s="4" t="s">
         <v>2</v>
@@ -51272,7 +51269,7 @@
         <v>264</v>
       </c>
       <c r="C51" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="D51" s="30" t="s">
         <v>266</v>
@@ -51289,16 +51286,16 @@
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
       <c r="J51" s="38" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="K51" s="8" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="L51" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="N51" s="4" t="s">
         <v>7</v>
@@ -51326,7 +51323,7 @@
         <v>264</v>
       </c>
       <c r="C52" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="D52" s="30" t="s">
         <v>270</v>
@@ -51343,16 +51340,16 @@
       <c r="H52" s="7"/>
       <c r="I52" s="7"/>
       <c r="J52" s="38" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="K52" s="8" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="L52" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="N52" s="4" t="s">
         <v>7</v>
@@ -51397,16 +51394,16 @@
       <c r="H53" s="7"/>
       <c r="I53" s="7"/>
       <c r="J53" s="38" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="K53" s="8" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="L53" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N53" s="4" t="s">
         <v>7</v>
@@ -51451,16 +51448,16 @@
       <c r="H54" s="7"/>
       <c r="I54" s="7"/>
       <c r="J54" s="38" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K54" s="8" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="L54" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N54" s="4" t="s">
         <v>7</v>
@@ -51505,16 +51502,16 @@
       <c r="H55" s="7"/>
       <c r="I55" s="7"/>
       <c r="J55" s="38" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K55" s="8" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="L55" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M55" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N55" s="4" t="s">
         <v>7</v>
@@ -51542,7 +51539,7 @@
         <v>264</v>
       </c>
       <c r="C56" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="D56" s="30" t="s">
         <v>286</v>
@@ -51559,16 +51556,16 @@
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
       <c r="J56" s="38" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="K56" s="8" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="L56" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M56" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N56" s="4" t="s">
         <v>7</v>
@@ -51596,7 +51593,7 @@
         <v>264</v>
       </c>
       <c r="C57" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="D57" s="30" t="s">
         <v>289</v>
@@ -51613,16 +51610,16 @@
       <c r="H57" s="7"/>
       <c r="I57" s="7"/>
       <c r="J57" s="38" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="K57" s="8" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="L57" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N57" s="4" t="s">
         <v>7</v>
@@ -51647,28 +51644,26 @@
         <v>263</v>
       </c>
       <c r="B58" t="s">
-        <v>310</v>
-      </c>
-      <c r="C58" t="s">
-        <v>321</v>
-      </c>
+        <v>309</v>
+      </c>
+      <c r="C58"/>
       <c r="D58" s="10" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H58" s="10"/>
       <c r="I58" s="7"/>
       <c r="J58" s="7"/>
       <c r="K58" s="1" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="L58" s="12"/>
       <c r="M58" s="4" t="s">
@@ -51678,7 +51673,7 @@
         <v>12</v>
       </c>
       <c r="O58" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="P58" s="5"/>
       <c r="Q58" s="5"/>
@@ -51699,31 +51694,29 @@
         <v>263</v>
       </c>
       <c r="B59" t="s">
-        <v>313</v>
-      </c>
-      <c r="C59" t="s">
+        <v>312</v>
+      </c>
+      <c r="C59"/>
+      <c r="D59" t="s">
+        <v>317</v>
+      </c>
+      <c r="E59" t="s">
+        <v>316</v>
+      </c>
+      <c r="F59" t="s">
+        <v>315</v>
+      </c>
+      <c r="G59" s="10" t="s">
         <v>314</v>
-      </c>
-      <c r="D59" t="s">
-        <v>318</v>
-      </c>
-      <c r="E59" t="s">
-        <v>317</v>
-      </c>
-      <c r="F59" t="s">
-        <v>316</v>
-      </c>
-      <c r="G59" s="10" t="s">
-        <v>315</v>
       </c>
       <c r="H59" s="10"/>
       <c r="I59" s="7"/>
       <c r="J59" s="7"/>
       <c r="K59" s="1" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="L59" s="12" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M59" s="4" t="s">
         <v>4</v>
@@ -51731,7 +51724,9 @@
       <c r="N59" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O59" s="3"/>
+      <c r="O59" s="3" t="s">
+        <v>313</v>
+      </c>
       <c r="P59" s="5"/>
       <c r="Q59" s="5"/>
       <c r="R59" s="5"/>
@@ -51751,28 +51746,26 @@
         <v>263</v>
       </c>
       <c r="B60" t="s">
+        <v>319</v>
+      </c>
+      <c r="C60"/>
+      <c r="D60" t="s">
+        <v>323</v>
+      </c>
+      <c r="E60" t="s">
+        <v>322</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="G60" t="s">
         <v>320</v>
-      </c>
-      <c r="C60" t="s">
-        <v>321</v>
-      </c>
-      <c r="D60" t="s">
-        <v>325</v>
-      </c>
-      <c r="E60" t="s">
-        <v>324</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="G60" t="s">
-        <v>322</v>
       </c>
       <c r="H60" s="7"/>
       <c r="I60" s="7"/>
       <c r="J60" s="7"/>
       <c r="K60" s="8" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="L60" s="4"/>
       <c r="M60" s="4" t="s">
@@ -51782,7 +51775,7 @@
         <v>12</v>
       </c>
       <c r="O60" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="P60" s="5"/>
       <c r="Q60" s="5"/>
@@ -51803,20 +51796,20 @@
         <v>263</v>
       </c>
       <c r="B61" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C61" s="10"/>
       <c r="D61" s="10" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="H61" s="10" t="s">
         <v>183</v>
@@ -51824,7 +51817,7 @@
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
       <c r="K61" s="8" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="L61" s="11" t="s">
         <v>10</v>
@@ -51855,28 +51848,26 @@
         <v>263</v>
       </c>
       <c r="B62" t="s">
+        <v>328</v>
+      </c>
+      <c r="C62"/>
+      <c r="D62" t="s">
+        <v>329</v>
+      </c>
+      <c r="E62" t="s">
         <v>330</v>
       </c>
-      <c r="C62" t="s">
-        <v>321</v>
-      </c>
-      <c r="D62" t="s">
+      <c r="F62" s="7" t="s">
         <v>331</v>
       </c>
-      <c r="E62" t="s">
-        <v>332</v>
-      </c>
-      <c r="F62" s="7" t="s">
-        <v>333</v>
-      </c>
       <c r="G62" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="H62" s="7"/>
       <c r="I62" s="7"/>
       <c r="J62" s="7"/>
       <c r="K62" s="8" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="L62" s="4"/>
       <c r="M62" s="4" t="s">
@@ -51886,7 +51877,7 @@
         <v>12</v>
       </c>
       <c r="O62" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="P62" s="5"/>
       <c r="Q62" s="5"/>
@@ -51907,36 +51898,36 @@
         <v>263</v>
       </c>
       <c r="B63" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C63" t="s">
         <v>299</v>
       </c>
       <c r="D63" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="G63" s="10" t="s">
         <v>336</v>
-      </c>
-      <c r="E63" s="10" t="s">
-        <v>337</v>
-      </c>
-      <c r="F63" s="10" t="s">
-        <v>335</v>
-      </c>
-      <c r="G63" s="10" t="s">
-        <v>338</v>
       </c>
       <c r="H63" s="10"/>
       <c r="I63" s="7"/>
       <c r="J63" s="38" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K63" s="8" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="L63" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N63" s="4" t="s">
         <v>7</v>
@@ -51961,36 +51952,36 @@
         <v>263</v>
       </c>
       <c r="B64" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C64" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="H64" s="10"/>
       <c r="I64" s="7"/>
       <c r="J64" s="38" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="K64" s="8" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="L64" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N64" s="4" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Closes #2225 tidy up SUBGROUP column (#2226)
2225 tidy up SUBGROUP column

Co-authored-by: Ben Straub <ben.x.straub@gsk.com>
</commit_message>
<xml_diff>
--- a/inst/adlb_grading/adlb_grading_spec.xlsx
+++ b/inst/adlb_grading/adlb_grading_spec.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\millerg1\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\millerg1\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="6090" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="6090" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NCICTCAEv4" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1640" uniqueCount="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="685">
   <si>
     <t>Anemia</t>
   </si>
@@ -1024,9 +1024,6 @@
     <t>Absolute Lymphocyte Count, Low</t>
   </si>
   <si>
-    <t>&gt; 5 years of age (not HIV infected)</t>
-  </si>
-  <si>
     <t>&lt;350/mm3; &lt;0.350 x 10e9 /L</t>
   </si>
   <si>
@@ -1070,9 +1067,6 @@
   </si>
   <si>
     <t>PTT, High</t>
-  </si>
-  <si>
-    <t>not on anticoagulation therapy</t>
   </si>
   <si>
     <t>&gt;=3.00 x ULN</t>
@@ -2955,6 +2949,9 @@
 !is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig) &amp; signif(AVAL, signif_dig) &lt;= signif(BASE, signif_dig) ~ "0"
 )</t>
   </si>
+  <si>
+    <t>&gt; 5 years of age</t>
+  </si>
 </sst>
 </file>
 
@@ -3532,7 +3529,7 @@
         <v>182</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>2</v>
@@ -3584,7 +3581,7 @@
         <v>11</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>10</v>
@@ -3636,7 +3633,7 @@
         <v>186</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
@@ -3686,7 +3683,7 @@
         <v>23</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
@@ -3736,7 +3733,7 @@
         <v>27</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
@@ -3786,7 +3783,7 @@
         <v>29</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4" t="s">
@@ -3836,7 +3833,7 @@
         <v>34</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="4" t="s">
@@ -3886,7 +3883,7 @@
         <v>39</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>10</v>
@@ -3938,7 +3935,7 @@
         <v>46</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="J10" s="14" t="s">
         <v>42</v>
@@ -3990,7 +3987,7 @@
         <v>51</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="4" t="s">
@@ -4040,7 +4037,7 @@
         <v>58</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="4" t="s">
@@ -4090,7 +4087,7 @@
         <v>63</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>2</v>
@@ -4142,7 +4139,7 @@
         <v>65</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="4" t="s">
@@ -4192,7 +4189,7 @@
         <v>68</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="J15" s="12"/>
       <c r="K15" s="4" t="s">
@@ -4242,7 +4239,7 @@
         <v>190</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>2</v>
@@ -4294,7 +4291,7 @@
         <v>77</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="J17" s="12"/>
       <c r="K17" s="4" t="s">
@@ -4346,7 +4343,7 @@
         <v>82</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="J18" s="12"/>
       <c r="K18" s="4" t="s">
@@ -4396,7 +4393,7 @@
         <v>86</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="J19" s="11" t="s">
         <v>10</v>
@@ -4448,7 +4445,7 @@
         <v>192</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="J20" s="11" t="s">
         <v>10</v>
@@ -4500,7 +4497,7 @@
         <v>95</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="J21" s="11" t="s">
         <v>10</v>
@@ -4552,7 +4549,7 @@
         <v>101</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="J22" s="11" t="s">
         <v>10</v>
@@ -4604,7 +4601,7 @@
         <v>103</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="J23" s="12"/>
       <c r="K23" s="4" t="s">
@@ -4654,7 +4651,7 @@
         <v>109</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="J24" s="11" t="s">
         <v>10</v>
@@ -4706,7 +4703,7 @@
         <v>198</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="J25" s="17" t="s">
         <v>212</v>
@@ -4760,7 +4757,7 @@
         <v>198</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="J26" s="17" t="s">
         <v>212</v>
@@ -4814,7 +4811,7 @@
         <v>199</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="J27" s="17" t="s">
         <v>212</v>
@@ -4868,7 +4865,7 @@
         <v>199</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="J28" s="17" t="s">
         <v>212</v>
@@ -4922,7 +4919,7 @@
         <v>200</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="J29" s="17" t="s">
         <v>212</v>
@@ -4974,7 +4971,7 @@
         <v>201</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="J30" s="17" t="s">
         <v>212</v>
@@ -5026,7 +5023,7 @@
         <v>202</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="J31" s="17" t="s">
         <v>212</v>
@@ -5078,7 +5075,7 @@
         <v>203</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="J32" s="17" t="s">
         <v>212</v>
@@ -5130,7 +5127,7 @@
         <v>204</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="J33" s="17" t="s">
         <v>219</v>
@@ -5184,7 +5181,7 @@
         <v>205</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="J34" s="17" t="s">
         <v>2</v>
@@ -5236,7 +5233,7 @@
         <v>206</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="J35" s="17" t="s">
         <v>212</v>
@@ -5290,7 +5287,7 @@
         <v>206</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="J36" s="17" t="s">
         <v>212</v>
@@ -5344,7 +5341,7 @@
         <v>207</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="J37" s="17" t="s">
         <v>212</v>
@@ -5396,7 +5393,7 @@
         <v>208</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="J38" s="17" t="s">
         <v>212</v>
@@ -5450,7 +5447,7 @@
         <v>209</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="J39" s="17" t="s">
         <v>212</v>
@@ -5502,7 +5499,7 @@
         <v>210</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="J40" s="17" t="s">
         <v>212</v>
@@ -5554,7 +5551,7 @@
         <v>211</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="J41" s="17" t="s">
         <v>212</v>
@@ -26138,7 +26135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z972"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -26233,7 +26230,7 @@
         <v>182</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>2</v>
@@ -26285,7 +26282,7 @@
         <v>11</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>10</v>
@@ -26337,7 +26334,7 @@
         <v>186</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
@@ -26387,7 +26384,7 @@
         <v>23</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
@@ -26437,7 +26434,7 @@
         <v>27</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
@@ -26487,7 +26484,7 @@
         <v>29</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4" t="s">
@@ -26537,7 +26534,7 @@
         <v>34</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="4" t="s">
@@ -26587,7 +26584,7 @@
         <v>39</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>10</v>
@@ -26639,7 +26636,7 @@
         <v>46</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="J10" s="14" t="s">
         <v>42</v>
@@ -26691,7 +26688,7 @@
         <v>51</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="4" t="s">
@@ -26741,7 +26738,7 @@
         <v>58</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="4" t="s">
@@ -26791,7 +26788,7 @@
         <v>63</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>2</v>
@@ -26843,7 +26840,7 @@
         <v>65</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="4" t="s">
@@ -26893,7 +26890,7 @@
         <v>68</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="J15" s="12"/>
       <c r="K15" s="4" t="s">
@@ -26943,7 +26940,7 @@
         <v>247</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>2</v>
@@ -26995,7 +26992,7 @@
         <v>77</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="J17" s="12"/>
       <c r="K17" s="4" t="s">
@@ -27047,7 +27044,7 @@
         <v>82</v>
       </c>
       <c r="I18" s="26" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="J18" s="27"/>
       <c r="K18" s="27" t="s">
@@ -27099,7 +27096,7 @@
         <v>86</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="J19" s="11" t="s">
         <v>10</v>
@@ -27151,7 +27148,7 @@
         <v>192</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="J20" s="11" t="s">
         <v>10</v>
@@ -27203,7 +27200,7 @@
         <v>95</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="J21" s="11" t="s">
         <v>10</v>
@@ -27255,7 +27252,7 @@
         <v>101</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="J22" s="11" t="s">
         <v>10</v>
@@ -27307,7 +27304,7 @@
         <v>103</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="J23" s="12"/>
       <c r="K23" s="4" t="s">
@@ -27359,7 +27356,7 @@
         <v>109</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="J24" s="11" t="s">
         <v>10</v>
@@ -27411,7 +27408,7 @@
         <v>198</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="J25" s="17" t="s">
         <v>212</v>
@@ -27465,7 +27462,7 @@
         <v>198</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="J26" s="17" t="s">
         <v>212</v>
@@ -27519,7 +27516,7 @@
         <v>200</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="J27" s="17" t="s">
         <v>212</v>
@@ -27571,7 +27568,7 @@
         <v>201</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="J28" s="17" t="s">
         <v>212</v>
@@ -27623,7 +27620,7 @@
         <v>202</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="J29" s="17" t="s">
         <v>212</v>
@@ -27675,7 +27672,7 @@
         <v>203</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="J30" s="17" t="s">
         <v>212</v>
@@ -27727,7 +27724,7 @@
         <v>204</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="J31" s="17"/>
       <c r="K31" s="4" t="s">
@@ -27779,7 +27776,7 @@
         <v>205</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="J32" s="17" t="s">
         <v>2</v>
@@ -27831,7 +27828,7 @@
         <v>206</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="J33" s="17" t="s">
         <v>212</v>
@@ -27885,7 +27882,7 @@
         <v>206</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="J34" s="17" t="s">
         <v>212</v>
@@ -27939,7 +27936,7 @@
         <v>207</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="J35" s="17" t="s">
         <v>212</v>
@@ -27991,7 +27988,7 @@
         <v>208</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="J36" s="17" t="s">
         <v>212</v>
@@ -28045,7 +28042,7 @@
         <v>209</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="J37" s="17" t="s">
         <v>212</v>
@@ -28097,7 +28094,7 @@
         <v>210</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="J38" s="17" t="s">
         <v>212</v>
@@ -48683,8 +48680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB998"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -48708,7 +48705,7 @@
         <v>193</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>224</v>
@@ -48762,27 +48759,27 @@
     </row>
     <row r="2" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2"/>
       <c r="E2" t="s">
+        <v>542</v>
+      </c>
+      <c r="F2" t="s">
+        <v>543</v>
+      </c>
+      <c r="G2" t="s">
         <v>544</v>
-      </c>
-      <c r="F2" t="s">
-        <v>545</v>
-      </c>
-      <c r="G2" t="s">
-        <v>546</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="8" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L2" s="4"/>
       <c r="M2" s="4" t="s">
@@ -48792,7 +48789,7 @@
         <v>7</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
@@ -48810,27 +48807,27 @@
     </row>
     <row r="3" spans="1:28" ht="126" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="G3" s="32"/>
       <c r="H3" s="10"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="8" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>2</v>
@@ -48858,29 +48855,29 @@
     </row>
     <row r="4" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B4" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="31" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G4" s="32" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="8" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4" t="s">
@@ -48906,27 +48903,27 @@
     </row>
     <row r="5" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B5" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5"/>
       <c r="E5" t="s">
+        <v>547</v>
+      </c>
+      <c r="F5" t="s">
+        <v>548</v>
+      </c>
+      <c r="G5" t="s">
         <v>549</v>
-      </c>
-      <c r="F5" t="s">
-        <v>550</v>
-      </c>
-      <c r="G5" t="s">
-        <v>551</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="4" t="s">
@@ -48936,7 +48933,7 @@
         <v>12</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
@@ -48954,29 +48951,29 @@
     </row>
     <row r="6" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B6" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="8" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4" t="s">
@@ -49002,29 +48999,29 @@
     </row>
     <row r="7" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B7" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="33" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="G7" s="33" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="L7" s="12"/>
       <c r="M7" s="4" t="s">
@@ -49050,29 +49047,29 @@
     </row>
     <row r="8" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B8" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="8" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4" t="s">
@@ -49098,29 +49095,29 @@
     </row>
     <row r="9" spans="1:28" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B9" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="8" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>42</v>
@@ -49148,39 +49145,39 @@
     </row>
     <row r="10" spans="1:28" s="44" customFormat="1" ht="101" x14ac:dyDescent="0.35">
       <c r="A10" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="32"/>
       <c r="F10" s="37" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="H10" s="36"/>
       <c r="I10" s="38"/>
       <c r="J10" s="38" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="K10" s="39" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="L10" s="40"/>
       <c r="M10" s="4" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="N10" s="41" t="s">
         <v>12</v>
       </c>
       <c r="O10" s="37" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="P10" s="43"/>
       <c r="Q10" s="43"/>
@@ -49198,44 +49195,44 @@
     </row>
     <row r="11" spans="1:28" s="44" customFormat="1" ht="151" x14ac:dyDescent="0.35">
       <c r="A11" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B11" s="37" t="s">
+        <v>361</v>
+      </c>
+      <c r="C11" s="37" t="s">
         <v>363</v>
       </c>
-      <c r="C11" s="37" t="s">
-        <v>365</v>
-      </c>
       <c r="D11" s="32" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F11" s="32" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="G11" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="H11"/>
       <c r="J11" s="38" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="K11" s="39" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="L11" s="40" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="N11" s="41" t="s">
         <v>12</v>
       </c>
       <c r="O11" s="42" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="P11" s="43"/>
       <c r="Q11" s="43"/>
@@ -49253,37 +49250,37 @@
     </row>
     <row r="12" spans="1:28" s="44" customFormat="1" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A12" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B12" t="s">
+        <v>371</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>362</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>374</v>
+      </c>
+      <c r="E12" s="34" t="s">
         <v>373</v>
       </c>
-      <c r="C12" s="37" t="s">
-        <v>364</v>
-      </c>
-      <c r="D12" s="33" t="s">
-        <v>376</v>
-      </c>
-      <c r="E12" s="34" t="s">
-        <v>375</v>
-      </c>
       <c r="F12" s="33" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="G12" s="33" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="H12" s="36"/>
       <c r="I12" s="38"/>
       <c r="J12" s="38" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="L12" s="40"/>
       <c r="M12" s="4" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="N12" s="41" t="s">
         <v>12</v>
@@ -49305,13 +49302,13 @@
     </row>
     <row r="13" spans="1:28" s="44" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B13" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D13" s="33"/>
       <c r="E13" s="34"/>
@@ -49320,20 +49317,20 @@
       <c r="H13" s="36"/>
       <c r="I13" s="38"/>
       <c r="J13" s="38" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="L13" s="40"/>
       <c r="M13" s="4" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="N13" s="41" t="s">
         <v>12</v>
       </c>
       <c r="O13" s="37" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="P13" s="43"/>
       <c r="Q13" s="43"/>
@@ -49351,39 +49348,39 @@
     </row>
     <row r="14" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A14" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B14" s="15" t="s">
+        <v>380</v>
+      </c>
+      <c r="C14" t="s">
+        <v>558</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="E14" s="19" t="s">
         <v>382</v>
       </c>
-      <c r="C14" t="s">
-        <v>560</v>
-      </c>
-      <c r="D14" s="19" t="s">
+      <c r="F14" s="19" t="s">
         <v>383</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="G14" s="19" t="s">
         <v>384</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>385</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>386</v>
       </c>
       <c r="H14" s="19"/>
       <c r="I14" s="18"/>
       <c r="J14" s="38" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="L14" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N14" s="4" t="s">
         <v>12</v>
@@ -49405,39 +49402,39 @@
     </row>
     <row r="15" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A15" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C15" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="18"/>
       <c r="J15" s="38" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="L15" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>12</v>
@@ -49459,29 +49456,29 @@
     </row>
     <row r="16" spans="1:28" ht="138" x14ac:dyDescent="0.3">
       <c r="A16" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="19" t="s">
+        <v>376</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>379</v>
+      </c>
+      <c r="F16" s="19" t="s">
         <v>378</v>
       </c>
-      <c r="E16" s="19" t="s">
-        <v>381</v>
-      </c>
-      <c r="F16" s="19" t="s">
-        <v>380</v>
-      </c>
       <c r="G16" s="19" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
       <c r="K16" s="1" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="L16" s="14" t="s">
         <v>42</v>
@@ -49509,39 +49506,39 @@
     </row>
     <row r="17" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A17" s="45" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B17" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C17" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="D17" t="s">
+        <v>393</v>
+      </c>
+      <c r="E17" t="s">
+        <v>394</v>
+      </c>
+      <c r="F17" t="s">
         <v>395</v>
       </c>
-      <c r="E17" t="s">
+      <c r="G17" t="s">
         <v>396</v>
-      </c>
-      <c r="F17" t="s">
-        <v>397</v>
-      </c>
-      <c r="G17" t="s">
-        <v>398</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="18"/>
       <c r="J17" s="38" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="L17" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>7</v>
@@ -49563,39 +49560,39 @@
     </row>
     <row r="18" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A18" s="45" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B18" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C18" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D18" t="s">
+        <v>397</v>
+      </c>
+      <c r="E18" t="s">
+        <v>398</v>
+      </c>
+      <c r="F18" t="s">
         <v>399</v>
       </c>
-      <c r="E18" t="s">
+      <c r="G18" t="s">
         <v>400</v>
-      </c>
-      <c r="F18" t="s">
-        <v>401</v>
-      </c>
-      <c r="G18" t="s">
-        <v>402</v>
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="18"/>
       <c r="J18" s="38" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="L18" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N18" s="4" t="s">
         <v>7</v>
@@ -49617,29 +49614,29 @@
     </row>
     <row r="19" spans="1:28" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A19" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B19" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
+        <v>389</v>
+      </c>
+      <c r="E19" t="s">
+        <v>390</v>
+      </c>
+      <c r="F19" t="s">
         <v>391</v>
       </c>
-      <c r="E19" t="s">
+      <c r="G19" t="s">
         <v>392</v>
-      </c>
-      <c r="F19" t="s">
-        <v>393</v>
-      </c>
-      <c r="G19" t="s">
-        <v>394</v>
       </c>
       <c r="H19" s="19"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="1" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="L19" s="14" t="s">
         <v>42</v>
@@ -49667,29 +49664,29 @@
     </row>
     <row r="20" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A20" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B20" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="1" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="L20" s="12"/>
       <c r="M20" s="4" t="s">
@@ -49715,29 +49712,29 @@
     </row>
     <row r="21" spans="1:28" ht="251" x14ac:dyDescent="0.35">
       <c r="A21" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B21" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="E21" t="s">
+        <v>408</v>
+      </c>
+      <c r="F21" t="s">
         <v>409</v>
       </c>
-      <c r="E21" t="s">
-        <v>410</v>
-      </c>
-      <c r="F21" t="s">
-        <v>411</v>
-      </c>
       <c r="G21" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="H21" s="10"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
       <c r="K21" s="1" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="L21" s="12"/>
       <c r="M21" s="4" t="s">
@@ -49763,29 +49760,29 @@
     </row>
     <row r="22" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A22" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B22" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C22" s="16"/>
       <c r="D22" t="s">
+        <v>411</v>
+      </c>
+      <c r="E22" t="s">
+        <v>412</v>
+      </c>
+      <c r="F22" t="s">
         <v>413</v>
       </c>
-      <c r="E22" t="s">
-        <v>414</v>
-      </c>
-      <c r="F22" t="s">
-        <v>415</v>
-      </c>
       <c r="G22" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="18"/>
       <c r="J22" s="18"/>
       <c r="K22" s="1" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="L22" s="14" t="s">
         <v>42</v>
@@ -49813,29 +49810,29 @@
     </row>
     <row r="23" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A23" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B23" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C23" s="16"/>
       <c r="D23" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E23" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F23" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="G23" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="H23" s="20"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="K23" s="1" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="L23" s="14" t="s">
         <v>42</v>
@@ -49863,39 +49860,39 @@
     </row>
     <row r="24" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A24" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B24" t="s">
+        <v>417</v>
+      </c>
+      <c r="C24" t="s">
+        <v>418</v>
+      </c>
+      <c r="D24" t="s">
         <v>419</v>
       </c>
-      <c r="C24" t="s">
+      <c r="E24" t="s">
         <v>420</v>
       </c>
-      <c r="D24" t="s">
+      <c r="F24" t="s">
         <v>421</v>
       </c>
-      <c r="E24" t="s">
+      <c r="G24" t="s">
         <v>422</v>
-      </c>
-      <c r="F24" t="s">
-        <v>423</v>
-      </c>
-      <c r="G24" t="s">
-        <v>424</v>
       </c>
       <c r="H24" s="20"/>
       <c r="I24" s="18"/>
       <c r="J24" s="38" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="L24" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="N24" s="4" t="s">
         <v>7</v>
@@ -49917,39 +49914,39 @@
     </row>
     <row r="25" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A25" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B25" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C25" s="30" t="s">
+        <v>423</v>
+      </c>
+      <c r="D25" s="30" t="s">
         <v>425</v>
       </c>
-      <c r="D25" s="30" t="s">
-        <v>427</v>
-      </c>
       <c r="E25" s="30" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="F25" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="G25" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="H25" s="20"/>
       <c r="I25" s="18"/>
       <c r="J25" s="38" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="L25" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="N25" s="4" t="s">
         <v>7</v>
@@ -49971,28 +49968,28 @@
     </row>
     <row r="26" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A26" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B26" s="30" t="s">
+        <v>426</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>427</v>
+      </c>
+      <c r="E26" s="30" t="s">
         <v>428</v>
       </c>
-      <c r="D26" s="30" t="s">
+      <c r="F26" s="35" t="s">
         <v>429</v>
       </c>
-      <c r="E26" s="30" t="s">
+      <c r="G26" s="30" t="s">
         <v>430</v>
-      </c>
-      <c r="F26" s="35" t="s">
-        <v>431</v>
-      </c>
-      <c r="G26" s="30" t="s">
-        <v>432</v>
       </c>
       <c r="H26" s="20"/>
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
       <c r="K26" s="1" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="L26" s="14"/>
       <c r="M26" s="4" t="s">
@@ -50002,7 +49999,7 @@
         <v>12</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
@@ -50020,29 +50017,29 @@
     </row>
     <row r="27" spans="1:28" s="29" customFormat="1" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A27" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C27" s="17"/>
       <c r="D27" s="30" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F27" s="33" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="H27" s="17"/>
       <c r="I27" s="17"/>
       <c r="J27" s="17"/>
       <c r="K27" s="26" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="L27" s="27"/>
       <c r="M27" s="27" t="s">
@@ -50068,37 +50065,37 @@
     </row>
     <row r="28" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A28" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B28" t="s">
+        <v>436</v>
+      </c>
+      <c r="C28" t="s">
+        <v>437</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>440</v>
+      </c>
+      <c r="E28" s="30" t="s">
+        <v>439</v>
+      </c>
+      <c r="F28" s="10" t="s">
         <v>438</v>
-      </c>
-      <c r="C28" t="s">
-        <v>439</v>
-      </c>
-      <c r="D28" s="30" t="s">
-        <v>442</v>
-      </c>
-      <c r="E28" s="30" t="s">
-        <v>441</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>440</v>
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
       <c r="I28" s="7"/>
       <c r="J28" s="38" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="L28" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>12</v>
@@ -50120,37 +50117,37 @@
     </row>
     <row r="29" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A29" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B29" t="s">
+        <v>436</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>441</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>443</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>442</v>
+      </c>
+      <c r="F29" s="10" t="s">
         <v>438</v>
-      </c>
-      <c r="C29" s="30" t="s">
-        <v>443</v>
-      </c>
-      <c r="D29" s="30" t="s">
-        <v>445</v>
-      </c>
-      <c r="E29" s="30" t="s">
-        <v>444</v>
-      </c>
-      <c r="F29" s="10" t="s">
-        <v>440</v>
       </c>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
       <c r="I29" s="7"/>
       <c r="J29" s="38" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="L29" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="N29" s="4" t="s">
         <v>12</v>
@@ -50172,37 +50169,37 @@
     </row>
     <row r="30" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A30" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B30" s="30" t="s">
+        <v>444</v>
+      </c>
+      <c r="C30" t="s">
+        <v>437</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>445</v>
+      </c>
+      <c r="E30" s="30" t="s">
         <v>446</v>
       </c>
-      <c r="C30" t="s">
-        <v>439</v>
-      </c>
-      <c r="D30" s="30" t="s">
+      <c r="F30" s="30" t="s">
         <v>447</v>
-      </c>
-      <c r="E30" s="30" t="s">
-        <v>448</v>
-      </c>
-      <c r="F30" s="30" t="s">
-        <v>449</v>
       </c>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
       <c r="I30" s="7"/>
       <c r="J30" s="38" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="L30" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="N30" s="4" t="s">
         <v>12</v>
@@ -50224,37 +50221,37 @@
     </row>
     <row r="31" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A31" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C31" s="30" t="s">
+        <v>448</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>449</v>
+      </c>
+      <c r="E31" s="30" t="s">
         <v>450</v>
       </c>
-      <c r="D31" s="30" t="s">
-        <v>451</v>
-      </c>
-      <c r="E31" s="30" t="s">
-        <v>452</v>
-      </c>
       <c r="F31" s="30" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
       <c r="I31" s="7"/>
       <c r="J31" s="38" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="K31" s="8" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="L31" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="N31" s="4" t="s">
         <v>12</v>
@@ -50276,13 +50273,13 @@
     </row>
     <row r="32" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A32" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C32" s="47" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="D32" s="30"/>
       <c r="E32" s="30"/>
@@ -50291,22 +50288,22 @@
       <c r="H32" s="10"/>
       <c r="I32" s="7"/>
       <c r="J32" s="38" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="L32" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="N32" s="4" t="s">
         <v>12</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
@@ -50324,29 +50321,29 @@
     </row>
     <row r="33" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A33" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C33" s="16"/>
       <c r="D33" s="30" t="s">
+        <v>452</v>
+      </c>
+      <c r="E33" s="30" t="s">
+        <v>453</v>
+      </c>
+      <c r="F33" s="30" t="s">
         <v>454</v>
       </c>
-      <c r="E33" s="30" t="s">
+      <c r="G33" s="30" t="s">
         <v>455</v>
-      </c>
-      <c r="F33" s="30" t="s">
-        <v>456</v>
-      </c>
-      <c r="G33" s="30" t="s">
-        <v>457</v>
       </c>
       <c r="H33" s="20"/>
       <c r="I33" s="18"/>
       <c r="J33" s="18"/>
       <c r="K33" s="1" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="L33" s="14" t="s">
         <v>42</v>
@@ -50374,29 +50371,29 @@
     </row>
     <row r="34" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A34" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C34" s="16"/>
       <c r="D34" s="30" t="s">
+        <v>457</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>458</v>
+      </c>
+      <c r="F34" s="30" t="s">
         <v>459</v>
       </c>
-      <c r="E34" s="30" t="s">
+      <c r="G34" s="30" t="s">
         <v>460</v>
-      </c>
-      <c r="F34" s="30" t="s">
-        <v>461</v>
-      </c>
-      <c r="G34" s="30" t="s">
-        <v>462</v>
       </c>
       <c r="H34" s="20"/>
       <c r="I34" s="18"/>
       <c r="J34" s="18"/>
       <c r="K34" s="1" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L34" s="14" t="s">
         <v>42</v>
@@ -50424,39 +50421,39 @@
     </row>
     <row r="35" spans="1:28" ht="151" x14ac:dyDescent="0.35">
       <c r="A35" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B35" s="30" t="s">
+        <v>461</v>
+      </c>
+      <c r="C35" s="30" t="s">
+        <v>462</v>
+      </c>
+      <c r="D35" s="30" t="s">
         <v>463</v>
       </c>
-      <c r="C35" s="30" t="s">
+      <c r="E35" s="30" t="s">
         <v>464</v>
       </c>
-      <c r="D35" s="30" t="s">
+      <c r="F35" s="30" t="s">
         <v>465</v>
       </c>
-      <c r="E35" s="30" t="s">
+      <c r="G35" s="30" t="s">
         <v>466</v>
-      </c>
-      <c r="F35" s="30" t="s">
-        <v>467</v>
-      </c>
-      <c r="G35" s="30" t="s">
-        <v>468</v>
       </c>
       <c r="H35" s="20"/>
       <c r="I35" s="18"/>
       <c r="J35" s="38" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="L35" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>7</v>
@@ -50478,39 +50475,39 @@
     </row>
     <row r="36" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A36" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C36" s="30" t="s">
+        <v>467</v>
+      </c>
+      <c r="D36" s="30" t="s">
+        <v>471</v>
+      </c>
+      <c r="E36" s="30" t="s">
+        <v>470</v>
+      </c>
+      <c r="F36" s="30" t="s">
         <v>469</v>
       </c>
-      <c r="D36" s="30" t="s">
-        <v>473</v>
-      </c>
-      <c r="E36" s="30" t="s">
-        <v>472</v>
-      </c>
-      <c r="F36" s="30" t="s">
-        <v>471</v>
-      </c>
       <c r="G36" s="30" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="H36" s="20"/>
       <c r="I36" s="18"/>
       <c r="J36" s="38" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="L36" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="N36" s="4" t="s">
         <v>7</v>
@@ -50532,39 +50529,39 @@
     </row>
     <row r="37" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A37" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B37" s="30" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C37" s="30" t="s">
+        <v>472</v>
+      </c>
+      <c r="D37" s="30" t="s">
         <v>474</v>
       </c>
-      <c r="D37" s="30" t="s">
-        <v>476</v>
-      </c>
       <c r="E37" s="30" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="F37" s="30" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="G37" s="30" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="H37" s="20"/>
       <c r="I37" s="18"/>
       <c r="J37" s="38" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L37" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="N37" s="4" t="s">
         <v>7</v>
@@ -50586,29 +50583,29 @@
     </row>
     <row r="38" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A38" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B38" s="30" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C38" s="30"/>
       <c r="D38" s="30" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F38" s="30" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="G38" s="30" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="H38" s="20"/>
       <c r="I38" s="18"/>
       <c r="J38" s="18"/>
       <c r="K38" s="1" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="L38" s="14" t="s">
         <v>42</v>
@@ -50636,29 +50633,29 @@
     </row>
     <row r="39" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A39" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B39" s="30" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C39" s="30"/>
       <c r="D39" s="30" t="s">
+        <v>476</v>
+      </c>
+      <c r="E39" s="30" t="s">
+        <v>479</v>
+      </c>
+      <c r="F39" s="30" t="s">
         <v>478</v>
       </c>
-      <c r="E39" s="30" t="s">
-        <v>481</v>
-      </c>
-      <c r="F39" s="30" t="s">
-        <v>480</v>
-      </c>
       <c r="G39" s="30" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H39" s="20"/>
       <c r="I39" s="18"/>
       <c r="J39" s="18"/>
       <c r="K39" s="1" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="L39" s="14" t="s">
         <v>42</v>
@@ -50686,29 +50683,29 @@
     </row>
     <row r="40" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A40" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B40" s="30" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C40" s="16"/>
       <c r="D40" s="30" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="F40" s="30" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="G40" s="20" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="H40" s="20"/>
       <c r="I40" s="18"/>
       <c r="J40" s="18"/>
       <c r="K40" s="1" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="L40" s="14" t="s">
         <v>42</v>
@@ -50736,29 +50733,29 @@
     </row>
     <row r="41" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A41" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C41" s="16"/>
       <c r="D41" s="30" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="F41" s="30" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="G41" s="33" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="H41" s="20"/>
       <c r="I41" s="18"/>
       <c r="J41" s="18"/>
       <c r="K41" s="1" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="L41" s="14" t="s">
         <v>42</v>
@@ -50786,32 +50783,32 @@
     </row>
     <row r="42" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A42" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C42" s="15"/>
       <c r="D42" s="30" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="F42" s="30" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="G42" s="30" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="H42" s="19"/>
       <c r="I42" s="18"/>
       <c r="J42" s="18"/>
       <c r="K42" s="1" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="L42" s="14" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="M42" s="4" t="s">
         <v>4</v>
@@ -50820,7 +50817,7 @@
         <v>12</v>
       </c>
       <c r="O42" s="3" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="P42" s="5"/>
       <c r="Q42" s="5"/>
@@ -50841,42 +50838,42 @@
         <v>263</v>
       </c>
       <c r="B43" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C43" t="s">
-        <v>305</v>
+        <v>684</v>
       </c>
       <c r="D43" s="10" t="s">
+        <v>507</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>508</v>
+      </c>
+      <c r="F43" s="10" t="s">
         <v>509</v>
       </c>
-      <c r="E43" s="10" t="s">
+      <c r="G43" s="10" t="s">
         <v>510</v>
-      </c>
-      <c r="F43" s="10" t="s">
-        <v>511</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>512</v>
       </c>
       <c r="H43" s="10"/>
       <c r="I43" s="7"/>
       <c r="J43" s="38" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="L43" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N43" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O43" s="3" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="P43" s="5"/>
       <c r="Q43" s="5"/>
@@ -50897,10 +50894,10 @@
         <v>263</v>
       </c>
       <c r="B44" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C44" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
@@ -50909,22 +50906,22 @@
       <c r="H44" s="10"/>
       <c r="I44" s="7"/>
       <c r="J44" s="38" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="K44" s="8" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="L44" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N44" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O44" s="3" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="P44" s="5"/>
       <c r="Q44" s="5"/>
@@ -50948,39 +50945,39 @@
         <v>304</v>
       </c>
       <c r="C45" t="s">
+        <v>684</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>512</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="G45" s="7" t="s">
         <v>305</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>514</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>306</v>
       </c>
       <c r="H45" s="7"/>
       <c r="I45" s="7"/>
       <c r="J45" s="38" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="L45" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N45" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O45" s="3" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="P45" s="5"/>
       <c r="Q45" s="5"/>
@@ -51004,7 +51001,7 @@
         <v>304</v>
       </c>
       <c r="C46" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
@@ -51013,22 +51010,22 @@
       <c r="H46" s="7"/>
       <c r="I46" s="7"/>
       <c r="J46" s="38" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="K46" s="8" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="L46" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N46" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O46" s="3" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="P46" s="5"/>
       <c r="Q46" s="5"/>
@@ -51055,13 +51052,13 @@
         <v>299</v>
       </c>
       <c r="D47" s="10" t="s">
+        <v>513</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>514</v>
+      </c>
+      <c r="F47" s="10" t="s">
         <v>515</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>516</v>
-      </c>
-      <c r="F47" s="10" t="s">
-        <v>517</v>
       </c>
       <c r="G47" s="10" t="s">
         <v>300</v>
@@ -51071,16 +51068,16 @@
       </c>
       <c r="I47" s="7"/>
       <c r="J47" s="38" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K47" s="8" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="L47" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N47" s="4" t="s">
         <v>7</v>
@@ -51111,13 +51108,13 @@
         <v>301</v>
       </c>
       <c r="D48" s="10" t="s">
+        <v>516</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>517</v>
+      </c>
+      <c r="F48" s="10" t="s">
         <v>518</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>519</v>
-      </c>
-      <c r="F48" s="10" t="s">
-        <v>520</v>
       </c>
       <c r="G48" s="10" t="s">
         <v>302</v>
@@ -51127,16 +51124,16 @@
       </c>
       <c r="I48" s="7"/>
       <c r="J48" s="38" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K48" s="8" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="L48" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N48" s="4" t="s">
         <v>7</v>
@@ -51164,16 +51161,16 @@
         <v>298</v>
       </c>
       <c r="C49" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="D49" s="10" t="s">
+        <v>519</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>520</v>
+      </c>
+      <c r="F49" s="10" t="s">
         <v>521</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>522</v>
-      </c>
-      <c r="F49" s="10" t="s">
-        <v>523</v>
       </c>
       <c r="G49" s="10" t="s">
         <v>303</v>
@@ -51183,16 +51180,16 @@
       </c>
       <c r="I49" s="7"/>
       <c r="J49" s="38" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="L49" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N49" s="4" t="s">
         <v>7</v>
@@ -51238,7 +51235,7 @@
       <c r="I50" s="7"/>
       <c r="J50" s="7"/>
       <c r="K50" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="L50" s="4" t="s">
         <v>2</v>
@@ -51272,7 +51269,7 @@
         <v>264</v>
       </c>
       <c r="C51" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="D51" s="30" t="s">
         <v>266</v>
@@ -51289,16 +51286,16 @@
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
       <c r="J51" s="38" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="K51" s="8" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="L51" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="N51" s="4" t="s">
         <v>7</v>
@@ -51326,7 +51323,7 @@
         <v>264</v>
       </c>
       <c r="C52" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="D52" s="30" t="s">
         <v>270</v>
@@ -51343,16 +51340,16 @@
       <c r="H52" s="7"/>
       <c r="I52" s="7"/>
       <c r="J52" s="38" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="K52" s="8" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="L52" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="N52" s="4" t="s">
         <v>7</v>
@@ -51397,16 +51394,16 @@
       <c r="H53" s="7"/>
       <c r="I53" s="7"/>
       <c r="J53" s="38" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="K53" s="8" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="L53" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N53" s="4" t="s">
         <v>7</v>
@@ -51451,16 +51448,16 @@
       <c r="H54" s="7"/>
       <c r="I54" s="7"/>
       <c r="J54" s="38" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K54" s="8" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="L54" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N54" s="4" t="s">
         <v>7</v>
@@ -51505,16 +51502,16 @@
       <c r="H55" s="7"/>
       <c r="I55" s="7"/>
       <c r="J55" s="38" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K55" s="8" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="L55" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M55" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N55" s="4" t="s">
         <v>7</v>
@@ -51542,7 +51539,7 @@
         <v>264</v>
       </c>
       <c r="C56" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="D56" s="30" t="s">
         <v>286</v>
@@ -51559,16 +51556,16 @@
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
       <c r="J56" s="38" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="K56" s="8" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="L56" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M56" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N56" s="4" t="s">
         <v>7</v>
@@ -51596,7 +51593,7 @@
         <v>264</v>
       </c>
       <c r="C57" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="D57" s="30" t="s">
         <v>289</v>
@@ -51613,16 +51610,16 @@
       <c r="H57" s="7"/>
       <c r="I57" s="7"/>
       <c r="J57" s="38" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="K57" s="8" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="L57" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N57" s="4" t="s">
         <v>7</v>
@@ -51647,28 +51644,26 @@
         <v>263</v>
       </c>
       <c r="B58" t="s">
-        <v>310</v>
-      </c>
-      <c r="C58" t="s">
-        <v>321</v>
-      </c>
+        <v>309</v>
+      </c>
+      <c r="C58"/>
       <c r="D58" s="10" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H58" s="10"/>
       <c r="I58" s="7"/>
       <c r="J58" s="7"/>
       <c r="K58" s="1" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="L58" s="12"/>
       <c r="M58" s="4" t="s">
@@ -51678,7 +51673,7 @@
         <v>12</v>
       </c>
       <c r="O58" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="P58" s="5"/>
       <c r="Q58" s="5"/>
@@ -51699,31 +51694,29 @@
         <v>263</v>
       </c>
       <c r="B59" t="s">
-        <v>313</v>
-      </c>
-      <c r="C59" t="s">
+        <v>312</v>
+      </c>
+      <c r="C59"/>
+      <c r="D59" t="s">
+        <v>317</v>
+      </c>
+      <c r="E59" t="s">
+        <v>316</v>
+      </c>
+      <c r="F59" t="s">
+        <v>315</v>
+      </c>
+      <c r="G59" s="10" t="s">
         <v>314</v>
-      </c>
-      <c r="D59" t="s">
-        <v>318</v>
-      </c>
-      <c r="E59" t="s">
-        <v>317</v>
-      </c>
-      <c r="F59" t="s">
-        <v>316</v>
-      </c>
-      <c r="G59" s="10" t="s">
-        <v>315</v>
       </c>
       <c r="H59" s="10"/>
       <c r="I59" s="7"/>
       <c r="J59" s="7"/>
       <c r="K59" s="1" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="L59" s="12" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M59" s="4" t="s">
         <v>4</v>
@@ -51731,7 +51724,9 @@
       <c r="N59" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O59" s="3"/>
+      <c r="O59" s="3" t="s">
+        <v>313</v>
+      </c>
       <c r="P59" s="5"/>
       <c r="Q59" s="5"/>
       <c r="R59" s="5"/>
@@ -51751,28 +51746,26 @@
         <v>263</v>
       </c>
       <c r="B60" t="s">
+        <v>319</v>
+      </c>
+      <c r="C60"/>
+      <c r="D60" t="s">
+        <v>323</v>
+      </c>
+      <c r="E60" t="s">
+        <v>322</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="G60" t="s">
         <v>320</v>
-      </c>
-      <c r="C60" t="s">
-        <v>321</v>
-      </c>
-      <c r="D60" t="s">
-        <v>325</v>
-      </c>
-      <c r="E60" t="s">
-        <v>324</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="G60" t="s">
-        <v>322</v>
       </c>
       <c r="H60" s="7"/>
       <c r="I60" s="7"/>
       <c r="J60" s="7"/>
       <c r="K60" s="8" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="L60" s="4"/>
       <c r="M60" s="4" t="s">
@@ -51782,7 +51775,7 @@
         <v>12</v>
       </c>
       <c r="O60" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="P60" s="5"/>
       <c r="Q60" s="5"/>
@@ -51803,20 +51796,20 @@
         <v>263</v>
       </c>
       <c r="B61" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C61" s="10"/>
       <c r="D61" s="10" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="H61" s="10" t="s">
         <v>183</v>
@@ -51824,7 +51817,7 @@
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
       <c r="K61" s="8" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="L61" s="11" t="s">
         <v>10</v>
@@ -51855,28 +51848,26 @@
         <v>263</v>
       </c>
       <c r="B62" t="s">
+        <v>328</v>
+      </c>
+      <c r="C62"/>
+      <c r="D62" t="s">
+        <v>329</v>
+      </c>
+      <c r="E62" t="s">
         <v>330</v>
       </c>
-      <c r="C62" t="s">
-        <v>321</v>
-      </c>
-      <c r="D62" t="s">
+      <c r="F62" s="7" t="s">
         <v>331</v>
       </c>
-      <c r="E62" t="s">
-        <v>332</v>
-      </c>
-      <c r="F62" s="7" t="s">
-        <v>333</v>
-      </c>
       <c r="G62" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="H62" s="7"/>
       <c r="I62" s="7"/>
       <c r="J62" s="7"/>
       <c r="K62" s="8" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="L62" s="4"/>
       <c r="M62" s="4" t="s">
@@ -51886,7 +51877,7 @@
         <v>12</v>
       </c>
       <c r="O62" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="P62" s="5"/>
       <c r="Q62" s="5"/>
@@ -51907,36 +51898,36 @@
         <v>263</v>
       </c>
       <c r="B63" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C63" t="s">
         <v>299</v>
       </c>
       <c r="D63" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="G63" s="10" t="s">
         <v>336</v>
-      </c>
-      <c r="E63" s="10" t="s">
-        <v>337</v>
-      </c>
-      <c r="F63" s="10" t="s">
-        <v>335</v>
-      </c>
-      <c r="G63" s="10" t="s">
-        <v>338</v>
       </c>
       <c r="H63" s="10"/>
       <c r="I63" s="7"/>
       <c r="J63" s="38" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K63" s="8" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="L63" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N63" s="4" t="s">
         <v>7</v>
@@ -51961,36 +51952,36 @@
         <v>263</v>
       </c>
       <c r="B64" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C64" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="H64" s="10"/>
       <c r="I64" s="7"/>
       <c r="J64" s="38" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="K64" s="8" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="L64" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N64" s="4" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
2284 fix grade in DAIDS
</commit_message>
<xml_diff>
--- a/inst/adlb_grading/adlb_grading_spec.xlsx
+++ b/inst/adlb_grading/adlb_grading_spec.xlsx
@@ -2238,16 +2238,6 @@
   <si>
     <t>case_when(
 is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-signif(AVAL, signif_dig) &lt; 0.35 ~ "4",
-signif(AVAL, signif_dig) &lt; 0.5 ~ "3",
-signif(AVAL, signif_dig) &lt; 0.6 ~ "2",
-signif(AVAL, signif_dig) &lt; 0.65 ~ "1",
-signif(AVAL, signif_dig) &lt;= 0.65 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
 signif(AVAL, signif_dig) &lt; 0.4 ~ "4",
 signif(AVAL, signif_dig) &lt; 0.6 ~ "3",
 signif(AVAL, signif_dig) &lt; 0.8 ~ "2",
@@ -2952,6 +2942,16 @@
   <si>
     <t>&gt; 5 years of age</t>
   </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 0.35 ~ "4",
+signif(AVAL, signif_dig) &lt; 0.5 ~ "3",
+signif(AVAL, signif_dig) &lt; 0.6 ~ "2",
+signif(AVAL, signif_dig) &lt; 0.65 ~ "1",
+signif(AVAL, signif_dig) &gt;= 0.65 ~ "0"
+)</t>
+  </si>
 </sst>
 </file>
 
@@ -3529,7 +3529,7 @@
         <v>182</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>2</v>
@@ -3581,7 +3581,7 @@
         <v>11</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>10</v>
@@ -3633,7 +3633,7 @@
         <v>186</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
@@ -3683,7 +3683,7 @@
         <v>23</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
@@ -3733,7 +3733,7 @@
         <v>27</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
@@ -3783,7 +3783,7 @@
         <v>29</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4" t="s">
@@ -3833,7 +3833,7 @@
         <v>34</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="4" t="s">
@@ -3883,7 +3883,7 @@
         <v>39</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>10</v>
@@ -3935,7 +3935,7 @@
         <v>46</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="J10" s="14" t="s">
         <v>42</v>
@@ -3987,7 +3987,7 @@
         <v>51</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="4" t="s">
@@ -4037,7 +4037,7 @@
         <v>58</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="4" t="s">
@@ -4087,7 +4087,7 @@
         <v>63</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>2</v>
@@ -4139,7 +4139,7 @@
         <v>65</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="4" t="s">
@@ -4189,7 +4189,7 @@
         <v>68</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="J15" s="12"/>
       <c r="K15" s="4" t="s">
@@ -4239,7 +4239,7 @@
         <v>190</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>2</v>
@@ -4291,7 +4291,7 @@
         <v>77</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="J17" s="12"/>
       <c r="K17" s="4" t="s">
@@ -4343,7 +4343,7 @@
         <v>82</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="J18" s="12"/>
       <c r="K18" s="4" t="s">
@@ -4393,7 +4393,7 @@
         <v>86</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J19" s="11" t="s">
         <v>10</v>
@@ -4445,7 +4445,7 @@
         <v>192</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J20" s="11" t="s">
         <v>10</v>
@@ -4497,7 +4497,7 @@
         <v>95</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J21" s="11" t="s">
         <v>10</v>
@@ -4549,7 +4549,7 @@
         <v>101</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J22" s="11" t="s">
         <v>10</v>
@@ -4601,7 +4601,7 @@
         <v>103</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="J23" s="12"/>
       <c r="K23" s="4" t="s">
@@ -4651,7 +4651,7 @@
         <v>109</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="J24" s="11" t="s">
         <v>10</v>
@@ -4703,7 +4703,7 @@
         <v>198</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="J25" s="17" t="s">
         <v>212</v>
@@ -4757,7 +4757,7 @@
         <v>198</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="J26" s="17" t="s">
         <v>212</v>
@@ -4811,7 +4811,7 @@
         <v>199</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="J27" s="17" t="s">
         <v>212</v>
@@ -4865,7 +4865,7 @@
         <v>199</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="J28" s="17" t="s">
         <v>212</v>
@@ -4919,7 +4919,7 @@
         <v>200</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="J29" s="17" t="s">
         <v>212</v>
@@ -4971,7 +4971,7 @@
         <v>201</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="J30" s="17" t="s">
         <v>212</v>
@@ -5023,7 +5023,7 @@
         <v>202</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="J31" s="17" t="s">
         <v>212</v>
@@ -5075,7 +5075,7 @@
         <v>203</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="J32" s="17" t="s">
         <v>212</v>
@@ -5127,7 +5127,7 @@
         <v>204</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="J33" s="17" t="s">
         <v>219</v>
@@ -5181,7 +5181,7 @@
         <v>205</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="J34" s="17" t="s">
         <v>2</v>
@@ -5233,7 +5233,7 @@
         <v>206</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="J35" s="17" t="s">
         <v>212</v>
@@ -5341,7 +5341,7 @@
         <v>207</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="J37" s="17" t="s">
         <v>212</v>
@@ -5393,7 +5393,7 @@
         <v>208</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="J38" s="17" t="s">
         <v>212</v>
@@ -5447,7 +5447,7 @@
         <v>209</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="J39" s="17" t="s">
         <v>212</v>
@@ -5499,7 +5499,7 @@
         <v>210</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="J40" s="17" t="s">
         <v>212</v>
@@ -5551,7 +5551,7 @@
         <v>211</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="J41" s="17" t="s">
         <v>212</v>
@@ -26230,7 +26230,7 @@
         <v>182</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>2</v>
@@ -26282,7 +26282,7 @@
         <v>11</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>10</v>
@@ -26334,7 +26334,7 @@
         <v>186</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
@@ -26384,7 +26384,7 @@
         <v>23</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
@@ -26434,7 +26434,7 @@
         <v>27</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
@@ -26484,7 +26484,7 @@
         <v>29</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4" t="s">
@@ -26534,7 +26534,7 @@
         <v>34</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="4" t="s">
@@ -26584,7 +26584,7 @@
         <v>39</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>10</v>
@@ -26636,7 +26636,7 @@
         <v>46</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="J10" s="14" t="s">
         <v>42</v>
@@ -26688,7 +26688,7 @@
         <v>51</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="4" t="s">
@@ -26738,7 +26738,7 @@
         <v>58</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="4" t="s">
@@ -26788,7 +26788,7 @@
         <v>63</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>2</v>
@@ -26840,7 +26840,7 @@
         <v>65</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="4" t="s">
@@ -26890,7 +26890,7 @@
         <v>68</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="J15" s="12"/>
       <c r="K15" s="4" t="s">
@@ -26940,7 +26940,7 @@
         <v>247</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>2</v>
@@ -26992,7 +26992,7 @@
         <v>77</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="J17" s="12"/>
       <c r="K17" s="4" t="s">
@@ -27044,7 +27044,7 @@
         <v>82</v>
       </c>
       <c r="I18" s="26" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="J18" s="27"/>
       <c r="K18" s="27" t="s">
@@ -27096,7 +27096,7 @@
         <v>86</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J19" s="11" t="s">
         <v>10</v>
@@ -27148,7 +27148,7 @@
         <v>192</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J20" s="11" t="s">
         <v>10</v>
@@ -27200,7 +27200,7 @@
         <v>95</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J21" s="11" t="s">
         <v>10</v>
@@ -27252,7 +27252,7 @@
         <v>101</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J22" s="11" t="s">
         <v>10</v>
@@ -27304,7 +27304,7 @@
         <v>103</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="J23" s="12"/>
       <c r="K23" s="4" t="s">
@@ -27356,7 +27356,7 @@
         <v>109</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="J24" s="11" t="s">
         <v>10</v>
@@ -27408,7 +27408,7 @@
         <v>198</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="J25" s="17" t="s">
         <v>212</v>
@@ -27462,7 +27462,7 @@
         <v>198</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="J26" s="17" t="s">
         <v>212</v>
@@ -27516,7 +27516,7 @@
         <v>200</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="J27" s="17" t="s">
         <v>212</v>
@@ -27568,7 +27568,7 @@
         <v>201</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="J28" s="17" t="s">
         <v>212</v>
@@ -27620,7 +27620,7 @@
         <v>202</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="J29" s="17" t="s">
         <v>212</v>
@@ -27672,7 +27672,7 @@
         <v>203</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="J30" s="17" t="s">
         <v>212</v>
@@ -27724,7 +27724,7 @@
         <v>204</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="J31" s="17"/>
       <c r="K31" s="4" t="s">
@@ -27776,7 +27776,7 @@
         <v>205</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="J32" s="17" t="s">
         <v>2</v>
@@ -27828,7 +27828,7 @@
         <v>206</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="J33" s="17" t="s">
         <v>212</v>
@@ -27936,7 +27936,7 @@
         <v>207</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="J35" s="17" t="s">
         <v>212</v>
@@ -27988,7 +27988,7 @@
         <v>208</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="J36" s="17" t="s">
         <v>212</v>
@@ -28042,7 +28042,7 @@
         <v>209</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="J37" s="17" t="s">
         <v>212</v>
@@ -28094,7 +28094,7 @@
         <v>210</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="J38" s="17" t="s">
         <v>212</v>
@@ -48680,8 +48680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="B33" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -50501,7 +50501,7 @@
         <v>571</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="L36" s="14" t="s">
         <v>42</v>
@@ -50841,7 +50841,7 @@
         <v>308</v>
       </c>
       <c r="C43" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D43" s="10" t="s">
         <v>507</v>
@@ -50945,7 +50945,7 @@
         <v>304</v>
       </c>
       <c r="C45" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>512</v>
@@ -50965,7 +50965,7 @@
         <v>573</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>618</v>
+        <v>684</v>
       </c>
       <c r="L45" s="11" t="s">
         <v>10</v>
@@ -51071,7 +51071,7 @@
         <v>531</v>
       </c>
       <c r="K47" s="8" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="L47" s="11" t="s">
         <v>10</v>
@@ -51127,7 +51127,7 @@
         <v>532</v>
       </c>
       <c r="K48" s="8" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="L48" s="11" t="s">
         <v>10</v>
@@ -51183,7 +51183,7 @@
         <v>533</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="L49" s="11" t="s">
         <v>10</v>
@@ -51235,7 +51235,7 @@
       <c r="I50" s="7"/>
       <c r="J50" s="7"/>
       <c r="K50" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="L50" s="4" t="s">
         <v>2</v>
@@ -51289,7 +51289,7 @@
         <v>575</v>
       </c>
       <c r="K51" s="8" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="L51" s="4" t="s">
         <v>2</v>
@@ -51343,7 +51343,7 @@
         <v>576</v>
       </c>
       <c r="K52" s="8" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="L52" s="4" t="s">
         <v>2</v>
@@ -51397,7 +51397,7 @@
         <v>577</v>
       </c>
       <c r="K53" s="8" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="L53" s="4" t="s">
         <v>2</v>
@@ -51451,7 +51451,7 @@
         <v>534</v>
       </c>
       <c r="K54" s="8" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="L54" s="4" t="s">
         <v>2</v>
@@ -51505,7 +51505,7 @@
         <v>535</v>
       </c>
       <c r="K55" s="8" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="L55" s="4" t="s">
         <v>2</v>
@@ -51559,7 +51559,7 @@
         <v>536</v>
       </c>
       <c r="K56" s="8" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="L56" s="4" t="s">
         <v>2</v>
@@ -51613,7 +51613,7 @@
         <v>537</v>
       </c>
       <c r="K57" s="8" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="L57" s="4" t="s">
         <v>2</v>
@@ -51663,7 +51663,7 @@
       <c r="I58" s="7"/>
       <c r="J58" s="7"/>
       <c r="K58" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="L58" s="12"/>
       <c r="M58" s="4" t="s">
@@ -51713,7 +51713,7 @@
       <c r="I59" s="7"/>
       <c r="J59" s="7"/>
       <c r="K59" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="L59" s="12" t="s">
         <v>318</v>
@@ -51817,7 +51817,7 @@
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
       <c r="K61" s="8" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="L61" s="11" t="s">
         <v>10</v>
@@ -51921,7 +51921,7 @@
         <v>531</v>
       </c>
       <c r="K63" s="8" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="L63" s="11" t="s">
         <v>10</v>
@@ -51975,7 +51975,7 @@
         <v>537</v>
       </c>
       <c r="K64" s="8" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="L64" s="11" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
2284 fix grade in DAIDS (#2285)
</commit_message>
<xml_diff>
--- a/inst/adlb_grading/adlb_grading_spec.xlsx
+++ b/inst/adlb_grading/adlb_grading_spec.xlsx
@@ -2238,16 +2238,6 @@
   <si>
     <t>case_when(
 is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
-signif(AVAL, signif_dig) &lt; 0.35 ~ "4",
-signif(AVAL, signif_dig) &lt; 0.5 ~ "3",
-signif(AVAL, signif_dig) &lt; 0.6 ~ "2",
-signif(AVAL, signif_dig) &lt; 0.65 ~ "1",
-signif(AVAL, signif_dig) &lt;= 0.65 ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
 signif(AVAL, signif_dig) &lt; 0.4 ~ "4",
 signif(AVAL, signif_dig) &lt; 0.6 ~ "3",
 signif(AVAL, signif_dig) &lt; 0.8 ~ "2",
@@ -2952,6 +2942,16 @@
   <si>
     <t>&gt; 5 years of age</t>
   </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(BRTHDT) | is.na(LBDT) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 0.35 ~ "4",
+signif(AVAL, signif_dig) &lt; 0.5 ~ "3",
+signif(AVAL, signif_dig) &lt; 0.6 ~ "2",
+signif(AVAL, signif_dig) &lt; 0.65 ~ "1",
+signif(AVAL, signif_dig) &gt;= 0.65 ~ "0"
+)</t>
+  </si>
 </sst>
 </file>
 
@@ -3529,7 +3529,7 @@
         <v>182</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>2</v>
@@ -3581,7 +3581,7 @@
         <v>11</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>10</v>
@@ -3633,7 +3633,7 @@
         <v>186</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
@@ -3683,7 +3683,7 @@
         <v>23</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
@@ -3733,7 +3733,7 @@
         <v>27</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
@@ -3783,7 +3783,7 @@
         <v>29</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4" t="s">
@@ -3833,7 +3833,7 @@
         <v>34</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="4" t="s">
@@ -3883,7 +3883,7 @@
         <v>39</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>10</v>
@@ -3935,7 +3935,7 @@
         <v>46</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="J10" s="14" t="s">
         <v>42</v>
@@ -3987,7 +3987,7 @@
         <v>51</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="4" t="s">
@@ -4037,7 +4037,7 @@
         <v>58</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="4" t="s">
@@ -4087,7 +4087,7 @@
         <v>63</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>2</v>
@@ -4139,7 +4139,7 @@
         <v>65</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="4" t="s">
@@ -4189,7 +4189,7 @@
         <v>68</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="J15" s="12"/>
       <c r="K15" s="4" t="s">
@@ -4239,7 +4239,7 @@
         <v>190</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>2</v>
@@ -4291,7 +4291,7 @@
         <v>77</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="J17" s="12"/>
       <c r="K17" s="4" t="s">
@@ -4343,7 +4343,7 @@
         <v>82</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="J18" s="12"/>
       <c r="K18" s="4" t="s">
@@ -4393,7 +4393,7 @@
         <v>86</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J19" s="11" t="s">
         <v>10</v>
@@ -4445,7 +4445,7 @@
         <v>192</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J20" s="11" t="s">
         <v>10</v>
@@ -4497,7 +4497,7 @@
         <v>95</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J21" s="11" t="s">
         <v>10</v>
@@ -4549,7 +4549,7 @@
         <v>101</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J22" s="11" t="s">
         <v>10</v>
@@ -4601,7 +4601,7 @@
         <v>103</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="J23" s="12"/>
       <c r="K23" s="4" t="s">
@@ -4651,7 +4651,7 @@
         <v>109</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="J24" s="11" t="s">
         <v>10</v>
@@ -4703,7 +4703,7 @@
         <v>198</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="J25" s="17" t="s">
         <v>212</v>
@@ -4757,7 +4757,7 @@
         <v>198</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="J26" s="17" t="s">
         <v>212</v>
@@ -4811,7 +4811,7 @@
         <v>199</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="J27" s="17" t="s">
         <v>212</v>
@@ -4865,7 +4865,7 @@
         <v>199</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="J28" s="17" t="s">
         <v>212</v>
@@ -4919,7 +4919,7 @@
         <v>200</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="J29" s="17" t="s">
         <v>212</v>
@@ -4971,7 +4971,7 @@
         <v>201</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="J30" s="17" t="s">
         <v>212</v>
@@ -5023,7 +5023,7 @@
         <v>202</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="J31" s="17" t="s">
         <v>212</v>
@@ -5075,7 +5075,7 @@
         <v>203</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="J32" s="17" t="s">
         <v>212</v>
@@ -5127,7 +5127,7 @@
         <v>204</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="J33" s="17" t="s">
         <v>219</v>
@@ -5181,7 +5181,7 @@
         <v>205</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="J34" s="17" t="s">
         <v>2</v>
@@ -5233,7 +5233,7 @@
         <v>206</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="J35" s="17" t="s">
         <v>212</v>
@@ -5341,7 +5341,7 @@
         <v>207</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="J37" s="17" t="s">
         <v>212</v>
@@ -5393,7 +5393,7 @@
         <v>208</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="J38" s="17" t="s">
         <v>212</v>
@@ -5447,7 +5447,7 @@
         <v>209</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="J39" s="17" t="s">
         <v>212</v>
@@ -5499,7 +5499,7 @@
         <v>210</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="J40" s="17" t="s">
         <v>212</v>
@@ -5551,7 +5551,7 @@
         <v>211</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="J41" s="17" t="s">
         <v>212</v>
@@ -26230,7 +26230,7 @@
         <v>182</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>2</v>
@@ -26282,7 +26282,7 @@
         <v>11</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>10</v>
@@ -26334,7 +26334,7 @@
         <v>186</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
@@ -26384,7 +26384,7 @@
         <v>23</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
@@ -26434,7 +26434,7 @@
         <v>27</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
@@ -26484,7 +26484,7 @@
         <v>29</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4" t="s">
@@ -26534,7 +26534,7 @@
         <v>34</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="4" t="s">
@@ -26584,7 +26584,7 @@
         <v>39</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>10</v>
@@ -26636,7 +26636,7 @@
         <v>46</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="J10" s="14" t="s">
         <v>42</v>
@@ -26688,7 +26688,7 @@
         <v>51</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="4" t="s">
@@ -26738,7 +26738,7 @@
         <v>58</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="4" t="s">
@@ -26788,7 +26788,7 @@
         <v>63</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>2</v>
@@ -26840,7 +26840,7 @@
         <v>65</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="4" t="s">
@@ -26890,7 +26890,7 @@
         <v>68</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="J15" s="12"/>
       <c r="K15" s="4" t="s">
@@ -26940,7 +26940,7 @@
         <v>247</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>2</v>
@@ -26992,7 +26992,7 @@
         <v>77</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="J17" s="12"/>
       <c r="K17" s="4" t="s">
@@ -27044,7 +27044,7 @@
         <v>82</v>
       </c>
       <c r="I18" s="26" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="J18" s="27"/>
       <c r="K18" s="27" t="s">
@@ -27096,7 +27096,7 @@
         <v>86</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J19" s="11" t="s">
         <v>10</v>
@@ -27148,7 +27148,7 @@
         <v>192</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J20" s="11" t="s">
         <v>10</v>
@@ -27200,7 +27200,7 @@
         <v>95</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J21" s="11" t="s">
         <v>10</v>
@@ -27252,7 +27252,7 @@
         <v>101</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J22" s="11" t="s">
         <v>10</v>
@@ -27304,7 +27304,7 @@
         <v>103</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="J23" s="12"/>
       <c r="K23" s="4" t="s">
@@ -27356,7 +27356,7 @@
         <v>109</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="J24" s="11" t="s">
         <v>10</v>
@@ -27408,7 +27408,7 @@
         <v>198</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="J25" s="17" t="s">
         <v>212</v>
@@ -27462,7 +27462,7 @@
         <v>198</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="J26" s="17" t="s">
         <v>212</v>
@@ -27516,7 +27516,7 @@
         <v>200</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="J27" s="17" t="s">
         <v>212</v>
@@ -27568,7 +27568,7 @@
         <v>201</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="J28" s="17" t="s">
         <v>212</v>
@@ -27620,7 +27620,7 @@
         <v>202</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="J29" s="17" t="s">
         <v>212</v>
@@ -27672,7 +27672,7 @@
         <v>203</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="J30" s="17" t="s">
         <v>212</v>
@@ -27724,7 +27724,7 @@
         <v>204</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="J31" s="17"/>
       <c r="K31" s="4" t="s">
@@ -27776,7 +27776,7 @@
         <v>205</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="J32" s="17" t="s">
         <v>2</v>
@@ -27828,7 +27828,7 @@
         <v>206</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="J33" s="17" t="s">
         <v>212</v>
@@ -27936,7 +27936,7 @@
         <v>207</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="J35" s="17" t="s">
         <v>212</v>
@@ -27988,7 +27988,7 @@
         <v>208</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="J36" s="17" t="s">
         <v>212</v>
@@ -28042,7 +28042,7 @@
         <v>209</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="J37" s="17" t="s">
         <v>212</v>
@@ -28094,7 +28094,7 @@
         <v>210</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="J38" s="17" t="s">
         <v>212</v>
@@ -48680,8 +48680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="B33" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -50501,7 +50501,7 @@
         <v>571</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="L36" s="14" t="s">
         <v>42</v>
@@ -50841,7 +50841,7 @@
         <v>308</v>
       </c>
       <c r="C43" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D43" s="10" t="s">
         <v>507</v>
@@ -50945,7 +50945,7 @@
         <v>304</v>
       </c>
       <c r="C45" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>512</v>
@@ -50965,7 +50965,7 @@
         <v>573</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>618</v>
+        <v>684</v>
       </c>
       <c r="L45" s="11" t="s">
         <v>10</v>
@@ -51071,7 +51071,7 @@
         <v>531</v>
       </c>
       <c r="K47" s="8" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="L47" s="11" t="s">
         <v>10</v>
@@ -51127,7 +51127,7 @@
         <v>532</v>
       </c>
       <c r="K48" s="8" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="L48" s="11" t="s">
         <v>10</v>
@@ -51183,7 +51183,7 @@
         <v>533</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="L49" s="11" t="s">
         <v>10</v>
@@ -51235,7 +51235,7 @@
       <c r="I50" s="7"/>
       <c r="J50" s="7"/>
       <c r="K50" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="L50" s="4" t="s">
         <v>2</v>
@@ -51289,7 +51289,7 @@
         <v>575</v>
       </c>
       <c r="K51" s="8" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="L51" s="4" t="s">
         <v>2</v>
@@ -51343,7 +51343,7 @@
         <v>576</v>
       </c>
       <c r="K52" s="8" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="L52" s="4" t="s">
         <v>2</v>
@@ -51397,7 +51397,7 @@
         <v>577</v>
       </c>
       <c r="K53" s="8" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="L53" s="4" t="s">
         <v>2</v>
@@ -51451,7 +51451,7 @@
         <v>534</v>
       </c>
       <c r="K54" s="8" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="L54" s="4" t="s">
         <v>2</v>
@@ -51505,7 +51505,7 @@
         <v>535</v>
       </c>
       <c r="K55" s="8" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="L55" s="4" t="s">
         <v>2</v>
@@ -51559,7 +51559,7 @@
         <v>536</v>
       </c>
       <c r="K56" s="8" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="L56" s="4" t="s">
         <v>2</v>
@@ -51613,7 +51613,7 @@
         <v>537</v>
       </c>
       <c r="K57" s="8" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="L57" s="4" t="s">
         <v>2</v>
@@ -51663,7 +51663,7 @@
       <c r="I58" s="7"/>
       <c r="J58" s="7"/>
       <c r="K58" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="L58" s="12"/>
       <c r="M58" s="4" t="s">
@@ -51713,7 +51713,7 @@
       <c r="I59" s="7"/>
       <c r="J59" s="7"/>
       <c r="K59" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="L59" s="12" t="s">
         <v>318</v>
@@ -51817,7 +51817,7 @@
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
       <c r="K61" s="8" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="L61" s="11" t="s">
         <v>10</v>
@@ -51921,7 +51921,7 @@
         <v>531</v>
       </c>
       <c r="K63" s="8" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="L63" s="11" t="s">
         <v>10</v>
@@ -51975,7 +51975,7 @@
         <v>537</v>
       </c>
       <c r="K64" s="8" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="L64" s="11" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
2534 fixed bug for INR Increased
</commit_message>
<xml_diff>
--- a/inst/adlb_grading/adlb_grading_spec.xlsx
+++ b/inst/adlb_grading/adlb_grading_spec.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="6090" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="6090" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NCICTCAEv4" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DAIDS!$C$1:$C$998</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">NCICTCAEv5!$B$1:$B$972</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="687">
   <si>
     <t>Anemia</t>
   </si>
@@ -773,12 +774,6 @@
   </si>
   <si>
     <t>A finding based on laboratory test results that indicate increased levels of hemoglobin above normal.</t>
-  </si>
-  <si>
-    <t>&gt;1.5 - 2.5 x ULN; &gt;1.5 - 2.5 x baseline if on anticoagulation; dose adjustment indicated</t>
-  </si>
-  <si>
-    <t>&gt;1.2 - 1.5 x ULN; &gt;1 - 1.5 x baseline if on anticoagulation; monitoring only indicated</t>
   </si>
   <si>
     <t>&gt;5.0 x ULN and with signs or symptoms</t>
@@ -2855,19 +2850,6 @@
   </si>
   <si>
     <t>case_when(
-is.na(AVAL) ~ NA_character_,
-!is.na(ANRHI) &amp; signif(AVAL, signif_dig) &gt; signif(2.5*ANRHI, signif_dig) ~ "3",
-!is.na(BASE) &amp; signif(AVAL, signif_dig) &gt; signif(2.5*BASE, signif_dig) ~ "3",
-!is.na(ANRHI) &amp; signif(AVAL, signif_dig) &gt; signif(1.5*ANRHI, signif_dig) ~ "2",
-!is.na(BASE) &amp; signif(AVAL, signif_dig) &gt; signif(1.5*BASE, signif_dig) ~ "2",
-!is.na(ANRHI) &amp; signif(AVAL, signif_dig) &gt; signif(1.2*ANRHI, signif_dig) ~ "1",
-!is.na(BASE) &amp; signif(AVAL, signif_dig) &gt; signif(BASE, signif_dig) ~ "1",
-!is.na(ANRHI) &amp; signif(AVAL, signif_dig) &lt;= signif(1.2*ANRHI, signif_dig) &amp; !is.na(BASE) &amp; signif(AVAL, signif_dig) &lt;= signif(BASE, signif_dig) ~ "0",
-is.na(ANRHI) | is.na(BASE) ~ NA_character_
-)</t>
-  </si>
-  <si>
-    <t>case_when(
 is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
 signif(AVAL, signif_dig) &gt; signif(5*ANRHI, signif_dig) ~ "4",
 signif(AVAL, signif_dig) &gt; signif(2*ANRHI, signif_dig) ~ "3",
@@ -2951,6 +2933,31 @@
 signif(AVAL, signif_dig) &lt; 0.65 ~ "1",
 signif(AVAL, signif_dig) &gt;= 0.65 ~ "0"
 )</t>
+  </si>
+  <si>
+    <t>&gt;1.2 - 1.5; &gt;1 - 1.5 x baseline if on anticoagulation; monitoring only indicated</t>
+  </si>
+  <si>
+    <t>&gt;1.5 - 2.5; &gt;1.5 - 2.5 x baseline if on anticoagulation; dose adjustment indicated</t>
+  </si>
+  <si>
+    <t>&gt;2.5; &gt;2.5 times above baseline if on anticoagulation</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+signif(AVAL, signif_dig) &gt; signif(2.5, signif_dig) ~ "3",
+!is.na(BASE) &amp; signif(AVAL, signif_dig) &gt; signif(2.5*BASE, signif_dig) ~ "3",
+signif(AVAL, signif_dig) &gt; signif(1.5, signif_dig) ~ "2",
+!is.na(BASE) &amp; signif(AVAL, signif_dig) &gt; signif(1.5*BASE, signif_dig) ~ "2",
+signif(AVAL, signif_dig) &gt; signif(1.2, signif_dig) ~ "1",
+!is.na(BASE) &amp; signif(AVAL, signif_dig) &gt; signif(BASE, signif_dig) ~ "1",
+signif(AVAL, signif_dig) &lt;= signif(1.2, signif_dig) &amp; !is.na(BASE) &amp; signif(AVAL, signif_dig) &lt;= signif(BASE, signif_dig) ~ "0",
+is.na(BASE) ~ NA_character_
+)</t>
+  </si>
+  <si>
+    <t>AVAL, BASE</t>
   </si>
 </sst>
 </file>
@@ -3529,7 +3536,7 @@
         <v>182</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>2</v>
@@ -3581,7 +3588,7 @@
         <v>11</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>10</v>
@@ -3633,7 +3640,7 @@
         <v>186</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
@@ -3683,7 +3690,7 @@
         <v>23</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
@@ -3733,7 +3740,7 @@
         <v>27</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
@@ -3783,7 +3790,7 @@
         <v>29</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4" t="s">
@@ -3833,7 +3840,7 @@
         <v>34</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="4" t="s">
@@ -3883,7 +3890,7 @@
         <v>39</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>10</v>
@@ -3935,7 +3942,7 @@
         <v>46</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="J10" s="14" t="s">
         <v>42</v>
@@ -3987,7 +3994,7 @@
         <v>51</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="4" t="s">
@@ -4037,7 +4044,7 @@
         <v>58</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="4" t="s">
@@ -4087,7 +4094,7 @@
         <v>63</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>2</v>
@@ -4139,7 +4146,7 @@
         <v>65</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="4" t="s">
@@ -4189,7 +4196,7 @@
         <v>68</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="J15" s="12"/>
       <c r="K15" s="4" t="s">
@@ -4239,7 +4246,7 @@
         <v>190</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>2</v>
@@ -4291,7 +4298,7 @@
         <v>77</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="J17" s="12"/>
       <c r="K17" s="4" t="s">
@@ -4343,7 +4350,7 @@
         <v>82</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="J18" s="12"/>
       <c r="K18" s="4" t="s">
@@ -4393,7 +4400,7 @@
         <v>86</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="J19" s="11" t="s">
         <v>10</v>
@@ -4445,7 +4452,7 @@
         <v>192</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="J20" s="11" t="s">
         <v>10</v>
@@ -4497,7 +4504,7 @@
         <v>95</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="J21" s="11" t="s">
         <v>10</v>
@@ -4549,7 +4556,7 @@
         <v>101</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="J22" s="11" t="s">
         <v>10</v>
@@ -4601,7 +4608,7 @@
         <v>103</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="J23" s="12"/>
       <c r="K23" s="4" t="s">
@@ -4651,7 +4658,7 @@
         <v>109</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="J24" s="11" t="s">
         <v>10</v>
@@ -4703,7 +4710,7 @@
         <v>198</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="J25" s="17" t="s">
         <v>212</v>
@@ -4757,7 +4764,7 @@
         <v>198</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="J26" s="17" t="s">
         <v>212</v>
@@ -4811,7 +4818,7 @@
         <v>199</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="J27" s="17" t="s">
         <v>212</v>
@@ -4865,7 +4872,7 @@
         <v>199</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="J28" s="17" t="s">
         <v>212</v>
@@ -4919,7 +4926,7 @@
         <v>200</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="J29" s="17" t="s">
         <v>212</v>
@@ -4971,7 +4978,7 @@
         <v>201</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="J30" s="17" t="s">
         <v>212</v>
@@ -5023,7 +5030,7 @@
         <v>202</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="J31" s="17" t="s">
         <v>212</v>
@@ -5075,7 +5082,7 @@
         <v>203</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="J32" s="17" t="s">
         <v>212</v>
@@ -5127,7 +5134,7 @@
         <v>204</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="J33" s="17" t="s">
         <v>219</v>
@@ -5181,7 +5188,7 @@
         <v>205</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="J34" s="17" t="s">
         <v>2</v>
@@ -5233,7 +5240,7 @@
         <v>206</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="J35" s="17" t="s">
         <v>212</v>
@@ -5287,7 +5294,7 @@
         <v>206</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="J36" s="17" t="s">
         <v>212</v>
@@ -5341,7 +5348,7 @@
         <v>207</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="J37" s="17" t="s">
         <v>212</v>
@@ -5393,7 +5400,7 @@
         <v>208</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="J38" s="17" t="s">
         <v>212</v>
@@ -5447,7 +5454,7 @@
         <v>209</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="J39" s="17" t="s">
         <v>212</v>
@@ -5499,7 +5506,7 @@
         <v>210</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="J40" s="17" t="s">
         <v>212</v>
@@ -5551,7 +5558,7 @@
         <v>211</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="J41" s="17" t="s">
         <v>212</v>
@@ -26135,8 +26142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z972"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -26230,7 +26237,7 @@
         <v>182</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>2</v>
@@ -26282,7 +26289,7 @@
         <v>11</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>10</v>
@@ -26334,7 +26341,7 @@
         <v>186</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
@@ -26384,7 +26391,7 @@
         <v>23</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
@@ -26434,7 +26441,7 @@
         <v>27</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
@@ -26484,7 +26491,7 @@
         <v>29</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4" t="s">
@@ -26534,7 +26541,7 @@
         <v>34</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="4" t="s">
@@ -26584,7 +26591,7 @@
         <v>39</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>10</v>
@@ -26636,7 +26643,7 @@
         <v>46</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="J10" s="14" t="s">
         <v>42</v>
@@ -26688,7 +26695,7 @@
         <v>51</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="4" t="s">
@@ -26738,7 +26745,7 @@
         <v>58</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="4" t="s">
@@ -26788,7 +26795,7 @@
         <v>63</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>2</v>
@@ -26840,7 +26847,7 @@
         <v>65</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="4" t="s">
@@ -26890,7 +26897,7 @@
         <v>68</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="J15" s="12"/>
       <c r="K15" s="4" t="s">
@@ -26940,7 +26947,7 @@
         <v>247</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>2</v>
@@ -26966,7 +26973,7 @@
       <c r="Y16" s="5"/>
       <c r="Z16" s="5"/>
     </row>
-    <row r="17" spans="1:26" ht="250.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" ht="238" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>185</v>
       </c>
@@ -26974,13 +26981,13 @@
         <v>73</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>249</v>
+        <v>682</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>248</v>
+        <v>683</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>76</v>
+        <v>684</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>183</v>
@@ -26992,11 +26999,11 @@
         <v>77</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>676</v>
+        <v>685</v>
       </c>
       <c r="J17" s="12"/>
       <c r="K17" s="4" t="s">
-        <v>15</v>
+        <v>686</v>
       </c>
       <c r="L17" s="4" t="s">
         <v>12</v>
@@ -27029,13 +27036,13 @@
         <v>14</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G18" s="17" t="s">
         <v>183</v>
@@ -27044,7 +27051,7 @@
         <v>82</v>
       </c>
       <c r="I18" s="26" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="J18" s="27"/>
       <c r="K18" s="27" t="s">
@@ -27054,7 +27061,7 @@
         <v>12</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="N18" s="28"/>
       <c r="O18" s="28"/>
@@ -27096,7 +27103,7 @@
         <v>86</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="J19" s="11" t="s">
         <v>10</v>
@@ -27148,7 +27155,7 @@
         <v>192</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="J20" s="11" t="s">
         <v>10</v>
@@ -27200,7 +27207,7 @@
         <v>95</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="J21" s="11" t="s">
         <v>10</v>
@@ -27252,7 +27259,7 @@
         <v>101</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="J22" s="11" t="s">
         <v>10</v>
@@ -27289,13 +27296,13 @@
         <v>14</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F23" s="24" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>183</v>
@@ -27304,7 +27311,7 @@
         <v>103</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="J23" s="12"/>
       <c r="K23" s="4" t="s">
@@ -27314,7 +27321,7 @@
         <v>12</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
@@ -27356,7 +27363,7 @@
         <v>109</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="J24" s="11" t="s">
         <v>10</v>
@@ -27408,7 +27415,7 @@
         <v>198</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="J25" s="17" t="s">
         <v>212</v>
@@ -27462,7 +27469,7 @@
         <v>198</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="J26" s="17" t="s">
         <v>212</v>
@@ -27501,7 +27508,7 @@
         <v>121</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E27" s="24" t="s">
         <v>123</v>
@@ -27516,7 +27523,7 @@
         <v>200</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="J27" s="17" t="s">
         <v>212</v>
@@ -27568,7 +27575,7 @@
         <v>201</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="J28" s="17" t="s">
         <v>212</v>
@@ -27605,7 +27612,7 @@
         <v>130</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E29" s="20" t="s">
         <v>132</v>
@@ -27620,7 +27627,7 @@
         <v>202</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="J29" s="17" t="s">
         <v>212</v>
@@ -27672,7 +27679,7 @@
         <v>203</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="J30" s="17" t="s">
         <v>212</v>
@@ -27706,16 +27713,16 @@
         <v>139</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D31" s="24" t="s">
         <v>197</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F31" s="22" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G31" s="19" t="s">
         <v>181</v>
@@ -27724,7 +27731,7 @@
         <v>204</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="J31" s="17"/>
       <c r="K31" s="4" t="s">
@@ -27776,7 +27783,7 @@
         <v>205</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="J32" s="17" t="s">
         <v>2</v>
@@ -27828,7 +27835,7 @@
         <v>206</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="J33" s="17" t="s">
         <v>212</v>
@@ -27882,7 +27889,7 @@
         <v>206</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="J34" s="17" t="s">
         <v>212</v>
@@ -27936,7 +27943,7 @@
         <v>207</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="J35" s="17" t="s">
         <v>212</v>
@@ -27973,7 +27980,7 @@
         <v>158</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E36" s="20" t="s">
         <v>160</v>
@@ -27988,7 +27995,7 @@
         <v>208</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="J36" s="17" t="s">
         <v>212</v>
@@ -28000,7 +28007,7 @@
         <v>7</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
@@ -28042,7 +28049,7 @@
         <v>209</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="J37" s="17" t="s">
         <v>212</v>
@@ -28079,10 +28086,10 @@
         <v>168</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F38" s="24" t="s">
         <v>170</v>
@@ -28094,7 +28101,7 @@
         <v>210</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="J38" s="17" t="s">
         <v>212</v>
@@ -28106,7 +28113,7 @@
         <v>7</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
@@ -48671,6 +48678,7 @@
       <c r="Z972" s="5"/>
     </row>
   </sheetData>
+  <autoFilter ref="B1:B972"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -48680,8 +48688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B33" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView topLeftCell="B33" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -48705,7 +48713,7 @@
         <v>193</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>224</v>
@@ -48726,7 +48734,7 @@
         <v>6</v>
       </c>
       <c r="J1" s="46" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>223</v>
@@ -48759,27 +48767,27 @@
     </row>
     <row r="2" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B2" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2"/>
       <c r="E2" t="s">
+        <v>540</v>
+      </c>
+      <c r="F2" t="s">
+        <v>541</v>
+      </c>
+      <c r="G2" t="s">
         <v>542</v>
-      </c>
-      <c r="F2" t="s">
-        <v>543</v>
-      </c>
-      <c r="G2" t="s">
-        <v>544</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="8" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="L2" s="4"/>
       <c r="M2" s="4" t="s">
@@ -48789,7 +48797,7 @@
         <v>7</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
@@ -48807,27 +48815,27 @@
     </row>
     <row r="3" spans="1:28" ht="126" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B3" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E3" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="G3" s="32"/>
       <c r="H3" s="10"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="8" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>2</v>
@@ -48855,29 +48863,29 @@
     </row>
     <row r="4" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B4" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="31" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G4" s="32" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="8" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4" t="s">
@@ -48903,27 +48911,27 @@
     </row>
     <row r="5" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B5" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5"/>
       <c r="E5" t="s">
+        <v>545</v>
+      </c>
+      <c r="F5" t="s">
+        <v>546</v>
+      </c>
+      <c r="G5" t="s">
         <v>547</v>
-      </c>
-      <c r="F5" t="s">
-        <v>548</v>
-      </c>
-      <c r="G5" t="s">
-        <v>549</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="4" t="s">
@@ -48933,7 +48941,7 @@
         <v>12</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
@@ -48951,29 +48959,29 @@
     </row>
     <row r="6" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B6" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="8" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4" t="s">
@@ -48999,29 +49007,29 @@
     </row>
     <row r="7" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B7" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="33" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G7" s="33" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="1" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="L7" s="12"/>
       <c r="M7" s="4" t="s">
@@ -49047,29 +49055,29 @@
     </row>
     <row r="8" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B8" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="8" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4" t="s">
@@ -49095,29 +49103,29 @@
     </row>
     <row r="9" spans="1:28" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B9" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="8" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>42</v>
@@ -49145,39 +49153,39 @@
     </row>
     <row r="10" spans="1:28" s="44" customFormat="1" ht="101" x14ac:dyDescent="0.35">
       <c r="A10" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="32"/>
       <c r="F10" s="37" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="H10" s="36"/>
       <c r="I10" s="38"/>
       <c r="J10" s="38" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="K10" s="39" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="L10" s="40"/>
       <c r="M10" s="4" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="N10" s="41" t="s">
         <v>12</v>
       </c>
       <c r="O10" s="37" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="P10" s="43"/>
       <c r="Q10" s="43"/>
@@ -49195,44 +49203,44 @@
     </row>
     <row r="11" spans="1:28" s="44" customFormat="1" ht="151" x14ac:dyDescent="0.35">
       <c r="A11" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B11" s="37" t="s">
+        <v>359</v>
+      </c>
+      <c r="C11" s="37" t="s">
         <v>361</v>
       </c>
-      <c r="C11" s="37" t="s">
-        <v>363</v>
-      </c>
       <c r="D11" s="32" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F11" s="32" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="G11" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="H11"/>
       <c r="J11" s="38" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="K11" s="39" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="L11" s="40" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="N11" s="41" t="s">
         <v>12</v>
       </c>
       <c r="O11" s="42" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="P11" s="43"/>
       <c r="Q11" s="43"/>
@@ -49250,37 +49258,37 @@
     </row>
     <row r="12" spans="1:28" s="44" customFormat="1" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A12" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B12" t="s">
+        <v>369</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>360</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>372</v>
+      </c>
+      <c r="E12" s="34" t="s">
         <v>371</v>
       </c>
-      <c r="C12" s="37" t="s">
-        <v>362</v>
-      </c>
-      <c r="D12" s="33" t="s">
-        <v>374</v>
-      </c>
-      <c r="E12" s="34" t="s">
-        <v>373</v>
-      </c>
       <c r="F12" s="33" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="G12" s="33" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="H12" s="36"/>
       <c r="I12" s="38"/>
       <c r="J12" s="38" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="L12" s="40"/>
       <c r="M12" s="4" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="N12" s="41" t="s">
         <v>12</v>
@@ -49302,13 +49310,13 @@
     </row>
     <row r="13" spans="1:28" s="44" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B13" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D13" s="33"/>
       <c r="E13" s="34"/>
@@ -49317,20 +49325,20 @@
       <c r="H13" s="36"/>
       <c r="I13" s="38"/>
       <c r="J13" s="38" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="L13" s="40"/>
       <c r="M13" s="4" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="N13" s="41" t="s">
         <v>12</v>
       </c>
       <c r="O13" s="37" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="P13" s="43"/>
       <c r="Q13" s="43"/>
@@ -49348,39 +49356,39 @@
     </row>
     <row r="14" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A14" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B14" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="C14" t="s">
+        <v>556</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>379</v>
+      </c>
+      <c r="E14" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="C14" t="s">
-        <v>558</v>
-      </c>
-      <c r="D14" s="19" t="s">
+      <c r="F14" s="19" t="s">
         <v>381</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="G14" s="19" t="s">
         <v>382</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>383</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>384</v>
       </c>
       <c r="H14" s="19"/>
       <c r="I14" s="18"/>
       <c r="J14" s="38" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="L14" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N14" s="4" t="s">
         <v>12</v>
@@ -49402,39 +49410,39 @@
     </row>
     <row r="15" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A15" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C15" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="18"/>
       <c r="J15" s="38" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="L15" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>12</v>
@@ -49456,29 +49464,29 @@
     </row>
     <row r="16" spans="1:28" ht="138" x14ac:dyDescent="0.3">
       <c r="A16" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="19" t="s">
+        <v>374</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>377</v>
+      </c>
+      <c r="F16" s="19" t="s">
         <v>376</v>
       </c>
-      <c r="E16" s="19" t="s">
-        <v>379</v>
-      </c>
-      <c r="F16" s="19" t="s">
-        <v>378</v>
-      </c>
       <c r="G16" s="19" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
       <c r="K16" s="1" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="L16" s="14" t="s">
         <v>42</v>
@@ -49506,39 +49514,39 @@
     </row>
     <row r="17" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A17" s="45" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B17" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C17" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="D17" t="s">
+        <v>391</v>
+      </c>
+      <c r="E17" t="s">
+        <v>392</v>
+      </c>
+      <c r="F17" t="s">
         <v>393</v>
       </c>
-      <c r="E17" t="s">
+      <c r="G17" t="s">
         <v>394</v>
-      </c>
-      <c r="F17" t="s">
-        <v>395</v>
-      </c>
-      <c r="G17" t="s">
-        <v>396</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="18"/>
       <c r="J17" s="38" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="L17" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>7</v>
@@ -49560,39 +49568,39 @@
     </row>
     <row r="18" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A18" s="45" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B18" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C18" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D18" t="s">
+        <v>395</v>
+      </c>
+      <c r="E18" t="s">
+        <v>396</v>
+      </c>
+      <c r="F18" t="s">
         <v>397</v>
       </c>
-      <c r="E18" t="s">
+      <c r="G18" t="s">
         <v>398</v>
-      </c>
-      <c r="F18" t="s">
-        <v>399</v>
-      </c>
-      <c r="G18" t="s">
-        <v>400</v>
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="18"/>
       <c r="J18" s="38" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="L18" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N18" s="4" t="s">
         <v>7</v>
@@ -49614,29 +49622,29 @@
     </row>
     <row r="19" spans="1:28" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A19" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B19" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
+        <v>387</v>
+      </c>
+      <c r="E19" t="s">
+        <v>388</v>
+      </c>
+      <c r="F19" t="s">
         <v>389</v>
       </c>
-      <c r="E19" t="s">
+      <c r="G19" t="s">
         <v>390</v>
-      </c>
-      <c r="F19" t="s">
-        <v>391</v>
-      </c>
-      <c r="G19" t="s">
-        <v>392</v>
       </c>
       <c r="H19" s="19"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="1" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="L19" s="14" t="s">
         <v>42</v>
@@ -49664,29 +49672,29 @@
     </row>
     <row r="20" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A20" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B20" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="1" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="L20" s="12"/>
       <c r="M20" s="4" t="s">
@@ -49712,29 +49720,29 @@
     </row>
     <row r="21" spans="1:28" ht="251" x14ac:dyDescent="0.35">
       <c r="A21" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B21" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="E21" t="s">
+        <v>406</v>
+      </c>
+      <c r="F21" t="s">
         <v>407</v>
       </c>
-      <c r="E21" t="s">
-        <v>408</v>
-      </c>
-      <c r="F21" t="s">
-        <v>409</v>
-      </c>
       <c r="G21" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="H21" s="10"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
       <c r="K21" s="1" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="L21" s="12"/>
       <c r="M21" s="4" t="s">
@@ -49760,29 +49768,29 @@
     </row>
     <row r="22" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A22" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B22" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C22" s="16"/>
       <c r="D22" t="s">
+        <v>409</v>
+      </c>
+      <c r="E22" t="s">
+        <v>410</v>
+      </c>
+      <c r="F22" t="s">
         <v>411</v>
       </c>
-      <c r="E22" t="s">
-        <v>412</v>
-      </c>
-      <c r="F22" t="s">
-        <v>413</v>
-      </c>
       <c r="G22" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="18"/>
       <c r="J22" s="18"/>
       <c r="K22" s="1" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="L22" s="14" t="s">
         <v>42</v>
@@ -49810,29 +49818,29 @@
     </row>
     <row r="23" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A23" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B23" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C23" s="16"/>
       <c r="D23" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E23" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F23" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="G23" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="H23" s="20"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="K23" s="1" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="L23" s="14" t="s">
         <v>42</v>
@@ -49860,39 +49868,39 @@
     </row>
     <row r="24" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A24" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B24" t="s">
+        <v>415</v>
+      </c>
+      <c r="C24" t="s">
+        <v>416</v>
+      </c>
+      <c r="D24" t="s">
         <v>417</v>
       </c>
-      <c r="C24" t="s">
+      <c r="E24" t="s">
         <v>418</v>
       </c>
-      <c r="D24" t="s">
+      <c r="F24" t="s">
         <v>419</v>
       </c>
-      <c r="E24" t="s">
+      <c r="G24" t="s">
         <v>420</v>
-      </c>
-      <c r="F24" t="s">
-        <v>421</v>
-      </c>
-      <c r="G24" t="s">
-        <v>422</v>
       </c>
       <c r="H24" s="20"/>
       <c r="I24" s="18"/>
       <c r="J24" s="38" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="L24" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="N24" s="4" t="s">
         <v>7</v>
@@ -49914,39 +49922,39 @@
     </row>
     <row r="25" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A25" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B25" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C25" s="30" t="s">
+        <v>421</v>
+      </c>
+      <c r="D25" s="30" t="s">
         <v>423</v>
       </c>
-      <c r="D25" s="30" t="s">
-        <v>425</v>
-      </c>
       <c r="E25" s="30" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F25" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="G25" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="H25" s="20"/>
       <c r="I25" s="18"/>
       <c r="J25" s="38" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="L25" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="N25" s="4" t="s">
         <v>7</v>
@@ -49968,28 +49976,28 @@
     </row>
     <row r="26" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A26" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B26" s="30" t="s">
+        <v>424</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>425</v>
+      </c>
+      <c r="E26" s="30" t="s">
         <v>426</v>
       </c>
-      <c r="D26" s="30" t="s">
+      <c r="F26" s="35" t="s">
         <v>427</v>
       </c>
-      <c r="E26" s="30" t="s">
+      <c r="G26" s="30" t="s">
         <v>428</v>
-      </c>
-      <c r="F26" s="35" t="s">
-        <v>429</v>
-      </c>
-      <c r="G26" s="30" t="s">
-        <v>430</v>
       </c>
       <c r="H26" s="20"/>
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
       <c r="K26" s="1" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="L26" s="14"/>
       <c r="M26" s="4" t="s">
@@ -49999,7 +50007,7 @@
         <v>12</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
@@ -50017,29 +50025,29 @@
     </row>
     <row r="27" spans="1:28" s="29" customFormat="1" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A27" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C27" s="17"/>
       <c r="D27" s="30" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="F27" s="33" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="H27" s="17"/>
       <c r="I27" s="17"/>
       <c r="J27" s="17"/>
       <c r="K27" s="26" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="L27" s="27"/>
       <c r="M27" s="27" t="s">
@@ -50065,37 +50073,37 @@
     </row>
     <row r="28" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A28" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B28" t="s">
+        <v>434</v>
+      </c>
+      <c r="C28" t="s">
+        <v>435</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>438</v>
+      </c>
+      <c r="E28" s="30" t="s">
+        <v>437</v>
+      </c>
+      <c r="F28" s="10" t="s">
         <v>436</v>
-      </c>
-      <c r="C28" t="s">
-        <v>437</v>
-      </c>
-      <c r="D28" s="30" t="s">
-        <v>440</v>
-      </c>
-      <c r="E28" s="30" t="s">
-        <v>439</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>438</v>
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
       <c r="I28" s="7"/>
       <c r="J28" s="38" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="L28" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>12</v>
@@ -50117,37 +50125,37 @@
     </row>
     <row r="29" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A29" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B29" t="s">
+        <v>434</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>439</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>441</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>440</v>
+      </c>
+      <c r="F29" s="10" t="s">
         <v>436</v>
-      </c>
-      <c r="C29" s="30" t="s">
-        <v>441</v>
-      </c>
-      <c r="D29" s="30" t="s">
-        <v>443</v>
-      </c>
-      <c r="E29" s="30" t="s">
-        <v>442</v>
-      </c>
-      <c r="F29" s="10" t="s">
-        <v>438</v>
       </c>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
       <c r="I29" s="7"/>
       <c r="J29" s="38" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="L29" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="N29" s="4" t="s">
         <v>12</v>
@@ -50169,37 +50177,37 @@
     </row>
     <row r="30" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A30" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B30" s="30" t="s">
+        <v>442</v>
+      </c>
+      <c r="C30" t="s">
+        <v>435</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>443</v>
+      </c>
+      <c r="E30" s="30" t="s">
         <v>444</v>
       </c>
-      <c r="C30" t="s">
-        <v>437</v>
-      </c>
-      <c r="D30" s="30" t="s">
+      <c r="F30" s="30" t="s">
         <v>445</v>
-      </c>
-      <c r="E30" s="30" t="s">
-        <v>446</v>
-      </c>
-      <c r="F30" s="30" t="s">
-        <v>447</v>
       </c>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
       <c r="I30" s="7"/>
       <c r="J30" s="38" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="L30" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="N30" s="4" t="s">
         <v>12</v>
@@ -50221,37 +50229,37 @@
     </row>
     <row r="31" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A31" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C31" s="30" t="s">
+        <v>446</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>447</v>
+      </c>
+      <c r="E31" s="30" t="s">
         <v>448</v>
       </c>
-      <c r="D31" s="30" t="s">
-        <v>449</v>
-      </c>
-      <c r="E31" s="30" t="s">
-        <v>450</v>
-      </c>
       <c r="F31" s="30" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
       <c r="I31" s="7"/>
       <c r="J31" s="38" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="K31" s="8" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="L31" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="N31" s="4" t="s">
         <v>12</v>
@@ -50273,13 +50281,13 @@
     </row>
     <row r="32" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A32" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C32" s="47" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="D32" s="30"/>
       <c r="E32" s="30"/>
@@ -50288,22 +50296,22 @@
       <c r="H32" s="10"/>
       <c r="I32" s="7"/>
       <c r="J32" s="38" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="L32" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="N32" s="4" t="s">
         <v>12</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
@@ -50321,29 +50329,29 @@
     </row>
     <row r="33" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A33" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C33" s="16"/>
       <c r="D33" s="30" t="s">
+        <v>450</v>
+      </c>
+      <c r="E33" s="30" t="s">
+        <v>451</v>
+      </c>
+      <c r="F33" s="30" t="s">
         <v>452</v>
       </c>
-      <c r="E33" s="30" t="s">
+      <c r="G33" s="30" t="s">
         <v>453</v>
-      </c>
-      <c r="F33" s="30" t="s">
-        <v>454</v>
-      </c>
-      <c r="G33" s="30" t="s">
-        <v>455</v>
       </c>
       <c r="H33" s="20"/>
       <c r="I33" s="18"/>
       <c r="J33" s="18"/>
       <c r="K33" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="L33" s="14" t="s">
         <v>42</v>
@@ -50371,29 +50379,29 @@
     </row>
     <row r="34" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A34" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C34" s="16"/>
       <c r="D34" s="30" t="s">
+        <v>455</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>456</v>
+      </c>
+      <c r="F34" s="30" t="s">
         <v>457</v>
       </c>
-      <c r="E34" s="30" t="s">
+      <c r="G34" s="30" t="s">
         <v>458</v>
-      </c>
-      <c r="F34" s="30" t="s">
-        <v>459</v>
-      </c>
-      <c r="G34" s="30" t="s">
-        <v>460</v>
       </c>
       <c r="H34" s="20"/>
       <c r="I34" s="18"/>
       <c r="J34" s="18"/>
       <c r="K34" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="L34" s="14" t="s">
         <v>42</v>
@@ -50421,39 +50429,39 @@
     </row>
     <row r="35" spans="1:28" ht="151" x14ac:dyDescent="0.35">
       <c r="A35" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B35" s="30" t="s">
+        <v>459</v>
+      </c>
+      <c r="C35" s="30" t="s">
+        <v>460</v>
+      </c>
+      <c r="D35" s="30" t="s">
         <v>461</v>
       </c>
-      <c r="C35" s="30" t="s">
+      <c r="E35" s="30" t="s">
         <v>462</v>
       </c>
-      <c r="D35" s="30" t="s">
+      <c r="F35" s="30" t="s">
         <v>463</v>
       </c>
-      <c r="E35" s="30" t="s">
+      <c r="G35" s="30" t="s">
         <v>464</v>
-      </c>
-      <c r="F35" s="30" t="s">
-        <v>465</v>
-      </c>
-      <c r="G35" s="30" t="s">
-        <v>466</v>
       </c>
       <c r="H35" s="20"/>
       <c r="I35" s="18"/>
       <c r="J35" s="38" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="L35" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>7</v>
@@ -50475,39 +50483,39 @@
     </row>
     <row r="36" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A36" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C36" s="30" t="s">
+        <v>465</v>
+      </c>
+      <c r="D36" s="30" t="s">
+        <v>469</v>
+      </c>
+      <c r="E36" s="30" t="s">
+        <v>468</v>
+      </c>
+      <c r="F36" s="30" t="s">
         <v>467</v>
       </c>
-      <c r="D36" s="30" t="s">
-        <v>471</v>
-      </c>
-      <c r="E36" s="30" t="s">
-        <v>470</v>
-      </c>
-      <c r="F36" s="30" t="s">
-        <v>469</v>
-      </c>
       <c r="G36" s="30" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="H36" s="20"/>
       <c r="I36" s="18"/>
       <c r="J36" s="38" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="L36" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="N36" s="4" t="s">
         <v>7</v>
@@ -50529,39 +50537,39 @@
     </row>
     <row r="37" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A37" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B37" s="30" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C37" s="30" t="s">
+        <v>470</v>
+      </c>
+      <c r="D37" s="30" t="s">
         <v>472</v>
       </c>
-      <c r="D37" s="30" t="s">
-        <v>474</v>
-      </c>
       <c r="E37" s="30" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="F37" s="30" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="G37" s="30" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="H37" s="20"/>
       <c r="I37" s="18"/>
       <c r="J37" s="38" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L37" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="N37" s="4" t="s">
         <v>7</v>
@@ -50583,29 +50591,29 @@
     </row>
     <row r="38" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A38" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B38" s="30" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C38" s="30"/>
       <c r="D38" s="30" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="F38" s="30" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="G38" s="30" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="H38" s="20"/>
       <c r="I38" s="18"/>
       <c r="J38" s="18"/>
       <c r="K38" s="1" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="L38" s="14" t="s">
         <v>42</v>
@@ -50633,29 +50641,29 @@
     </row>
     <row r="39" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A39" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B39" s="30" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C39" s="30"/>
       <c r="D39" s="30" t="s">
+        <v>474</v>
+      </c>
+      <c r="E39" s="30" t="s">
+        <v>477</v>
+      </c>
+      <c r="F39" s="30" t="s">
         <v>476</v>
       </c>
-      <c r="E39" s="30" t="s">
-        <v>479</v>
-      </c>
-      <c r="F39" s="30" t="s">
-        <v>478</v>
-      </c>
       <c r="G39" s="30" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="H39" s="20"/>
       <c r="I39" s="18"/>
       <c r="J39" s="18"/>
       <c r="K39" s="1" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L39" s="14" t="s">
         <v>42</v>
@@ -50683,29 +50691,29 @@
     </row>
     <row r="40" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A40" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B40" s="30" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C40" s="16"/>
       <c r="D40" s="30" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="F40" s="30" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="G40" s="20" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="H40" s="20"/>
       <c r="I40" s="18"/>
       <c r="J40" s="18"/>
       <c r="K40" s="1" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="L40" s="14" t="s">
         <v>42</v>
@@ -50733,29 +50741,29 @@
     </row>
     <row r="41" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A41" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C41" s="16"/>
       <c r="D41" s="30" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="F41" s="30" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G41" s="33" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="H41" s="20"/>
       <c r="I41" s="18"/>
       <c r="J41" s="18"/>
       <c r="K41" s="1" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="L41" s="14" t="s">
         <v>42</v>
@@ -50783,32 +50791,32 @@
     </row>
     <row r="42" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A42" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C42" s="15"/>
       <c r="D42" s="30" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="F42" s="30" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="G42" s="30" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H42" s="19"/>
       <c r="I42" s="18"/>
       <c r="J42" s="18"/>
       <c r="K42" s="1" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="L42" s="14" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="M42" s="4" t="s">
         <v>4</v>
@@ -50817,7 +50825,7 @@
         <v>12</v>
       </c>
       <c r="O42" s="3" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="P42" s="5"/>
       <c r="Q42" s="5"/>
@@ -50835,45 +50843,45 @@
     </row>
     <row r="43" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A43" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B43" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C43" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="D43" s="10" t="s">
+        <v>505</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>506</v>
+      </c>
+      <c r="F43" s="10" t="s">
         <v>507</v>
       </c>
-      <c r="E43" s="10" t="s">
+      <c r="G43" s="10" t="s">
         <v>508</v>
-      </c>
-      <c r="F43" s="10" t="s">
-        <v>509</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>510</v>
       </c>
       <c r="H43" s="10"/>
       <c r="I43" s="7"/>
       <c r="J43" s="38" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="L43" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N43" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O43" s="3" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="P43" s="5"/>
       <c r="Q43" s="5"/>
@@ -50891,13 +50899,13 @@
     </row>
     <row r="44" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B44" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C44" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
@@ -50906,22 +50914,22 @@
       <c r="H44" s="10"/>
       <c r="I44" s="7"/>
       <c r="J44" s="38" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="K44" s="8" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="L44" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N44" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O44" s="3" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="P44" s="5"/>
       <c r="Q44" s="5"/>
@@ -50939,45 +50947,45 @@
     </row>
     <row r="45" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B45" t="s">
+        <v>302</v>
+      </c>
+      <c r="C45" t="s">
+        <v>680</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>510</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="F45" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="C45" t="s">
-        <v>683</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>512</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>306</v>
-      </c>
       <c r="G45" s="7" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H45" s="7"/>
       <c r="I45" s="7"/>
       <c r="J45" s="38" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="L45" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N45" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O45" s="3" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="P45" s="5"/>
       <c r="Q45" s="5"/>
@@ -50995,13 +51003,13 @@
     </row>
     <row r="46" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B46" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C46" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
@@ -51010,22 +51018,22 @@
       <c r="H46" s="7"/>
       <c r="I46" s="7"/>
       <c r="J46" s="38" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="K46" s="8" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="L46" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N46" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O46" s="3" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="P46" s="5"/>
       <c r="Q46" s="5"/>
@@ -51043,41 +51051,41 @@
     </row>
     <row r="47" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B47" t="s">
+        <v>296</v>
+      </c>
+      <c r="C47" t="s">
+        <v>297</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>511</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>512</v>
+      </c>
+      <c r="F47" s="10" t="s">
+        <v>513</v>
+      </c>
+      <c r="G47" s="10" t="s">
         <v>298</v>
-      </c>
-      <c r="C47" t="s">
-        <v>299</v>
-      </c>
-      <c r="D47" s="10" t="s">
-        <v>513</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>514</v>
-      </c>
-      <c r="F47" s="10" t="s">
-        <v>515</v>
-      </c>
-      <c r="G47" s="10" t="s">
-        <v>300</v>
       </c>
       <c r="H47" s="10" t="s">
         <v>183</v>
       </c>
       <c r="I47" s="7"/>
       <c r="J47" s="38" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="K47" s="8" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="L47" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N47" s="4" t="s">
         <v>7</v>
@@ -51099,41 +51107,41 @@
     </row>
     <row r="48" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B48" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C48" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D48" s="10" t="s">
+        <v>514</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>515</v>
+      </c>
+      <c r="F48" s="10" t="s">
         <v>516</v>
       </c>
-      <c r="E48" s="10" t="s">
-        <v>517</v>
-      </c>
-      <c r="F48" s="10" t="s">
-        <v>518</v>
-      </c>
       <c r="G48" s="10" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H48" s="10" t="s">
         <v>183</v>
       </c>
       <c r="I48" s="7"/>
       <c r="J48" s="38" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="K48" s="8" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="L48" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N48" s="4" t="s">
         <v>7</v>
@@ -51155,41 +51163,41 @@
     </row>
     <row r="49" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B49" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C49" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="D49" s="10" t="s">
+        <v>517</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>518</v>
+      </c>
+      <c r="F49" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E49" s="10" t="s">
-        <v>520</v>
-      </c>
-      <c r="F49" s="10" t="s">
-        <v>521</v>
-      </c>
       <c r="G49" s="10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="H49" s="10" t="s">
         <v>183</v>
       </c>
       <c r="I49" s="7"/>
       <c r="J49" s="38" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="L49" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N49" s="4" t="s">
         <v>7</v>
@@ -51211,23 +51219,23 @@
     </row>
     <row r="50" spans="1:28" ht="226" x14ac:dyDescent="0.35">
       <c r="A50" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B50" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C50"/>
       <c r="D50" t="s">
+        <v>292</v>
+      </c>
+      <c r="E50" t="s">
+        <v>293</v>
+      </c>
+      <c r="F50" t="s">
         <v>294</v>
       </c>
-      <c r="E50" t="s">
+      <c r="G50" t="s">
         <v>295</v>
-      </c>
-      <c r="F50" t="s">
-        <v>296</v>
-      </c>
-      <c r="G50" t="s">
-        <v>297</v>
       </c>
       <c r="H50" s="10" t="s">
         <v>183</v>
@@ -51235,7 +51243,7 @@
       <c r="I50" s="7"/>
       <c r="J50" s="7"/>
       <c r="K50" s="1" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="L50" s="4" t="s">
         <v>2</v>
@@ -51263,39 +51271,39 @@
     </row>
     <row r="51" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A51" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B51" t="s">
+        <v>262</v>
+      </c>
+      <c r="C51" t="s">
+        <v>560</v>
+      </c>
+      <c r="D51" s="30" t="s">
         <v>264</v>
       </c>
-      <c r="C51" t="s">
-        <v>562</v>
-      </c>
-      <c r="D51" s="30" t="s">
+      <c r="E51" s="30" t="s">
+        <v>265</v>
+      </c>
+      <c r="F51" s="30" t="s">
         <v>266</v>
       </c>
-      <c r="E51" s="30" t="s">
+      <c r="G51" s="30" t="s">
         <v>267</v>
-      </c>
-      <c r="F51" s="30" t="s">
-        <v>268</v>
-      </c>
-      <c r="G51" s="30" t="s">
-        <v>269</v>
       </c>
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
       <c r="J51" s="38" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="K51" s="8" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="L51" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="N51" s="4" t="s">
         <v>7</v>
@@ -51317,39 +51325,39 @@
     </row>
     <row r="52" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A52" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B52" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C52" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="D52" s="30" t="s">
+        <v>268</v>
+      </c>
+      <c r="E52" s="30" t="s">
+        <v>269</v>
+      </c>
+      <c r="F52" s="30" t="s">
         <v>270</v>
       </c>
-      <c r="E52" s="30" t="s">
+      <c r="G52" s="30" t="s">
         <v>271</v>
-      </c>
-      <c r="F52" s="30" t="s">
-        <v>272</v>
-      </c>
-      <c r="G52" s="30" t="s">
-        <v>273</v>
       </c>
       <c r="H52" s="7"/>
       <c r="I52" s="7"/>
       <c r="J52" s="38" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="K52" s="8" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="L52" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="N52" s="4" t="s">
         <v>7</v>
@@ -51371,39 +51379,39 @@
     </row>
     <row r="53" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A53" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B53" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C53" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D53" s="30" t="s">
+        <v>268</v>
+      </c>
+      <c r="E53" s="30" t="s">
+        <v>269</v>
+      </c>
+      <c r="F53" s="30" t="s">
         <v>270</v>
       </c>
-      <c r="E53" s="30" t="s">
+      <c r="G53" s="30" t="s">
         <v>271</v>
-      </c>
-      <c r="F53" s="30" t="s">
-        <v>272</v>
-      </c>
-      <c r="G53" s="30" t="s">
-        <v>273</v>
       </c>
       <c r="H53" s="7"/>
       <c r="I53" s="7"/>
       <c r="J53" s="38" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="K53" s="8" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="L53" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N53" s="4" t="s">
         <v>7</v>
@@ -51425,39 +51433,39 @@
     </row>
     <row r="54" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A54" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B54" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C54" t="s">
+        <v>273</v>
+      </c>
+      <c r="D54" s="30" t="s">
+        <v>274</v>
+      </c>
+      <c r="E54" s="30" t="s">
         <v>275</v>
       </c>
-      <c r="D54" s="30" t="s">
+      <c r="F54" s="30" t="s">
         <v>276</v>
       </c>
-      <c r="E54" s="30" t="s">
+      <c r="G54" s="30" t="s">
         <v>277</v>
-      </c>
-      <c r="F54" s="30" t="s">
-        <v>278</v>
-      </c>
-      <c r="G54" s="30" t="s">
-        <v>279</v>
       </c>
       <c r="H54" s="7"/>
       <c r="I54" s="7"/>
       <c r="J54" s="38" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K54" s="8" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="L54" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N54" s="4" t="s">
         <v>7</v>
@@ -51479,39 +51487,39 @@
     </row>
     <row r="55" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B55" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C55" t="s">
+        <v>278</v>
+      </c>
+      <c r="D55" s="30" t="s">
+        <v>279</v>
+      </c>
+      <c r="E55" s="30" t="s">
         <v>280</v>
       </c>
-      <c r="D55" s="30" t="s">
-        <v>281</v>
-      </c>
-      <c r="E55" s="30" t="s">
+      <c r="F55" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="G55" s="30" t="s">
         <v>282</v>
-      </c>
-      <c r="F55" s="30" t="s">
-        <v>285</v>
-      </c>
-      <c r="G55" s="30" t="s">
-        <v>284</v>
       </c>
       <c r="H55" s="7"/>
       <c r="I55" s="7"/>
       <c r="J55" s="38" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K55" s="8" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="L55" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M55" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N55" s="4" t="s">
         <v>7</v>
@@ -51533,39 +51541,39 @@
     </row>
     <row r="56" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B56" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C56" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="D56" s="30" t="s">
+        <v>284</v>
+      </c>
+      <c r="E56" s="30" t="s">
+        <v>285</v>
+      </c>
+      <c r="F56" s="30" t="s">
+        <v>281</v>
+      </c>
+      <c r="G56" s="30" t="s">
         <v>286</v>
-      </c>
-      <c r="E56" s="30" t="s">
-        <v>287</v>
-      </c>
-      <c r="F56" s="30" t="s">
-        <v>283</v>
-      </c>
-      <c r="G56" s="30" t="s">
-        <v>288</v>
       </c>
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
       <c r="J56" s="38" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K56" s="8" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="L56" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M56" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N56" s="4" t="s">
         <v>7</v>
@@ -51587,39 +51595,39 @@
     </row>
     <row r="57" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A57" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B57" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C57" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="D57" s="30" t="s">
+        <v>287</v>
+      </c>
+      <c r="E57" s="30" t="s">
+        <v>288</v>
+      </c>
+      <c r="F57" s="30" t="s">
         <v>289</v>
       </c>
-      <c r="E57" s="30" t="s">
+      <c r="G57" s="30" t="s">
         <v>290</v>
-      </c>
-      <c r="F57" s="30" t="s">
-        <v>291</v>
-      </c>
-      <c r="G57" s="30" t="s">
-        <v>292</v>
       </c>
       <c r="H57" s="7"/>
       <c r="I57" s="7"/>
       <c r="J57" s="38" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K57" s="8" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="L57" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N57" s="4" t="s">
         <v>7</v>
@@ -51641,29 +51649,29 @@
     </row>
     <row r="58" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A58" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B58" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C58"/>
       <c r="D58" s="10" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H58" s="10"/>
       <c r="I58" s="7"/>
       <c r="J58" s="7"/>
       <c r="K58" s="1" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="L58" s="12"/>
       <c r="M58" s="4" t="s">
@@ -51673,7 +51681,7 @@
         <v>12</v>
       </c>
       <c r="O58" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="P58" s="5"/>
       <c r="Q58" s="5"/>
@@ -51691,32 +51699,32 @@
     </row>
     <row r="59" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A59" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B59" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C59"/>
       <c r="D59" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E59" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F59" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="H59" s="10"/>
       <c r="I59" s="7"/>
       <c r="J59" s="7"/>
       <c r="K59" s="1" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="L59" s="12" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="M59" s="4" t="s">
         <v>4</v>
@@ -51725,7 +51733,7 @@
         <v>12</v>
       </c>
       <c r="O59" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="P59" s="5"/>
       <c r="Q59" s="5"/>
@@ -51743,29 +51751,29 @@
     </row>
     <row r="60" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A60" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B60" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C60"/>
       <c r="D60" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E60" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G60" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="H60" s="7"/>
       <c r="I60" s="7"/>
       <c r="J60" s="7"/>
       <c r="K60" s="8" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="L60" s="4"/>
       <c r="M60" s="4" t="s">
@@ -51775,7 +51783,7 @@
         <v>12</v>
       </c>
       <c r="O60" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="P60" s="5"/>
       <c r="Q60" s="5"/>
@@ -51793,23 +51801,23 @@
     </row>
     <row r="61" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A61" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B61" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C61" s="10"/>
       <c r="D61" s="10" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="H61" s="10" t="s">
         <v>183</v>
@@ -51817,7 +51825,7 @@
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
       <c r="K61" s="8" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="L61" s="11" t="s">
         <v>10</v>
@@ -51845,29 +51853,29 @@
     </row>
     <row r="62" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A62" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B62" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C62"/>
       <c r="D62" t="s">
+        <v>327</v>
+      </c>
+      <c r="E62" t="s">
+        <v>328</v>
+      </c>
+      <c r="F62" s="7" t="s">
         <v>329</v>
       </c>
-      <c r="E62" t="s">
-        <v>330</v>
-      </c>
-      <c r="F62" s="7" t="s">
-        <v>331</v>
-      </c>
       <c r="G62" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="H62" s="7"/>
       <c r="I62" s="7"/>
       <c r="J62" s="7"/>
       <c r="K62" s="8" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="L62" s="4"/>
       <c r="M62" s="4" t="s">
@@ -51877,7 +51885,7 @@
         <v>12</v>
       </c>
       <c r="O62" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="P62" s="5"/>
       <c r="Q62" s="5"/>
@@ -51895,39 +51903,39 @@
     </row>
     <row r="63" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A63" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B63" t="s">
+        <v>330</v>
+      </c>
+      <c r="C63" t="s">
+        <v>297</v>
+      </c>
+      <c r="D63" s="10" t="s">
         <v>332</v>
       </c>
-      <c r="C63" t="s">
-        <v>299</v>
-      </c>
-      <c r="D63" s="10" t="s">
+      <c r="E63" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="G63" s="10" t="s">
         <v>334</v>
-      </c>
-      <c r="E63" s="10" t="s">
-        <v>335</v>
-      </c>
-      <c r="F63" s="10" t="s">
-        <v>333</v>
-      </c>
-      <c r="G63" s="10" t="s">
-        <v>336</v>
       </c>
       <c r="H63" s="10"/>
       <c r="I63" s="7"/>
       <c r="J63" s="38" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="K63" s="8" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="L63" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N63" s="4" t="s">
         <v>7</v>
@@ -51949,39 +51957,39 @@
     </row>
     <row r="64" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A64" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B64" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C64" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="H64" s="10"/>
       <c r="I64" s="7"/>
       <c r="J64" s="38" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K64" s="8" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="L64" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N64" s="4" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Closes #2534 fixed bug for INR Increased (#2553)
* 2534 fixed bug for INR Increased

* 2534 empty commit to trigger checks
</commit_message>
<xml_diff>
--- a/inst/adlb_grading/adlb_grading_spec.xlsx
+++ b/inst/adlb_grading/adlb_grading_spec.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="6090" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="6090" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NCICTCAEv4" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DAIDS!$C$1:$C$998</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">NCICTCAEv5!$B$1:$B$972</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="687">
   <si>
     <t>Anemia</t>
   </si>
@@ -773,12 +774,6 @@
   </si>
   <si>
     <t>A finding based on laboratory test results that indicate increased levels of hemoglobin above normal.</t>
-  </si>
-  <si>
-    <t>&gt;1.5 - 2.5 x ULN; &gt;1.5 - 2.5 x baseline if on anticoagulation; dose adjustment indicated</t>
-  </si>
-  <si>
-    <t>&gt;1.2 - 1.5 x ULN; &gt;1 - 1.5 x baseline if on anticoagulation; monitoring only indicated</t>
   </si>
   <si>
     <t>&gt;5.0 x ULN and with signs or symptoms</t>
@@ -2855,19 +2850,6 @@
   </si>
   <si>
     <t>case_when(
-is.na(AVAL) ~ NA_character_,
-!is.na(ANRHI) &amp; signif(AVAL, signif_dig) &gt; signif(2.5*ANRHI, signif_dig) ~ "3",
-!is.na(BASE) &amp; signif(AVAL, signif_dig) &gt; signif(2.5*BASE, signif_dig) ~ "3",
-!is.na(ANRHI) &amp; signif(AVAL, signif_dig) &gt; signif(1.5*ANRHI, signif_dig) ~ "2",
-!is.na(BASE) &amp; signif(AVAL, signif_dig) &gt; signif(1.5*BASE, signif_dig) ~ "2",
-!is.na(ANRHI) &amp; signif(AVAL, signif_dig) &gt; signif(1.2*ANRHI, signif_dig) ~ "1",
-!is.na(BASE) &amp; signif(AVAL, signif_dig) &gt; signif(BASE, signif_dig) ~ "1",
-!is.na(ANRHI) &amp; signif(AVAL, signif_dig) &lt;= signif(1.2*ANRHI, signif_dig) &amp; !is.na(BASE) &amp; signif(AVAL, signif_dig) &lt;= signif(BASE, signif_dig) ~ "0",
-is.na(ANRHI) | is.na(BASE) ~ NA_character_
-)</t>
-  </si>
-  <si>
-    <t>case_when(
 is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
 signif(AVAL, signif_dig) &gt; signif(5*ANRHI, signif_dig) ~ "4",
 signif(AVAL, signif_dig) &gt; signif(2*ANRHI, signif_dig) ~ "3",
@@ -2951,6 +2933,31 @@
 signif(AVAL, signif_dig) &lt; 0.65 ~ "1",
 signif(AVAL, signif_dig) &gt;= 0.65 ~ "0"
 )</t>
+  </si>
+  <si>
+    <t>&gt;1.2 - 1.5; &gt;1 - 1.5 x baseline if on anticoagulation; monitoring only indicated</t>
+  </si>
+  <si>
+    <t>&gt;1.5 - 2.5; &gt;1.5 - 2.5 x baseline if on anticoagulation; dose adjustment indicated</t>
+  </si>
+  <si>
+    <t>&gt;2.5; &gt;2.5 times above baseline if on anticoagulation</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+signif(AVAL, signif_dig) &gt; signif(2.5, signif_dig) ~ "3",
+!is.na(BASE) &amp; signif(AVAL, signif_dig) &gt; signif(2.5*BASE, signif_dig) ~ "3",
+signif(AVAL, signif_dig) &gt; signif(1.5, signif_dig) ~ "2",
+!is.na(BASE) &amp; signif(AVAL, signif_dig) &gt; signif(1.5*BASE, signif_dig) ~ "2",
+signif(AVAL, signif_dig) &gt; signif(1.2, signif_dig) ~ "1",
+!is.na(BASE) &amp; signif(AVAL, signif_dig) &gt; signif(BASE, signif_dig) ~ "1",
+signif(AVAL, signif_dig) &lt;= signif(1.2, signif_dig) &amp; !is.na(BASE) &amp; signif(AVAL, signif_dig) &lt;= signif(BASE, signif_dig) ~ "0",
+is.na(BASE) ~ NA_character_
+)</t>
+  </si>
+  <si>
+    <t>AVAL, BASE</t>
   </si>
 </sst>
 </file>
@@ -3529,7 +3536,7 @@
         <v>182</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>2</v>
@@ -3581,7 +3588,7 @@
         <v>11</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>10</v>
@@ -3633,7 +3640,7 @@
         <v>186</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
@@ -3683,7 +3690,7 @@
         <v>23</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
@@ -3733,7 +3740,7 @@
         <v>27</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
@@ -3783,7 +3790,7 @@
         <v>29</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4" t="s">
@@ -3833,7 +3840,7 @@
         <v>34</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="4" t="s">
@@ -3883,7 +3890,7 @@
         <v>39</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>10</v>
@@ -3935,7 +3942,7 @@
         <v>46</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="J10" s="14" t="s">
         <v>42</v>
@@ -3987,7 +3994,7 @@
         <v>51</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="4" t="s">
@@ -4037,7 +4044,7 @@
         <v>58</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="4" t="s">
@@ -4087,7 +4094,7 @@
         <v>63</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>2</v>
@@ -4139,7 +4146,7 @@
         <v>65</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="4" t="s">
@@ -4189,7 +4196,7 @@
         <v>68</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="J15" s="12"/>
       <c r="K15" s="4" t="s">
@@ -4239,7 +4246,7 @@
         <v>190</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>2</v>
@@ -4291,7 +4298,7 @@
         <v>77</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="J17" s="12"/>
       <c r="K17" s="4" t="s">
@@ -4343,7 +4350,7 @@
         <v>82</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="J18" s="12"/>
       <c r="K18" s="4" t="s">
@@ -4393,7 +4400,7 @@
         <v>86</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="J19" s="11" t="s">
         <v>10</v>
@@ -4445,7 +4452,7 @@
         <v>192</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="J20" s="11" t="s">
         <v>10</v>
@@ -4497,7 +4504,7 @@
         <v>95</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="J21" s="11" t="s">
         <v>10</v>
@@ -4549,7 +4556,7 @@
         <v>101</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="J22" s="11" t="s">
         <v>10</v>
@@ -4601,7 +4608,7 @@
         <v>103</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="J23" s="12"/>
       <c r="K23" s="4" t="s">
@@ -4651,7 +4658,7 @@
         <v>109</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="J24" s="11" t="s">
         <v>10</v>
@@ -4703,7 +4710,7 @@
         <v>198</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="J25" s="17" t="s">
         <v>212</v>
@@ -4757,7 +4764,7 @@
         <v>198</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="J26" s="17" t="s">
         <v>212</v>
@@ -4811,7 +4818,7 @@
         <v>199</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="J27" s="17" t="s">
         <v>212</v>
@@ -4865,7 +4872,7 @@
         <v>199</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="J28" s="17" t="s">
         <v>212</v>
@@ -4919,7 +4926,7 @@
         <v>200</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="J29" s="17" t="s">
         <v>212</v>
@@ -4971,7 +4978,7 @@
         <v>201</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="J30" s="17" t="s">
         <v>212</v>
@@ -5023,7 +5030,7 @@
         <v>202</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="J31" s="17" t="s">
         <v>212</v>
@@ -5075,7 +5082,7 @@
         <v>203</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="J32" s="17" t="s">
         <v>212</v>
@@ -5127,7 +5134,7 @@
         <v>204</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="J33" s="17" t="s">
         <v>219</v>
@@ -5181,7 +5188,7 @@
         <v>205</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="J34" s="17" t="s">
         <v>2</v>
@@ -5233,7 +5240,7 @@
         <v>206</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="J35" s="17" t="s">
         <v>212</v>
@@ -5287,7 +5294,7 @@
         <v>206</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="J36" s="17" t="s">
         <v>212</v>
@@ -5341,7 +5348,7 @@
         <v>207</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="J37" s="17" t="s">
         <v>212</v>
@@ -5393,7 +5400,7 @@
         <v>208</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="J38" s="17" t="s">
         <v>212</v>
@@ -5447,7 +5454,7 @@
         <v>209</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="J39" s="17" t="s">
         <v>212</v>
@@ -5499,7 +5506,7 @@
         <v>210</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="J40" s="17" t="s">
         <v>212</v>
@@ -5551,7 +5558,7 @@
         <v>211</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="J41" s="17" t="s">
         <v>212</v>
@@ -26135,8 +26142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z972"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -26230,7 +26237,7 @@
         <v>182</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>2</v>
@@ -26282,7 +26289,7 @@
         <v>11</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>10</v>
@@ -26334,7 +26341,7 @@
         <v>186</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
@@ -26384,7 +26391,7 @@
         <v>23</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
@@ -26434,7 +26441,7 @@
         <v>27</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
@@ -26484,7 +26491,7 @@
         <v>29</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4" t="s">
@@ -26534,7 +26541,7 @@
         <v>34</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="4" t="s">
@@ -26584,7 +26591,7 @@
         <v>39</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>10</v>
@@ -26636,7 +26643,7 @@
         <v>46</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="J10" s="14" t="s">
         <v>42</v>
@@ -26688,7 +26695,7 @@
         <v>51</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="4" t="s">
@@ -26738,7 +26745,7 @@
         <v>58</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="4" t="s">
@@ -26788,7 +26795,7 @@
         <v>63</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>2</v>
@@ -26840,7 +26847,7 @@
         <v>65</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="4" t="s">
@@ -26890,7 +26897,7 @@
         <v>68</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="J15" s="12"/>
       <c r="K15" s="4" t="s">
@@ -26940,7 +26947,7 @@
         <v>247</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>2</v>
@@ -26966,7 +26973,7 @@
       <c r="Y16" s="5"/>
       <c r="Z16" s="5"/>
     </row>
-    <row r="17" spans="1:26" ht="250.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" ht="238" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>185</v>
       </c>
@@ -26974,13 +26981,13 @@
         <v>73</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>249</v>
+        <v>682</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>248</v>
+        <v>683</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>76</v>
+        <v>684</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>183</v>
@@ -26992,11 +26999,11 @@
         <v>77</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>676</v>
+        <v>685</v>
       </c>
       <c r="J17" s="12"/>
       <c r="K17" s="4" t="s">
-        <v>15</v>
+        <v>686</v>
       </c>
       <c r="L17" s="4" t="s">
         <v>12</v>
@@ -27029,13 +27036,13 @@
         <v>14</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G18" s="17" t="s">
         <v>183</v>
@@ -27044,7 +27051,7 @@
         <v>82</v>
       </c>
       <c r="I18" s="26" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="J18" s="27"/>
       <c r="K18" s="27" t="s">
@@ -27054,7 +27061,7 @@
         <v>12</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="N18" s="28"/>
       <c r="O18" s="28"/>
@@ -27096,7 +27103,7 @@
         <v>86</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="J19" s="11" t="s">
         <v>10</v>
@@ -27148,7 +27155,7 @@
         <v>192</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="J20" s="11" t="s">
         <v>10</v>
@@ -27200,7 +27207,7 @@
         <v>95</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="J21" s="11" t="s">
         <v>10</v>
@@ -27252,7 +27259,7 @@
         <v>101</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="J22" s="11" t="s">
         <v>10</v>
@@ -27289,13 +27296,13 @@
         <v>14</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F23" s="24" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>183</v>
@@ -27304,7 +27311,7 @@
         <v>103</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="J23" s="12"/>
       <c r="K23" s="4" t="s">
@@ -27314,7 +27321,7 @@
         <v>12</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
@@ -27356,7 +27363,7 @@
         <v>109</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="J24" s="11" t="s">
         <v>10</v>
@@ -27408,7 +27415,7 @@
         <v>198</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="J25" s="17" t="s">
         <v>212</v>
@@ -27462,7 +27469,7 @@
         <v>198</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="J26" s="17" t="s">
         <v>212</v>
@@ -27501,7 +27508,7 @@
         <v>121</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E27" s="24" t="s">
         <v>123</v>
@@ -27516,7 +27523,7 @@
         <v>200</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="J27" s="17" t="s">
         <v>212</v>
@@ -27568,7 +27575,7 @@
         <v>201</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="J28" s="17" t="s">
         <v>212</v>
@@ -27605,7 +27612,7 @@
         <v>130</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E29" s="20" t="s">
         <v>132</v>
@@ -27620,7 +27627,7 @@
         <v>202</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="J29" s="17" t="s">
         <v>212</v>
@@ -27672,7 +27679,7 @@
         <v>203</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="J30" s="17" t="s">
         <v>212</v>
@@ -27706,16 +27713,16 @@
         <v>139</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D31" s="24" t="s">
         <v>197</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F31" s="22" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G31" s="19" t="s">
         <v>181</v>
@@ -27724,7 +27731,7 @@
         <v>204</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="J31" s="17"/>
       <c r="K31" s="4" t="s">
@@ -27776,7 +27783,7 @@
         <v>205</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="J32" s="17" t="s">
         <v>2</v>
@@ -27828,7 +27835,7 @@
         <v>206</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="J33" s="17" t="s">
         <v>212</v>
@@ -27882,7 +27889,7 @@
         <v>206</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="J34" s="17" t="s">
         <v>212</v>
@@ -27936,7 +27943,7 @@
         <v>207</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="J35" s="17" t="s">
         <v>212</v>
@@ -27973,7 +27980,7 @@
         <v>158</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E36" s="20" t="s">
         <v>160</v>
@@ -27988,7 +27995,7 @@
         <v>208</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="J36" s="17" t="s">
         <v>212</v>
@@ -28000,7 +28007,7 @@
         <v>7</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
@@ -28042,7 +28049,7 @@
         <v>209</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="J37" s="17" t="s">
         <v>212</v>
@@ -28079,10 +28086,10 @@
         <v>168</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F38" s="24" t="s">
         <v>170</v>
@@ -28094,7 +28101,7 @@
         <v>210</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="J38" s="17" t="s">
         <v>212</v>
@@ -28106,7 +28113,7 @@
         <v>7</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
@@ -48671,6 +48678,7 @@
       <c r="Z972" s="5"/>
     </row>
   </sheetData>
+  <autoFilter ref="B1:B972"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -48680,8 +48688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B33" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView topLeftCell="B33" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -48705,7 +48713,7 @@
         <v>193</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>224</v>
@@ -48726,7 +48734,7 @@
         <v>6</v>
       </c>
       <c r="J1" s="46" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>223</v>
@@ -48759,27 +48767,27 @@
     </row>
     <row r="2" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B2" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2"/>
       <c r="E2" t="s">
+        <v>540</v>
+      </c>
+      <c r="F2" t="s">
+        <v>541</v>
+      </c>
+      <c r="G2" t="s">
         <v>542</v>
-      </c>
-      <c r="F2" t="s">
-        <v>543</v>
-      </c>
-      <c r="G2" t="s">
-        <v>544</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="8" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="L2" s="4"/>
       <c r="M2" s="4" t="s">
@@ -48789,7 +48797,7 @@
         <v>7</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
@@ -48807,27 +48815,27 @@
     </row>
     <row r="3" spans="1:28" ht="126" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B3" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E3" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="G3" s="32"/>
       <c r="H3" s="10"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="8" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>2</v>
@@ -48855,29 +48863,29 @@
     </row>
     <row r="4" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B4" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="31" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G4" s="32" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="8" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4" t="s">
@@ -48903,27 +48911,27 @@
     </row>
     <row r="5" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B5" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5"/>
       <c r="E5" t="s">
+        <v>545</v>
+      </c>
+      <c r="F5" t="s">
+        <v>546</v>
+      </c>
+      <c r="G5" t="s">
         <v>547</v>
-      </c>
-      <c r="F5" t="s">
-        <v>548</v>
-      </c>
-      <c r="G5" t="s">
-        <v>549</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="4" t="s">
@@ -48933,7 +48941,7 @@
         <v>12</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
@@ -48951,29 +48959,29 @@
     </row>
     <row r="6" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B6" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="8" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4" t="s">
@@ -48999,29 +49007,29 @@
     </row>
     <row r="7" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B7" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="33" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G7" s="33" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="1" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="L7" s="12"/>
       <c r="M7" s="4" t="s">
@@ -49047,29 +49055,29 @@
     </row>
     <row r="8" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B8" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="8" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4" t="s">
@@ -49095,29 +49103,29 @@
     </row>
     <row r="9" spans="1:28" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B9" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="8" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>42</v>
@@ -49145,39 +49153,39 @@
     </row>
     <row r="10" spans="1:28" s="44" customFormat="1" ht="101" x14ac:dyDescent="0.35">
       <c r="A10" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="32"/>
       <c r="F10" s="37" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="H10" s="36"/>
       <c r="I10" s="38"/>
       <c r="J10" s="38" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="K10" s="39" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="L10" s="40"/>
       <c r="M10" s="4" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="N10" s="41" t="s">
         <v>12</v>
       </c>
       <c r="O10" s="37" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="P10" s="43"/>
       <c r="Q10" s="43"/>
@@ -49195,44 +49203,44 @@
     </row>
     <row r="11" spans="1:28" s="44" customFormat="1" ht="151" x14ac:dyDescent="0.35">
       <c r="A11" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B11" s="37" t="s">
+        <v>359</v>
+      </c>
+      <c r="C11" s="37" t="s">
         <v>361</v>
       </c>
-      <c r="C11" s="37" t="s">
-        <v>363</v>
-      </c>
       <c r="D11" s="32" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F11" s="32" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="G11" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="H11"/>
       <c r="J11" s="38" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="K11" s="39" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="L11" s="40" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="N11" s="41" t="s">
         <v>12</v>
       </c>
       <c r="O11" s="42" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="P11" s="43"/>
       <c r="Q11" s="43"/>
@@ -49250,37 +49258,37 @@
     </row>
     <row r="12" spans="1:28" s="44" customFormat="1" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A12" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B12" t="s">
+        <v>369</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>360</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>372</v>
+      </c>
+      <c r="E12" s="34" t="s">
         <v>371</v>
       </c>
-      <c r="C12" s="37" t="s">
-        <v>362</v>
-      </c>
-      <c r="D12" s="33" t="s">
-        <v>374</v>
-      </c>
-      <c r="E12" s="34" t="s">
-        <v>373</v>
-      </c>
       <c r="F12" s="33" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="G12" s="33" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="H12" s="36"/>
       <c r="I12" s="38"/>
       <c r="J12" s="38" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="L12" s="40"/>
       <c r="M12" s="4" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="N12" s="41" t="s">
         <v>12</v>
@@ -49302,13 +49310,13 @@
     </row>
     <row r="13" spans="1:28" s="44" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B13" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D13" s="33"/>
       <c r="E13" s="34"/>
@@ -49317,20 +49325,20 @@
       <c r="H13" s="36"/>
       <c r="I13" s="38"/>
       <c r="J13" s="38" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="L13" s="40"/>
       <c r="M13" s="4" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="N13" s="41" t="s">
         <v>12</v>
       </c>
       <c r="O13" s="37" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="P13" s="43"/>
       <c r="Q13" s="43"/>
@@ -49348,39 +49356,39 @@
     </row>
     <row r="14" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A14" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B14" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="C14" t="s">
+        <v>556</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>379</v>
+      </c>
+      <c r="E14" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="C14" t="s">
-        <v>558</v>
-      </c>
-      <c r="D14" s="19" t="s">
+      <c r="F14" s="19" t="s">
         <v>381</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="G14" s="19" t="s">
         <v>382</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>383</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>384</v>
       </c>
       <c r="H14" s="19"/>
       <c r="I14" s="18"/>
       <c r="J14" s="38" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="L14" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N14" s="4" t="s">
         <v>12</v>
@@ -49402,39 +49410,39 @@
     </row>
     <row r="15" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A15" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C15" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="18"/>
       <c r="J15" s="38" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="L15" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>12</v>
@@ -49456,29 +49464,29 @@
     </row>
     <row r="16" spans="1:28" ht="138" x14ac:dyDescent="0.3">
       <c r="A16" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="19" t="s">
+        <v>374</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>377</v>
+      </c>
+      <c r="F16" s="19" t="s">
         <v>376</v>
       </c>
-      <c r="E16" s="19" t="s">
-        <v>379</v>
-      </c>
-      <c r="F16" s="19" t="s">
-        <v>378</v>
-      </c>
       <c r="G16" s="19" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
       <c r="K16" s="1" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="L16" s="14" t="s">
         <v>42</v>
@@ -49506,39 +49514,39 @@
     </row>
     <row r="17" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A17" s="45" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B17" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C17" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="D17" t="s">
+        <v>391</v>
+      </c>
+      <c r="E17" t="s">
+        <v>392</v>
+      </c>
+      <c r="F17" t="s">
         <v>393</v>
       </c>
-      <c r="E17" t="s">
+      <c r="G17" t="s">
         <v>394</v>
-      </c>
-      <c r="F17" t="s">
-        <v>395</v>
-      </c>
-      <c r="G17" t="s">
-        <v>396</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="18"/>
       <c r="J17" s="38" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="L17" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>7</v>
@@ -49560,39 +49568,39 @@
     </row>
     <row r="18" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A18" s="45" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B18" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C18" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D18" t="s">
+        <v>395</v>
+      </c>
+      <c r="E18" t="s">
+        <v>396</v>
+      </c>
+      <c r="F18" t="s">
         <v>397</v>
       </c>
-      <c r="E18" t="s">
+      <c r="G18" t="s">
         <v>398</v>
-      </c>
-      <c r="F18" t="s">
-        <v>399</v>
-      </c>
-      <c r="G18" t="s">
-        <v>400</v>
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="18"/>
       <c r="J18" s="38" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="L18" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N18" s="4" t="s">
         <v>7</v>
@@ -49614,29 +49622,29 @@
     </row>
     <row r="19" spans="1:28" ht="138.5" x14ac:dyDescent="0.35">
       <c r="A19" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B19" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
+        <v>387</v>
+      </c>
+      <c r="E19" t="s">
+        <v>388</v>
+      </c>
+      <c r="F19" t="s">
         <v>389</v>
       </c>
-      <c r="E19" t="s">
+      <c r="G19" t="s">
         <v>390</v>
-      </c>
-      <c r="F19" t="s">
-        <v>391</v>
-      </c>
-      <c r="G19" t="s">
-        <v>392</v>
       </c>
       <c r="H19" s="19"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="1" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="L19" s="14" t="s">
         <v>42</v>
@@ -49664,29 +49672,29 @@
     </row>
     <row r="20" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A20" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B20" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="1" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="L20" s="12"/>
       <c r="M20" s="4" t="s">
@@ -49712,29 +49720,29 @@
     </row>
     <row r="21" spans="1:28" ht="251" x14ac:dyDescent="0.35">
       <c r="A21" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B21" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="E21" t="s">
+        <v>406</v>
+      </c>
+      <c r="F21" t="s">
         <v>407</v>
       </c>
-      <c r="E21" t="s">
-        <v>408</v>
-      </c>
-      <c r="F21" t="s">
-        <v>409</v>
-      </c>
       <c r="G21" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="H21" s="10"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
       <c r="K21" s="1" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="L21" s="12"/>
       <c r="M21" s="4" t="s">
@@ -49760,29 +49768,29 @@
     </row>
     <row r="22" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A22" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B22" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C22" s="16"/>
       <c r="D22" t="s">
+        <v>409</v>
+      </c>
+      <c r="E22" t="s">
+        <v>410</v>
+      </c>
+      <c r="F22" t="s">
         <v>411</v>
       </c>
-      <c r="E22" t="s">
-        <v>412</v>
-      </c>
-      <c r="F22" t="s">
-        <v>413</v>
-      </c>
       <c r="G22" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="18"/>
       <c r="J22" s="18"/>
       <c r="K22" s="1" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="L22" s="14" t="s">
         <v>42</v>
@@ -49810,29 +49818,29 @@
     </row>
     <row r="23" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A23" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B23" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C23" s="16"/>
       <c r="D23" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E23" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F23" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="G23" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="H23" s="20"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="K23" s="1" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="L23" s="14" t="s">
         <v>42</v>
@@ -49860,39 +49868,39 @@
     </row>
     <row r="24" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A24" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B24" t="s">
+        <v>415</v>
+      </c>
+      <c r="C24" t="s">
+        <v>416</v>
+      </c>
+      <c r="D24" t="s">
         <v>417</v>
       </c>
-      <c r="C24" t="s">
+      <c r="E24" t="s">
         <v>418</v>
       </c>
-      <c r="D24" t="s">
+      <c r="F24" t="s">
         <v>419</v>
       </c>
-      <c r="E24" t="s">
+      <c r="G24" t="s">
         <v>420</v>
-      </c>
-      <c r="F24" t="s">
-        <v>421</v>
-      </c>
-      <c r="G24" t="s">
-        <v>422</v>
       </c>
       <c r="H24" s="20"/>
       <c r="I24" s="18"/>
       <c r="J24" s="38" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="L24" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="N24" s="4" t="s">
         <v>7</v>
@@ -49914,39 +49922,39 @@
     </row>
     <row r="25" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A25" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B25" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C25" s="30" t="s">
+        <v>421</v>
+      </c>
+      <c r="D25" s="30" t="s">
         <v>423</v>
       </c>
-      <c r="D25" s="30" t="s">
-        <v>425</v>
-      </c>
       <c r="E25" s="30" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F25" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="G25" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="H25" s="20"/>
       <c r="I25" s="18"/>
       <c r="J25" s="38" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="L25" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="N25" s="4" t="s">
         <v>7</v>
@@ -49968,28 +49976,28 @@
     </row>
     <row r="26" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A26" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B26" s="30" t="s">
+        <v>424</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>425</v>
+      </c>
+      <c r="E26" s="30" t="s">
         <v>426</v>
       </c>
-      <c r="D26" s="30" t="s">
+      <c r="F26" s="35" t="s">
         <v>427</v>
       </c>
-      <c r="E26" s="30" t="s">
+      <c r="G26" s="30" t="s">
         <v>428</v>
-      </c>
-      <c r="F26" s="35" t="s">
-        <v>429</v>
-      </c>
-      <c r="G26" s="30" t="s">
-        <v>430</v>
       </c>
       <c r="H26" s="20"/>
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
       <c r="K26" s="1" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="L26" s="14"/>
       <c r="M26" s="4" t="s">
@@ -49999,7 +50007,7 @@
         <v>12</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
@@ -50017,29 +50025,29 @@
     </row>
     <row r="27" spans="1:28" s="29" customFormat="1" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A27" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C27" s="17"/>
       <c r="D27" s="30" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="F27" s="33" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="H27" s="17"/>
       <c r="I27" s="17"/>
       <c r="J27" s="17"/>
       <c r="K27" s="26" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="L27" s="27"/>
       <c r="M27" s="27" t="s">
@@ -50065,37 +50073,37 @@
     </row>
     <row r="28" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A28" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B28" t="s">
+        <v>434</v>
+      </c>
+      <c r="C28" t="s">
+        <v>435</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>438</v>
+      </c>
+      <c r="E28" s="30" t="s">
+        <v>437</v>
+      </c>
+      <c r="F28" s="10" t="s">
         <v>436</v>
-      </c>
-      <c r="C28" t="s">
-        <v>437</v>
-      </c>
-      <c r="D28" s="30" t="s">
-        <v>440</v>
-      </c>
-      <c r="E28" s="30" t="s">
-        <v>439</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>438</v>
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
       <c r="I28" s="7"/>
       <c r="J28" s="38" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="L28" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>12</v>
@@ -50117,37 +50125,37 @@
     </row>
     <row r="29" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A29" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B29" t="s">
+        <v>434</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>439</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>441</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>440</v>
+      </c>
+      <c r="F29" s="10" t="s">
         <v>436</v>
-      </c>
-      <c r="C29" s="30" t="s">
-        <v>441</v>
-      </c>
-      <c r="D29" s="30" t="s">
-        <v>443</v>
-      </c>
-      <c r="E29" s="30" t="s">
-        <v>442</v>
-      </c>
-      <c r="F29" s="10" t="s">
-        <v>438</v>
       </c>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
       <c r="I29" s="7"/>
       <c r="J29" s="38" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="L29" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="N29" s="4" t="s">
         <v>12</v>
@@ -50169,37 +50177,37 @@
     </row>
     <row r="30" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A30" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B30" s="30" t="s">
+        <v>442</v>
+      </c>
+      <c r="C30" t="s">
+        <v>435</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>443</v>
+      </c>
+      <c r="E30" s="30" t="s">
         <v>444</v>
       </c>
-      <c r="C30" t="s">
-        <v>437</v>
-      </c>
-      <c r="D30" s="30" t="s">
+      <c r="F30" s="30" t="s">
         <v>445</v>
-      </c>
-      <c r="E30" s="30" t="s">
-        <v>446</v>
-      </c>
-      <c r="F30" s="30" t="s">
-        <v>447</v>
       </c>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
       <c r="I30" s="7"/>
       <c r="J30" s="38" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="L30" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="N30" s="4" t="s">
         <v>12</v>
@@ -50221,37 +50229,37 @@
     </row>
     <row r="31" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A31" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C31" s="30" t="s">
+        <v>446</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>447</v>
+      </c>
+      <c r="E31" s="30" t="s">
         <v>448</v>
       </c>
-      <c r="D31" s="30" t="s">
-        <v>449</v>
-      </c>
-      <c r="E31" s="30" t="s">
-        <v>450</v>
-      </c>
       <c r="F31" s="30" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
       <c r="I31" s="7"/>
       <c r="J31" s="38" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="K31" s="8" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="L31" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="N31" s="4" t="s">
         <v>12</v>
@@ -50273,13 +50281,13 @@
     </row>
     <row r="32" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A32" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C32" s="47" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="D32" s="30"/>
       <c r="E32" s="30"/>
@@ -50288,22 +50296,22 @@
       <c r="H32" s="10"/>
       <c r="I32" s="7"/>
       <c r="J32" s="38" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="L32" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="N32" s="4" t="s">
         <v>12</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
@@ -50321,29 +50329,29 @@
     </row>
     <row r="33" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A33" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C33" s="16"/>
       <c r="D33" s="30" t="s">
+        <v>450</v>
+      </c>
+      <c r="E33" s="30" t="s">
+        <v>451</v>
+      </c>
+      <c r="F33" s="30" t="s">
         <v>452</v>
       </c>
-      <c r="E33" s="30" t="s">
+      <c r="G33" s="30" t="s">
         <v>453</v>
-      </c>
-      <c r="F33" s="30" t="s">
-        <v>454</v>
-      </c>
-      <c r="G33" s="30" t="s">
-        <v>455</v>
       </c>
       <c r="H33" s="20"/>
       <c r="I33" s="18"/>
       <c r="J33" s="18"/>
       <c r="K33" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="L33" s="14" t="s">
         <v>42</v>
@@ -50371,29 +50379,29 @@
     </row>
     <row r="34" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A34" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C34" s="16"/>
       <c r="D34" s="30" t="s">
+        <v>455</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>456</v>
+      </c>
+      <c r="F34" s="30" t="s">
         <v>457</v>
       </c>
-      <c r="E34" s="30" t="s">
+      <c r="G34" s="30" t="s">
         <v>458</v>
-      </c>
-      <c r="F34" s="30" t="s">
-        <v>459</v>
-      </c>
-      <c r="G34" s="30" t="s">
-        <v>460</v>
       </c>
       <c r="H34" s="20"/>
       <c r="I34" s="18"/>
       <c r="J34" s="18"/>
       <c r="K34" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="L34" s="14" t="s">
         <v>42</v>
@@ -50421,39 +50429,39 @@
     </row>
     <row r="35" spans="1:28" ht="151" x14ac:dyDescent="0.35">
       <c r="A35" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B35" s="30" t="s">
+        <v>459</v>
+      </c>
+      <c r="C35" s="30" t="s">
+        <v>460</v>
+      </c>
+      <c r="D35" s="30" t="s">
         <v>461</v>
       </c>
-      <c r="C35" s="30" t="s">
+      <c r="E35" s="30" t="s">
         <v>462</v>
       </c>
-      <c r="D35" s="30" t="s">
+      <c r="F35" s="30" t="s">
         <v>463</v>
       </c>
-      <c r="E35" s="30" t="s">
+      <c r="G35" s="30" t="s">
         <v>464</v>
-      </c>
-      <c r="F35" s="30" t="s">
-        <v>465</v>
-      </c>
-      <c r="G35" s="30" t="s">
-        <v>466</v>
       </c>
       <c r="H35" s="20"/>
       <c r="I35" s="18"/>
       <c r="J35" s="38" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="L35" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>7</v>
@@ -50475,39 +50483,39 @@
     </row>
     <row r="36" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A36" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C36" s="30" t="s">
+        <v>465</v>
+      </c>
+      <c r="D36" s="30" t="s">
+        <v>469</v>
+      </c>
+      <c r="E36" s="30" t="s">
+        <v>468</v>
+      </c>
+      <c r="F36" s="30" t="s">
         <v>467</v>
       </c>
-      <c r="D36" s="30" t="s">
-        <v>471</v>
-      </c>
-      <c r="E36" s="30" t="s">
-        <v>470</v>
-      </c>
-      <c r="F36" s="30" t="s">
-        <v>469</v>
-      </c>
       <c r="G36" s="30" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="H36" s="20"/>
       <c r="I36" s="18"/>
       <c r="J36" s="38" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="L36" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="N36" s="4" t="s">
         <v>7</v>
@@ -50529,39 +50537,39 @@
     </row>
     <row r="37" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A37" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B37" s="30" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C37" s="30" t="s">
+        <v>470</v>
+      </c>
+      <c r="D37" s="30" t="s">
         <v>472</v>
       </c>
-      <c r="D37" s="30" t="s">
-        <v>474</v>
-      </c>
       <c r="E37" s="30" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="F37" s="30" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="G37" s="30" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="H37" s="20"/>
       <c r="I37" s="18"/>
       <c r="J37" s="38" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L37" s="14" t="s">
         <v>42</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="N37" s="4" t="s">
         <v>7</v>
@@ -50583,29 +50591,29 @@
     </row>
     <row r="38" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A38" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B38" s="30" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C38" s="30"/>
       <c r="D38" s="30" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="F38" s="30" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="G38" s="30" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="H38" s="20"/>
       <c r="I38" s="18"/>
       <c r="J38" s="18"/>
       <c r="K38" s="1" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="L38" s="14" t="s">
         <v>42</v>
@@ -50633,29 +50641,29 @@
     </row>
     <row r="39" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A39" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B39" s="30" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C39" s="30"/>
       <c r="D39" s="30" t="s">
+        <v>474</v>
+      </c>
+      <c r="E39" s="30" t="s">
+        <v>477</v>
+      </c>
+      <c r="F39" s="30" t="s">
         <v>476</v>
       </c>
-      <c r="E39" s="30" t="s">
-        <v>479</v>
-      </c>
-      <c r="F39" s="30" t="s">
-        <v>478</v>
-      </c>
       <c r="G39" s="30" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="H39" s="20"/>
       <c r="I39" s="18"/>
       <c r="J39" s="18"/>
       <c r="K39" s="1" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L39" s="14" t="s">
         <v>42</v>
@@ -50683,29 +50691,29 @@
     </row>
     <row r="40" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A40" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B40" s="30" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C40" s="16"/>
       <c r="D40" s="30" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="F40" s="30" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="G40" s="20" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="H40" s="20"/>
       <c r="I40" s="18"/>
       <c r="J40" s="18"/>
       <c r="K40" s="1" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="L40" s="14" t="s">
         <v>42</v>
@@ -50733,29 +50741,29 @@
     </row>
     <row r="41" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A41" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C41" s="16"/>
       <c r="D41" s="30" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="F41" s="30" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G41" s="33" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="H41" s="20"/>
       <c r="I41" s="18"/>
       <c r="J41" s="18"/>
       <c r="K41" s="1" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="L41" s="14" t="s">
         <v>42</v>
@@ -50783,32 +50791,32 @@
     </row>
     <row r="42" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A42" s="36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C42" s="15"/>
       <c r="D42" s="30" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="F42" s="30" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="G42" s="30" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H42" s="19"/>
       <c r="I42" s="18"/>
       <c r="J42" s="18"/>
       <c r="K42" s="1" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="L42" s="14" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="M42" s="4" t="s">
         <v>4</v>
@@ -50817,7 +50825,7 @@
         <v>12</v>
       </c>
       <c r="O42" s="3" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="P42" s="5"/>
       <c r="Q42" s="5"/>
@@ -50835,45 +50843,45 @@
     </row>
     <row r="43" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A43" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B43" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C43" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="D43" s="10" t="s">
+        <v>505</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>506</v>
+      </c>
+      <c r="F43" s="10" t="s">
         <v>507</v>
       </c>
-      <c r="E43" s="10" t="s">
+      <c r="G43" s="10" t="s">
         <v>508</v>
-      </c>
-      <c r="F43" s="10" t="s">
-        <v>509</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>510</v>
       </c>
       <c r="H43" s="10"/>
       <c r="I43" s="7"/>
       <c r="J43" s="38" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="L43" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N43" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O43" s="3" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="P43" s="5"/>
       <c r="Q43" s="5"/>
@@ -50891,13 +50899,13 @@
     </row>
     <row r="44" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B44" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C44" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
@@ -50906,22 +50914,22 @@
       <c r="H44" s="10"/>
       <c r="I44" s="7"/>
       <c r="J44" s="38" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="K44" s="8" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="L44" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N44" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O44" s="3" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="P44" s="5"/>
       <c r="Q44" s="5"/>
@@ -50939,45 +50947,45 @@
     </row>
     <row r="45" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B45" t="s">
+        <v>302</v>
+      </c>
+      <c r="C45" t="s">
+        <v>680</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>510</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="F45" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="C45" t="s">
-        <v>683</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>512</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>306</v>
-      </c>
       <c r="G45" s="7" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H45" s="7"/>
       <c r="I45" s="7"/>
       <c r="J45" s="38" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="L45" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N45" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O45" s="3" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="P45" s="5"/>
       <c r="Q45" s="5"/>
@@ -50995,13 +51003,13 @@
     </row>
     <row r="46" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B46" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C46" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
@@ -51010,22 +51018,22 @@
       <c r="H46" s="7"/>
       <c r="I46" s="7"/>
       <c r="J46" s="38" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="K46" s="8" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="L46" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N46" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O46" s="3" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="P46" s="5"/>
       <c r="Q46" s="5"/>
@@ -51043,41 +51051,41 @@
     </row>
     <row r="47" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B47" t="s">
+        <v>296</v>
+      </c>
+      <c r="C47" t="s">
+        <v>297</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>511</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>512</v>
+      </c>
+      <c r="F47" s="10" t="s">
+        <v>513</v>
+      </c>
+      <c r="G47" s="10" t="s">
         <v>298</v>
-      </c>
-      <c r="C47" t="s">
-        <v>299</v>
-      </c>
-      <c r="D47" s="10" t="s">
-        <v>513</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>514</v>
-      </c>
-      <c r="F47" s="10" t="s">
-        <v>515</v>
-      </c>
-      <c r="G47" s="10" t="s">
-        <v>300</v>
       </c>
       <c r="H47" s="10" t="s">
         <v>183</v>
       </c>
       <c r="I47" s="7"/>
       <c r="J47" s="38" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="K47" s="8" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="L47" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N47" s="4" t="s">
         <v>7</v>
@@ -51099,41 +51107,41 @@
     </row>
     <row r="48" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B48" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C48" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D48" s="10" t="s">
+        <v>514</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>515</v>
+      </c>
+      <c r="F48" s="10" t="s">
         <v>516</v>
       </c>
-      <c r="E48" s="10" t="s">
-        <v>517</v>
-      </c>
-      <c r="F48" s="10" t="s">
-        <v>518</v>
-      </c>
       <c r="G48" s="10" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H48" s="10" t="s">
         <v>183</v>
       </c>
       <c r="I48" s="7"/>
       <c r="J48" s="38" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="K48" s="8" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="L48" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N48" s="4" t="s">
         <v>7</v>
@@ -51155,41 +51163,41 @@
     </row>
     <row r="49" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B49" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C49" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="D49" s="10" t="s">
+        <v>517</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>518</v>
+      </c>
+      <c r="F49" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E49" s="10" t="s">
-        <v>520</v>
-      </c>
-      <c r="F49" s="10" t="s">
-        <v>521</v>
-      </c>
       <c r="G49" s="10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="H49" s="10" t="s">
         <v>183</v>
       </c>
       <c r="I49" s="7"/>
       <c r="J49" s="38" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="L49" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N49" s="4" t="s">
         <v>7</v>
@@ -51211,23 +51219,23 @@
     </row>
     <row r="50" spans="1:28" ht="226" x14ac:dyDescent="0.35">
       <c r="A50" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B50" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C50"/>
       <c r="D50" t="s">
+        <v>292</v>
+      </c>
+      <c r="E50" t="s">
+        <v>293</v>
+      </c>
+      <c r="F50" t="s">
         <v>294</v>
       </c>
-      <c r="E50" t="s">
+      <c r="G50" t="s">
         <v>295</v>
-      </c>
-      <c r="F50" t="s">
-        <v>296</v>
-      </c>
-      <c r="G50" t="s">
-        <v>297</v>
       </c>
       <c r="H50" s="10" t="s">
         <v>183</v>
@@ -51235,7 +51243,7 @@
       <c r="I50" s="7"/>
       <c r="J50" s="7"/>
       <c r="K50" s="1" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="L50" s="4" t="s">
         <v>2</v>
@@ -51263,39 +51271,39 @@
     </row>
     <row r="51" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A51" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B51" t="s">
+        <v>262</v>
+      </c>
+      <c r="C51" t="s">
+        <v>560</v>
+      </c>
+      <c r="D51" s="30" t="s">
         <v>264</v>
       </c>
-      <c r="C51" t="s">
-        <v>562</v>
-      </c>
-      <c r="D51" s="30" t="s">
+      <c r="E51" s="30" t="s">
+        <v>265</v>
+      </c>
+      <c r="F51" s="30" t="s">
         <v>266</v>
       </c>
-      <c r="E51" s="30" t="s">
+      <c r="G51" s="30" t="s">
         <v>267</v>
-      </c>
-      <c r="F51" s="30" t="s">
-        <v>268</v>
-      </c>
-      <c r="G51" s="30" t="s">
-        <v>269</v>
       </c>
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
       <c r="J51" s="38" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="K51" s="8" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="L51" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="N51" s="4" t="s">
         <v>7</v>
@@ -51317,39 +51325,39 @@
     </row>
     <row r="52" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A52" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B52" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C52" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="D52" s="30" t="s">
+        <v>268</v>
+      </c>
+      <c r="E52" s="30" t="s">
+        <v>269</v>
+      </c>
+      <c r="F52" s="30" t="s">
         <v>270</v>
       </c>
-      <c r="E52" s="30" t="s">
+      <c r="G52" s="30" t="s">
         <v>271</v>
-      </c>
-      <c r="F52" s="30" t="s">
-        <v>272</v>
-      </c>
-      <c r="G52" s="30" t="s">
-        <v>273</v>
       </c>
       <c r="H52" s="7"/>
       <c r="I52" s="7"/>
       <c r="J52" s="38" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="K52" s="8" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="L52" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="N52" s="4" t="s">
         <v>7</v>
@@ -51371,39 +51379,39 @@
     </row>
     <row r="53" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A53" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B53" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C53" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D53" s="30" t="s">
+        <v>268</v>
+      </c>
+      <c r="E53" s="30" t="s">
+        <v>269</v>
+      </c>
+      <c r="F53" s="30" t="s">
         <v>270</v>
       </c>
-      <c r="E53" s="30" t="s">
+      <c r="G53" s="30" t="s">
         <v>271</v>
-      </c>
-      <c r="F53" s="30" t="s">
-        <v>272</v>
-      </c>
-      <c r="G53" s="30" t="s">
-        <v>273</v>
       </c>
       <c r="H53" s="7"/>
       <c r="I53" s="7"/>
       <c r="J53" s="38" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="K53" s="8" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="L53" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N53" s="4" t="s">
         <v>7</v>
@@ -51425,39 +51433,39 @@
     </row>
     <row r="54" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A54" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B54" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C54" t="s">
+        <v>273</v>
+      </c>
+      <c r="D54" s="30" t="s">
+        <v>274</v>
+      </c>
+      <c r="E54" s="30" t="s">
         <v>275</v>
       </c>
-      <c r="D54" s="30" t="s">
+      <c r="F54" s="30" t="s">
         <v>276</v>
       </c>
-      <c r="E54" s="30" t="s">
+      <c r="G54" s="30" t="s">
         <v>277</v>
-      </c>
-      <c r="F54" s="30" t="s">
-        <v>278</v>
-      </c>
-      <c r="G54" s="30" t="s">
-        <v>279</v>
       </c>
       <c r="H54" s="7"/>
       <c r="I54" s="7"/>
       <c r="J54" s="38" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K54" s="8" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="L54" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N54" s="4" t="s">
         <v>7</v>
@@ -51479,39 +51487,39 @@
     </row>
     <row r="55" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B55" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C55" t="s">
+        <v>278</v>
+      </c>
+      <c r="D55" s="30" t="s">
+        <v>279</v>
+      </c>
+      <c r="E55" s="30" t="s">
         <v>280</v>
       </c>
-      <c r="D55" s="30" t="s">
-        <v>281</v>
-      </c>
-      <c r="E55" s="30" t="s">
+      <c r="F55" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="G55" s="30" t="s">
         <v>282</v>
-      </c>
-      <c r="F55" s="30" t="s">
-        <v>285</v>
-      </c>
-      <c r="G55" s="30" t="s">
-        <v>284</v>
       </c>
       <c r="H55" s="7"/>
       <c r="I55" s="7"/>
       <c r="J55" s="38" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K55" s="8" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="L55" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M55" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N55" s="4" t="s">
         <v>7</v>
@@ -51533,39 +51541,39 @@
     </row>
     <row r="56" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B56" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C56" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="D56" s="30" t="s">
+        <v>284</v>
+      </c>
+      <c r="E56" s="30" t="s">
+        <v>285</v>
+      </c>
+      <c r="F56" s="30" t="s">
+        <v>281</v>
+      </c>
+      <c r="G56" s="30" t="s">
         <v>286</v>
-      </c>
-      <c r="E56" s="30" t="s">
-        <v>287</v>
-      </c>
-      <c r="F56" s="30" t="s">
-        <v>283</v>
-      </c>
-      <c r="G56" s="30" t="s">
-        <v>288</v>
       </c>
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
       <c r="J56" s="38" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K56" s="8" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="L56" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M56" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N56" s="4" t="s">
         <v>7</v>
@@ -51587,39 +51595,39 @@
     </row>
     <row r="57" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A57" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B57" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C57" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="D57" s="30" t="s">
+        <v>287</v>
+      </c>
+      <c r="E57" s="30" t="s">
+        <v>288</v>
+      </c>
+      <c r="F57" s="30" t="s">
         <v>289</v>
       </c>
-      <c r="E57" s="30" t="s">
+      <c r="G57" s="30" t="s">
         <v>290</v>
-      </c>
-      <c r="F57" s="30" t="s">
-        <v>291</v>
-      </c>
-      <c r="G57" s="30" t="s">
-        <v>292</v>
       </c>
       <c r="H57" s="7"/>
       <c r="I57" s="7"/>
       <c r="J57" s="38" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K57" s="8" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="L57" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N57" s="4" t="s">
         <v>7</v>
@@ -51641,29 +51649,29 @@
     </row>
     <row r="58" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A58" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B58" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C58"/>
       <c r="D58" s="10" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H58" s="10"/>
       <c r="I58" s="7"/>
       <c r="J58" s="7"/>
       <c r="K58" s="1" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="L58" s="12"/>
       <c r="M58" s="4" t="s">
@@ -51673,7 +51681,7 @@
         <v>12</v>
       </c>
       <c r="O58" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="P58" s="5"/>
       <c r="Q58" s="5"/>
@@ -51691,32 +51699,32 @@
     </row>
     <row r="59" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A59" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B59" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C59"/>
       <c r="D59" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E59" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F59" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="H59" s="10"/>
       <c r="I59" s="7"/>
       <c r="J59" s="7"/>
       <c r="K59" s="1" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="L59" s="12" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="M59" s="4" t="s">
         <v>4</v>
@@ -51725,7 +51733,7 @@
         <v>12</v>
       </c>
       <c r="O59" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="P59" s="5"/>
       <c r="Q59" s="5"/>
@@ -51743,29 +51751,29 @@
     </row>
     <row r="60" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A60" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B60" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C60"/>
       <c r="D60" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E60" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G60" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="H60" s="7"/>
       <c r="I60" s="7"/>
       <c r="J60" s="7"/>
       <c r="K60" s="8" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="L60" s="4"/>
       <c r="M60" s="4" t="s">
@@ -51775,7 +51783,7 @@
         <v>12</v>
       </c>
       <c r="O60" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="P60" s="5"/>
       <c r="Q60" s="5"/>
@@ -51793,23 +51801,23 @@
     </row>
     <row r="61" spans="1:28" ht="101" x14ac:dyDescent="0.35">
       <c r="A61" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B61" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C61" s="10"/>
       <c r="D61" s="10" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="H61" s="10" t="s">
         <v>183</v>
@@ -51817,7 +51825,7 @@
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
       <c r="K61" s="8" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="L61" s="11" t="s">
         <v>10</v>
@@ -51845,29 +51853,29 @@
     </row>
     <row r="62" spans="1:28" ht="163.5" x14ac:dyDescent="0.35">
       <c r="A62" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B62" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C62"/>
       <c r="D62" t="s">
+        <v>327</v>
+      </c>
+      <c r="E62" t="s">
+        <v>328</v>
+      </c>
+      <c r="F62" s="7" t="s">
         <v>329</v>
       </c>
-      <c r="E62" t="s">
-        <v>330</v>
-      </c>
-      <c r="F62" s="7" t="s">
-        <v>331</v>
-      </c>
       <c r="G62" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="H62" s="7"/>
       <c r="I62" s="7"/>
       <c r="J62" s="7"/>
       <c r="K62" s="8" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="L62" s="4"/>
       <c r="M62" s="4" t="s">
@@ -51877,7 +51885,7 @@
         <v>12</v>
       </c>
       <c r="O62" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="P62" s="5"/>
       <c r="Q62" s="5"/>
@@ -51895,39 +51903,39 @@
     </row>
     <row r="63" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A63" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B63" t="s">
+        <v>330</v>
+      </c>
+      <c r="C63" t="s">
+        <v>297</v>
+      </c>
+      <c r="D63" s="10" t="s">
         <v>332</v>
       </c>
-      <c r="C63" t="s">
-        <v>299</v>
-      </c>
-      <c r="D63" s="10" t="s">
+      <c r="E63" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="G63" s="10" t="s">
         <v>334</v>
-      </c>
-      <c r="E63" s="10" t="s">
-        <v>335</v>
-      </c>
-      <c r="F63" s="10" t="s">
-        <v>333</v>
-      </c>
-      <c r="G63" s="10" t="s">
-        <v>336</v>
       </c>
       <c r="H63" s="10"/>
       <c r="I63" s="7"/>
       <c r="J63" s="38" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="K63" s="8" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="L63" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N63" s="4" t="s">
         <v>7</v>
@@ -51949,39 +51957,39 @@
     </row>
     <row r="64" spans="1:28" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A64" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B64" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C64" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="H64" s="10"/>
       <c r="I64" s="7"/>
       <c r="J64" s="38" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K64" s="8" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="L64" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N64" s="4" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
2492 use ANRIND for abnormal baseline
</commit_message>
<xml_diff>
--- a/inst/adlb_grading/adlb_grading_spec.xlsx
+++ b/inst/adlb_grading/adlb_grading_spec.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="688">
   <si>
     <t>Anemia</t>
   </si>
@@ -2791,36 +2791,6 @@
   <si>
     <t>case_when(
 is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(20*ANRHI, signif_dig) ~ "4",
-(!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(20*BASE, signif_dig) ~ "4",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(5*ANRHI, signif_dig) ~ "3",
-(!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(5*BASE, signif_dig) ~ "3",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(3*ANRHI, signif_dig) ~ "2",
-(!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(3*BASE, signif_dig) ~ "2",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
-(!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt;= signif(1.5*BASE, signif_dig) ~ "1",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0",
-(!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &lt; signif(1.5*BASE, signif_dig) ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(20*ANRHI, signif_dig) ~ "4",
-(!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(20*BASE, signif_dig) ~ "4",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(5*ANRHI, signif_dig) ~ "3",
-(!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(5*BASE, signif_dig) ~ "3",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(2.5*ANRHI, signif_dig) ~ "2",
-(!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(2.5*BASE, signif_dig) ~ "2",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
-(!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt;= signif(2*BASE, signif_dig) ~ "1",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0",
-!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig) &amp; signif(AVAL, signif_dig) &lt; signif(2*BASE, signif_dig) ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
 signif(AVAL, signif_dig) &gt; signif(10*ANRHI, signif_dig) ~ "4",
 signif(AVAL, signif_dig) &gt; signif(5*ANRHI, signif_dig) ~ "3",
 signif(AVAL, signif_dig) &gt; signif(2.5*ANRHI, signif_dig) ~ "2",
@@ -2892,36 +2862,6 @@
 )</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(20*ANRHI, signif_dig) ~ "4",
-!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig) &amp; signif(AVAL, signif_dig) &gt; signif(20*BASE, signif_dig) ~ "4",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(5*ANRHI, signif_dig) ~ "3",
-!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig) &amp; signif(AVAL, signif_dig) &gt; signif(5*BASE, signif_dig) ~ "3",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(2.5*ANRHI, signif_dig) ~ "2",
-!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig) &amp; signif(AVAL, signif_dig) &gt; signif(2.5*BASE, signif_dig) ~ "2",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
-!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig) &amp; signif(AVAL, signif_dig) &gt; signif(2*BASE, signif_dig) ~ "1",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0",
-!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig) &amp; signif(AVAL, signif_dig) &lt;= signif(2*BASE, signif_dig) ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(10*ANRHI, signif_dig) ~ "4",
-!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig) &amp; signif(AVAL, signif_dig) &gt; signif(10*BASE, signif_dig) ~ "4",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(3*ANRHI, signif_dig) ~ "3",
-!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig) &amp; signif(AVAL, signif_dig) &gt; signif(3*BASE, signif_dig) ~ "3",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(1.5*ANRHI, signif_dig) ~ "2",
-!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig) &amp; signif(AVAL, signif_dig) &gt; signif(1.5*BASE, signif_dig) ~ "2",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
-!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig) &amp; signif(AVAL, signif_dig) &gt; signif(BASE, signif_dig) ~ "1",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0",
-!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig) &amp; signif(AVAL, signif_dig) &lt;= signif(BASE, signif_dig) ~ "0"
-)</t>
-  </si>
-  <si>
     <t>&gt; 5 years of age</t>
   </si>
   <si>
@@ -2958,6 +2898,69 @@
   </si>
   <si>
     <t>AVAL, BASE</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
+(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(20*ANRHI, signif_dig) ~ "4",
+BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(20*BASE, signif_dig) ~ "4",
+(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(5*ANRHI, signif_dig) ~ "3",
+BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(5*BASE, signif_dig) ~ "3",
+(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(3*ANRHI, signif_dig) ~ "2",
+BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(3*BASE, signif_dig) ~ "2",
+(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
+BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt;= signif(1.5*BASE, signif_dig) ~ "1",
+(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0",
+BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &lt; signif(1.5*BASE, signif_dig) ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>AVAL, ANRHI, BASE, BNRIND</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
+(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(20*ANRHI, signif_dig) ~ "4",
+BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(20*BASE, signif_dig) ~ "4",
+(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(5*ANRHI, signif_dig) ~ "3",
+BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(5*BASE, signif_dig) ~ "3",
+(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(2.5*ANRHI, signif_dig) ~ "2",
+BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(2.5*BASE, signif_dig) ~ "2",
+(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
+BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt;= signif(2*BASE, signif_dig) ~ "1",
+(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0",
+BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &lt; signif(2*BASE, signif_dig) ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
+(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(10*ANRHI, signif_dig) ~ "4",
+BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(10*BASE, signif_dig) ~ "4",
+(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(3*ANRHI, signif_dig) ~ "3",
+BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(3*BASE, signif_dig) ~ "3",
+(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(1.5*ANRHI, signif_dig) ~ "2",
+BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(1.5*BASE, signif_dig) ~ "2",
+(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
+BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(BASE, signif_dig) ~ "1",
+(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0",
+BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &lt;= signif(BASE, signif_dig) ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
+(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(20*ANRHI, signif_dig) ~ "4",
+BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(20*BASE, signif_dig) ~ "4",
+(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(5*ANRHI, signif_dig) ~ "3",
+BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(5*BASE, signif_dig) ~ "3",
+(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(2.5*ANRHI, signif_dig) ~ "2",
+BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(2.5*BASE, signif_dig) ~ "2",
+(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
+BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(2*BASE, signif_dig) ~ "1",
+(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0",
+BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &lt;= signif(2*BASE, signif_dig) ~ "0"
+)</t>
   </si>
 </sst>
 </file>
@@ -26142,8 +26145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z972"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="C14" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -26365,7 +26368,7 @@
       <c r="Y4" s="5"/>
       <c r="Z4" s="5"/>
     </row>
-    <row r="5" spans="1:26" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="288" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>185</v>
       </c>
@@ -26391,11 +26394,11 @@
         <v>23</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>669</v>
+        <v>683</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
-        <v>54</v>
+        <v>684</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>12</v>
@@ -26415,7 +26418,7 @@
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
     </row>
-    <row r="6" spans="1:26" ht="409.6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" ht="288.5" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>185</v>
       </c>
@@ -26441,11 +26444,11 @@
         <v>27</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>670</v>
+        <v>685</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
-        <v>54</v>
+        <v>684</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>12</v>
@@ -26465,7 +26468,7 @@
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
     </row>
-    <row r="7" spans="1:26" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="288" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>185</v>
       </c>
@@ -26491,11 +26494,11 @@
         <v>29</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>669</v>
+        <v>683</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4" t="s">
-        <v>54</v>
+        <v>684</v>
       </c>
       <c r="L7" s="4" t="s">
         <v>12</v>
@@ -26515,7 +26518,7 @@
       <c r="Y7" s="5"/>
       <c r="Z7" s="5"/>
     </row>
-    <row r="8" spans="1:26" ht="409.6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" ht="288.5" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>185</v>
       </c>
@@ -26541,11 +26544,11 @@
         <v>34</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>679</v>
+        <v>686</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="4" t="s">
-        <v>54</v>
+        <v>684</v>
       </c>
       <c r="L8" s="4" t="s">
         <v>12</v>
@@ -26695,7 +26698,7 @@
         <v>51</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="4" t="s">
@@ -26745,7 +26748,7 @@
         <v>58</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="4" t="s">
@@ -26795,7 +26798,7 @@
         <v>63</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>2</v>
@@ -26821,7 +26824,7 @@
       <c r="Y13" s="5"/>
       <c r="Z13" s="5"/>
     </row>
-    <row r="14" spans="1:26" ht="409.6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" ht="288.5" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>185</v>
       </c>
@@ -26847,11 +26850,11 @@
         <v>65</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>678</v>
+        <v>687</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="4" t="s">
-        <v>15</v>
+        <v>684</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>12</v>
@@ -26947,7 +26950,7 @@
         <v>247</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>2</v>
@@ -26981,13 +26984,13 @@
         <v>73</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>183</v>
@@ -26999,11 +27002,11 @@
         <v>77</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="J17" s="12"/>
       <c r="K17" s="4" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="L17" s="4" t="s">
         <v>12</v>
@@ -27051,7 +27054,7 @@
         <v>82</v>
       </c>
       <c r="I18" s="26" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="J18" s="27"/>
       <c r="K18" s="27" t="s">
@@ -27311,7 +27314,7 @@
         <v>103</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="J23" s="12"/>
       <c r="K23" s="4" t="s">
@@ -27731,7 +27734,7 @@
         <v>204</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="J31" s="17"/>
       <c r="K31" s="4" t="s">
@@ -28101,7 +28104,7 @@
         <v>210</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="J38" s="17" t="s">
         <v>212</v>
@@ -50849,7 +50852,7 @@
         <v>306</v>
       </c>
       <c r="C43" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="D43" s="10" t="s">
         <v>505</v>
@@ -50953,7 +50956,7 @@
         <v>302</v>
       </c>
       <c r="C45" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>510</v>
@@ -50973,7 +50976,7 @@
         <v>571</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="L45" s="11" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
2492 abnormal_indicator added to metadata and function
</commit_message>
<xml_diff>
--- a/inst/adlb_grading/adlb_grading_spec.xlsx
+++ b/inst/adlb_grading/adlb_grading_spec.xlsx
@@ -20,7 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DAIDS!$C$1:$C$998</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">NCICTCAEv5!$B$1:$B$972</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" refMode="R1C1"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7miMf568I5zSj3ueLWeKTzSDumdwrA=="/>
@@ -2950,16 +2950,16 @@
   <si>
     <t>case_when(
 is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
-(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(20*ANRHI, signif_dig) ~ "4",
-BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(20*BASE, signif_dig) ~ "4",
-(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(5*ANRHI, signif_dig) ~ "3",
-BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(5*BASE, signif_dig) ~ "3",
-(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(2.5*ANRHI, signif_dig) ~ "2",
-BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(2.5*BASE, signif_dig) ~ "2",
-(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
-BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(2*BASE, signif_dig) ~ "1",
-(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0",
-BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &lt;= signif(2*BASE, signif_dig) ~ "0"
+(is.na(BNRIND) | BNRIND != abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(20*ANRHI, signif_dig) ~ "4",
+BNRIND == abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(20*BASE, signif_dig) ~ "4",
+(is.na(BNRIND) | BNRIND != abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(5*ANRHI, signif_dig) ~ "3",
+BNRIND == abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(5*BASE, signif_dig) ~ "3",
+(is.na(BNRIND) | BNRIND != abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(2.5*ANRHI, signif_dig) ~ "2",
+BNRIND == abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(2.5*BASE, signif_dig) ~ "2",
+(is.na(BNRIND) | BNRIND != abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
+BNRIND == abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(2*BASE, signif_dig) ~ "1",
+(is.na(BNRIND) | BNRIND != abnormal_indicator) &amp; signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0",
+BNRIND == abnormal_indicator &amp; signif(AVAL, signif_dig) &lt;= signif(2*BASE, signif_dig) ~ "0"
 )</t>
   </si>
 </sst>
@@ -26145,8 +26145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z972"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C14" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -26824,7 +26824,7 @@
       <c r="Y13" s="5"/>
       <c r="Z13" s="5"/>
     </row>
-    <row r="14" spans="1:26" ht="288.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" ht="351" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>185</v>
       </c>

</xml_diff>

<commit_message>
2492 make final updates including Vignette
</commit_message>
<xml_diff>
--- a/inst/adlb_grading/adlb_grading_spec.xlsx
+++ b/inst/adlb_grading/adlb_grading_spec.xlsx
@@ -2900,66 +2900,66 @@
     <t>AVAL, BASE</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
-(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(20*ANRHI, signif_dig) ~ "4",
-BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(20*BASE, signif_dig) ~ "4",
-(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(5*ANRHI, signif_dig) ~ "3",
-BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(5*BASE, signif_dig) ~ "3",
-(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(3*ANRHI, signif_dig) ~ "2",
-BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(3*BASE, signif_dig) ~ "2",
-(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
-BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt;= signif(1.5*BASE, signif_dig) ~ "1",
-(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0",
-BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &lt; signif(1.5*BASE, signif_dig) ~ "0"
-)</t>
-  </si>
-  <si>
     <t>AVAL, ANRHI, BASE, BNRIND</t>
   </si>
   <si>
     <t>case_when(
 is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
-(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(20*ANRHI, signif_dig) ~ "4",
-BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(20*BASE, signif_dig) ~ "4",
-(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(5*ANRHI, signif_dig) ~ "3",
-BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(5*BASE, signif_dig) ~ "3",
-(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(2.5*ANRHI, signif_dig) ~ "2",
-BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(2.5*BASE, signif_dig) ~ "2",
-(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
-BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt;= signif(2*BASE, signif_dig) ~ "1",
-(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0",
-BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &lt; signif(2*BASE, signif_dig) ~ "0"
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(20*ANRHI, signif_dig) ~ "4",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(20*BASE, signif_dig) ~ "4",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(5*ANRHI, signif_dig) ~ "3",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(5*BASE, signif_dig) ~ "3",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(2.5*ANRHI, signif_dig) ~ "2",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(2.5*BASE, signif_dig) ~ "2",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(2*BASE, signif_dig) ~ "1",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &lt;= signif(2*BASE, signif_dig) ~ "0"
 )</t>
   </si>
   <si>
     <t>case_when(
 is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
-(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(10*ANRHI, signif_dig) ~ "4",
-BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(10*BASE, signif_dig) ~ "4",
-(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(3*ANRHI, signif_dig) ~ "3",
-BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(3*BASE, signif_dig) ~ "3",
-(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(1.5*ANRHI, signif_dig) ~ "2",
-BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(1.5*BASE, signif_dig) ~ "2",
-(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
-BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &gt; signif(BASE, signif_dig) ~ "1",
-(is.na(BNRIND) | BNRIND != "HIGH") &amp; signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0",
-BNRIND == "HIGH" &amp; signif(AVAL, signif_dig) &lt;= signif(BASE, signif_dig) ~ "0"
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(20*ANRHI, signif_dig) ~ "4",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(20*BASE, signif_dig) ~ "4",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(5*ANRHI, signif_dig) ~ "3",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(5*BASE, signif_dig) ~ "3",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(3*ANRHI, signif_dig) ~ "2",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(3*BASE, signif_dig) ~ "2",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt;= signif(1.5*BASE, signif_dig) ~ "1",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &lt; signif(1.5*BASE, signif_dig) ~ "0"
 )</t>
   </si>
   <si>
     <t>case_when(
 is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
-(is.na(BNRIND) | BNRIND != abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(20*ANRHI, signif_dig) ~ "4",
-BNRIND == abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(20*BASE, signif_dig) ~ "4",
-(is.na(BNRIND) | BNRIND != abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(5*ANRHI, signif_dig) ~ "3",
-BNRIND == abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(5*BASE, signif_dig) ~ "3",
-(is.na(BNRIND) | BNRIND != abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(2.5*ANRHI, signif_dig) ~ "2",
-BNRIND == abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(2.5*BASE, signif_dig) ~ "2",
-(is.na(BNRIND) | BNRIND != abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
-BNRIND == abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(2*BASE, signif_dig) ~ "1",
-(is.na(BNRIND) | BNRIND != abnormal_indicator) &amp; signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0",
-BNRIND == abnormal_indicator &amp; signif(AVAL, signif_dig) &lt;= signif(2*BASE, signif_dig) ~ "0"
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(20*ANRHI, signif_dig) ~ "4",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(20*BASE, signif_dig) ~ "4",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(5*ANRHI, signif_dig) ~ "3",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(5*BASE, signif_dig) ~ "3",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(2.5*ANRHI, signif_dig) ~ "2",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(2.5*BASE, signif_dig) ~ "2",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt;= signif(2*BASE, signif_dig) ~ "1",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &lt; signif(2*BASE, signif_dig) ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(10*ANRHI, signif_dig) ~ "4",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(10*BASE, signif_dig) ~ "4",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(3*ANRHI, signif_dig) ~ "3",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(3*BASE, signif_dig) ~ "3",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(1.5*ANRHI, signif_dig) ~ "2",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(1.5*BASE, signif_dig) ~ "2",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(BASE, signif_dig) ~ "1",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &lt;= signif(BASE, signif_dig) ~ "0"
 )</t>
   </si>
 </sst>
@@ -26145,8 +26145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z972"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -26394,11 +26394,11 @@
         <v>23</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>12</v>
@@ -26444,11 +26444,11 @@
         <v>27</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>12</v>
@@ -26494,11 +26494,11 @@
         <v>29</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="L7" s="4" t="s">
         <v>12</v>
@@ -26544,11 +26544,11 @@
         <v>34</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="4" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="L8" s="4" t="s">
         <v>12</v>
@@ -26824,7 +26824,7 @@
       <c r="Y13" s="5"/>
       <c r="Z13" s="5"/>
     </row>
-    <row r="14" spans="1:26" ht="351" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" ht="288.5" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>185</v>
       </c>
@@ -26850,11 +26850,11 @@
         <v>65</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="4" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Closes #2492 use ANRIND for abnormal baseline (#2555)
* 2492 use ANRIND for abnormal baseline

* 2492 abnormal_indicator added to metadata and function

* 2492 fix LINTR

* 2492 make final updates including Vignette

* Update NEWS.md

---------

Co-authored-by: Ben Straub <ben.x.straub@gsk.com>
</commit_message>
<xml_diff>
--- a/inst/adlb_grading/adlb_grading_spec.xlsx
+++ b/inst/adlb_grading/adlb_grading_spec.xlsx
@@ -20,7 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DAIDS!$C$1:$C$998</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">NCICTCAEv5!$B$1:$B$972</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" refMode="R1C1"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7miMf568I5zSj3ueLWeKTzSDumdwrA=="/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="688">
   <si>
     <t>Anemia</t>
   </si>
@@ -2791,36 +2791,6 @@
   <si>
     <t>case_when(
 is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(20*ANRHI, signif_dig) ~ "4",
-(!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(20*BASE, signif_dig) ~ "4",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(5*ANRHI, signif_dig) ~ "3",
-(!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(5*BASE, signif_dig) ~ "3",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(3*ANRHI, signif_dig) ~ "2",
-(!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(3*BASE, signif_dig) ~ "2",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
-(!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt;= signif(1.5*BASE, signif_dig) ~ "1",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0",
-(!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &lt; signif(1.5*BASE, signif_dig) ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(20*ANRHI, signif_dig) ~ "4",
-(!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(20*BASE, signif_dig) ~ "4",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(5*ANRHI, signif_dig) ~ "3",
-(!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(5*BASE, signif_dig) ~ "3",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(2.5*ANRHI, signif_dig) ~ "2",
-(!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(2.5*BASE, signif_dig) ~ "2",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
-(!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt;= signif(2*BASE, signif_dig) ~ "1",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0",
-!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig) &amp; signif(AVAL, signif_dig) &lt; signif(2*BASE, signif_dig) ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
 signif(AVAL, signif_dig) &gt; signif(10*ANRHI, signif_dig) ~ "4",
 signif(AVAL, signif_dig) &gt; signif(5*ANRHI, signif_dig) ~ "3",
 signif(AVAL, signif_dig) &gt; signif(2.5*ANRHI, signif_dig) ~ "2",
@@ -2892,36 +2862,6 @@
 )</t>
   </si>
   <si>
-    <t>case_when(
-is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(20*ANRHI, signif_dig) ~ "4",
-!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig) &amp; signif(AVAL, signif_dig) &gt; signif(20*BASE, signif_dig) ~ "4",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(5*ANRHI, signif_dig) ~ "3",
-!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig) &amp; signif(AVAL, signif_dig) &gt; signif(5*BASE, signif_dig) ~ "3",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(2.5*ANRHI, signif_dig) ~ "2",
-!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig) &amp; signif(AVAL, signif_dig) &gt; signif(2.5*BASE, signif_dig) ~ "2",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
-!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig) &amp; signif(AVAL, signif_dig) &gt; signif(2*BASE, signif_dig) ~ "1",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0",
-!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig) &amp; signif(AVAL, signif_dig) &lt;= signif(2*BASE, signif_dig) ~ "0"
-)</t>
-  </si>
-  <si>
-    <t>case_when(
-is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(10*ANRHI, signif_dig) ~ "4",
-!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig) &amp; signif(AVAL, signif_dig) &gt; signif(10*BASE, signif_dig) ~ "4",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(3*ANRHI, signif_dig) ~ "3",
-!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig) &amp; signif(AVAL, signif_dig) &gt; signif(3*BASE, signif_dig) ~ "3",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(1.5*ANRHI, signif_dig) ~ "2",
-!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig) &amp; signif(AVAL, signif_dig) &gt; signif(1.5*BASE, signif_dig) ~ "2",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
-!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig) &amp; signif(AVAL, signif_dig) &gt; signif(BASE, signif_dig) ~ "1",
-(is.na(BASE) | signif(BASE, signif_dig) &lt;= signif(ANRHI, signif_dig)) &amp; signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0",
-!is.na(BASE) &amp; signif(BASE, signif_dig) &gt; signif(ANRHI, signif_dig) &amp; signif(AVAL, signif_dig) &lt;= signif(BASE, signif_dig) ~ "0"
-)</t>
-  </si>
-  <si>
     <t>&gt; 5 years of age</t>
   </si>
   <si>
@@ -2958,6 +2898,69 @@
   </si>
   <si>
     <t>AVAL, BASE</t>
+  </si>
+  <si>
+    <t>AVAL, ANRHI, BASE, BNRIND</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(20*ANRHI, signif_dig) ~ "4",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(20*BASE, signif_dig) ~ "4",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(5*ANRHI, signif_dig) ~ "3",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(5*BASE, signif_dig) ~ "3",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(2.5*ANRHI, signif_dig) ~ "2",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(2.5*BASE, signif_dig) ~ "2",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(2*BASE, signif_dig) ~ "1",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &lt;= signif(2*BASE, signif_dig) ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(20*ANRHI, signif_dig) ~ "4",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(20*BASE, signif_dig) ~ "4",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(5*ANRHI, signif_dig) ~ "3",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(5*BASE, signif_dig) ~ "3",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(3*ANRHI, signif_dig) ~ "2",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(3*BASE, signif_dig) ~ "2",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt;= signif(1.5*BASE, signif_dig) ~ "1",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &lt; signif(1.5*BASE, signif_dig) ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(20*ANRHI, signif_dig) ~ "4",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(20*BASE, signif_dig) ~ "4",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(5*ANRHI, signif_dig) ~ "3",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(5*BASE, signif_dig) ~ "3",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(2.5*ANRHI, signif_dig) ~ "2",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(2.5*BASE, signif_dig) ~ "2",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt;= signif(2*BASE, signif_dig) ~ "1",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &lt; signif(2*BASE, signif_dig) ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) | is.na(ANRHI) ~ NA_character_,
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(10*ANRHI, signif_dig) ~ "4",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(10*BASE, signif_dig) ~ "4",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(3*ANRHI, signif_dig) ~ "3",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(3*BASE, signif_dig) ~ "3",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(1.5*ANRHI, signif_dig) ~ "2",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(1.5*BASE, signif_dig) ~ "2",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &gt; signif(BASE, signif_dig) ~ "1",
+!(BNRIND %in% abnormal_indicator) &amp; signif(AVAL, signif_dig) &lt;= signif(ANRHI, signif_dig) ~ "0",
+BNRIND %in% abnormal_indicator &amp; signif(AVAL, signif_dig) &lt;= signif(BASE, signif_dig) ~ "0"
+)</t>
   </si>
 </sst>
 </file>
@@ -26142,8 +26145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z972"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -26365,7 +26368,7 @@
       <c r="Y4" s="5"/>
       <c r="Z4" s="5"/>
     </row>
-    <row r="5" spans="1:26" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="288" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>185</v>
       </c>
@@ -26391,11 +26394,11 @@
         <v>23</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>669</v>
+        <v>685</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
-        <v>54</v>
+        <v>683</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>12</v>
@@ -26415,7 +26418,7 @@
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
     </row>
-    <row r="6" spans="1:26" ht="409.6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" ht="288.5" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>185</v>
       </c>
@@ -26441,11 +26444,11 @@
         <v>27</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>670</v>
+        <v>686</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
-        <v>54</v>
+        <v>683</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>12</v>
@@ -26465,7 +26468,7 @@
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
     </row>
-    <row r="7" spans="1:26" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="288" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>185</v>
       </c>
@@ -26491,11 +26494,11 @@
         <v>29</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>669</v>
+        <v>685</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4" t="s">
-        <v>54</v>
+        <v>683</v>
       </c>
       <c r="L7" s="4" t="s">
         <v>12</v>
@@ -26515,7 +26518,7 @@
       <c r="Y7" s="5"/>
       <c r="Z7" s="5"/>
     </row>
-    <row r="8" spans="1:26" ht="409.6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" ht="288.5" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>185</v>
       </c>
@@ -26541,11 +26544,11 @@
         <v>34</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>679</v>
+        <v>687</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="4" t="s">
-        <v>54</v>
+        <v>683</v>
       </c>
       <c r="L8" s="4" t="s">
         <v>12</v>
@@ -26695,7 +26698,7 @@
         <v>51</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="4" t="s">
@@ -26745,7 +26748,7 @@
         <v>58</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="4" t="s">
@@ -26795,7 +26798,7 @@
         <v>63</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>2</v>
@@ -26821,7 +26824,7 @@
       <c r="Y13" s="5"/>
       <c r="Z13" s="5"/>
     </row>
-    <row r="14" spans="1:26" ht="409.6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" ht="288.5" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>185</v>
       </c>
@@ -26847,11 +26850,11 @@
         <v>65</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>678</v>
+        <v>684</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="4" t="s">
-        <v>15</v>
+        <v>683</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>12</v>
@@ -26947,7 +26950,7 @@
         <v>247</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>2</v>
@@ -26981,13 +26984,13 @@
         <v>73</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>183</v>
@@ -26999,11 +27002,11 @@
         <v>77</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="J17" s="12"/>
       <c r="K17" s="4" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="L17" s="4" t="s">
         <v>12</v>
@@ -27051,7 +27054,7 @@
         <v>82</v>
       </c>
       <c r="I18" s="26" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="J18" s="27"/>
       <c r="K18" s="27" t="s">
@@ -27311,7 +27314,7 @@
         <v>103</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="J23" s="12"/>
       <c r="K23" s="4" t="s">
@@ -27731,7 +27734,7 @@
         <v>204</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="J31" s="17"/>
       <c r="K31" s="4" t="s">
@@ -28101,7 +28104,7 @@
         <v>210</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="J38" s="17" t="s">
         <v>212</v>
@@ -50849,7 +50852,7 @@
         <v>306</v>
       </c>
       <c r="C43" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="D43" s="10" t="s">
         <v>505</v>
@@ -50953,7 +50956,7 @@
         <v>302</v>
       </c>
       <c r="C45" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>510</v>
@@ -50973,7 +50976,7 @@
         <v>571</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="L45" s="11" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
2768 add Acidosis and Alkalosis to NCI v4 and v5
</commit_message>
<xml_diff>
--- a/inst/adlb_grading/adlb_grading_spec.xlsx
+++ b/inst/adlb_grading/adlb_grading_spec.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\millerg1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{98A8C04D-E463-41A6-80E7-2B7A6D55D24E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE06370B-02B5-4690-9613-57E748A4B7B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29715" yWindow="465" windowWidth="27360" windowHeight="12390" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28995" yWindow="60" windowWidth="28380" windowHeight="15285" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NCICTCAEv4" sheetId="2" r:id="rId1"/>
@@ -22,10 +22,21 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">DAIDS!$C$1:$C$998</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">NCICTCAEv5!$B$1:$B$972</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">NCICTCAEv5!$B$1:$B$974</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7miMf568I5zSj3ueLWeKTzSDumdwrA=="/>
     </ext>
@@ -34,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3531" uniqueCount="764">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3619" uniqueCount="772">
   <si>
     <t>Anemia</t>
   </si>
@@ -3668,6 +3679,42 @@
 signif(AVAL, signif_dig) &lt; 600 ~ "2",
 signif(AVAL, signif_dig) &lt; 650 ~ "1",
 signif(AVAL, signif_dig) &gt;= 650 ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>pH &lt;normal, but &gt;=7.3</t>
+  </si>
+  <si>
+    <t>pH &lt;7.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A disorder characterized by abnormally high acidity (high hydrogen-ion concentration) of the blood and other body tissues. </t>
+  </si>
+  <si>
+    <t>pH &gt;normal, but &lt;=7.5</t>
+  </si>
+  <si>
+    <t>pH &gt;7.5</t>
+  </si>
+  <si>
+    <t>A disorder characterized by abnormally high alkalinity (low hydrogen-ion concentration) of the blood and other body tissues.</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+signif(AVAL, signif_dig) &gt; 7.5 ~ "3",
+is.na(ANRHI) ~ NA_character_,
+signif(AVAL, signif_dig) &gt; signif(ANRHI, signif_dig) ~ "1",
+signif(AVAL, signif_dig) &gt;= signif(ANRLO, signif_dig) ~ "0"
+)</t>
+  </si>
+  <si>
+    <t>case_when(
+is.na(AVAL) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; 7.3 ~ "3",
+is.na(ANRLO) ~ NA_character_,
+signif(AVAL, signif_dig) &lt; signif(ANRLO, signif_dig) ~ "1",
+signif(AVAL, signif_dig) &gt;= signif(ANRLO, signif_dig) ~ "0"
 )</t>
   </si>
 </sst>
@@ -4139,10 +4186,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M975"/>
+  <dimension ref="A1:M977"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5050,115 +5097,105 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="138" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
         <v>195</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>111</v>
+        <v>538</v>
+      </c>
+      <c r="C25" t="s">
+        <v>764</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>112</v>
+        <v>183</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>113</v>
+        <v>765</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>114</v>
+        <v>255</v>
       </c>
       <c r="G25" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>197</v>
+        <v>766</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>666</v>
-      </c>
-      <c r="J25" s="14" t="s">
-        <v>211</v>
-      </c>
+        <v>771</v>
+      </c>
+      <c r="J25" s="14"/>
       <c r="K25" s="4" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="M25" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="138" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
         <v>195</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>111</v>
+        <v>543</v>
+      </c>
+      <c r="C26" t="s">
+        <v>767</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>112</v>
+        <v>183</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>113</v>
+        <v>768</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>114</v>
+        <v>255</v>
       </c>
       <c r="G26" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>197</v>
+        <v>769</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>649</v>
-      </c>
-      <c r="J26" s="14" t="s">
-        <v>211</v>
-      </c>
+        <v>770</v>
+      </c>
+      <c r="J26" s="14"/>
       <c r="K26" s="4" t="s">
         <v>15</v>
       </c>
       <c r="L26" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M26" s="3" t="s">
-        <v>219</v>
-      </c>
     </row>
     <row r="27" spans="1:13" ht="138" x14ac:dyDescent="0.3">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="B27" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="F27" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="G27" s="16" t="s">
+      <c r="B27" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="G27" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>650</v>
+        <v>666</v>
       </c>
       <c r="J27" s="14" t="s">
         <v>211</v>
@@ -5170,48 +5207,48 @@
         <v>12</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="75.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="13" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="138" x14ac:dyDescent="0.3">
+      <c r="A28" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="B28" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="F28" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="G28" s="16" t="s">
+      <c r="B28" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="G28" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="J28" s="14" t="s">
         <v>211</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="L28" s="4" t="s">
         <v>12</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="138" x14ac:dyDescent="0.3">
@@ -5219,28 +5256,28 @@
         <v>195</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>120</v>
+        <v>213</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G29" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H29" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="J29" s="14" t="s">
         <v>211</v>
@@ -5251,43 +5288,49 @@
       <c r="L29" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" ht="125.5" x14ac:dyDescent="0.3">
+      <c r="M29" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="75.5" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
         <v>195</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>196</v>
+        <v>117</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="G30" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="J30" s="14" t="s">
         <v>211</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="L30" s="4" t="s">
         <v>12</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="138" x14ac:dyDescent="0.3">
@@ -5295,28 +5338,28 @@
         <v>195</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G31" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="J31" s="14" t="s">
         <v>211</v>
@@ -5328,74 +5371,74 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="100.5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" ht="125.5" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
         <v>195</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>136</v>
+        <v>196</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="G32" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="J32" s="14" t="s">
         <v>211</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="L32" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="113" x14ac:dyDescent="0.3">
-      <c r="A33" s="12" t="s">
+    <row r="33" spans="1:13" ht="138" x14ac:dyDescent="0.3">
+      <c r="A33" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G33" s="14" t="s">
+      <c r="B33" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="G33" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="J33" s="14" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="K33" s="4" t="s">
         <v>15</v>
@@ -5403,119 +5446,116 @@
       <c r="L33" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M33" s="3" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="125.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:13" ht="100.5" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
         <v>195</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>180</v>
+        <v>138</v>
       </c>
       <c r="G34" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="J34" s="14" t="s">
-        <v>2</v>
+        <v>211</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="138" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="113" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
         <v>195</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>149</v>
+        <v>196</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="G35" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="J35" s="14" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="138" x14ac:dyDescent="0.3">
-      <c r="A36" s="12" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="125.5" x14ac:dyDescent="0.3">
+      <c r="A36" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="B36" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="E36" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="F36" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="G36" s="14" t="s">
+      <c r="B36" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="G36" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>586</v>
+        <v>657</v>
       </c>
       <c r="J36" s="14" t="s">
-        <v>211</v>
+        <v>2</v>
       </c>
       <c r="K36" s="4" t="s">
         <v>3</v>
@@ -5523,37 +5563,34 @@
       <c r="L36" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M36" s="3" t="s">
-        <v>219</v>
-      </c>
     </row>
     <row r="37" spans="1:13" ht="138" x14ac:dyDescent="0.3">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="B37" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="C37" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="D37" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="E37" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="F37" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="G37" s="16" t="s">
+      <c r="B37" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="G37" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H37" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="J37" s="14" t="s">
         <v>211</v>
@@ -5564,34 +5601,37 @@
       <c r="L37" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" ht="125.5" x14ac:dyDescent="0.3">
-      <c r="A38" s="13" t="s">
+      <c r="M37" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="138" x14ac:dyDescent="0.3">
+      <c r="A38" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="B38" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="D38" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="G38" s="16" t="s">
+      <c r="B38" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="G38" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>667</v>
+        <v>586</v>
       </c>
       <c r="J38" s="14" t="s">
         <v>211</v>
@@ -5603,7 +5643,7 @@
         <v>7</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="138" x14ac:dyDescent="0.3">
@@ -5611,28 +5651,28 @@
         <v>195</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="F39" s="16" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="G39" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="J39" s="14" t="s">
         <v>211</v>
@@ -5649,28 +5689,28 @@
         <v>195</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>196</v>
+        <v>159</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="G40" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H40" s="15" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>661</v>
+        <v>667</v>
       </c>
       <c r="J40" s="14" t="s">
         <v>211</v>
@@ -5680,6 +5720,9 @@
       </c>
       <c r="L40" s="4" t="s">
         <v>7</v>
+      </c>
+      <c r="M40" s="3" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="138" x14ac:dyDescent="0.3">
@@ -5687,28 +5730,28 @@
         <v>195</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="F41" s="16" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="G41" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="J41" s="14" t="s">
         <v>211</v>
@@ -5720,15 +5763,81 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="13" x14ac:dyDescent="0.3">
-      <c r="J42" s="11"/>
-      <c r="K42" s="4"/>
-      <c r="L42" s="4"/>
-    </row>
-    <row r="43" spans="1:13" ht="13" x14ac:dyDescent="0.3">
-      <c r="J43" s="11"/>
-      <c r="K43" s="4"/>
-      <c r="L43" s="4"/>
+    <row r="42" spans="1:13" ht="125.5" x14ac:dyDescent="0.3">
+      <c r="A42" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="F42" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="G42" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="H42" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="J42" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="K42" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L42" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="138" x14ac:dyDescent="0.3">
+      <c r="A43" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="F43" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="G43" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="H43" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="J43" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L43" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="44" spans="1:13" ht="13" x14ac:dyDescent="0.3">
       <c r="J44" s="11"/>
@@ -10389,6 +10498,16 @@
       <c r="J975" s="11"/>
       <c r="K975" s="4"/>
       <c r="L975" s="4"/>
+    </row>
+    <row r="976" spans="10:12" ht="13" x14ac:dyDescent="0.3">
+      <c r="J976" s="11"/>
+      <c r="K976" s="4"/>
+      <c r="L976" s="4"/>
+    </row>
+    <row r="977" spans="10:12" ht="13" x14ac:dyDescent="0.3">
+      <c r="J977" s="11"/>
+      <c r="K977" s="4"/>
+      <c r="L977" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10398,10 +10517,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89BDAB5A-4072-4726-8F9D-2A23A573C446}">
-  <dimension ref="A1:M981"/>
+  <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -11555,115 +11674,105 @@
         <v>747</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="138" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
         <v>195</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>111</v>
+        <v>538</v>
+      </c>
+      <c r="C31" t="s">
+        <v>764</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>112</v>
+        <v>183</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>113</v>
+        <v>765</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>114</v>
+        <v>255</v>
       </c>
       <c r="G31" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>197</v>
+        <v>766</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>697</v>
-      </c>
-      <c r="J31" s="14" t="s">
-        <v>693</v>
-      </c>
+        <v>771</v>
+      </c>
+      <c r="J31" s="14"/>
       <c r="K31" s="4" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="M31" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="138" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
         <v>195</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>111</v>
+        <v>543</v>
+      </c>
+      <c r="C32" t="s">
+        <v>767</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>112</v>
+        <v>183</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>113</v>
+        <v>768</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>114</v>
+        <v>255</v>
       </c>
       <c r="G32" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>197</v>
+        <v>769</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>698</v>
-      </c>
-      <c r="J32" s="14" t="s">
-        <v>693</v>
-      </c>
+        <v>770</v>
+      </c>
+      <c r="J32" s="14"/>
       <c r="K32" s="4" t="s">
         <v>15</v>
       </c>
       <c r="L32" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M32" s="3" t="s">
-        <v>699</v>
-      </c>
     </row>
     <row r="33" spans="1:13" ht="138" x14ac:dyDescent="0.3">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="B33" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="F33" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="G33" s="16" t="s">
+      <c r="B33" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="G33" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="J33" s="14" t="s">
         <v>693</v>
@@ -11675,48 +11784,48 @@
         <v>12</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="75.5" x14ac:dyDescent="0.3">
-      <c r="A34" s="13" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="138" x14ac:dyDescent="0.3">
+      <c r="A34" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="B34" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="F34" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="G34" s="16" t="s">
+      <c r="B34" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="G34" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="J34" s="14" t="s">
         <v>693</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="L34" s="4" t="s">
         <v>12</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>220</v>
+        <v>699</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="138" x14ac:dyDescent="0.3">
@@ -11724,31 +11833,31 @@
         <v>195</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>120</v>
+        <v>213</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F35" s="16" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G35" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>652</v>
+        <v>700</v>
       </c>
       <c r="J35" s="14" t="s">
-        <v>211</v>
+        <v>693</v>
       </c>
       <c r="K35" s="4" t="s">
         <v>15</v>
@@ -11756,43 +11865,49 @@
       <c r="L35" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" ht="125.5" x14ac:dyDescent="0.3">
+      <c r="M35" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="75.5" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
         <v>195</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>196</v>
+        <v>117</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="F36" s="16" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="G36" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="J36" s="14" t="s">
         <v>693</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="L36" s="4" t="s">
         <v>12</v>
+      </c>
+      <c r="M36" s="3" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="138" x14ac:dyDescent="0.3">
@@ -11800,28 +11915,28 @@
         <v>195</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="F37" s="16" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G37" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H37" s="15" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="J37" s="14" t="s">
         <v>211</v>
@@ -11833,74 +11948,74 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="100.5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" ht="125.5" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
         <v>195</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>136</v>
+        <v>196</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="F38" s="16" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="G38" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="J38" s="14" t="s">
         <v>693</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="L38" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="113" x14ac:dyDescent="0.3">
-      <c r="A39" s="12" t="s">
+    <row r="39" spans="1:13" ht="138" x14ac:dyDescent="0.3">
+      <c r="A39" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="B39" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="E39" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="F39" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G39" s="14" t="s">
+      <c r="B39" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="E39" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="F39" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="G39" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>704</v>
+        <v>654</v>
       </c>
       <c r="J39" s="14" t="s">
-        <v>693</v>
+        <v>211</v>
       </c>
       <c r="K39" s="4" t="s">
         <v>15</v>
@@ -11908,119 +12023,116 @@
       <c r="L39" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M39" s="3" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" ht="125.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:13" ht="100.5" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
         <v>195</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>180</v>
+        <v>138</v>
       </c>
       <c r="G40" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H40" s="15" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="J40" s="14" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" ht="138" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="113" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
         <v>195</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>149</v>
+        <v>196</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="G41" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="J41" s="14" t="s">
         <v>693</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="138" x14ac:dyDescent="0.3">
-      <c r="A42" s="12" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="125.5" x14ac:dyDescent="0.3">
+      <c r="A42" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="B42" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="C42" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="E42" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="F42" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="G42" s="14" t="s">
+      <c r="B42" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="F42" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="G42" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H42" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="J42" s="14" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>3</v>
@@ -12028,37 +12140,34 @@
       <c r="L42" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M42" s="3" t="s">
-        <v>699</v>
-      </c>
     </row>
     <row r="43" spans="1:13" ht="138" x14ac:dyDescent="0.3">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="B43" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="C43" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="D43" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="E43" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="F43" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="G43" s="16" t="s">
+      <c r="B43" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="G43" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H43" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="J43" s="14" t="s">
         <v>693</v>
@@ -12069,37 +12178,40 @@
       <c r="L43" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" ht="125.5" x14ac:dyDescent="0.3">
-      <c r="A44" s="13" t="s">
+      <c r="M43" s="3" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="138" x14ac:dyDescent="0.3">
+      <c r="A44" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="B44" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="C44" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="D44" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="E44" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="F44" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="G44" s="16" t="s">
+      <c r="B44" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="G44" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H44" s="15" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>667</v>
+        <v>708</v>
       </c>
       <c r="J44" s="14" t="s">
-        <v>211</v>
+        <v>693</v>
       </c>
       <c r="K44" s="4" t="s">
         <v>3</v>
@@ -12108,7 +12220,7 @@
         <v>7</v>
       </c>
       <c r="M44" s="3" t="s">
-        <v>216</v>
+        <v>699</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="138" x14ac:dyDescent="0.3">
@@ -12116,28 +12228,28 @@
         <v>195</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="F45" s="16" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="G45" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H45" s="15" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="J45" s="14" t="s">
         <v>693</v>
@@ -12154,28 +12266,28 @@
         <v>195</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>196</v>
+        <v>159</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="F46" s="16" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="G46" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H46" s="15" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>661</v>
+        <v>667</v>
       </c>
       <c r="J46" s="14" t="s">
         <v>211</v>
@@ -12185,6 +12297,9 @@
       </c>
       <c r="L46" s="4" t="s">
         <v>7</v>
+      </c>
+      <c r="M46" s="3" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="138" x14ac:dyDescent="0.3">
@@ -12192,28 +12307,28 @@
         <v>195</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="E47" s="16" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="F47" s="16" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="G47" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H47" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="J47" s="14" t="s">
         <v>693</v>
@@ -12225,87 +12340,153 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="J48" s="11"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
-    </row>
-    <row r="49" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J49" s="11"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
-    </row>
-    <row r="50" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" ht="125.5" x14ac:dyDescent="0.3">
+      <c r="A48" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="F48" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="G48" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="H48" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="J48" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="K48" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L48" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="138" x14ac:dyDescent="0.3">
+      <c r="A49" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="C49" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="E49" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="F49" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="G49" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="H49" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="J49" s="14" t="s">
+        <v>693</v>
+      </c>
+      <c r="K49" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L49" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J50" s="11"/>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
     </row>
-    <row r="51" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J51" s="11"/>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
     </row>
-    <row r="52" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J52" s="11"/>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
     </row>
-    <row r="53" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J53" s="11"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
     </row>
-    <row r="54" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J54" s="11"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
     </row>
-    <row r="55" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J55" s="11"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
     </row>
-    <row r="56" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J56" s="11"/>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
     </row>
-    <row r="57" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J57" s="11"/>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
     </row>
-    <row r="58" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J58" s="11"/>
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
     </row>
-    <row r="59" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J59" s="11"/>
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
     </row>
-    <row r="60" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J60" s="11"/>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
     </row>
-    <row r="61" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J61" s="11"/>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
     </row>
-    <row r="62" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J62" s="11"/>
       <c r="K62" s="4"/>
       <c r="L62" s="4"/>
     </row>
-    <row r="63" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J63" s="11"/>
       <c r="K63" s="4"/>
       <c r="L63" s="4"/>
     </row>
-    <row r="64" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J64" s="11"/>
       <c r="K64" s="4"/>
       <c r="L64" s="4"/>
@@ -16894,6 +17075,16 @@
       <c r="J981" s="11"/>
       <c r="K981" s="4"/>
       <c r="L981" s="4"/>
+    </row>
+    <row r="982" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J982" s="11"/>
+      <c r="K982" s="4"/>
+      <c r="L982" s="4"/>
+    </row>
+    <row r="983" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J983" s="11"/>
+      <c r="K983" s="4"/>
+      <c r="L983" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16902,10 +17093,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M972"/>
+  <dimension ref="A1:M974"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -17819,115 +18010,105 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="138" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
         <v>195</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>111</v>
+        <v>538</v>
+      </c>
+      <c r="C25" t="s">
+        <v>764</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>112</v>
+        <v>183</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>113</v>
+        <v>765</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>114</v>
+        <v>255</v>
       </c>
       <c r="G25" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>197</v>
+        <v>766</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>666</v>
-      </c>
-      <c r="J25" s="14" t="s">
-        <v>211</v>
-      </c>
+        <v>771</v>
+      </c>
+      <c r="J25" s="14"/>
       <c r="K25" s="4" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="M25" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="138" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
         <v>195</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>111</v>
+        <v>543</v>
+      </c>
+      <c r="C26" t="s">
+        <v>767</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>112</v>
+        <v>183</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>113</v>
+        <v>768</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>114</v>
+        <v>255</v>
       </c>
       <c r="G26" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>197</v>
+        <v>769</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>649</v>
-      </c>
-      <c r="J26" s="14" t="s">
-        <v>211</v>
-      </c>
+        <v>770</v>
+      </c>
+      <c r="J26" s="14"/>
       <c r="K26" s="4" t="s">
         <v>15</v>
       </c>
       <c r="L26" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M26" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="138.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="13" t="s">
+    </row>
+    <row r="27" spans="1:13" ht="138" x14ac:dyDescent="0.3">
+      <c r="A27" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="B27" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="D27" s="20" t="s">
-        <v>251</v>
-      </c>
-      <c r="E27" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="F27" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="G27" s="16" t="s">
+      <c r="B27" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="G27" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>652</v>
+        <v>666</v>
       </c>
       <c r="J27" s="14" t="s">
         <v>211</v>
@@ -17938,34 +18119,37 @@
       <c r="L27" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" ht="125.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="13" t="s">
+      <c r="M27" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="138" x14ac:dyDescent="0.3">
+      <c r="A28" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="B28" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="F28" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="G28" s="16" t="s">
+      <c r="B28" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="G28" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="J28" s="14" t="s">
         <v>211</v>
@@ -17975,6 +18159,9 @@
       </c>
       <c r="L28" s="4" t="s">
         <v>12</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="138.5" x14ac:dyDescent="0.35">
@@ -17982,28 +18169,28 @@
         <v>195</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>130</v>
+        <v>120</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>121</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>252</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="F29" s="16" t="s">
-        <v>133</v>
+        <v>251</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="F29" s="20" t="s">
+        <v>124</v>
       </c>
       <c r="G29" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H29" s="15" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="J29" s="14" t="s">
         <v>211</v>
@@ -18015,192 +18202,189 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="100.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" ht="125.5" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
         <v>195</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>136</v>
+        <v>196</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="G30" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="J30" s="14" t="s">
         <v>211</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="L30" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="101" x14ac:dyDescent="0.35">
-      <c r="A31" s="12" t="s">
+    <row r="31" spans="1:13" ht="138.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="B31" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>253</v>
+      <c r="B31" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="E31" s="20" t="s">
-        <v>254</v>
-      </c>
-      <c r="F31" s="18" t="s">
-        <v>255</v>
-      </c>
-      <c r="G31" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="G31" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>672</v>
-      </c>
-      <c r="J31" s="14"/>
+        <v>654</v>
+      </c>
+      <c r="J31" s="14" t="s">
+        <v>211</v>
+      </c>
       <c r="K31" s="4" t="s">
         <v>15</v>
       </c>
       <c r="L31" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M31" s="3" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="125.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:13" ht="100.5" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
         <v>195</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>180</v>
+        <v>138</v>
       </c>
       <c r="G32" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="J32" s="14" t="s">
-        <v>2</v>
+        <v>211</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="138" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="101" x14ac:dyDescent="0.35">
       <c r="A33" s="12" t="s">
         <v>195</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>151</v>
+        <v>139</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>255</v>
       </c>
       <c r="G33" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>658</v>
-      </c>
-      <c r="J33" s="14" t="s">
-        <v>211</v>
-      </c>
+        <v>672</v>
+      </c>
+      <c r="J33" s="14"/>
       <c r="K33" s="4" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="138" x14ac:dyDescent="0.3">
-      <c r="A34" s="12" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="125.5" x14ac:dyDescent="0.3">
+      <c r="A34" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="B34" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="G34" s="14" t="s">
+      <c r="B34" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="G34" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>586</v>
+        <v>657</v>
       </c>
       <c r="J34" s="14" t="s">
-        <v>211</v>
+        <v>2</v>
       </c>
       <c r="K34" s="4" t="s">
         <v>3</v>
@@ -18208,37 +18392,34 @@
       <c r="L34" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M34" s="3" t="s">
-        <v>219</v>
-      </c>
     </row>
     <row r="35" spans="1:13" ht="138" x14ac:dyDescent="0.3">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="B35" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="F35" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="G35" s="16" t="s">
+      <c r="B35" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="G35" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="J35" s="14" t="s">
         <v>211</v>
@@ -18249,34 +18430,37 @@
       <c r="L35" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" ht="126" x14ac:dyDescent="0.35">
-      <c r="A36" s="13" t="s">
+      <c r="M35" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="138" x14ac:dyDescent="0.3">
+      <c r="A36" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="B36" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>256</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="F36" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="G36" s="16" t="s">
+      <c r="B36" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="G36" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>667</v>
+        <v>586</v>
       </c>
       <c r="J36" s="14" t="s">
         <v>211</v>
@@ -18288,7 +18472,7 @@
         <v>7</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>257</v>
+        <v>219</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="138" x14ac:dyDescent="0.3">
@@ -18296,28 +18480,28 @@
         <v>195</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="F37" s="16" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="G37" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H37" s="15" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="J37" s="14" t="s">
         <v>211</v>
@@ -18334,28 +18518,28 @@
         <v>195</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="C38" s="20" t="s">
-        <v>168</v>
+        <v>157</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>158</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>258</v>
-      </c>
-      <c r="E38" s="18" t="s">
-        <v>259</v>
-      </c>
-      <c r="F38" s="20" t="s">
-        <v>170</v>
+        <v>256</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>161</v>
       </c>
       <c r="G38" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>673</v>
+        <v>667</v>
       </c>
       <c r="J38" s="14" t="s">
         <v>211</v>
@@ -18370,15 +18554,84 @@
         <v>257</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="J39" s="11"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="J40" s="11"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
+    <row r="39" spans="1:13" ht="138" x14ac:dyDescent="0.3">
+      <c r="A39" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="E39" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="F39" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="G39" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="H39" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="J39" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L39" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="126" x14ac:dyDescent="0.35">
+      <c r="A40" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>258</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="G40" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="H40" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="J40" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L40" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M40" s="3" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J41" s="11"/>
@@ -23040,8 +23293,18 @@
       <c r="K972" s="4"/>
       <c r="L972" s="4"/>
     </row>
+    <row r="973" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J973" s="11"/>
+      <c r="K973" s="4"/>
+      <c r="L973" s="4"/>
+    </row>
+    <row r="974" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J974" s="11"/>
+      <c r="K974" s="4"/>
+      <c r="L974" s="4"/>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:B972" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="B1:B974" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -23049,10 +23312,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E42768F3-2D0D-4ACC-A88F-D1070A9BA453}">
-  <dimension ref="A1:M978"/>
+  <dimension ref="A1:M980"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -24212,118 +24475,108 @@
         <v>747</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="138" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
         <v>195</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>111</v>
+        <v>538</v>
+      </c>
+      <c r="C31" t="s">
+        <v>764</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>112</v>
+        <v>183</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>113</v>
+        <v>765</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>114</v>
+        <v>255</v>
       </c>
       <c r="G31" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>197</v>
+        <v>766</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>697</v>
-      </c>
-      <c r="J31" s="14" t="s">
-        <v>693</v>
-      </c>
+        <v>771</v>
+      </c>
+      <c r="J31" s="14"/>
       <c r="K31" s="4" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="M31" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="138" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="113.5" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
         <v>195</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>111</v>
+        <v>543</v>
+      </c>
+      <c r="C32" t="s">
+        <v>767</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>112</v>
+        <v>183</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>113</v>
+        <v>768</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>114</v>
+        <v>255</v>
       </c>
       <c r="G32" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>197</v>
+        <v>769</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>714</v>
-      </c>
-      <c r="J32" s="14" t="s">
-        <v>693</v>
-      </c>
+        <v>770</v>
+      </c>
+      <c r="J32" s="14"/>
       <c r="K32" s="4" t="s">
         <v>15</v>
       </c>
       <c r="L32" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M32" s="3" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="138.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="13" t="s">
+    </row>
+    <row r="33" spans="1:13" ht="138" x14ac:dyDescent="0.3">
+      <c r="A33" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="B33" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="C33" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>251</v>
-      </c>
-      <c r="E33" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="F33" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="G33" s="16" t="s">
+      <c r="B33" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="G33" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>652</v>
+        <v>697</v>
       </c>
       <c r="J33" s="14" t="s">
-        <v>211</v>
+        <v>693</v>
       </c>
       <c r="K33" s="4" t="s">
         <v>15</v>
@@ -24331,34 +24584,37 @@
       <c r="L33" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" ht="125.5" x14ac:dyDescent="0.3">
-      <c r="A34" s="13" t="s">
+      <c r="M33" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="138" x14ac:dyDescent="0.3">
+      <c r="A34" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="B34" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="F34" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="G34" s="16" t="s">
+      <c r="B34" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="G34" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>702</v>
+        <v>714</v>
       </c>
       <c r="J34" s="14" t="s">
         <v>693</v>
@@ -24368,6 +24624,9 @@
       </c>
       <c r="L34" s="4" t="s">
         <v>12</v>
+      </c>
+      <c r="M34" s="3" t="s">
+        <v>699</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="138.5" x14ac:dyDescent="0.35">
@@ -24375,28 +24634,28 @@
         <v>195</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>130</v>
+        <v>120</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>121</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>252</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="F35" s="16" t="s">
-        <v>133</v>
+        <v>251</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="F35" s="20" t="s">
+        <v>124</v>
       </c>
       <c r="G35" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="J35" s="14" t="s">
         <v>211</v>
@@ -24408,192 +24667,189 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="100.5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" ht="125.5" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
         <v>195</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>136</v>
+        <v>196</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="F36" s="16" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="G36" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="J36" s="14" t="s">
         <v>693</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="L36" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="101" x14ac:dyDescent="0.35">
-      <c r="A37" s="12" t="s">
+    <row r="37" spans="1:13" ht="138.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="B37" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C37" s="20" t="s">
-        <v>253</v>
+      <c r="B37" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="E37" s="20" t="s">
-        <v>254</v>
-      </c>
-      <c r="F37" s="18" t="s">
-        <v>255</v>
-      </c>
-      <c r="G37" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="G37" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H37" s="15" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>672</v>
-      </c>
-      <c r="J37" s="14"/>
+        <v>654</v>
+      </c>
+      <c r="J37" s="14" t="s">
+        <v>211</v>
+      </c>
       <c r="K37" s="4" t="s">
         <v>15</v>
       </c>
       <c r="L37" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M37" s="3" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="125.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:13" ht="100.5" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
         <v>195</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F38" s="16" t="s">
-        <v>180</v>
+        <v>138</v>
       </c>
       <c r="G38" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="J38" s="14" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="138" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="101" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
         <v>195</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="E39" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="F39" s="14" t="s">
-        <v>151</v>
+        <v>139</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>255</v>
       </c>
       <c r="G39" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>706</v>
-      </c>
-      <c r="J39" s="14" t="s">
-        <v>693</v>
-      </c>
+        <v>672</v>
+      </c>
+      <c r="J39" s="14"/>
       <c r="K39" s="4" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" ht="138" x14ac:dyDescent="0.3">
-      <c r="A40" s="12" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="125.5" x14ac:dyDescent="0.3">
+      <c r="A40" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="B40" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="E40" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="F40" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="G40" s="14" t="s">
+      <c r="B40" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="E40" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="F40" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="G40" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H40" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="J40" s="14" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
       <c r="K40" s="4" t="s">
         <v>3</v>
@@ -24601,37 +24857,34 @@
       <c r="L40" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M40" s="3" t="s">
-        <v>699</v>
-      </c>
     </row>
     <row r="41" spans="1:13" ht="138" x14ac:dyDescent="0.3">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="B41" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="D41" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="E41" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="F41" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="G41" s="16" t="s">
+      <c r="B41" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="G41" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="J41" s="14" t="s">
         <v>693</v>
@@ -24642,37 +24895,40 @@
       <c r="L41" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" ht="126" x14ac:dyDescent="0.35">
-      <c r="A42" s="13" t="s">
+      <c r="M41" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="138" x14ac:dyDescent="0.3">
+      <c r="A42" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="B42" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="C42" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="D42" s="20" t="s">
-        <v>256</v>
-      </c>
-      <c r="E42" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="F42" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="G42" s="16" t="s">
+      <c r="B42" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="G42" s="14" t="s">
         <v>181</v>
       </c>
       <c r="H42" s="15" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>667</v>
+        <v>708</v>
       </c>
       <c r="J42" s="14" t="s">
-        <v>211</v>
+        <v>693</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>3</v>
@@ -24681,7 +24937,7 @@
         <v>7</v>
       </c>
       <c r="M42" s="3" t="s">
-        <v>257</v>
+        <v>699</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="138" x14ac:dyDescent="0.3">
@@ -24689,28 +24945,28 @@
         <v>195</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="F43" s="16" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="G43" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H43" s="15" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="J43" s="14" t="s">
         <v>693</v>
@@ -24727,28 +24983,28 @@
         <v>195</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="C44" s="20" t="s">
-        <v>168</v>
+        <v>157</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>158</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>258</v>
-      </c>
-      <c r="E44" s="18" t="s">
-        <v>259</v>
-      </c>
-      <c r="F44" s="20" t="s">
-        <v>170</v>
+        <v>256</v>
+      </c>
+      <c r="E44" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="F44" s="16" t="s">
+        <v>161</v>
       </c>
       <c r="G44" s="16" t="s">
         <v>181</v>
       </c>
       <c r="H44" s="15" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>673</v>
+        <v>667</v>
       </c>
       <c r="J44" s="14" t="s">
         <v>211</v>
@@ -24763,15 +25019,84 @@
         <v>257</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="J45" s="11"/>
-      <c r="K45" s="4"/>
-      <c r="L45" s="4"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="J46" s="11"/>
-      <c r="K46" s="4"/>
-      <c r="L46" s="4"/>
+    <row r="45" spans="1:13" ht="138" x14ac:dyDescent="0.3">
+      <c r="A45" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="F45" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="G45" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="H45" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="J45" s="14" t="s">
+        <v>693</v>
+      </c>
+      <c r="K45" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L45" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="126" x14ac:dyDescent="0.35">
+      <c r="A46" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>258</v>
+      </c>
+      <c r="E46" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="F46" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="G46" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="H46" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="J46" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="K46" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L46" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M46" s="3" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J47" s="11"/>
@@ -29432,6 +29757,16 @@
       <c r="J978" s="11"/>
       <c r="K978" s="4"/>
       <c r="L978" s="4"/>
+    </row>
+    <row r="979" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J979" s="11"/>
+      <c r="K979" s="4"/>
+      <c r="L979" s="4"/>
+    </row>
+    <row r="980" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J980" s="11"/>
+      <c r="K980" s="4"/>
+      <c r="L980" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -29442,8 +29777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O998"/>
   <sheetViews>
-    <sheetView topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -36566,7 +36901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03D8D31F-DB06-4E94-9371-46539D804E26}">
   <dimension ref="A1:O1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D47" workbookViewId="0">
+    <sheetView topLeftCell="D47" workbookViewId="0">
       <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>

</xml_diff>